<commit_message>
003 Week 3 data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>WINTER BEST PAIRS COMP(SUNDAY)</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>PAUL DIXON</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>TONI SHIRLEY</t>
@@ -688,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -747,6 +744,9 @@
     <xf borderId="20" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="20" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="21" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -763,6 +763,9 @@
     <xf borderId="25" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="26" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="26" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -1477,7 +1480,9 @@
         <v>31.0</v>
       </c>
       <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="F12" s="30">
+        <v>31.0</v>
+      </c>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
@@ -1497,53 +1502,55 @@
       <c r="W12" s="29"/>
       <c r="X12" s="29"/>
       <c r="Y12" s="29"/>
-      <c r="Z12" s="30"/>
-      <c r="AA12" s="30"/>
-      <c r="AB12" s="31">
+      <c r="Z12" s="31"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="32">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>31</v>
-      </c>
-      <c r="AC12" s="32">
+        <v>62</v>
+      </c>
+      <c r="AC12" s="33">
         <f>SUM(AB12:AB13)</f>
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="AD12" s="5"/>
     </row>
     <row r="13">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="36">
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37">
         <v>32.0</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="36"/>
-      <c r="X13" s="36"/>
-      <c r="Y13" s="36"/>
-      <c r="Z13" s="37"/>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="31">
+      <c r="E13" s="37"/>
+      <c r="F13" s="38">
+        <v>35.0</v>
+      </c>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="37"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="39"/>
+      <c r="AB13" s="32">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -1578,51 +1585,51 @@
       <c r="W14" s="29"/>
       <c r="X14" s="29"/>
       <c r="Y14" s="29"/>
-      <c r="Z14" s="30"/>
-      <c r="AA14" s="30"/>
-      <c r="AB14" s="31">
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="32">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AC14" s="32">
+      <c r="AC14" s="33">
         <f>SUM(AB14:AB15)</f>
         <v>61</v>
       </c>
       <c r="AD14" s="5"/>
     </row>
     <row r="15">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36">
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37">
         <v>37.0</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="36"/>
-      <c r="Y15" s="36"/>
-      <c r="Z15" s="37"/>
-      <c r="AA15" s="37"/>
-      <c r="AB15" s="31">
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
+      <c r="Z15" s="39"/>
+      <c r="AA15" s="39"/>
+      <c r="AB15" s="32">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
@@ -1639,7 +1646,9 @@
         <v>31.0</v>
       </c>
       <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="F16" s="30">
+        <v>42.0</v>
+      </c>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
@@ -1659,53 +1668,55 @@
       <c r="W16" s="29"/>
       <c r="X16" s="29"/>
       <c r="Y16" s="29"/>
-      <c r="Z16" s="30"/>
-      <c r="AA16" s="30"/>
-      <c r="AB16" s="31">
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="31"/>
+      <c r="AB16" s="32">
         <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="AC16" s="32">
+        <v>73</v>
+      </c>
+      <c r="AC16" s="33">
         <f>SUM(AB16:AB17)</f>
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="AD16" s="5"/>
     </row>
     <row r="17">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="36">
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37">
         <v>31.0</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
-      <c r="X17" s="36"/>
-      <c r="Y17" s="36"/>
-      <c r="Z17" s="37"/>
-      <c r="AA17" s="37"/>
-      <c r="AB17" s="31">
+      <c r="E17" s="37"/>
+      <c r="F17" s="38">
+        <v>32.0</v>
+      </c>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="37"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="37"/>
+      <c r="Z17" s="39"/>
+      <c r="AA17" s="39"/>
+      <c r="AB17" s="32">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
@@ -1716,11 +1727,11 @@
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="28"/>
-      <c r="D18" s="29" t="s">
-        <v>36</v>
-      </c>
+      <c r="D18" s="29"/>
       <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
+      <c r="F18" s="30">
+        <v>33.0</v>
+      </c>
       <c r="G18" s="29"/>
       <c r="H18" s="29"/>
       <c r="I18" s="29"/>
@@ -1740,51 +1751,51 @@
       <c r="W18" s="29"/>
       <c r="X18" s="29"/>
       <c r="Y18" s="29"/>
-      <c r="Z18" s="30"/>
-      <c r="AA18" s="30"/>
-      <c r="AB18" s="31">
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC18" s="32">
+        <v>33</v>
+      </c>
+      <c r="AC18" s="33">
         <f>SUM(AB18:AB19)</f>
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="AD18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="36">
+      <c r="A19" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37">
         <v>28.0</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="36"/>
-      <c r="U19" s="36"/>
-      <c r="V19" s="36"/>
-      <c r="W19" s="36"/>
-      <c r="X19" s="36"/>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="37"/>
-      <c r="AA19" s="37"/>
-      <c r="AB19" s="31">
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="37"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="37"/>
+      <c r="Z19" s="39"/>
+      <c r="AA19" s="39"/>
+      <c r="AB19" s="32">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
@@ -1793,15 +1804,17 @@
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="27"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="30">
+        <v>32.0</v>
+      </c>
+      <c r="F20" s="30">
+        <v>33.0</v>
+      </c>
       <c r="G20" s="29"/>
       <c r="H20" s="29"/>
       <c r="I20" s="29"/>
@@ -1821,62 +1834,66 @@
       <c r="W20" s="29"/>
       <c r="X20" s="29"/>
       <c r="Y20" s="29"/>
-      <c r="Z20" s="30"/>
-      <c r="AA20" s="30"/>
-      <c r="AB20" s="31">
+      <c r="Z20" s="31"/>
+      <c r="AA20" s="31"/>
+      <c r="AB20" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC20" s="32">
+        <v>65</v>
+      </c>
+      <c r="AC20" s="33">
         <f>SUM(AB20:AB21)</f>
-        <v>36</v>
+        <v>173</v>
       </c>
       <c r="AD20" s="5"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="41">
+      <c r="A21" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43">
         <v>36.0</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="37"/>
-      <c r="AA21" s="37"/>
-      <c r="AB21" s="31">
+      <c r="E21" s="38">
+        <v>39.0</v>
+      </c>
+      <c r="F21" s="38">
+        <v>33.0</v>
+      </c>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="37"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="37"/>
+      <c r="Z21" s="39"/>
+      <c r="AA21" s="39"/>
+      <c r="AB21" s="32">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="43"/>
+      <c r="A22" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="45"/>
       <c r="C22" s="19"/>
       <c r="D22" s="29">
         <v>33.0</v>
@@ -1902,68 +1919,70 @@
       <c r="W22" s="29"/>
       <c r="X22" s="29"/>
       <c r="Y22" s="29"/>
-      <c r="Z22" s="30"/>
-      <c r="AA22" s="30"/>
-      <c r="AB22" s="31">
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="32">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="AC22" s="32">
+      <c r="AC22" s="33">
         <f>SUM(AB22:AB23)</f>
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="AD22" s="5"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="44" t="s">
-        <v>41</v>
+      <c r="A23" s="46" t="s">
+        <v>40</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="36">
+      <c r="C23" s="47"/>
+      <c r="D23" s="37">
         <v>25.0</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="36"/>
-      <c r="W23" s="36"/>
-      <c r="X23" s="36"/>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="37"/>
-      <c r="AA23" s="37"/>
-      <c r="AB23" s="31">
+      <c r="E23" s="37"/>
+      <c r="F23" s="38">
+        <v>30.0</v>
+      </c>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="37"/>
+      <c r="W23" s="37"/>
+      <c r="X23" s="37"/>
+      <c r="Y23" s="37"/>
+      <c r="Z23" s="39"/>
+      <c r="AA23" s="39"/>
+      <c r="AB23" s="32">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="AC23" s="6"/>
       <c r="AD23" s="8"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
-      <c r="D24" s="29" t="s">
-        <v>36</v>
-      </c>
+      <c r="D24" s="29"/>
       <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
+      <c r="F24" s="30">
+        <v>33.0</v>
+      </c>
       <c r="G24" s="29"/>
       <c r="H24" s="29"/>
       <c r="I24" s="29"/>
@@ -1983,60 +2002,62 @@
       <c r="W24" s="29"/>
       <c r="X24" s="29"/>
       <c r="Y24" s="29"/>
-      <c r="Z24" s="30"/>
-      <c r="AA24" s="30"/>
-      <c r="AB24" s="31">
+      <c r="Z24" s="31"/>
+      <c r="AA24" s="31"/>
+      <c r="AB24" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC24" s="32">
+        <v>33</v>
+      </c>
+      <c r="AC24" s="33">
         <f>SUM(AB24:AB25)</f>
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="AD24" s="5"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="36">
+      <c r="A25" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="35"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="37">
         <v>36.0</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="36"/>
-      <c r="U25" s="36"/>
-      <c r="V25" s="36"/>
-      <c r="W25" s="36"/>
-      <c r="X25" s="36"/>
-      <c r="Y25" s="36"/>
-      <c r="Z25" s="37"/>
-      <c r="AA25" s="37"/>
-      <c r="AB25" s="31">
+      <c r="E25" s="37"/>
+      <c r="F25" s="38">
+        <v>33.0</v>
+      </c>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="Y25" s="37"/>
+      <c r="Z25" s="39"/>
+      <c r="AA25" s="39"/>
+      <c r="AB25" s="32">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -2044,7 +2065,9 @@
         <v>35.0</v>
       </c>
       <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="F26" s="30">
+        <v>36.0</v>
+      </c>
       <c r="G26" s="29"/>
       <c r="H26" s="29"/>
       <c r="I26" s="29"/>
@@ -2064,68 +2087,74 @@
       <c r="W26" s="29"/>
       <c r="X26" s="29"/>
       <c r="Y26" s="29"/>
-      <c r="Z26" s="30"/>
-      <c r="AA26" s="30"/>
-      <c r="AB26" s="31">
+      <c r="Z26" s="31"/>
+      <c r="AA26" s="31"/>
+      <c r="AB26" s="32">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="AC26" s="32">
+        <v>71</v>
+      </c>
+      <c r="AC26" s="33">
         <f>SUM(AB26:AB27)</f>
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="AD26" s="5"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="36">
+      <c r="A27" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="35"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37">
         <v>42.0</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="36"/>
-      <c r="R27" s="36"/>
-      <c r="S27" s="36"/>
-      <c r="T27" s="36"/>
-      <c r="U27" s="36"/>
-      <c r="V27" s="36"/>
-      <c r="W27" s="36"/>
-      <c r="X27" s="36"/>
-      <c r="Y27" s="36"/>
-      <c r="Z27" s="37"/>
-      <c r="AA27" s="37"/>
-      <c r="AB27" s="31">
+      <c r="E27" s="37"/>
+      <c r="F27" s="38">
+        <v>29.0</v>
+      </c>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="37"/>
+      <c r="W27" s="37"/>
+      <c r="X27" s="37"/>
+      <c r="Y27" s="37"/>
+      <c r="Z27" s="39"/>
+      <c r="AA27" s="39"/>
+      <c r="AB27" s="32">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="27"/>
       <c r="C28" s="28"/>
       <c r="D28" s="29">
         <v>29.0</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="E28" s="30">
+        <v>31.0</v>
+      </c>
+      <c r="F28" s="30">
+        <v>33.0</v>
+      </c>
       <c r="G28" s="29"/>
       <c r="H28" s="29"/>
       <c r="I28" s="29"/>
@@ -2145,68 +2174,72 @@
       <c r="W28" s="29"/>
       <c r="X28" s="29"/>
       <c r="Y28" s="29"/>
-      <c r="Z28" s="30"/>
-      <c r="AA28" s="30"/>
-      <c r="AB28" s="31">
+      <c r="Z28" s="31"/>
+      <c r="AA28" s="31"/>
+      <c r="AB28" s="32">
         <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="AC28" s="32">
+        <v>93</v>
+      </c>
+      <c r="AC28" s="33">
         <f>SUM(AB28:AB29)</f>
-        <v>53</v>
+        <v>179</v>
       </c>
       <c r="AD28" s="5"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36">
+      <c r="A29" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37">
         <v>24.0</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="36"/>
-      <c r="O29" s="36"/>
-      <c r="P29" s="36"/>
-      <c r="Q29" s="36"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="36"/>
-      <c r="T29" s="36"/>
-      <c r="U29" s="36"/>
-      <c r="V29" s="36"/>
-      <c r="W29" s="36"/>
-      <c r="X29" s="36"/>
-      <c r="Y29" s="36"/>
-      <c r="Z29" s="37"/>
-      <c r="AA29" s="37"/>
-      <c r="AB29" s="31">
+      <c r="E29" s="38">
+        <v>30.0</v>
+      </c>
+      <c r="F29" s="38">
+        <v>32.0</v>
+      </c>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="37"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="37"/>
+      <c r="X29" s="37"/>
+      <c r="Y29" s="37"/>
+      <c r="Z29" s="39"/>
+      <c r="AA29" s="39"/>
+      <c r="AB29" s="32">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="27"/>
       <c r="C30" s="28"/>
-      <c r="D30" s="29" t="s">
-        <v>36</v>
-      </c>
+      <c r="D30" s="29"/>
       <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="F30" s="30">
+        <v>27.0</v>
+      </c>
       <c r="G30" s="29"/>
       <c r="H30" s="29"/>
       <c r="I30" s="29"/>
@@ -2226,59 +2259,61 @@
       <c r="W30" s="29"/>
       <c r="X30" s="29"/>
       <c r="Y30" s="29"/>
-      <c r="Z30" s="30"/>
-      <c r="AA30" s="30"/>
-      <c r="AB30" s="31">
+      <c r="Z30" s="31"/>
+      <c r="AA30" s="31"/>
+      <c r="AB30" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC30" s="32">
+        <v>27</v>
+      </c>
+      <c r="AC30" s="33">
         <f>SUM(AB30:AB31)</f>
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="AD30" s="5"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="36">
+      <c r="A31" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37">
         <v>33.0</v>
       </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="36"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="T31" s="36"/>
-      <c r="U31" s="36"/>
-      <c r="V31" s="36"/>
-      <c r="W31" s="36"/>
-      <c r="X31" s="36"/>
-      <c r="Y31" s="36"/>
-      <c r="Z31" s="46"/>
-      <c r="AA31" s="46"/>
-      <c r="AB31" s="47">
+      <c r="E31" s="37"/>
+      <c r="F31" s="38">
+        <v>34.0</v>
+      </c>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="37"/>
+      <c r="O31" s="37"/>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="37"/>
+      <c r="W31" s="37"/>
+      <c r="X31" s="37"/>
+      <c r="Y31" s="37"/>
+      <c r="Z31" s="48"/>
+      <c r="AA31" s="48"/>
+      <c r="AB31" s="49">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="48"/>
+      <c r="A32" s="50"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2308,27 +2343,27 @@
       <c r="AD32" s="1"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="52"/>
+      <c r="C33" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="52"/>
-      <c r="E33" s="50"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="52"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="L33" s="54"/>
-      <c r="M33" s="54"/>
-      <c r="N33" s="54"/>
-      <c r="O33" s="55"/>
+      <c r="K33" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="57"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -2346,9 +2381,9 @@
       <c r="AD33" s="1"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="48"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2378,16 +2413,16 @@
       <c r="AD34" s="1"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="48"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="58"/>
+      <c r="E35" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="60"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2395,84 +2430,84 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q35" s="57"/>
-      <c r="R35" s="57"/>
-      <c r="S35" s="58"/>
+      <c r="P35" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q35" s="59"/>
+      <c r="R35" s="59"/>
+      <c r="S35" s="60"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="59"/>
+      <c r="X35" s="61"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="48"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="60" t="s">
-        <v>55</v>
+      <c r="A36" s="50"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="62" t="s">
+        <v>54</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="61">
+      <c r="E36" s="63">
         <v>80.0</v>
       </c>
-      <c r="F36" s="52"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="62"/>
-      <c r="J36" s="62"/>
-      <c r="K36" s="62"/>
-      <c r="L36" s="62"/>
-      <c r="M36" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="O36" s="62"/>
-      <c r="P36" s="61">
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="64"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="O36" s="64"/>
+      <c r="P36" s="63">
         <v>50.0</v>
       </c>
-      <c r="Q36" s="52"/>
-      <c r="R36" s="52"/>
-      <c r="S36" s="50"/>
+      <c r="Q36" s="54"/>
+      <c r="R36" s="54"/>
+      <c r="S36" s="52"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="63"/>
+      <c r="X36" s="65"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="48"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="60" t="s">
-        <v>56</v>
+      <c r="A37" s="50"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="62" t="s">
+        <v>55</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="61">
+      <c r="E37" s="63">
         <v>50.0</v>
       </c>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="62"/>
-      <c r="K37" s="62"/>
-      <c r="L37" s="62"/>
-      <c r="M37" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="O37" s="62"/>
-      <c r="P37" s="61">
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="64"/>
+      <c r="J37" s="64"/>
+      <c r="K37" s="64"/>
+      <c r="L37" s="64"/>
+      <c r="M37" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="O37" s="64"/>
+      <c r="P37" s="63">
         <v>30.0</v>
       </c>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="52"/>
-      <c r="S37" s="50"/>
+      <c r="Q37" s="54"/>
+      <c r="R37" s="54"/>
+      <c r="S37" s="52"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -2486,18 +2521,18 @@
       <c r="AD37" s="1"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="48"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="60" t="s">
-        <v>57</v>
+      <c r="A38" s="50"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="62" t="s">
+        <v>56</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="61">
+      <c r="E38" s="63">
         <v>40.0</v>
       </c>
-      <c r="F38" s="52"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="50"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="52"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -2505,7 +2540,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="64"/>
+      <c r="P38" s="66"/>
       <c r="Q38" s="21"/>
       <c r="R38" s="21"/>
       <c r="S38" s="21"/>
@@ -2522,14 +2557,14 @@
       <c r="AD38" s="1"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="D39" s="65"/>
-      <c r="E39" s="64"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="66"/>
       <c r="F39" s="21"/>
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-      <c r="O39" s="65"/>
+      <c r="O39" s="67"/>
       <c r="S39" s="1"/>
       <c r="W39" s="1"/>
     </row>
@@ -3600,112 +3635,112 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="66" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="69" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="67" t="s">
+      <c r="B2" s="70">
+        <f>Sheet1!AC26</f>
+        <v>142</v>
+      </c>
+      <c r="C2" s="69"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="68">
-        <f>Sheet1!AC26</f>
-        <v>77</v>
-      </c>
-      <c r="C2" s="67"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="67" t="s">
+      <c r="B3" s="70">
+        <f>Sheet1!AC12</f>
+        <v>129</v>
+      </c>
+      <c r="C3" s="69"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="68">
-        <f>Sheet1!AC12</f>
-        <v>63</v>
-      </c>
-      <c r="C3" s="67"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="67" t="s">
+      <c r="B4" s="70">
+        <f>Sheet1!AC16</f>
+        <v>136</v>
+      </c>
+      <c r="C4" s="69"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="68">
-        <f>Sheet1!AC16</f>
-        <v>62</v>
-      </c>
-      <c r="C4" s="67"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="68">
+      <c r="B5" s="70">
         <f>Sheet1!AC14</f>
         <v>61</v>
       </c>
-      <c r="C5" s="67"/>
+      <c r="C5" s="69"/>
     </row>
     <row r="6">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="70">
+        <f>Sheet1!AC22</f>
+        <v>88</v>
+      </c>
+      <c r="C6" s="69"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="68">
-        <f>Sheet1!AC22</f>
-        <v>58</v>
-      </c>
-      <c r="C6" s="67"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="67" t="s">
+      <c r="B7" s="70">
+        <f>Sheet1!AC28</f>
+        <v>179</v>
+      </c>
+      <c r="C7" s="69"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="68">
-        <f>Sheet1!AC28</f>
-        <v>53</v>
-      </c>
-      <c r="C7" s="67"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="67" t="s">
+      <c r="B8" s="70">
+        <f>Sheet1!AC20</f>
+        <v>173</v>
+      </c>
+      <c r="C8" s="69"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="68">
-        <f>Sheet1!AC20</f>
-        <v>36</v>
-      </c>
-      <c r="C8" s="67"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="67" t="s">
+      <c r="B9" s="70">
+        <f>Sheet1!AC24</f>
+        <v>102</v>
+      </c>
+      <c r="C9" s="69"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="68">
-        <f>Sheet1!AC24</f>
-        <v>36</v>
-      </c>
-      <c r="C9" s="67"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="67" t="s">
+      <c r="B10" s="70">
+        <f>Sheet1!AC30</f>
+        <v>94</v>
+      </c>
+      <c r="C10" s="69"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="68">
-        <f>Sheet1!AC30</f>
-        <v>33</v>
-      </c>
-      <c r="C10" s="67"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="68">
+      <c r="B11" s="70">
         <f>Sheet1!AC18</f>
-        <v>28</v>
-      </c>
-      <c r="C11" s="67"/>
+        <v>61</v>
+      </c>
+      <c r="C11" s="69"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
004 Average Calc Fix
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="cwJIlWbq0KKQeybK1Bo/imG8HjW0sgm7bTMSj3Jld9w="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="emksQva/QHKVBg8Jg7dXnxTaw3GJ01mCWEWrwbnszq8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>WINTER BEST PAIRS COMP(SUNDAY)</t>
   </si>
@@ -106,6 +106,9 @@
     <t>SCORE</t>
   </si>
   <si>
+    <t>RNDS PLAYED</t>
+  </si>
+  <si>
     <t>BAZ MASON</t>
   </si>
   <si>
@@ -194,6 +197,9 @@
   </si>
   <si>
     <t>TEAM TOTAL</t>
+  </si>
+  <si>
+    <t>PLAYED</t>
   </si>
   <si>
     <t>MAL &amp; KEN</t>
@@ -685,7 +691,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -714,6 +720,9 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -736,6 +745,9 @@
     <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -756,6 +768,9 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="23" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -820,9 +835,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -1060,7 +1072,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="3" width="8.71"/>
-    <col customWidth="1" min="4" max="30" width="3.71"/>
+    <col customWidth="1" min="4" max="31" width="3.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1211,1109 +1223,1199 @@
         <v>2</v>
       </c>
       <c r="AD4" s="13"/>
+      <c r="AE4" s="14"/>
     </row>
     <row r="5">
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="16"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="14"/>
     </row>
     <row r="6">
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="16"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="14"/>
     </row>
     <row r="7">
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="15"/>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="16"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="14"/>
     </row>
     <row r="8">
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="15"/>
-      <c r="AC8" s="15"/>
-      <c r="AD8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="14"/>
     </row>
     <row r="9">
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="15"/>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="16"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="17"/>
+      <c r="AE9" s="14"/>
     </row>
     <row r="10">
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="17"/>
-      <c r="Y10" s="17"/>
-      <c r="Z10" s="17"/>
-      <c r="AA10" s="17"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="19"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="19"/>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="14"/>
     </row>
     <row r="11">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="22" t="s">
+      <c r="L11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="M11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="N11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="O11" s="22" t="s">
+      <c r="O11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="P11" s="22" t="s">
+      <c r="P11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="Q11" s="22" t="s">
+      <c r="Q11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="R11" s="22" t="s">
+      <c r="R11" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="S11" s="22" t="s">
+      <c r="S11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="T11" s="22" t="s">
+      <c r="T11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="U11" s="22" t="s">
+      <c r="U11" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="V11" s="22" t="s">
+      <c r="V11" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="W11" s="22" t="s">
+      <c r="W11" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="X11" s="22" t="s">
+      <c r="X11" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="Y11" s="22" t="s">
+      <c r="Y11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="Z11" s="23" t="s">
+      <c r="Z11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="AA11" s="23" t="s">
+      <c r="AA11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="AB11" s="24" t="s">
+      <c r="AB11" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="AC11" s="25"/>
+      <c r="AC11" s="26"/>
       <c r="AD11" s="13"/>
+      <c r="AE11" s="27" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29">
+      <c r="A12" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="31">
         <v>31.0</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30">
+      <c r="E12" s="31"/>
+      <c r="F12" s="32">
         <v>31.0</v>
       </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="31"/>
-      <c r="AA12" s="31"/>
-      <c r="AB12" s="32">
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="31"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="33"/>
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
         <v>62</v>
       </c>
-      <c r="AC12" s="33">
+      <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
         <v>129</v>
       </c>
       <c r="AD12" s="5"/>
+      <c r="AE12" s="36">
+        <f t="shared" ref="AE12:AE31" si="2">countif(D12:AA12,"&lt;&gt;"&amp;"")</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="37">
+      <c r="A13" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40">
         <v>32.0</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38">
+      <c r="E13" s="40"/>
+      <c r="F13" s="41">
         <v>35.0</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
-      <c r="V13" s="37"/>
-      <c r="W13" s="37"/>
-      <c r="X13" s="37"/>
-      <c r="Y13" s="37"/>
-      <c r="Z13" s="39"/>
-      <c r="AA13" s="39"/>
-      <c r="AB13" s="32">
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+      <c r="X13" s="40"/>
+      <c r="Y13" s="40"/>
+      <c r="Z13" s="42"/>
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="34">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
+      <c r="AE13" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29">
+      <c r="A14" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31">
         <v>24.0</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="U14" s="29"/>
-      <c r="V14" s="29"/>
-      <c r="W14" s="29"/>
-      <c r="X14" s="29"/>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="31"/>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="32">
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="33"/>
+      <c r="AA14" s="33"/>
+      <c r="AB14" s="34">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AC14" s="33">
+      <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
         <v>61</v>
       </c>
       <c r="AD14" s="5"/>
+      <c r="AE14" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="37">
+      <c r="A15" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40">
         <v>37.0</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="39"/>
-      <c r="AA15" s="39"/>
-      <c r="AB15" s="32">
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="40"/>
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="42"/>
+      <c r="AA15" s="42"/>
+      <c r="AB15" s="34">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
+      <c r="AE15" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29">
+      <c r="A16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="31">
         <v>31.0</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30">
+      <c r="E16" s="31"/>
+      <c r="F16" s="32">
         <v>42.0</v>
       </c>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="29"/>
-      <c r="T16" s="29"/>
-      <c r="U16" s="29"/>
-      <c r="V16" s="29"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="31"/>
-      <c r="AA16" s="31"/>
-      <c r="AB16" s="32">
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="33"/>
+      <c r="AA16" s="33"/>
+      <c r="AB16" s="34">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="AC16" s="33">
+      <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
         <v>136</v>
       </c>
       <c r="AD16" s="5"/>
+      <c r="AE16" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37">
+      <c r="A17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40">
         <v>31.0</v>
       </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38">
+      <c r="E17" s="40"/>
+      <c r="F17" s="41">
         <v>32.0</v>
       </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="37"/>
-      <c r="U17" s="37"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="37"/>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="37"/>
-      <c r="Z17" s="39"/>
-      <c r="AA17" s="39"/>
-      <c r="AB17" s="32">
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="40"/>
+      <c r="X17" s="40"/>
+      <c r="Y17" s="40"/>
+      <c r="Z17" s="42"/>
+      <c r="AA17" s="42"/>
+      <c r="AB17" s="34">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
+      <c r="AE17" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30">
+      <c r="A18" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32">
         <v>33.0</v>
       </c>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
-      <c r="W18" s="29"/>
-      <c r="X18" s="29"/>
-      <c r="Y18" s="29"/>
-      <c r="Z18" s="31"/>
-      <c r="AA18" s="31"/>
-      <c r="AB18" s="32">
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="33"/>
+      <c r="AA18" s="33"/>
+      <c r="AB18" s="34">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="AC18" s="33">
+      <c r="AC18" s="35">
         <f>SUM(AB18:AB19)</f>
         <v>61</v>
       </c>
       <c r="AD18" s="5"/>
+      <c r="AE18" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37">
+      <c r="A19" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40">
         <v>28.0</v>
       </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="37"/>
-      <c r="T19" s="37"/>
-      <c r="U19" s="37"/>
-      <c r="V19" s="37"/>
-      <c r="W19" s="37"/>
-      <c r="X19" s="37"/>
-      <c r="Y19" s="37"/>
-      <c r="Z19" s="39"/>
-      <c r="AA19" s="39"/>
-      <c r="AB19" s="32">
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="40"/>
+      <c r="W19" s="40"/>
+      <c r="X19" s="40"/>
+      <c r="Y19" s="40"/>
+      <c r="Z19" s="42"/>
+      <c r="AA19" s="42"/>
+      <c r="AB19" s="34">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="AC19" s="6"/>
       <c r="AD19" s="8"/>
+      <c r="AE19" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="30">
+      <c r="A20" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="32">
         <v>32.0</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="32">
         <v>33.0</v>
       </c>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
-      <c r="W20" s="29"/>
-      <c r="X20" s="29"/>
-      <c r="Y20" s="29"/>
-      <c r="Z20" s="31"/>
-      <c r="AA20" s="31"/>
-      <c r="AB20" s="32">
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
+      <c r="Z20" s="33"/>
+      <c r="AA20" s="33"/>
+      <c r="AB20" s="34">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="AC20" s="33">
+      <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
         <v>173</v>
       </c>
       <c r="AD20" s="5"/>
+      <c r="AE20" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="43">
+      <c r="A21" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="46">
         <v>36.0</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="41">
         <v>39.0</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="41">
         <v>33.0</v>
       </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="37"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="39"/>
-      <c r="AA21" s="39"/>
-      <c r="AB21" s="32">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="40"/>
+      <c r="W21" s="40"/>
+      <c r="X21" s="40"/>
+      <c r="Y21" s="40"/>
+      <c r="Z21" s="42"/>
+      <c r="AA21" s="42"/>
+      <c r="AB21" s="34">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
+      <c r="AE21" s="36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="29">
+      <c r="A22" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="48"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="31">
         <v>33.0</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29"/>
-      <c r="T22" s="29"/>
-      <c r="U22" s="29"/>
-      <c r="V22" s="29"/>
-      <c r="W22" s="29"/>
-      <c r="X22" s="29"/>
-      <c r="Y22" s="29"/>
-      <c r="Z22" s="31"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="32">
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="33"/>
+      <c r="AA22" s="33"/>
+      <c r="AB22" s="34">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="AC22" s="33">
+      <c r="AC22" s="35">
         <f>SUM(AB22:AB23)</f>
         <v>88</v>
       </c>
       <c r="AD22" s="5"/>
+      <c r="AE22" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="46" t="s">
-        <v>40</v>
+      <c r="A23" s="49" t="s">
+        <v>41</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="37">
+      <c r="C23" s="50"/>
+      <c r="D23" s="40">
         <v>25.0</v>
       </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="38">
+      <c r="E23" s="40"/>
+      <c r="F23" s="41">
         <v>30.0</v>
       </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="37"/>
-      <c r="T23" s="37"/>
-      <c r="U23" s="37"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="37"/>
-      <c r="Y23" s="37"/>
-      <c r="Z23" s="39"/>
-      <c r="AA23" s="39"/>
-      <c r="AB23" s="32">
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="40"/>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="40"/>
+      <c r="Z23" s="42"/>
+      <c r="AA23" s="42"/>
+      <c r="AB23" s="34">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="AC23" s="6"/>
       <c r="AD23" s="8"/>
+      <c r="AE23" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30">
+      <c r="A24" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32">
         <v>33.0</v>
       </c>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="29"/>
-      <c r="P24" s="29"/>
-      <c r="Q24" s="29"/>
-      <c r="R24" s="29"/>
-      <c r="S24" s="29"/>
-      <c r="T24" s="29"/>
-      <c r="U24" s="29"/>
-      <c r="V24" s="29"/>
-      <c r="W24" s="29"/>
-      <c r="X24" s="29"/>
-      <c r="Y24" s="29"/>
-      <c r="Z24" s="31"/>
-      <c r="AA24" s="31"/>
-      <c r="AB24" s="32">
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="33"/>
+      <c r="AA24" s="33"/>
+      <c r="AB24" s="34">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="AC24" s="33">
+      <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
         <v>102</v>
       </c>
       <c r="AD24" s="5"/>
+      <c r="AE24" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="37">
+      <c r="A25" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40">
         <v>36.0</v>
       </c>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38">
+      <c r="E25" s="40"/>
+      <c r="F25" s="41">
         <v>33.0</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="37"/>
-      <c r="T25" s="37"/>
-      <c r="U25" s="37"/>
-      <c r="V25" s="37"/>
-      <c r="W25" s="37"/>
-      <c r="X25" s="37"/>
-      <c r="Y25" s="37"/>
-      <c r="Z25" s="39"/>
-      <c r="AA25" s="39"/>
-      <c r="AB25" s="32">
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="40"/>
+      <c r="V25" s="40"/>
+      <c r="W25" s="40"/>
+      <c r="X25" s="40"/>
+      <c r="Y25" s="40"/>
+      <c r="Z25" s="42"/>
+      <c r="AA25" s="42"/>
+      <c r="AB25" s="34">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
+      <c r="AE25" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29">
+      <c r="A26" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="31">
         <v>35.0</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30">
+      <c r="E26" s="31"/>
+      <c r="F26" s="32">
         <v>36.0</v>
       </c>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
-      <c r="O26" s="29"/>
-      <c r="P26" s="29"/>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="29"/>
-      <c r="S26" s="29"/>
-      <c r="T26" s="29"/>
-      <c r="U26" s="29"/>
-      <c r="V26" s="29"/>
-      <c r="W26" s="29"/>
-      <c r="X26" s="29"/>
-      <c r="Y26" s="29"/>
-      <c r="Z26" s="31"/>
-      <c r="AA26" s="31"/>
-      <c r="AB26" s="32">
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="31"/>
+      <c r="W26" s="31"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="33"/>
+      <c r="AA26" s="33"/>
+      <c r="AB26" s="34">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="AC26" s="33">
+      <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
         <v>142</v>
       </c>
       <c r="AD26" s="5"/>
+      <c r="AE26" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37">
+      <c r="A27" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40">
         <v>42.0</v>
       </c>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38">
+      <c r="E27" s="40"/>
+      <c r="F27" s="41">
         <v>29.0</v>
       </c>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="37"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="37"/>
-      <c r="U27" s="37"/>
-      <c r="V27" s="37"/>
-      <c r="W27" s="37"/>
-      <c r="X27" s="37"/>
-      <c r="Y27" s="37"/>
-      <c r="Z27" s="39"/>
-      <c r="AA27" s="39"/>
-      <c r="AB27" s="32">
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="40"/>
+      <c r="N27" s="40"/>
+      <c r="O27" s="40"/>
+      <c r="P27" s="40"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+      <c r="S27" s="40"/>
+      <c r="T27" s="40"/>
+      <c r="U27" s="40"/>
+      <c r="V27" s="40"/>
+      <c r="W27" s="40"/>
+      <c r="X27" s="40"/>
+      <c r="Y27" s="40"/>
+      <c r="Z27" s="42"/>
+      <c r="AA27" s="42"/>
+      <c r="AB27" s="34">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
+      <c r="AE27" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29">
+      <c r="A28" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="31">
         <v>29.0</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="32">
         <v>31.0</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="32">
         <v>33.0</v>
       </c>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="29"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
-      <c r="U28" s="29"/>
-      <c r="V28" s="29"/>
-      <c r="W28" s="29"/>
-      <c r="X28" s="29"/>
-      <c r="Y28" s="29"/>
-      <c r="Z28" s="31"/>
-      <c r="AA28" s="31"/>
-      <c r="AB28" s="32">
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="31"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="31"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="31"/>
+      <c r="X28" s="31"/>
+      <c r="Y28" s="31"/>
+      <c r="Z28" s="33"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="34">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="AC28" s="33">
+      <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
         <v>179</v>
       </c>
       <c r="AD28" s="5"/>
+      <c r="AE28" s="36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="37">
+      <c r="A29" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40">
         <v>24.0</v>
       </c>
-      <c r="E29" s="38">
+      <c r="E29" s="41">
         <v>30.0</v>
       </c>
-      <c r="F29" s="38">
+      <c r="F29" s="41">
         <v>32.0</v>
       </c>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="37"/>
-      <c r="R29" s="37"/>
-      <c r="S29" s="37"/>
-      <c r="T29" s="37"/>
-      <c r="U29" s="37"/>
-      <c r="V29" s="37"/>
-      <c r="W29" s="37"/>
-      <c r="X29" s="37"/>
-      <c r="Y29" s="37"/>
-      <c r="Z29" s="39"/>
-      <c r="AA29" s="39"/>
-      <c r="AB29" s="32">
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="40"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="40"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="40"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="40"/>
+      <c r="Z29" s="42"/>
+      <c r="AA29" s="42"/>
+      <c r="AB29" s="34">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
+      <c r="AE29" s="36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="30">
+      <c r="A30" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32">
         <v>27.0</v>
       </c>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
-      <c r="O30" s="29"/>
-      <c r="P30" s="29"/>
-      <c r="Q30" s="29"/>
-      <c r="R30" s="29"/>
-      <c r="S30" s="29"/>
-      <c r="T30" s="29"/>
-      <c r="U30" s="29"/>
-      <c r="V30" s="29"/>
-      <c r="W30" s="29"/>
-      <c r="X30" s="29"/>
-      <c r="Y30" s="29"/>
-      <c r="Z30" s="31"/>
-      <c r="AA30" s="31"/>
-      <c r="AB30" s="32">
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="31"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
+      <c r="X30" s="31"/>
+      <c r="Y30" s="31"/>
+      <c r="Z30" s="33"/>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="34">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="AC30" s="33">
+      <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
         <v>94</v>
       </c>
       <c r="AD30" s="5"/>
+      <c r="AE30" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37">
+      <c r="A31" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="40">
         <v>33.0</v>
       </c>
-      <c r="E31" s="37"/>
-      <c r="F31" s="38">
+      <c r="E31" s="40"/>
+      <c r="F31" s="41">
         <v>34.0</v>
       </c>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="37"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="37"/>
-      <c r="P31" s="37"/>
-      <c r="Q31" s="37"/>
-      <c r="R31" s="37"/>
-      <c r="S31" s="37"/>
-      <c r="T31" s="37"/>
-      <c r="U31" s="37"/>
-      <c r="V31" s="37"/>
-      <c r="W31" s="37"/>
-      <c r="X31" s="37"/>
-      <c r="Y31" s="37"/>
-      <c r="Z31" s="48"/>
-      <c r="AA31" s="48"/>
-      <c r="AB31" s="49">
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+      <c r="T31" s="40"/>
+      <c r="U31" s="40"/>
+      <c r="V31" s="40"/>
+      <c r="W31" s="40"/>
+      <c r="X31" s="40"/>
+      <c r="Y31" s="40"/>
+      <c r="Z31" s="51"/>
+      <c r="AA31" s="51"/>
+      <c r="AB31" s="52">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
+      <c r="AE31" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="50"/>
+      <c r="A32" s="53"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2341,29 +2443,30 @@
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="52"/>
-      <c r="C33" s="53" t="s">
+      <c r="A33" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="54"/>
-      <c r="E33" s="52"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="57"/>
+      <c r="E33" s="55"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="57"/>
+      <c r="K33" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="L33" s="59"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="60"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -2379,11 +2482,12 @@
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="50"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="50"/>
+      <c r="A34" s="53"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2411,18 +2515,19 @@
       <c r="AB34" s="1"/>
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="50"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="59"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="60"/>
+      <c r="E35" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="63"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2430,84 +2535,86 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q35" s="59"/>
-      <c r="R35" s="59"/>
-      <c r="S35" s="60"/>
+      <c r="P35" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q35" s="62"/>
+      <c r="R35" s="62"/>
+      <c r="S35" s="63"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="61"/>
+      <c r="X35" s="64"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="50"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="62" t="s">
-        <v>54</v>
+      <c r="A36" s="53"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="65" t="s">
+        <v>55</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="63">
+      <c r="E36" s="66">
         <v>80.0</v>
       </c>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="52"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="64"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="O36" s="64"/>
-      <c r="P36" s="63">
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="O36" s="36"/>
+      <c r="P36" s="66">
         <v>50.0</v>
       </c>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="54"/>
-      <c r="S36" s="52"/>
+      <c r="Q36" s="57"/>
+      <c r="R36" s="57"/>
+      <c r="S36" s="55"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="65"/>
+      <c r="X36" s="67"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="50"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="62" t="s">
-        <v>55</v>
+      <c r="A37" s="53"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="65" t="s">
+        <v>56</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="63">
+      <c r="E37" s="66">
         <v>50.0</v>
       </c>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="64"/>
-      <c r="K37" s="64"/>
-      <c r="L37" s="64"/>
-      <c r="M37" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="O37" s="64"/>
-      <c r="P37" s="63">
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="36"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="O37" s="36"/>
+      <c r="P37" s="66">
         <v>30.0</v>
       </c>
-      <c r="Q37" s="54"/>
-      <c r="R37" s="54"/>
-      <c r="S37" s="52"/>
+      <c r="Q37" s="57"/>
+      <c r="R37" s="57"/>
+      <c r="S37" s="55"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -2519,20 +2626,21 @@
       <c r="AB37" s="1"/>
       <c r="AC37" s="1"/>
       <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="50"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="62" t="s">
-        <v>56</v>
+      <c r="A38" s="53"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="65" t="s">
+        <v>57</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="63">
+      <c r="E38" s="66">
         <v>40.0</v>
       </c>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="52"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="55"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -2540,10 +2648,10 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="66"/>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="21"/>
-      <c r="S38" s="21"/>
+      <c r="P38" s="68"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
@@ -2555,16 +2663,17 @@
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="D39" s="67"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-      <c r="O39" s="67"/>
+      <c r="O39" s="69"/>
       <c r="S39" s="1"/>
       <c r="W39" s="1"/>
     </row>
@@ -3632,115 +3741,168 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="25.29"/>
     <col customWidth="1" min="2" max="2" width="15.14"/>
+    <col customWidth="1" min="3" max="3" width="10.14"/>
+    <col customWidth="1" min="4" max="4" width="7.57"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>58</v>
       </c>
+      <c r="B1" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="70">
+      <c r="A2" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="72">
         <f>Sheet1!AC26</f>
         <v>142</v>
       </c>
-      <c r="C2" s="69"/>
+      <c r="C2" s="70">
+        <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
+        <v>4</v>
+      </c>
+      <c r="E2" s="70"/>
     </row>
     <row r="3">
-      <c r="A3" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="70">
+      <c r="A3" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="72">
         <f>Sheet1!AC12</f>
         <v>129</v>
       </c>
-      <c r="C3" s="69"/>
+      <c r="C3" s="70">
+        <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
+        <v>4</v>
+      </c>
+      <c r="E3" s="70"/>
     </row>
     <row r="4">
-      <c r="A4" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="70">
+      <c r="A4" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="72">
         <f>Sheet1!AC16</f>
         <v>136</v>
       </c>
-      <c r="C4" s="69"/>
+      <c r="C4" s="70">
+        <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
+        <v>4</v>
+      </c>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
     </row>
     <row r="5">
-      <c r="A5" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="70">
+      <c r="A5" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="72">
         <f>Sheet1!AC14</f>
         <v>61</v>
       </c>
-      <c r="C5" s="69"/>
+      <c r="C5" s="70">
+        <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
     </row>
     <row r="6">
-      <c r="A6" s="69" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="70">
+      <c r="A6" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="72">
         <f>Sheet1!AC22</f>
         <v>88</v>
       </c>
-      <c r="C6" s="69"/>
+      <c r="C6" s="70">
+        <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
+        <v>3</v>
+      </c>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
     </row>
     <row r="7">
-      <c r="A7" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="70">
+      <c r="A7" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="72">
         <f>Sheet1!AC28</f>
         <v>179</v>
       </c>
-      <c r="C7" s="69"/>
+      <c r="C7" s="70">
+        <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
+        <v>6</v>
+      </c>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
     </row>
     <row r="8">
-      <c r="A8" s="69" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="70">
+      <c r="A8" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="72">
         <f>Sheet1!AC20</f>
         <v>173</v>
       </c>
-      <c r="C8" s="69"/>
+      <c r="C8" s="70">
+        <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
+        <v>5</v>
+      </c>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
     </row>
     <row r="9">
-      <c r="A9" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="70">
+      <c r="A9" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="72">
         <f>Sheet1!AC24</f>
         <v>102</v>
       </c>
-      <c r="C9" s="69"/>
+      <c r="C9" s="70">
+        <f>COUNTIF(Sheet1!D24:AA25,"&lt;&gt;"&amp;"")</f>
+        <v>3</v>
+      </c>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
     </row>
     <row r="10">
-      <c r="A10" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="70">
+      <c r="A10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="72">
         <f>Sheet1!AC30</f>
         <v>94</v>
       </c>
-      <c r="C10" s="69"/>
+      <c r="C10" s="70">
+        <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
     </row>
     <row r="11">
-      <c r="A11" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="70">
+      <c r="A11" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="72">
         <f>Sheet1!AC18</f>
         <v>61</v>
       </c>
-      <c r="C11" s="69"/>
+      <c r="C11" s="70">
+        <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
+        <v>2</v>
+      </c>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
005 Week 4 update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -5,19 +5,20 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="xxDO NOT EDITxx" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="HANDICAPS" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="emksQva/QHKVBg8Jg7dXnxTaw3GJ01mCWEWrwbnszq8="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="X/xjmHFd2A+dABkjvFq2tQqB37tSlgFtRxrGmCp92xg="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
   <si>
     <t>WINTER BEST PAIRS COMP(SUNDAY)</t>
   </si>
@@ -196,40 +197,40 @@
     <t>TEAM</t>
   </si>
   <si>
-    <t>TEAM TOTAL</t>
-  </si>
-  <si>
     <t>PLAYED</t>
   </si>
   <si>
+    <t>BAZ &amp; MICK</t>
+  </si>
+  <si>
+    <t>RYAN &amp; STUART</t>
+  </si>
+  <si>
+    <t>LES &amp; JOHN</t>
+  </si>
+  <si>
+    <t>PAUL &amp; TONI</t>
+  </si>
+  <si>
+    <t>ALBIE &amp; CHRIS</t>
+  </si>
+  <si>
+    <t>STEWART &amp; TONY</t>
+  </si>
+  <si>
+    <t>ADY &amp; STEVE</t>
+  </si>
+  <si>
     <t>MAL &amp; KEN</t>
   </si>
   <si>
-    <t>BAZ &amp; MICK</t>
-  </si>
-  <si>
-    <t>LES &amp; JOHN</t>
-  </si>
-  <si>
-    <t>RYAN &amp; STUART</t>
-  </si>
-  <si>
-    <t>STEWART &amp; TONY</t>
-  </si>
-  <si>
     <t>PAUL &amp; FRED</t>
   </si>
   <si>
-    <t>ALBIE &amp; CHRIS</t>
-  </si>
-  <si>
-    <t>ADY &amp; STEVE</t>
-  </si>
-  <si>
     <t>SCOTT &amp; ANDY</t>
   </si>
   <si>
-    <t>PAUL &amp; TONI</t>
+    <t>HANDICAP</t>
   </si>
 </sst>
 </file>
@@ -691,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -850,6 +851,7 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -864,6 +866,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1072,7 +1078,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="3" width="8.71"/>
-    <col customWidth="1" min="4" max="31" width="3.71"/>
+    <col customWidth="1" min="4" max="28" width="4.29"/>
+    <col customWidth="1" min="29" max="31" width="3.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1505,7 +1512,9 @@
       <c r="F12" s="32">
         <v>31.0</v>
       </c>
-      <c r="G12" s="31"/>
+      <c r="G12" s="32">
+        <v>32.0</v>
+      </c>
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
@@ -1528,16 +1537,16 @@
       <c r="AA12" s="33"/>
       <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>129</v>
+        <v>196</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36">
         <f t="shared" ref="AE12:AE31" si="2">countif(D12:AA12,"&lt;&gt;"&amp;"")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -1553,7 +1562,9 @@
       <c r="F13" s="41">
         <v>35.0</v>
       </c>
-      <c r="G13" s="40"/>
+      <c r="G13" s="41">
+        <v>35.0</v>
+      </c>
       <c r="H13" s="40"/>
       <c r="I13" s="40"/>
       <c r="J13" s="40"/>
@@ -1576,13 +1587,13 @@
       <c r="AA13" s="42"/>
       <c r="AB13" s="34">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
       <c r="AE13" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -1623,7 +1634,7 @@
       </c>
       <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="36">
@@ -1642,7 +1653,9 @@
       </c>
       <c r="E15" s="40"/>
       <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="G15" s="41">
+        <v>31.0</v>
+      </c>
       <c r="H15" s="40"/>
       <c r="I15" s="40"/>
       <c r="J15" s="40"/>
@@ -1665,13 +1678,13 @@
       <c r="AA15" s="42"/>
       <c r="AB15" s="34">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
       <c r="AE15" s="36">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -1687,7 +1700,9 @@
       <c r="F16" s="32">
         <v>42.0</v>
       </c>
-      <c r="G16" s="31"/>
+      <c r="G16" s="32">
+        <v>29.0</v>
+      </c>
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
@@ -1710,16 +1725,16 @@
       <c r="AA16" s="33"/>
       <c r="AB16" s="34">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>136</v>
+        <v>191</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -1735,7 +1750,9 @@
       <c r="F17" s="41">
         <v>32.0</v>
       </c>
-      <c r="G17" s="40"/>
+      <c r="G17" s="41">
+        <v>26.0</v>
+      </c>
       <c r="H17" s="40"/>
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
@@ -1758,13 +1775,13 @@
       <c r="AA17" s="42"/>
       <c r="AB17" s="34">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
       <c r="AE17" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -1778,7 +1795,9 @@
       <c r="F18" s="32">
         <v>33.0</v>
       </c>
-      <c r="G18" s="31"/>
+      <c r="G18" s="32">
+        <v>31.0</v>
+      </c>
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
@@ -1801,16 +1820,16 @@
       <c r="AA18" s="33"/>
       <c r="AB18" s="34">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="AC18" s="35">
         <f>SUM(AB18:AB19)</f>
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="36">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1824,7 +1843,9 @@
       </c>
       <c r="E19" s="40"/>
       <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
+      <c r="G19" s="41">
+        <v>33.0</v>
+      </c>
       <c r="H19" s="40"/>
       <c r="I19" s="40"/>
       <c r="J19" s="40"/>
@@ -1847,13 +1868,13 @@
       <c r="AA19" s="42"/>
       <c r="AB19" s="34">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="AC19" s="6"/>
       <c r="AD19" s="8"/>
       <c r="AE19" s="36">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -1869,7 +1890,9 @@
       <c r="F20" s="32">
         <v>33.0</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="32">
+        <v>35.0</v>
+      </c>
       <c r="H20" s="31"/>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
@@ -1892,16 +1915,16 @@
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>173</v>
+        <v>237</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -1919,7 +1942,9 @@
       <c r="F21" s="41">
         <v>33.0</v>
       </c>
-      <c r="G21" s="40"/>
+      <c r="G21" s="41">
+        <v>29.0</v>
+      </c>
       <c r="H21" s="40"/>
       <c r="I21" s="40"/>
       <c r="J21" s="40"/>
@@ -1942,13 +1967,13 @@
       <c r="AA21" s="42"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
       <c r="AE21" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -1962,7 +1987,9 @@
       </c>
       <c r="E22" s="31"/>
       <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
+      <c r="G22" s="32">
+        <v>35.0</v>
+      </c>
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
       <c r="J22" s="31"/>
@@ -1985,16 +2012,16 @@
       <c r="AA22" s="33"/>
       <c r="AB22" s="34">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="AC22" s="35">
         <f>SUM(AB22:AB23)</f>
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="AD22" s="5"/>
       <c r="AE22" s="36">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -2053,7 +2080,9 @@
       <c r="F24" s="32">
         <v>33.0</v>
       </c>
-      <c r="G24" s="31"/>
+      <c r="G24" s="32">
+        <v>37.0</v>
+      </c>
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
@@ -2076,16 +2105,16 @@
       <c r="AA24" s="33"/>
       <c r="AB24" s="34">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="36">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -2101,7 +2130,9 @@
       <c r="F25" s="41">
         <v>33.0</v>
       </c>
-      <c r="G25" s="40"/>
+      <c r="G25" s="41">
+        <v>33.0</v>
+      </c>
       <c r="H25" s="40"/>
       <c r="I25" s="40"/>
       <c r="J25" s="40"/>
@@ -2124,13 +2155,13 @@
       <c r="AA25" s="42"/>
       <c r="AB25" s="34">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
       <c r="AE25" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -2146,7 +2177,9 @@
       <c r="F26" s="32">
         <v>36.0</v>
       </c>
-      <c r="G26" s="31"/>
+      <c r="G26" s="32">
+        <v>36.0</v>
+      </c>
       <c r="H26" s="31"/>
       <c r="I26" s="31"/>
       <c r="J26" s="31"/>
@@ -2169,16 +2202,16 @@
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -2194,7 +2227,9 @@
       <c r="F27" s="41">
         <v>29.0</v>
       </c>
-      <c r="G27" s="40"/>
+      <c r="G27" s="41">
+        <v>40.0</v>
+      </c>
       <c r="H27" s="40"/>
       <c r="I27" s="40"/>
       <c r="J27" s="40"/>
@@ -2217,13 +2252,13 @@
       <c r="AA27" s="42"/>
       <c r="AB27" s="34">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
       <c r="AE27" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -2241,7 +2276,9 @@
       <c r="F28" s="32">
         <v>33.0</v>
       </c>
-      <c r="G28" s="31"/>
+      <c r="G28" s="32">
+        <v>30.0</v>
+      </c>
       <c r="H28" s="31"/>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
@@ -2264,16 +2301,16 @@
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>179</v>
+        <v>246</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -2291,7 +2328,9 @@
       <c r="F29" s="41">
         <v>32.0</v>
       </c>
-      <c r="G29" s="40"/>
+      <c r="G29" s="41">
+        <v>37.0</v>
+      </c>
       <c r="H29" s="40"/>
       <c r="I29" s="40"/>
       <c r="J29" s="40"/>
@@ -2314,13 +2353,13 @@
       <c r="AA29" s="42"/>
       <c r="AB29" s="34">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
       <c r="AE29" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -2334,7 +2373,9 @@
       <c r="F30" s="32">
         <v>27.0</v>
       </c>
-      <c r="G30" s="31"/>
+      <c r="G30" s="32">
+        <v>33.0</v>
+      </c>
       <c r="H30" s="31"/>
       <c r="I30" s="31"/>
       <c r="J30" s="31"/>
@@ -2357,16 +2398,16 @@
       <c r="AA30" s="33"/>
       <c r="AB30" s="34">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -2382,7 +2423,9 @@
       <c r="F31" s="41">
         <v>34.0</v>
       </c>
-      <c r="G31" s="40"/>
+      <c r="G31" s="41">
+        <v>30.0</v>
+      </c>
       <c r="H31" s="40"/>
       <c r="I31" s="40"/>
       <c r="J31" s="40"/>
@@ -2405,13 +2448,13 @@
       <c r="AA31" s="51"/>
       <c r="AB31" s="52">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
       <c r="AE31" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -3738,12 +3781,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="25.29"/>
-    <col customWidth="1" min="2" max="2" width="15.14"/>
-    <col customWidth="1" min="3" max="3" width="10.14"/>
-    <col customWidth="1" min="4" max="4" width="7.57"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="70" t="s">
@@ -3752,157 +3789,282 @@
       <c r="B1" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="70" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="72">
-        <f>Sheet1!AC26</f>
-        <v>142</v>
-      </c>
-      <c r="C2" s="70">
-        <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>4</v>
-      </c>
-      <c r="E2" s="70"/>
+        <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="72">
-        <f>Sheet1!AC12</f>
-        <v>129</v>
-      </c>
-      <c r="C3" s="70">
-        <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>4</v>
-      </c>
-      <c r="E3" s="70"/>
+        <v>61</v>
+      </c>
+      <c r="B3" s="70">
+        <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="72">
-        <f>Sheet1!AC16</f>
-        <v>136</v>
-      </c>
-      <c r="C4" s="70">
+        <v>62</v>
+      </c>
+      <c r="B4" s="70">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>4</v>
-      </c>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="72">
-        <f>Sheet1!AC14</f>
-        <v>61</v>
-      </c>
-      <c r="C5" s="70">
-        <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
-        <v>2</v>
-      </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
+        <v>63</v>
+      </c>
+      <c r="B5" s="70">
+        <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="72">
-        <f>Sheet1!AC22</f>
-        <v>88</v>
-      </c>
-      <c r="C6" s="70">
-        <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>3</v>
-      </c>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
+        <v>64</v>
+      </c>
+      <c r="B6" s="70">
+        <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="72">
-        <f>Sheet1!AC28</f>
-        <v>179</v>
-      </c>
-      <c r="C7" s="70">
-        <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>6</v>
-      </c>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
+        <v>65</v>
+      </c>
+      <c r="B7" s="70">
+        <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="72">
-        <f>Sheet1!AC20</f>
-        <v>173</v>
-      </c>
-      <c r="C8" s="70">
-        <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
+        <v>66</v>
+      </c>
+      <c r="B8" s="70">
+        <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
         <v>5</v>
       </c>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
     </row>
     <row r="9">
       <c r="A9" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="72">
-        <f>Sheet1!AC24</f>
-        <v>102</v>
-      </c>
-      <c r="C9" s="70">
-        <f>COUNTIF(Sheet1!D24:AA25,"&lt;&gt;"&amp;"")</f>
-        <v>3</v>
-      </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="70"/>
+        <v>67</v>
+      </c>
+      <c r="B9" s="70">
+        <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="72">
-        <f>Sheet1!AC30</f>
-        <v>94</v>
-      </c>
-      <c r="C10" s="70">
-        <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>3</v>
-      </c>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
+        <v>68</v>
+      </c>
+      <c r="B10" s="70">
+        <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="70">
+        <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="22.14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="72">
-        <f>Sheet1!AC18</f>
-        <v>61</v>
-      </c>
-      <c r="C11" s="70">
-        <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>2</v>
-      </c>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="70">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="70">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="70">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="70">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="70">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="70">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="70">
+        <v>-2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="70">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="70">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="70">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="70">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="70">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="73" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="70">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="70">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="70">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="73" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="70">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="70">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="73" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="70">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="70">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="70">
+        <v>7.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
#006 Thursday Singles page added
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -4,21 +4,22 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="xxDO NOT EDITxx" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="HANDICAPS" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="THURSDAY SINGLES" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="xxDO NOT EDITxx" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="HANDICAPS" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="X/xjmHFd2A+dABkjvFq2tQqB37tSlgFtRxrGmCp92xg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="g0V7LTg/eSjx8a99N05z6zCx+DOe579pUdliY60dtT8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
   <si>
     <t>WINTER BEST PAIRS COMP(SUNDAY)</t>
   </si>
@@ -192,6 +193,27 @@
   </si>
   <si>
     <t>3RD</t>
+  </si>
+  <si>
+    <t>WINTER SINGLES (THURSDAY)</t>
+  </si>
+  <si>
+    <t>STEW TAYLOR</t>
+  </si>
+  <si>
+    <t>SIMON EDWARDS</t>
+  </si>
+  <si>
+    <t>DAVE BARNETT</t>
+  </si>
+  <si>
+    <t>MARTIN BROCK</t>
+  </si>
+  <si>
+    <t>GORDON PERRIN</t>
+  </si>
+  <si>
+    <t>JOHN KING</t>
   </si>
   <si>
     <t>TEAM</t>
@@ -240,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -288,12 +310,21 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,8 +343,14 @@
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border/>
     <border>
       <left style="medium">
@@ -688,11 +725,25 @@
       </top>
       <bottom/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="94">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -845,14 +896,74 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="9" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" textRotation="90" vertical="center"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="9" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" textRotation="90" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" textRotation="90" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" textRotation="90" vertical="center"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="33" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="33" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="33" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="33" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -870,6 +981,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1515,7 +1630,9 @@
       <c r="G12" s="32">
         <v>32.0</v>
       </c>
-      <c r="H12" s="31"/>
+      <c r="H12" s="32">
+        <v>31.0</v>
+      </c>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
@@ -1537,16 +1654,16 @@
       <c r="AA12" s="33"/>
       <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>196</v>
+        <v>258</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36">
         <f t="shared" ref="AE12:AE31" si="2">countif(D12:AA12,"&lt;&gt;"&amp;"")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -1565,7 +1682,9 @@
       <c r="G13" s="41">
         <v>35.0</v>
       </c>
-      <c r="H13" s="40"/>
+      <c r="H13" s="41">
+        <v>31.0</v>
+      </c>
       <c r="I13" s="40"/>
       <c r="J13" s="40"/>
       <c r="K13" s="40"/>
@@ -1587,13 +1706,13 @@
       <c r="AA13" s="42"/>
       <c r="AB13" s="34">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
       <c r="AE13" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -1608,7 +1727,9 @@
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
       <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="H14" s="32">
+        <v>39.0</v>
+      </c>
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
@@ -1630,16 +1751,16 @@
       <c r="AA14" s="33"/>
       <c r="AB14" s="34">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="36">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1656,7 +1777,9 @@
       <c r="G15" s="41">
         <v>31.0</v>
       </c>
-      <c r="H15" s="40"/>
+      <c r="H15" s="41">
+        <v>38.0</v>
+      </c>
       <c r="I15" s="40"/>
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
@@ -1678,13 +1801,13 @@
       <c r="AA15" s="42"/>
       <c r="AB15" s="34">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
       <c r="AE15" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -1703,7 +1826,9 @@
       <c r="G16" s="32">
         <v>29.0</v>
       </c>
-      <c r="H16" s="31"/>
+      <c r="H16" s="32">
+        <v>27.0</v>
+      </c>
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
@@ -1725,16 +1850,16 @@
       <c r="AA16" s="33"/>
       <c r="AB16" s="34">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>191</v>
+        <v>250</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -1753,7 +1878,9 @@
       <c r="G17" s="41">
         <v>26.0</v>
       </c>
-      <c r="H17" s="40"/>
+      <c r="H17" s="41">
+        <v>32.0</v>
+      </c>
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
@@ -1775,13 +1902,13 @@
       <c r="AA17" s="42"/>
       <c r="AB17" s="34">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
       <c r="AE17" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1798,7 +1925,9 @@
       <c r="G18" s="32">
         <v>31.0</v>
       </c>
-      <c r="H18" s="31"/>
+      <c r="H18" s="32">
+        <v>33.0</v>
+      </c>
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
@@ -1820,16 +1949,16 @@
       <c r="AA18" s="33"/>
       <c r="AB18" s="34">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="AC18" s="35">
         <f>SUM(AB18:AB19)</f>
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1893,7 +2022,9 @@
       <c r="G20" s="32">
         <v>35.0</v>
       </c>
-      <c r="H20" s="31"/>
+      <c r="H20" s="32">
+        <v>38.0</v>
+      </c>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
@@ -1915,16 +2046,16 @@
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>237</v>
+        <v>307</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -1945,7 +2076,9 @@
       <c r="G21" s="41">
         <v>29.0</v>
       </c>
-      <c r="H21" s="40"/>
+      <c r="H21" s="41">
+        <v>32.0</v>
+      </c>
       <c r="I21" s="40"/>
       <c r="J21" s="40"/>
       <c r="K21" s="40"/>
@@ -1967,13 +2100,13 @@
       <c r="AA21" s="42"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
       <c r="AE21" s="36">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -2016,7 +2149,7 @@
       </c>
       <c r="AC22" s="35">
         <f>SUM(AB22:AB23)</f>
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="AD22" s="5"/>
       <c r="AE22" s="36">
@@ -2038,7 +2171,9 @@
         <v>30.0</v>
       </c>
       <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
+      <c r="H23" s="41">
+        <v>28.0</v>
+      </c>
       <c r="I23" s="40"/>
       <c r="J23" s="40"/>
       <c r="K23" s="40"/>
@@ -2060,13 +2195,13 @@
       <c r="AA23" s="42"/>
       <c r="AB23" s="34">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="AC23" s="6"/>
       <c r="AD23" s="8"/>
       <c r="AE23" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -2109,7 +2244,7 @@
       </c>
       <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="36">
@@ -2133,7 +2268,9 @@
       <c r="G25" s="41">
         <v>33.0</v>
       </c>
-      <c r="H25" s="40"/>
+      <c r="H25" s="41">
+        <v>34.0</v>
+      </c>
       <c r="I25" s="40"/>
       <c r="J25" s="40"/>
       <c r="K25" s="40"/>
@@ -2155,13 +2292,13 @@
       <c r="AA25" s="42"/>
       <c r="AB25" s="34">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
       <c r="AE25" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -2180,7 +2317,9 @@
       <c r="G26" s="32">
         <v>36.0</v>
       </c>
-      <c r="H26" s="31"/>
+      <c r="H26" s="32">
+        <v>31.0</v>
+      </c>
       <c r="I26" s="31"/>
       <c r="J26" s="31"/>
       <c r="K26" s="31"/>
@@ -2202,16 +2341,16 @@
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>218</v>
+        <v>277</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -2230,7 +2369,9 @@
       <c r="G27" s="41">
         <v>40.0</v>
       </c>
-      <c r="H27" s="40"/>
+      <c r="H27" s="41">
+        <v>28.0</v>
+      </c>
       <c r="I27" s="40"/>
       <c r="J27" s="40"/>
       <c r="K27" s="40"/>
@@ -2252,13 +2393,13 @@
       <c r="AA27" s="42"/>
       <c r="AB27" s="34">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
       <c r="AE27" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -2279,7 +2420,9 @@
       <c r="G28" s="32">
         <v>30.0</v>
       </c>
-      <c r="H28" s="31"/>
+      <c r="H28" s="32">
+        <v>29.0</v>
+      </c>
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
       <c r="K28" s="31"/>
@@ -2301,16 +2444,16 @@
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>246</v>
+        <v>311</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -2331,7 +2474,9 @@
       <c r="G29" s="41">
         <v>37.0</v>
       </c>
-      <c r="H29" s="40"/>
+      <c r="H29" s="41">
+        <v>36.0</v>
+      </c>
       <c r="I29" s="40"/>
       <c r="J29" s="40"/>
       <c r="K29" s="40"/>
@@ -2353,13 +2498,13 @@
       <c r="AA29" s="42"/>
       <c r="AB29" s="34">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
       <c r="AE29" s="36">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -2376,7 +2521,9 @@
       <c r="G30" s="32">
         <v>33.0</v>
       </c>
-      <c r="H30" s="31"/>
+      <c r="H30" s="32">
+        <v>34.0</v>
+      </c>
       <c r="I30" s="31"/>
       <c r="J30" s="31"/>
       <c r="K30" s="31"/>
@@ -2398,16 +2545,16 @@
       <c r="AA30" s="33"/>
       <c r="AB30" s="34">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>157</v>
+        <v>220</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -2426,7 +2573,9 @@
       <c r="G31" s="41">
         <v>30.0</v>
       </c>
-      <c r="H31" s="40"/>
+      <c r="H31" s="41">
+        <v>29.0</v>
+      </c>
       <c r="I31" s="40"/>
       <c r="J31" s="40"/>
       <c r="K31" s="40"/>
@@ -2448,13 +2597,13 @@
       <c r="AA31" s="51"/>
       <c r="AB31" s="52">
         <f t="shared" si="1"/>
-        <v>97</v>
+        <v>126</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
       <c r="AE31" s="36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -3781,106 +3930,1100 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="30.0"/>
+    <col customWidth="1" min="2" max="27" width="5.57"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="70"/>
+      <c r="AA1" s="70"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="70"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="70"/>
+    </row>
+    <row r="3" ht="79.5" customHeight="1">
+      <c r="A3" s="70"/>
+      <c r="B3" s="72">
+        <v>45575.0</v>
+      </c>
+      <c r="C3" s="72">
+        <v>45582.0</v>
+      </c>
+      <c r="D3" s="73">
+        <v>45589.0</v>
+      </c>
+      <c r="E3" s="73">
+        <v>45596.0</v>
+      </c>
+      <c r="F3" s="73">
+        <v>45603.0</v>
+      </c>
+      <c r="G3" s="73">
+        <v>45610.0</v>
+      </c>
+      <c r="H3" s="73">
+        <v>45617.0</v>
+      </c>
+      <c r="I3" s="73">
+        <v>45624.0</v>
+      </c>
+      <c r="J3" s="73">
+        <v>45631.0</v>
+      </c>
+      <c r="K3" s="73">
+        <v>45638.0</v>
+      </c>
+      <c r="L3" s="73">
+        <v>45645.0</v>
+      </c>
+      <c r="M3" s="73">
+        <v>45659.0</v>
+      </c>
+      <c r="N3" s="73">
+        <v>45666.0</v>
+      </c>
+      <c r="O3" s="73">
+        <v>45673.0</v>
+      </c>
+      <c r="P3" s="72">
+        <v>45680.0</v>
+      </c>
+      <c r="Q3" s="72">
+        <v>45687.0</v>
+      </c>
+      <c r="R3" s="72">
+        <v>45694.0</v>
+      </c>
+      <c r="S3" s="72">
+        <v>45701.0</v>
+      </c>
+      <c r="T3" s="72">
+        <v>45708.0</v>
+      </c>
+      <c r="U3" s="72">
+        <v>45715.0</v>
+      </c>
+      <c r="V3" s="72">
+        <v>45722.0</v>
+      </c>
+      <c r="W3" s="72">
+        <v>45729.0</v>
+      </c>
+      <c r="X3" s="72">
+        <v>45736.0</v>
+      </c>
+      <c r="Y3" s="72">
+        <v>45743.0</v>
+      </c>
+      <c r="Z3" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="75"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="T4" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="V4" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="W4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="X4" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="79">
+        <v>30.0</v>
+      </c>
+      <c r="C5" s="79">
+        <v>37.0</v>
+      </c>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79">
+        <v>31.0</v>
+      </c>
+      <c r="F5" s="79">
+        <v>33.0</v>
+      </c>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79"/>
+      <c r="X5" s="79"/>
+      <c r="Y5" s="79"/>
+      <c r="Z5" s="80">
+        <f t="shared" ref="Z5:Z17" si="1">SUM(B5:W5)</f>
+        <v>131</v>
+      </c>
+      <c r="AA5" s="36">
+        <f t="shared" ref="AA5:AA17" si="2">countif(B5:Y5,"&lt;&gt;"&amp;"")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="79">
+        <v>36.0</v>
+      </c>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79">
+        <v>32.0</v>
+      </c>
+      <c r="E6" s="79"/>
+      <c r="F6" s="81">
+        <v>39.0</v>
+      </c>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="80">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="AA6" s="36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="78" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="71" t="s">
+      <c r="B7" s="79">
+        <v>33.0</v>
+      </c>
+      <c r="C7" s="79">
+        <v>28.0</v>
+      </c>
+      <c r="D7" s="79">
+        <v>32.0</v>
+      </c>
+      <c r="E7" s="79"/>
+      <c r="F7" s="81">
+        <v>33.0</v>
+      </c>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="79"/>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="79"/>
+      <c r="R7" s="79"/>
+      <c r="S7" s="79"/>
+      <c r="T7" s="79"/>
+      <c r="U7" s="79"/>
+      <c r="V7" s="79"/>
+      <c r="W7" s="79"/>
+      <c r="X7" s="79"/>
+      <c r="Y7" s="79"/>
+      <c r="Z7" s="80">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="AA7" s="36">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="79">
+        <v>37.0</v>
+      </c>
+      <c r="C8" s="79">
+        <v>35.0</v>
+      </c>
+      <c r="D8" s="79">
+        <v>32.0</v>
+      </c>
+      <c r="E8" s="79">
+        <v>31.0</v>
+      </c>
+      <c r="F8" s="81">
+        <v>31.0</v>
+      </c>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="79"/>
+      <c r="O8" s="79"/>
+      <c r="P8" s="79"/>
+      <c r="Q8" s="79"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="79"/>
+      <c r="T8" s="79"/>
+      <c r="U8" s="79"/>
+      <c r="V8" s="79"/>
+      <c r="W8" s="79"/>
+      <c r="X8" s="79"/>
+      <c r="Y8" s="79"/>
+      <c r="Z8" s="80">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+      <c r="AA8" s="36">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="79">
+        <v>30.0</v>
+      </c>
+      <c r="C9" s="79">
+        <v>33.0</v>
+      </c>
+      <c r="D9" s="79">
+        <v>30.0</v>
+      </c>
+      <c r="E9" s="79">
+        <v>26.0</v>
+      </c>
+      <c r="F9" s="81">
+        <v>28.0</v>
+      </c>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="79"/>
+      <c r="T9" s="79"/>
+      <c r="U9" s="79"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="79"/>
+      <c r="X9" s="79"/>
+      <c r="Y9" s="79"/>
+      <c r="Z9" s="80">
+        <f t="shared" si="1"/>
+        <v>147</v>
+      </c>
+      <c r="AA9" s="36">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79">
+        <v>31.0</v>
+      </c>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79">
+        <v>23.0</v>
+      </c>
+      <c r="F10" s="81">
+        <v>35.0</v>
+      </c>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="79"/>
+      <c r="U10" s="79"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="79"/>
+      <c r="X10" s="79"/>
+      <c r="Y10" s="79"/>
+      <c r="Z10" s="80">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="AA10" s="36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="72">
-        <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="71" t="s">
+      <c r="B11" s="79">
+        <v>41.0</v>
+      </c>
+      <c r="C11" s="79">
+        <v>31.0</v>
+      </c>
+      <c r="D11" s="79">
+        <v>32.0</v>
+      </c>
+      <c r="E11" s="79">
+        <v>29.0</v>
+      </c>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
+      <c r="O11" s="79"/>
+      <c r="P11" s="79"/>
+      <c r="Q11" s="79"/>
+      <c r="R11" s="79"/>
+      <c r="S11" s="79"/>
+      <c r="T11" s="79"/>
+      <c r="U11" s="79"/>
+      <c r="V11" s="79"/>
+      <c r="W11" s="79"/>
+      <c r="X11" s="79"/>
+      <c r="Y11" s="79"/>
+      <c r="Z11" s="80">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="AA11" s="36">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="70">
-        <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
+      <c r="B12" s="79">
+        <v>42.0</v>
+      </c>
+      <c r="C12" s="79">
+        <v>31.0</v>
+      </c>
+      <c r="D12" s="79">
+        <v>32.0</v>
+      </c>
+      <c r="E12" s="79">
+        <v>32.0</v>
+      </c>
+      <c r="F12" s="81">
+        <v>34.0</v>
+      </c>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="79"/>
+      <c r="P12" s="79"/>
+      <c r="Q12" s="79"/>
+      <c r="R12" s="79"/>
+      <c r="S12" s="79"/>
+      <c r="T12" s="79"/>
+      <c r="U12" s="79"/>
+      <c r="V12" s="79"/>
+      <c r="W12" s="79"/>
+      <c r="X12" s="79"/>
+      <c r="Y12" s="79"/>
+      <c r="Z12" s="80">
+        <f t="shared" si="1"/>
+        <v>171</v>
+      </c>
+      <c r="AA12" s="36">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="82"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79">
+        <v>33.0</v>
+      </c>
+      <c r="E13" s="79">
+        <v>36.0</v>
+      </c>
+      <c r="F13" s="81">
+        <v>27.0</v>
+      </c>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="79"/>
+      <c r="P13" s="79"/>
+      <c r="Q13" s="79"/>
+      <c r="R13" s="79"/>
+      <c r="S13" s="79"/>
+      <c r="T13" s="79"/>
+      <c r="U13" s="79"/>
+      <c r="V13" s="79"/>
+      <c r="W13" s="79"/>
+      <c r="X13" s="79"/>
+      <c r="Y13" s="79"/>
+      <c r="Z13" s="80">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="AA13" s="36">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="70">
-        <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="71" t="s">
+    <row r="14">
+      <c r="A14" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="70">
-        <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="71" t="s">
+      <c r="B14" s="79"/>
+      <c r="C14" s="79">
+        <v>22.0</v>
+      </c>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="81">
+        <v>36.0</v>
+      </c>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="79"/>
+      <c r="R14" s="79"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="79"/>
+      <c r="U14" s="79"/>
+      <c r="V14" s="79"/>
+      <c r="W14" s="79"/>
+      <c r="X14" s="79"/>
+      <c r="Y14" s="79"/>
+      <c r="Z14" s="80">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="AA14" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79">
+        <v>43.0</v>
+      </c>
+      <c r="D15" s="79">
+        <v>25.0</v>
+      </c>
+      <c r="E15" s="79"/>
+      <c r="F15" s="81">
+        <v>32.0</v>
+      </c>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="79"/>
+      <c r="Q15" s="79"/>
+      <c r="R15" s="79"/>
+      <c r="S15" s="79"/>
+      <c r="T15" s="79"/>
+      <c r="U15" s="79"/>
+      <c r="V15" s="79"/>
+      <c r="W15" s="79"/>
+      <c r="X15" s="79"/>
+      <c r="Y15" s="79"/>
+      <c r="Z15" s="80">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="AA15" s="36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="70">
-        <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="70">
-        <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="70">
-        <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="70">
-        <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="70">
-        <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="70">
-        <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>5</v>
-      </c>
+      <c r="B16" s="79"/>
+      <c r="C16" s="79">
+        <v>29.0</v>
+      </c>
+      <c r="D16" s="79">
+        <v>28.0</v>
+      </c>
+      <c r="E16" s="79"/>
+      <c r="F16" s="81">
+        <v>23.0</v>
+      </c>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="79"/>
+      <c r="P16" s="79"/>
+      <c r="Q16" s="79"/>
+      <c r="R16" s="79"/>
+      <c r="S16" s="79"/>
+      <c r="T16" s="79"/>
+      <c r="U16" s="79"/>
+      <c r="V16" s="79"/>
+      <c r="W16" s="79"/>
+      <c r="X16" s="79"/>
+      <c r="Y16" s="79"/>
+      <c r="Z16" s="80">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="AA16" s="36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="79"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79">
+        <v>41.0</v>
+      </c>
+      <c r="E17" s="79">
+        <v>37.0</v>
+      </c>
+      <c r="F17" s="81">
+        <v>38.0</v>
+      </c>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="79"/>
+      <c r="P17" s="79"/>
+      <c r="Q17" s="79"/>
+      <c r="R17" s="79"/>
+      <c r="S17" s="79"/>
+      <c r="T17" s="79"/>
+      <c r="U17" s="79"/>
+      <c r="V17" s="79"/>
+      <c r="W17" s="79"/>
+      <c r="X17" s="79"/>
+      <c r="Y17" s="79"/>
+      <c r="Z17" s="80">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="AA17" s="36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="83"/>
+      <c r="B18" s="77"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77"/>
+      <c r="K18" s="77"/>
+      <c r="L18" s="77"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="77"/>
+      <c r="O18" s="77"/>
+      <c r="P18" s="77"/>
+      <c r="Q18" s="77"/>
+      <c r="R18" s="77"/>
+      <c r="S18" s="77"/>
+      <c r="T18" s="77"/>
+      <c r="U18" s="77"/>
+      <c r="V18" s="77"/>
+      <c r="W18" s="77"/>
+      <c r="X18" s="77"/>
+      <c r="Y18" s="77"/>
+      <c r="Z18" s="77"/>
+      <c r="AA18" s="36"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="70"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="70"/>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="70"/>
+      <c r="S19" s="70"/>
+      <c r="T19" s="70"/>
+      <c r="U19" s="70"/>
+      <c r="V19" s="70"/>
+      <c r="W19" s="70"/>
+      <c r="X19" s="70"/>
+      <c r="Y19" s="70"/>
+      <c r="Z19" s="70"/>
+      <c r="AA19" s="36"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="84" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="85">
+        <v>10.0</v>
+      </c>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="86" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="70"/>
+      <c r="P20" s="70"/>
+      <c r="Q20" s="70"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
+      <c r="T20" s="70"/>
+      <c r="U20" s="70"/>
+      <c r="V20" s="70"/>
+      <c r="W20" s="70"/>
+      <c r="X20" s="70"/>
+      <c r="Y20" s="70"/>
+      <c r="Z20" s="70"/>
+      <c r="AA20" s="36"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="70"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="70"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="70"/>
+      <c r="P21" s="70"/>
+      <c r="Q21" s="70"/>
+      <c r="R21" s="70"/>
+      <c r="S21" s="70"/>
+      <c r="T21" s="70"/>
+      <c r="U21" s="70"/>
+      <c r="V21" s="70"/>
+      <c r="W21" s="70"/>
+      <c r="X21" s="70"/>
+      <c r="Y21" s="70"/>
+      <c r="Z21" s="70"/>
+      <c r="AA21" s="36"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="70"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="70"/>
+      <c r="M22" s="70"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="70"/>
+      <c r="P22" s="70"/>
+      <c r="Q22" s="70"/>
+      <c r="R22" s="70"/>
+      <c r="S22" s="70"/>
+      <c r="T22" s="70"/>
+      <c r="U22" s="70"/>
+      <c r="V22" s="70"/>
+      <c r="W22" s="70"/>
+      <c r="X22" s="70"/>
+      <c r="Y22" s="70"/>
+      <c r="Z22" s="70"/>
+      <c r="AA22" s="36"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="70"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="87" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="57"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="88">
+        <v>60.0</v>
+      </c>
+      <c r="K23" s="57"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="70"/>
+      <c r="N23" s="70"/>
+      <c r="O23" s="70"/>
+      <c r="P23" s="70"/>
+      <c r="Q23" s="70"/>
+      <c r="R23" s="70"/>
+      <c r="S23" s="70"/>
+      <c r="T23" s="70"/>
+      <c r="U23" s="70"/>
+      <c r="V23" s="70"/>
+      <c r="W23" s="70"/>
+      <c r="X23" s="70"/>
+      <c r="Y23" s="70"/>
+      <c r="Z23" s="70"/>
+      <c r="AA23" s="36"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="70"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="87" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="57"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="88">
+        <v>45.0</v>
+      </c>
+      <c r="K24" s="57"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="70"/>
+      <c r="N24" s="70"/>
+      <c r="O24" s="70"/>
+      <c r="P24" s="70"/>
+      <c r="Q24" s="70"/>
+      <c r="R24" s="70"/>
+      <c r="S24" s="70"/>
+      <c r="T24" s="70"/>
+      <c r="U24" s="70"/>
+      <c r="V24" s="70"/>
+      <c r="W24" s="70"/>
+      <c r="X24" s="70"/>
+      <c r="Y24" s="70"/>
+      <c r="Z24" s="70"/>
+      <c r="AA24" s="36"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="70"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="57"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="88">
+        <v>25.0</v>
+      </c>
+      <c r="K25" s="57"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="70"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="70"/>
+      <c r="P25" s="70"/>
+      <c r="Q25" s="70"/>
+      <c r="R25" s="70"/>
+      <c r="S25" s="70"/>
+      <c r="T25" s="70"/>
+      <c r="U25" s="70"/>
+      <c r="V25" s="70"/>
+      <c r="W25" s="70"/>
+      <c r="X25" s="70"/>
+      <c r="Y25" s="70"/>
+      <c r="Z25" s="70"/>
+      <c r="AA25" s="36"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="70"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="89">
+        <f>SUM(J23:L25)</f>
+        <v>130</v>
+      </c>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="70"/>
+      <c r="N26" s="70"/>
+      <c r="O26" s="70"/>
+      <c r="P26" s="70"/>
+      <c r="Q26" s="70"/>
+      <c r="R26" s="70"/>
+      <c r="S26" s="70"/>
+      <c r="T26" s="70"/>
+      <c r="U26" s="70"/>
+      <c r="V26" s="70"/>
+      <c r="W26" s="70"/>
+      <c r="X26" s="70"/>
+      <c r="Y26" s="70"/>
+      <c r="Z26" s="70"/>
+      <c r="AA26" s="70"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="D1:O2"/>
+    <mergeCell ref="F20:L21"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="F25:H25"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -3894,175 +5037,288 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="90" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="90" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="92">
+        <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="90">
+        <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="91" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="90">
+        <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="90">
+        <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="90">
+        <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="90">
+        <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="91" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="90">
+        <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="91" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="90">
+        <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="91" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="90">
+        <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="91" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="90">
+        <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="22.14"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="70" t="s">
-        <v>70</v>
+      <c r="B1" s="90" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="70">
+      <c r="B2" s="90">
         <v>11.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="70">
+      <c r="B3" s="90">
         <v>5.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="70">
+      <c r="B4" s="90">
         <v>12.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="70">
+      <c r="B5" s="90">
         <v>5.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="70">
+      <c r="B6" s="90">
         <v>16.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="70">
+      <c r="B7" s="90">
         <v>11.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="70">
+      <c r="B8" s="90">
         <v>-2.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="70">
+      <c r="B9" s="90">
         <v>12.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="70">
+      <c r="B10" s="90">
         <v>7.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="70">
+      <c r="B11" s="90">
         <v>17.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="70">
+      <c r="B12" s="90">
         <v>4.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="70">
+      <c r="B13" s="90">
         <v>8.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="70">
+      <c r="B14" s="90">
         <v>15.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="70">
+      <c r="B15" s="90">
         <v>19.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="70">
+      <c r="B16" s="90">
         <v>12.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="70">
+      <c r="B17" s="90">
         <v>26.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="70">
+      <c r="B18" s="90">
         <v>11.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="70">
+      <c r="B19" s="90">
         <v>8.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="70">
+      <c r="B20" s="90">
         <v>6.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="70">
+      <c r="B21" s="90">
         <v>7.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Week 4 Thursday update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -12,14 +12,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="g0V7LTg/eSjx8a99N05z6zCx+DOe579pUdliY60dtT8="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="4Wt5tiel+ejMppC3CNlgC6WsTwsKS1wmK611ETrU1tY="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
   <si>
     <t>WINTER BEST PAIRS COMP(SUNDAY)</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>JOHN KING</t>
+  </si>
+  <si>
+    <t>STEVE CONNOR</t>
+  </si>
+  <si>
+    <t>COLIN HOPKINS</t>
   </si>
   <si>
     <t>TEAM</t>
@@ -743,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -926,14 +932,17 @@
     <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="42" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="33" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -4108,7 +4117,9 @@
       <c r="F5" s="79">
         <v>33.0</v>
       </c>
-      <c r="G5" s="79"/>
+      <c r="G5" s="80">
+        <v>27.0</v>
+      </c>
       <c r="H5" s="79"/>
       <c r="I5" s="79"/>
       <c r="J5" s="79"/>
@@ -4127,9 +4138,9 @@
       <c r="W5" s="79"/>
       <c r="X5" s="79"/>
       <c r="Y5" s="79"/>
-      <c r="Z5" s="80">
-        <f t="shared" ref="Z5:Z17" si="1">SUM(B5:W5)</f>
-        <v>131</v>
+      <c r="Z5" s="81">
+        <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
+        <v>158</v>
       </c>
       <c r="AA5" s="36"/>
     </row>
@@ -4145,10 +4156,12 @@
         <v>32.0</v>
       </c>
       <c r="E6" s="79"/>
-      <c r="F6" s="81">
+      <c r="F6" s="80">
         <v>39.0</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80">
+        <v>35.0</v>
+      </c>
       <c r="H6" s="79"/>
       <c r="I6" s="79"/>
       <c r="J6" s="79"/>
@@ -4167,9 +4180,9 @@
       <c r="W6" s="79"/>
       <c r="X6" s="79"/>
       <c r="Y6" s="79"/>
-      <c r="Z6" s="80">
+      <c r="Z6" s="81">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="AA6" s="36"/>
     </row>
@@ -4187,10 +4200,12 @@
         <v>32.0</v>
       </c>
       <c r="E7" s="79"/>
-      <c r="F7" s="81">
+      <c r="F7" s="80">
         <v>33.0</v>
       </c>
-      <c r="G7" s="79"/>
+      <c r="G7" s="80">
+        <v>34.0</v>
+      </c>
       <c r="H7" s="79"/>
       <c r="I7" s="79"/>
       <c r="J7" s="79"/>
@@ -4209,9 +4224,9 @@
       <c r="W7" s="79"/>
       <c r="X7" s="79"/>
       <c r="Y7" s="79"/>
-      <c r="Z7" s="80">
+      <c r="Z7" s="81">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="AA7" s="36"/>
     </row>
@@ -4231,10 +4246,12 @@
       <c r="E8" s="79">
         <v>31.0</v>
       </c>
-      <c r="F8" s="81">
+      <c r="F8" s="80">
         <v>31.0</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80">
+        <v>33.0</v>
+      </c>
       <c r="H8" s="79"/>
       <c r="I8" s="79"/>
       <c r="J8" s="79"/>
@@ -4253,9 +4270,9 @@
       <c r="W8" s="79"/>
       <c r="X8" s="79"/>
       <c r="Y8" s="79"/>
-      <c r="Z8" s="80">
+      <c r="Z8" s="81">
         <f t="shared" si="1"/>
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="AA8" s="36"/>
     </row>
@@ -4275,10 +4292,12 @@
       <c r="E9" s="79">
         <v>26.0</v>
       </c>
-      <c r="F9" s="81">
+      <c r="F9" s="80">
         <v>28.0</v>
       </c>
-      <c r="G9" s="79"/>
+      <c r="G9" s="80">
+        <v>26.0</v>
+      </c>
       <c r="H9" s="79"/>
       <c r="I9" s="79"/>
       <c r="J9" s="79"/>
@@ -4297,9 +4316,9 @@
       <c r="W9" s="79"/>
       <c r="X9" s="79"/>
       <c r="Y9" s="79"/>
-      <c r="Z9" s="80">
+      <c r="Z9" s="81">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="AA9" s="36"/>
     </row>
@@ -4315,10 +4334,12 @@
       <c r="E10" s="79">
         <v>23.0</v>
       </c>
-      <c r="F10" s="81">
+      <c r="F10" s="80">
         <v>35.0</v>
       </c>
-      <c r="G10" s="79"/>
+      <c r="G10" s="80">
+        <v>29.0</v>
+      </c>
       <c r="H10" s="79"/>
       <c r="I10" s="79"/>
       <c r="J10" s="79"/>
@@ -4337,9 +4358,9 @@
       <c r="W10" s="79"/>
       <c r="X10" s="79"/>
       <c r="Y10" s="79"/>
-      <c r="Z10" s="80">
+      <c r="Z10" s="81">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="AA10" s="36"/>
     </row>
@@ -4379,7 +4400,7 @@
       <c r="W11" s="79"/>
       <c r="X11" s="79"/>
       <c r="Y11" s="79"/>
-      <c r="Z11" s="80">
+      <c r="Z11" s="81">
         <f t="shared" si="1"/>
         <v>133</v>
       </c>
@@ -4401,7 +4422,7 @@
       <c r="E12" s="79">
         <v>32.0</v>
       </c>
-      <c r="F12" s="81">
+      <c r="F12" s="80">
         <v>34.0</v>
       </c>
       <c r="G12" s="79"/>
@@ -4423,7 +4444,7 @@
       <c r="W12" s="79"/>
       <c r="X12" s="79"/>
       <c r="Y12" s="79"/>
-      <c r="Z12" s="80">
+      <c r="Z12" s="81">
         <f t="shared" si="1"/>
         <v>171</v>
       </c>
@@ -4441,10 +4462,12 @@
       <c r="E13" s="79">
         <v>36.0</v>
       </c>
-      <c r="F13" s="81">
+      <c r="F13" s="80">
         <v>27.0</v>
       </c>
-      <c r="G13" s="79"/>
+      <c r="G13" s="80">
+        <v>37.0</v>
+      </c>
       <c r="H13" s="79"/>
       <c r="I13" s="79"/>
       <c r="J13" s="79"/>
@@ -4463,9 +4486,9 @@
       <c r="W13" s="79"/>
       <c r="X13" s="79"/>
       <c r="Y13" s="79"/>
-      <c r="Z13" s="80">
+      <c r="Z13" s="81">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="AA13" s="36"/>
     </row>
@@ -4479,7 +4502,7 @@
       </c>
       <c r="D14" s="79"/>
       <c r="E14" s="79"/>
-      <c r="F14" s="81">
+      <c r="F14" s="80">
         <v>36.0</v>
       </c>
       <c r="G14" s="79"/>
@@ -4501,7 +4524,7 @@
       <c r="W14" s="79"/>
       <c r="X14" s="79"/>
       <c r="Y14" s="79"/>
-      <c r="Z14" s="80">
+      <c r="Z14" s="81">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
@@ -4519,10 +4542,12 @@
         <v>25.0</v>
       </c>
       <c r="E15" s="79"/>
-      <c r="F15" s="81">
+      <c r="F15" s="80">
         <v>32.0</v>
       </c>
-      <c r="G15" s="79"/>
+      <c r="G15" s="80">
+        <v>30.0</v>
+      </c>
       <c r="H15" s="79"/>
       <c r="I15" s="79"/>
       <c r="J15" s="79"/>
@@ -4541,9 +4566,9 @@
       <c r="W15" s="79"/>
       <c r="X15" s="79"/>
       <c r="Y15" s="79"/>
-      <c r="Z15" s="80">
+      <c r="Z15" s="81">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="AA15" s="36"/>
     </row>
@@ -4559,10 +4584,12 @@
         <v>28.0</v>
       </c>
       <c r="E16" s="79"/>
-      <c r="F16" s="81">
+      <c r="F16" s="80">
         <v>23.0</v>
       </c>
-      <c r="G16" s="79"/>
+      <c r="G16" s="80">
+        <v>30.0</v>
+      </c>
       <c r="H16" s="79"/>
       <c r="I16" s="79"/>
       <c r="J16" s="79"/>
@@ -4581,28 +4608,24 @@
       <c r="W16" s="79"/>
       <c r="X16" s="79"/>
       <c r="Y16" s="79"/>
-      <c r="Z16" s="80">
+      <c r="Z16" s="81">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="AA16" s="36"/>
     </row>
     <row r="17">
-      <c r="A17" s="78" t="s">
-        <v>47</v>
+      <c r="A17" s="83" t="s">
+        <v>64</v>
       </c>
       <c r="B17" s="79"/>
       <c r="C17" s="79"/>
-      <c r="D17" s="79">
-        <v>41.0</v>
-      </c>
-      <c r="E17" s="79">
-        <v>37.0</v>
-      </c>
-      <c r="F17" s="81">
-        <v>38.0</v>
-      </c>
-      <c r="G17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80">
+        <v>26.0</v>
+      </c>
       <c r="H17" s="79"/>
       <c r="I17" s="79"/>
       <c r="J17" s="79"/>
@@ -4621,103 +4644,115 @@
       <c r="W17" s="79"/>
       <c r="X17" s="79"/>
       <c r="Y17" s="79"/>
-      <c r="Z17" s="80">
+      <c r="Z17" s="81">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="AA17" s="36"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80">
+        <v>27.0</v>
+      </c>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="79"/>
+      <c r="R18" s="79"/>
+      <c r="S18" s="79"/>
+      <c r="T18" s="79"/>
+      <c r="U18" s="79"/>
+      <c r="V18" s="79"/>
+      <c r="W18" s="79"/>
+      <c r="X18" s="79"/>
+      <c r="Y18" s="79"/>
+      <c r="Z18" s="81">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="AA18" s="36"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="79"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79">
+        <v>41.0</v>
+      </c>
+      <c r="E19" s="79">
+        <v>37.0</v>
+      </c>
+      <c r="F19" s="80">
+        <v>38.0</v>
+      </c>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="79"/>
+      <c r="O19" s="79"/>
+      <c r="P19" s="79"/>
+      <c r="Q19" s="79"/>
+      <c r="R19" s="79"/>
+      <c r="S19" s="79"/>
+      <c r="T19" s="79"/>
+      <c r="U19" s="79"/>
+      <c r="V19" s="79"/>
+      <c r="W19" s="79"/>
+      <c r="X19" s="79"/>
+      <c r="Y19" s="79"/>
+      <c r="Z19" s="81">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="AA17" s="36"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="83"/>
-      <c r="B18" s="77"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="77"/>
-      <c r="E18" s="77"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="77"/>
-      <c r="J18" s="77"/>
-      <c r="K18" s="77"/>
-      <c r="L18" s="77"/>
-      <c r="M18" s="77"/>
-      <c r="N18" s="77"/>
-      <c r="O18" s="77"/>
-      <c r="P18" s="77"/>
-      <c r="Q18" s="77"/>
-      <c r="R18" s="77"/>
-      <c r="S18" s="77"/>
-      <c r="T18" s="77"/>
-      <c r="U18" s="77"/>
-      <c r="V18" s="77"/>
-      <c r="W18" s="77"/>
-      <c r="X18" s="77"/>
-      <c r="Y18" s="77"/>
-      <c r="Z18" s="77"/>
-      <c r="AA18" s="36"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="70"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
-      <c r="J19" s="70"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="70"/>
-      <c r="N19" s="70"/>
-      <c r="O19" s="70"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="70"/>
-      <c r="R19" s="70"/>
-      <c r="S19" s="70"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="70"/>
-      <c r="V19" s="70"/>
-      <c r="W19" s="70"/>
-      <c r="X19" s="70"/>
-      <c r="Y19" s="70"/>
-      <c r="Z19" s="70"/>
       <c r="AA19" s="36"/>
     </row>
     <row r="20">
-      <c r="A20" s="84" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="85">
-        <v>10.0</v>
-      </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="86" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="70"/>
-      <c r="N20" s="70"/>
-      <c r="O20" s="70"/>
-      <c r="P20" s="70"/>
-      <c r="Q20" s="70"/>
-      <c r="R20" s="70"/>
-      <c r="S20" s="70"/>
-      <c r="T20" s="70"/>
-      <c r="U20" s="70"/>
-      <c r="V20" s="70"/>
-      <c r="W20" s="70"/>
-      <c r="X20" s="70"/>
-      <c r="Y20" s="70"/>
-      <c r="Z20" s="70"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="77"/>
+      <c r="P20" s="77"/>
+      <c r="Q20" s="77"/>
+      <c r="R20" s="77"/>
+      <c r="S20" s="77"/>
+      <c r="T20" s="77"/>
+      <c r="U20" s="77"/>
+      <c r="V20" s="77"/>
+      <c r="W20" s="77"/>
+      <c r="X20" s="77"/>
+      <c r="Y20" s="77"/>
+      <c r="Z20" s="77"/>
       <c r="AA20" s="36"/>
     </row>
     <row r="21">
@@ -4726,13 +4761,13 @@
       <c r="C21" s="70"/>
       <c r="D21" s="70"/>
       <c r="E21" s="70"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
       <c r="M21" s="70"/>
       <c r="N21" s="70"/>
       <c r="O21" s="70"/>
@@ -4750,18 +4785,24 @@
       <c r="AA21" s="36"/>
     </row>
     <row r="22">
-      <c r="A22" s="70"/>
-      <c r="B22" s="70"/>
+      <c r="A22" s="85" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="86">
+        <v>10.0</v>
+      </c>
       <c r="C22" s="70"/>
       <c r="D22" s="70"/>
       <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="70"/>
+      <c r="F22" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5"/>
       <c r="M22" s="70"/>
       <c r="N22" s="70"/>
       <c r="O22" s="70"/>
@@ -4784,17 +4825,13 @@
       <c r="C23" s="70"/>
       <c r="D23" s="70"/>
       <c r="E23" s="70"/>
-      <c r="F23" s="87" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="57"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="88">
-        <v>60.0</v>
-      </c>
-      <c r="K23" s="57"/>
-      <c r="L23" s="55"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="8"/>
       <c r="M23" s="70"/>
       <c r="N23" s="70"/>
       <c r="O23" s="70"/>
@@ -4817,17 +4854,13 @@
       <c r="C24" s="70"/>
       <c r="D24" s="70"/>
       <c r="E24" s="70"/>
-      <c r="F24" s="87" t="s">
-        <v>55</v>
-      </c>
-      <c r="G24" s="57"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="77"/>
-      <c r="J24" s="88">
-        <v>45.0</v>
-      </c>
-      <c r="K24" s="57"/>
-      <c r="L24" s="55"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="70"/>
       <c r="M24" s="70"/>
       <c r="N24" s="70"/>
       <c r="O24" s="70"/>
@@ -4850,14 +4883,14 @@
       <c r="C25" s="70"/>
       <c r="D25" s="70"/>
       <c r="E25" s="70"/>
-      <c r="F25" s="87" t="s">
-        <v>56</v>
+      <c r="F25" s="88" t="s">
+        <v>54</v>
       </c>
       <c r="G25" s="57"/>
       <c r="H25" s="55"/>
       <c r="I25" s="77"/>
-      <c r="J25" s="88">
-        <v>25.0</v>
+      <c r="J25" s="89">
+        <v>60.0</v>
       </c>
       <c r="K25" s="57"/>
       <c r="L25" s="55"/>
@@ -4883,16 +4916,17 @@
       <c r="C26" s="70"/>
       <c r="D26" s="70"/>
       <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
+      <c r="F26" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="57"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="77"/>
       <c r="J26" s="89">
-        <f>SUM(J23:L25)</f>
-        <v>130</v>
-      </c>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
+        <v>45.0</v>
+      </c>
+      <c r="K26" s="57"/>
+      <c r="L26" s="55"/>
       <c r="M26" s="70"/>
       <c r="N26" s="70"/>
       <c r="O26" s="70"/>
@@ -4907,19 +4941,84 @@
       <c r="X26" s="70"/>
       <c r="Y26" s="70"/>
       <c r="Z26" s="70"/>
-      <c r="AA26" s="70"/>
+      <c r="AA26" s="36"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="70"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="57"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="77"/>
+      <c r="J27" s="89">
+        <v>25.0</v>
+      </c>
+      <c r="K27" s="57"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="70"/>
+      <c r="N27" s="70"/>
+      <c r="O27" s="70"/>
+      <c r="P27" s="70"/>
+      <c r="Q27" s="70"/>
+      <c r="R27" s="70"/>
+      <c r="S27" s="70"/>
+      <c r="T27" s="70"/>
+      <c r="U27" s="70"/>
+      <c r="V27" s="70"/>
+      <c r="W27" s="70"/>
+      <c r="X27" s="70"/>
+      <c r="Y27" s="70"/>
+      <c r="Z27" s="70"/>
+      <c r="AA27" s="36"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="70"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="90">
+        <f>SUM(J25:L27)</f>
+        <v>130</v>
+      </c>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="70"/>
+      <c r="N28" s="70"/>
+      <c r="O28" s="70"/>
+      <c r="P28" s="70"/>
+      <c r="Q28" s="70"/>
+      <c r="R28" s="70"/>
+      <c r="S28" s="70"/>
+      <c r="T28" s="70"/>
+      <c r="U28" s="70"/>
+      <c r="V28" s="70"/>
+      <c r="W28" s="70"/>
+      <c r="X28" s="70"/>
+      <c r="Y28" s="70"/>
+      <c r="Z28" s="70"/>
+      <c r="AA28" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="D1:O2"/>
+    <mergeCell ref="F22:L23"/>
+    <mergeCell ref="F25:H25"/>
     <mergeCell ref="J25:L25"/>
+    <mergeCell ref="F26:H26"/>
     <mergeCell ref="J26:L26"/>
-    <mergeCell ref="D1:O2"/>
-    <mergeCell ref="F20:L21"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F27:H27"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4936,99 +5035,99 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="90" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="90" t="s">
-        <v>65</v>
+      <c r="A1" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="91" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="92">
+      <c r="A2" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="93">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
         <v>8</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="91" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="90">
+      <c r="A3" s="92" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="91">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
         <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="91" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="90">
+      <c r="A4" s="92" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="91">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
         <v>8</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="91" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="90">
+      <c r="A5" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="91">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
         <v>5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="91" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="90">
+      <c r="A6" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="91">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
         <v>9</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="91" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="90">
+      <c r="A7" s="92" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="91">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
         <v>5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="91" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="90">
+      <c r="A8" s="92" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="91">
         <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="91" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="90">
+      <c r="A9" s="92" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="91">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
         <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="91" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="90">
+      <c r="A10" s="92" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="91">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
         <v>10</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="91" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="90">
+      <c r="A11" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="91">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
         <v>7</v>
       </c>
@@ -5053,238 +5152,254 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="90" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="90" t="s">
-        <v>77</v>
+      <c r="B1" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="90">
+      <c r="B2" s="91">
         <v>11.0</v>
       </c>
-      <c r="C2" s="90">
+      <c r="C2" s="91">
         <v>11.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="90">
+      <c r="B3" s="91">
         <v>5.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="90">
+      <c r="B4" s="91">
         <v>12.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="90">
+      <c r="B5" s="91">
         <v>5.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="90">
+      <c r="B6" s="91">
         <v>16.0</v>
       </c>
-      <c r="C6" s="90">
+      <c r="C6" s="91">
         <v>16.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="90">
+      <c r="B7" s="91">
         <v>11.0</v>
       </c>
-      <c r="C7" s="90">
+      <c r="C7" s="91">
         <v>11.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="90">
+      <c r="B8" s="91">
         <v>-2.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="90">
+      <c r="B9" s="91">
         <v>12.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="90">
+      <c r="B10" s="91">
         <v>7.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="90">
+      <c r="B11" s="91">
         <v>17.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="90">
+      <c r="B12" s="91">
         <v>4.0</v>
       </c>
-      <c r="C12" s="90">
+      <c r="C12" s="91">
         <v>4.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="90">
+      <c r="B13" s="91">
         <v>8.0</v>
       </c>
-      <c r="C13" s="90">
+      <c r="C13" s="91">
         <v>8.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="90">
+      <c r="B14" s="91">
         <v>15.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="93" t="s">
+      <c r="A15" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="90">
+      <c r="B15" s="91">
         <v>19.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="90">
+      <c r="B16" s="91">
         <v>12.0</v>
       </c>
-      <c r="C16" s="90">
+      <c r="C16" s="91">
         <v>12.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="90">
+      <c r="B17" s="91">
         <v>26.0</v>
       </c>
-      <c r="C17" s="90">
+      <c r="C17" s="91">
         <v>26.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="93" t="s">
+      <c r="A18" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="90">
+      <c r="B18" s="91">
         <v>11.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="93" t="s">
+      <c r="A19" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="90">
+      <c r="B19" s="91">
         <v>8.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="93" t="s">
+      <c r="A20" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="90">
+      <c r="B20" s="91">
         <v>6.0</v>
       </c>
-      <c r="C20" s="90">
+      <c r="C20" s="91">
         <v>6.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="90">
+      <c r="B21" s="91">
         <v>7.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="90">
+      <c r="C22" s="91">
         <v>14.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="90" t="s">
+      <c r="A23" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="90">
+      <c r="C23" s="91">
         <v>11.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="90">
+      <c r="C24" s="91">
         <v>14.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="90">
+      <c r="C25" s="91">
         <v>26.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="90" t="s">
+      <c r="A26" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="90">
+      <c r="C26" s="91">
         <v>24.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="91">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="91">
+        <v>21.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
010 Week 6 Pairs data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -1640,7 +1640,9 @@
       <c r="H12" s="32">
         <v>31.0</v>
       </c>
-      <c r="I12" s="31"/>
+      <c r="I12" s="32">
+        <v>32.0</v>
+      </c>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
@@ -1661,11 +1663,11 @@
       <c r="AA12" s="33"/>
       <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>258</v>
+        <v>290</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36"/>
@@ -1731,7 +1733,9 @@
       <c r="H14" s="32">
         <v>39.0</v>
       </c>
-      <c r="I14" s="31"/>
+      <c r="I14" s="32">
+        <v>33.0</v>
+      </c>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
@@ -1752,11 +1756,11 @@
       <c r="AA14" s="33"/>
       <c r="AB14" s="34">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
-        <v>169</v>
+        <v>232</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="36"/>
@@ -1778,7 +1782,9 @@
       <c r="H15" s="41">
         <v>38.0</v>
       </c>
-      <c r="I15" s="40"/>
+      <c r="I15" s="41">
+        <v>30.0</v>
+      </c>
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
       <c r="L15" s="40"/>
@@ -1799,7 +1805,7 @@
       <c r="AA15" s="42"/>
       <c r="AB15" s="34">
         <f t="shared" si="1"/>
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
@@ -1824,7 +1830,9 @@
       <c r="H16" s="32">
         <v>27.0</v>
       </c>
-      <c r="I16" s="31"/>
+      <c r="I16" s="32">
+        <v>28.0</v>
+      </c>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
@@ -1845,11 +1853,11 @@
       <c r="AA16" s="33"/>
       <c r="AB16" s="34">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>250</v>
+        <v>312</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36"/>
@@ -1873,7 +1881,9 @@
       <c r="H17" s="41">
         <v>32.0</v>
       </c>
-      <c r="I17" s="40"/>
+      <c r="I17" s="41">
+        <v>34.0</v>
+      </c>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
       <c r="L17" s="40"/>
@@ -1894,7 +1904,7 @@
       <c r="AA17" s="42"/>
       <c r="AB17" s="34">
         <f t="shared" si="1"/>
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
@@ -1917,7 +1927,9 @@
       <c r="H18" s="32">
         <v>33.0</v>
       </c>
-      <c r="I18" s="31"/>
+      <c r="I18" s="32">
+        <v>36.0</v>
+      </c>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
@@ -1938,11 +1950,11 @@
       <c r="AA18" s="33"/>
       <c r="AB18" s="34">
         <f t="shared" si="1"/>
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="AC18" s="35">
         <f>SUM(AB18:AB19)</f>
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="36"/>
@@ -2008,7 +2020,9 @@
       <c r="H20" s="32">
         <v>38.0</v>
       </c>
-      <c r="I20" s="31"/>
+      <c r="I20" s="32">
+        <v>38.0</v>
+      </c>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
       <c r="L20" s="31"/>
@@ -2029,11 +2043,11 @@
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>307</v>
+        <v>376</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36"/>
@@ -2059,7 +2073,9 @@
       <c r="H21" s="41">
         <v>32.0</v>
       </c>
-      <c r="I21" s="40"/>
+      <c r="I21" s="41">
+        <v>31.0</v>
+      </c>
       <c r="J21" s="40"/>
       <c r="K21" s="40"/>
       <c r="L21" s="40"/>
@@ -2080,7 +2096,7 @@
       <c r="AA21" s="42"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
@@ -2101,7 +2117,9 @@
         <v>35.0</v>
       </c>
       <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
+      <c r="I22" s="32">
+        <v>25.0</v>
+      </c>
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
@@ -2122,11 +2140,11 @@
       <c r="AA22" s="33"/>
       <c r="AB22" s="34">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="AC22" s="35">
         <f>SUM(AB22:AB23)</f>
-        <v>151</v>
+        <v>203</v>
       </c>
       <c r="AD22" s="5"/>
       <c r="AE22" s="36"/>
@@ -2148,7 +2166,9 @@
       <c r="H23" s="41">
         <v>28.0</v>
       </c>
-      <c r="I23" s="40"/>
+      <c r="I23" s="41">
+        <v>27.0</v>
+      </c>
       <c r="J23" s="40"/>
       <c r="K23" s="40"/>
       <c r="L23" s="40"/>
@@ -2169,7 +2189,7 @@
       <c r="AA23" s="42"/>
       <c r="AB23" s="34">
         <f t="shared" si="1"/>
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="AC23" s="6"/>
       <c r="AD23" s="8"/>
@@ -2215,7 +2235,7 @@
       </c>
       <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="36"/>
@@ -2239,7 +2259,9 @@
       <c r="H25" s="41">
         <v>34.0</v>
       </c>
-      <c r="I25" s="40"/>
+      <c r="I25" s="41">
+        <v>26.0</v>
+      </c>
       <c r="J25" s="40"/>
       <c r="K25" s="40"/>
       <c r="L25" s="40"/>
@@ -2260,7 +2282,7 @@
       <c r="AA25" s="42"/>
       <c r="AB25" s="34">
         <f t="shared" si="1"/>
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
@@ -2285,7 +2307,9 @@
       <c r="H26" s="32">
         <v>31.0</v>
       </c>
-      <c r="I26" s="31"/>
+      <c r="I26" s="32">
+        <v>30.0</v>
+      </c>
       <c r="J26" s="31"/>
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
@@ -2306,11 +2330,11 @@
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>277</v>
+        <v>328</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36"/>
@@ -2334,7 +2358,9 @@
       <c r="H27" s="41">
         <v>28.0</v>
       </c>
-      <c r="I27" s="40"/>
+      <c r="I27" s="41">
+        <v>21.0</v>
+      </c>
       <c r="J27" s="40"/>
       <c r="K27" s="40"/>
       <c r="L27" s="40"/>
@@ -2355,7 +2381,7 @@
       <c r="AA27" s="42"/>
       <c r="AB27" s="34">
         <f t="shared" si="1"/>
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
@@ -2382,7 +2408,9 @@
       <c r="H28" s="32">
         <v>29.0</v>
       </c>
-      <c r="I28" s="31"/>
+      <c r="I28" s="32">
+        <v>29.0</v>
+      </c>
       <c r="J28" s="31"/>
       <c r="K28" s="31"/>
       <c r="L28" s="31"/>
@@ -2403,11 +2431,11 @@
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>311</v>
+        <v>376</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36"/>
@@ -2433,7 +2461,9 @@
       <c r="H29" s="41">
         <v>36.0</v>
       </c>
-      <c r="I29" s="40"/>
+      <c r="I29" s="41">
+        <v>36.0</v>
+      </c>
       <c r="J29" s="40"/>
       <c r="K29" s="40"/>
       <c r="L29" s="40"/>
@@ -2454,7 +2484,7 @@
       <c r="AA29" s="42"/>
       <c r="AB29" s="34">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -2502,7 +2532,7 @@
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>220</v>
+        <v>259</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36"/>
@@ -2526,7 +2556,9 @@
       <c r="H31" s="41">
         <v>29.0</v>
       </c>
-      <c r="I31" s="40"/>
+      <c r="I31" s="41">
+        <v>39.0</v>
+      </c>
       <c r="J31" s="40"/>
       <c r="K31" s="40"/>
       <c r="L31" s="40"/>
@@ -2547,7 +2579,7 @@
       <c r="AA31" s="51"/>
       <c r="AB31" s="52">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
@@ -5048,7 +5080,7 @@
       </c>
       <c r="B2" s="93">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -5057,7 +5089,7 @@
       </c>
       <c r="B3" s="91">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -5066,7 +5098,7 @@
       </c>
       <c r="B4" s="91">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -5075,7 +5107,7 @@
       </c>
       <c r="B5" s="91">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -5084,7 +5116,7 @@
       </c>
       <c r="B6" s="91">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -5093,7 +5125,7 @@
       </c>
       <c r="B7" s="91">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -5111,7 +5143,7 @@
       </c>
       <c r="B9" s="91">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -5120,7 +5152,7 @@
       </c>
       <c r="B10" s="91">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -5129,7 +5161,7 @@
       </c>
       <c r="B11" s="91">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
011 Handicap data and list corrected
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -5,14 +5,14 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="THURSDAY SINGLES" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="xxDO NOT EDITxx" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="HANDICAPS" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="HANDICAPS" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="xxDO NOT EDITxx" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="4Wt5tiel+ejMppC3CNlgC6WsTwsKS1wmK611ETrU1tY="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="v/KD0ODkBienac8CW8rI205HTBNrDy3c9ezNXsDl4lg="/>
     </ext>
   </extLst>
 </workbook>
@@ -219,6 +219,12 @@
     <t>COLIN HOPKINS</t>
   </si>
   <si>
+    <t>HANDICAP</t>
+  </si>
+  <si>
+    <t>HANDICAP THURS</t>
+  </si>
+  <si>
     <t>TEAM</t>
   </si>
   <si>
@@ -253,12 +259,6 @@
   </si>
   <si>
     <t>SCOTT &amp; ANDY</t>
-  </si>
-  <si>
-    <t>HANDICAP</t>
-  </si>
-  <si>
-    <t>HANDICAP THURS</t>
   </si>
 </sst>
 </file>
@@ -749,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="99">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -965,13 +965,21 @@
     <xf borderId="16" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -5065,103 +5073,279 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="22.14"/>
+    <col customWidth="1" min="3" max="3" width="17.43"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="C1" s="92" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="92" t="s">
-        <v>68</v>
+      <c r="A2" s="91" t="s">
+        <v>29</v>
       </c>
       <c r="B2" s="93">
-        <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>9</v>
+        <v>11.0</v>
+      </c>
+      <c r="C2" s="94">
+        <v>11.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="92" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="91">
-        <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
-        <v>7</v>
-      </c>
+      <c r="A3" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="93">
+        <v>5.0</v>
+      </c>
+      <c r="C3" s="95"/>
     </row>
     <row r="4">
-      <c r="A4" s="92" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="91">
-        <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>10</v>
-      </c>
+      <c r="A4" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="93">
+        <v>11.0</v>
+      </c>
+      <c r="C4" s="95"/>
     </row>
     <row r="5">
-      <c r="A5" s="92" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="91">
-        <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>6</v>
-      </c>
+      <c r="A5" s="91" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="93">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="95"/>
     </row>
     <row r="6">
-      <c r="A6" s="92" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="91">
-        <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>11</v>
+      <c r="A6" s="91" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="93">
+        <v>16.0</v>
+      </c>
+      <c r="C6" s="94">
+        <v>16.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="92" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="91">
-        <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>7</v>
+      <c r="A7" s="91" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="93">
+        <v>12.0</v>
+      </c>
+      <c r="C7" s="94">
+        <v>12.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="92" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="91">
-        <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
-        <v>3</v>
-      </c>
+      <c r="A8" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="93">
+        <v>-2.0</v>
+      </c>
+      <c r="C8" s="95"/>
     </row>
     <row r="9">
-      <c r="A9" s="92" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="91">
-        <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>10</v>
-      </c>
+      <c r="A9" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="93">
+        <v>12.0</v>
+      </c>
+      <c r="C9" s="95"/>
     </row>
     <row r="10">
-      <c r="A10" s="92" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="91">
-        <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>12</v>
-      </c>
+      <c r="A10" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="93">
+        <v>6.0</v>
+      </c>
+      <c r="C10" s="95"/>
     </row>
     <row r="11">
-      <c r="A11" s="92" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="91">
-        <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+      <c r="A11" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="93">
+        <v>18.0</v>
+      </c>
+      <c r="C11" s="95"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="93">
+        <v>5.0</v>
+      </c>
+      <c r="C12" s="94">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="93">
+        <v>9.0</v>
+      </c>
+      <c r="C13" s="94">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="93">
+        <v>15.0</v>
+      </c>
+      <c r="C14" s="95"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="93">
+        <v>18.0</v>
+      </c>
+      <c r="C15" s="95"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="93">
+        <v>12.0</v>
+      </c>
+      <c r="C16" s="94">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="91" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="93">
+        <v>27.0</v>
+      </c>
+      <c r="C17" s="94">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="93">
+        <v>11.0</v>
+      </c>
+      <c r="C18" s="95"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="91" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="93">
+        <v>8.0</v>
+      </c>
+      <c r="C19" s="95"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="91" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="93">
+        <v>6.0</v>
+      </c>
+      <c r="C20" s="94">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="91" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="93">
+        <v>6.0</v>
+      </c>
+      <c r="C21" s="95"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="96"/>
+      <c r="C22" s="94">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="92" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="96"/>
+      <c r="C23" s="94">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="92" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="96"/>
+      <c r="C24" s="94">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="92" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="96"/>
+      <c r="C25" s="94">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="96"/>
+      <c r="C26" s="94">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="92" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="96"/>
+      <c r="C27" s="94">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="92" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="96"/>
+      <c r="C28" s="94">
+        <v>21.0</v>
       </c>
     </row>
   </sheetData>
@@ -5178,260 +5362,103 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="22.14"/>
-    <col customWidth="1" min="3" max="3" width="17.43"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="92" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="97" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="98">
+        <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="92">
+        <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="97" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="92">
+        <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="97" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="92">
+        <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="97" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="92">
+        <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="97" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="92">
+        <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="97" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="92">
+        <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="B1" s="91" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" s="97" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="92">
+        <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="91" t="s">
+      <c r="B10" s="92">
+        <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="97" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="91">
-        <v>11.0</v>
-      </c>
-      <c r="C2" s="91">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="94" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="91">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="94" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="91">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="91">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="94" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="91">
-        <v>16.0</v>
-      </c>
-      <c r="C6" s="91">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="94" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="91">
-        <v>11.0</v>
-      </c>
-      <c r="C7" s="91">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="94" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="91">
-        <v>-2.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="94" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="91">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="94" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="91">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="94" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="91">
-        <v>17.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="94" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="91">
-        <v>4.0</v>
-      </c>
-      <c r="C12" s="91">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="94" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="91">
-        <v>8.0</v>
-      </c>
-      <c r="C13" s="91">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="94" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="91">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="94" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="91">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="94" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="91">
-        <v>12.0</v>
-      </c>
-      <c r="C16" s="91">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="94" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="91">
-        <v>26.0</v>
-      </c>
-      <c r="C17" s="91">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="94" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="91">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="94" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="91">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="94" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="91">
-        <v>6.0</v>
-      </c>
-      <c r="C20" s="91">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="94" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="91">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="91" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="91">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="91" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="91">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="91" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="91">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="91" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="91">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="91" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="91">
-        <v>24.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="91" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="91">
-        <v>29.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="91" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="91">
-        <v>21.0</v>
+      <c r="B11" s="92">
+        <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
012 Week 7 data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -1938,7 +1938,7 @@
       <c r="I18" s="32">
         <v>36.0</v>
       </c>
-      <c r="J18" s="31"/>
+      <c r="J18" s="32"/>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
       <c r="M18" s="31"/>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="H19" s="40"/>
       <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
+      <c r="J19" s="41"/>
       <c r="K19" s="40"/>
       <c r="L19" s="40"/>
       <c r="M19" s="40"/>
@@ -2031,7 +2031,7 @@
       <c r="I20" s="32">
         <v>38.0</v>
       </c>
-      <c r="J20" s="31"/>
+      <c r="J20" s="32"/>
       <c r="K20" s="31"/>
       <c r="L20" s="31"/>
       <c r="M20" s="31"/>
@@ -2084,7 +2084,7 @@
       <c r="I21" s="41">
         <v>31.0</v>
       </c>
-      <c r="J21" s="40"/>
+      <c r="J21" s="41"/>
       <c r="K21" s="40"/>
       <c r="L21" s="40"/>
       <c r="M21" s="40"/>
@@ -2128,7 +2128,7 @@
       <c r="I22" s="32">
         <v>25.0</v>
       </c>
-      <c r="J22" s="31"/>
+      <c r="J22" s="32"/>
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
       <c r="M22" s="31"/>
@@ -2177,7 +2177,7 @@
       <c r="I23" s="41">
         <v>27.0</v>
       </c>
-      <c r="J23" s="40"/>
+      <c r="J23" s="41"/>
       <c r="K23" s="40"/>
       <c r="L23" s="40"/>
       <c r="M23" s="40"/>
@@ -4160,7 +4160,9 @@
       <c r="G5" s="80">
         <v>27.0</v>
       </c>
-      <c r="H5" s="79"/>
+      <c r="H5" s="80">
+        <v>27.0</v>
+      </c>
       <c r="I5" s="79"/>
       <c r="J5" s="79"/>
       <c r="K5" s="79"/>
@@ -4180,7 +4182,7 @@
       <c r="Y5" s="79"/>
       <c r="Z5" s="81">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="AA5" s="36"/>
     </row>
@@ -4202,7 +4204,9 @@
       <c r="G6" s="80">
         <v>35.0</v>
       </c>
-      <c r="H6" s="79"/>
+      <c r="H6" s="80">
+        <v>27.0</v>
+      </c>
       <c r="I6" s="79"/>
       <c r="J6" s="79"/>
       <c r="K6" s="79"/>
@@ -4222,7 +4226,7 @@
       <c r="Y6" s="79"/>
       <c r="Z6" s="81">
         <f t="shared" si="1"/>
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="AA6" s="36"/>
     </row>
@@ -4246,7 +4250,9 @@
       <c r="G7" s="80">
         <v>34.0</v>
       </c>
-      <c r="H7" s="79"/>
+      <c r="H7" s="80">
+        <v>26.0</v>
+      </c>
       <c r="I7" s="79"/>
       <c r="J7" s="79"/>
       <c r="K7" s="79"/>
@@ -4266,7 +4272,7 @@
       <c r="Y7" s="79"/>
       <c r="Z7" s="81">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="AA7" s="36"/>
     </row>
@@ -4292,7 +4298,9 @@
       <c r="G8" s="80">
         <v>33.0</v>
       </c>
-      <c r="H8" s="79"/>
+      <c r="H8" s="80">
+        <v>36.0</v>
+      </c>
       <c r="I8" s="79"/>
       <c r="J8" s="79"/>
       <c r="K8" s="79"/>
@@ -4312,7 +4320,7 @@
       <c r="Y8" s="79"/>
       <c r="Z8" s="81">
         <f t="shared" si="1"/>
-        <v>199</v>
+        <v>235</v>
       </c>
       <c r="AA8" s="36"/>
     </row>
@@ -4338,7 +4346,9 @@
       <c r="G9" s="80">
         <v>26.0</v>
       </c>
-      <c r="H9" s="79"/>
+      <c r="H9" s="80">
+        <v>20.0</v>
+      </c>
       <c r="I9" s="79"/>
       <c r="J9" s="79"/>
       <c r="K9" s="79"/>
@@ -4358,7 +4368,7 @@
       <c r="Y9" s="79"/>
       <c r="Z9" s="81">
         <f t="shared" si="1"/>
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="AA9" s="36"/>
     </row>
@@ -4380,7 +4390,9 @@
       <c r="G10" s="80">
         <v>29.0</v>
       </c>
-      <c r="H10" s="79"/>
+      <c r="H10" s="80">
+        <v>16.0</v>
+      </c>
       <c r="I10" s="79"/>
       <c r="J10" s="79"/>
       <c r="K10" s="79"/>
@@ -4400,7 +4412,7 @@
       <c r="Y10" s="79"/>
       <c r="Z10" s="81">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="AA10" s="36"/>
     </row>
@@ -4422,7 +4434,9 @@
       </c>
       <c r="F11" s="79"/>
       <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
+      <c r="H11" s="80">
+        <v>23.0</v>
+      </c>
       <c r="I11" s="79"/>
       <c r="J11" s="79"/>
       <c r="K11" s="79"/>
@@ -4442,7 +4456,7 @@
       <c r="Y11" s="79"/>
       <c r="Z11" s="81">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="AA11" s="36"/>
     </row>
@@ -4466,7 +4480,9 @@
         <v>34.0</v>
       </c>
       <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
+      <c r="H12" s="80">
+        <v>28.0</v>
+      </c>
       <c r="I12" s="79"/>
       <c r="J12" s="79"/>
       <c r="K12" s="79"/>
@@ -4486,7 +4502,7 @@
       <c r="Y12" s="79"/>
       <c r="Z12" s="81">
         <f t="shared" si="1"/>
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="AA12" s="36"/>
     </row>
@@ -4508,7 +4524,9 @@
       <c r="G13" s="80">
         <v>37.0</v>
       </c>
-      <c r="H13" s="79"/>
+      <c r="H13" s="80">
+        <v>31.0</v>
+      </c>
       <c r="I13" s="79"/>
       <c r="J13" s="79"/>
       <c r="K13" s="79"/>
@@ -4528,7 +4546,7 @@
       <c r="Y13" s="79"/>
       <c r="Z13" s="81">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="AA13" s="36"/>
     </row>
@@ -4588,7 +4606,9 @@
       <c r="G15" s="80">
         <v>30.0</v>
       </c>
-      <c r="H15" s="79"/>
+      <c r="H15" s="80">
+        <v>34.0</v>
+      </c>
       <c r="I15" s="79"/>
       <c r="J15" s="79"/>
       <c r="K15" s="79"/>
@@ -4608,7 +4628,7 @@
       <c r="Y15" s="79"/>
       <c r="Z15" s="81">
         <f t="shared" si="1"/>
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="AA15" s="36"/>
     </row>
@@ -5094,10 +5114,10 @@
         <v>29</v>
       </c>
       <c r="B2" s="93">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="C2" s="94">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="3">
@@ -5132,10 +5152,10 @@
         <v>33</v>
       </c>
       <c r="B6" s="93">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="C6" s="94">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="7">
@@ -5291,7 +5311,7 @@
       </c>
       <c r="B22" s="96"/>
       <c r="C22" s="94">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="23">
@@ -5300,7 +5320,7 @@
       </c>
       <c r="B23" s="96"/>
       <c r="C23" s="94">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="24">
@@ -5309,7 +5329,7 @@
       </c>
       <c r="B24" s="96"/>
       <c r="C24" s="94">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="25">

</xml_diff>

<commit_message>
014 Week 8 data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -1652,7 +1652,9 @@
         <v>32.0</v>
       </c>
       <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
+      <c r="K12" s="32">
+        <v>32.0</v>
+      </c>
       <c r="L12" s="31"/>
       <c r="M12" s="31"/>
       <c r="N12" s="31"/>
@@ -1671,11 +1673,11 @@
       <c r="AA12" s="33"/>
       <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>290</v>
+        <v>322</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36"/>
@@ -1768,7 +1770,7 @@
       </c>
       <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="36"/>
@@ -1794,7 +1796,9 @@
         <v>30.0</v>
       </c>
       <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
+      <c r="K15" s="41">
+        <v>36.0</v>
+      </c>
       <c r="L15" s="40"/>
       <c r="M15" s="40"/>
       <c r="N15" s="40"/>
@@ -1813,7 +1817,7 @@
       <c r="AA15" s="42"/>
       <c r="AB15" s="34">
         <f t="shared" si="1"/>
-        <v>136</v>
+        <v>172</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
@@ -1842,7 +1846,9 @@
         <v>28.0</v>
       </c>
       <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
+      <c r="K16" s="32">
+        <v>23.0</v>
+      </c>
       <c r="L16" s="31"/>
       <c r="M16" s="31"/>
       <c r="N16" s="31"/>
@@ -1861,11 +1867,11 @@
       <c r="AA16" s="33"/>
       <c r="AB16" s="34">
         <f t="shared" si="1"/>
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>312</v>
+        <v>366</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36"/>
@@ -1893,7 +1899,9 @@
         <v>34.0</v>
       </c>
       <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
+      <c r="K17" s="41">
+        <v>31.0</v>
+      </c>
       <c r="L17" s="40"/>
       <c r="M17" s="40"/>
       <c r="N17" s="40"/>
@@ -1912,7 +1920,7 @@
       <c r="AA17" s="42"/>
       <c r="AB17" s="34">
         <f t="shared" si="1"/>
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
@@ -2032,7 +2040,9 @@
         <v>38.0</v>
       </c>
       <c r="J20" s="32"/>
-      <c r="K20" s="31"/>
+      <c r="K20" s="32">
+        <v>37.0</v>
+      </c>
       <c r="L20" s="31"/>
       <c r="M20" s="31"/>
       <c r="N20" s="31"/>
@@ -2051,11 +2061,11 @@
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>376</v>
+        <v>455</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36"/>
@@ -2085,7 +2095,9 @@
         <v>31.0</v>
       </c>
       <c r="J21" s="41"/>
-      <c r="K21" s="40"/>
+      <c r="K21" s="41">
+        <v>42.0</v>
+      </c>
       <c r="L21" s="40"/>
       <c r="M21" s="40"/>
       <c r="N21" s="40"/>
@@ -2104,7 +2116,7 @@
       <c r="AA21" s="42"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>242</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
@@ -2129,7 +2141,9 @@
         <v>25.0</v>
       </c>
       <c r="J22" s="32"/>
-      <c r="K22" s="31"/>
+      <c r="K22" s="32">
+        <v>35.0</v>
+      </c>
       <c r="L22" s="31"/>
       <c r="M22" s="31"/>
       <c r="N22" s="31"/>
@@ -2148,11 +2162,11 @@
       <c r="AA22" s="33"/>
       <c r="AB22" s="34">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="AC22" s="35">
         <f>SUM(AB22:AB23)</f>
-        <v>203</v>
+        <v>238</v>
       </c>
       <c r="AD22" s="5"/>
       <c r="AE22" s="36"/>
@@ -2243,7 +2257,7 @@
       </c>
       <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
-        <v>232</v>
+        <v>263</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="36"/>
@@ -2271,7 +2285,9 @@
         <v>26.0</v>
       </c>
       <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
+      <c r="K25" s="41">
+        <v>31.0</v>
+      </c>
       <c r="L25" s="40"/>
       <c r="M25" s="40"/>
       <c r="N25" s="40"/>
@@ -2290,7 +2306,7 @@
       <c r="AA25" s="42"/>
       <c r="AB25" s="34">
         <f t="shared" si="1"/>
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
@@ -2319,7 +2335,9 @@
         <v>30.0</v>
       </c>
       <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
+      <c r="K26" s="32">
+        <v>30.0</v>
+      </c>
       <c r="L26" s="31"/>
       <c r="M26" s="31"/>
       <c r="N26" s="31"/>
@@ -2338,11 +2356,11 @@
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>328</v>
+        <v>397</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36"/>
@@ -2370,7 +2388,9 @@
         <v>21.0</v>
       </c>
       <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
+      <c r="K27" s="41">
+        <v>39.0</v>
+      </c>
       <c r="L27" s="40"/>
       <c r="M27" s="40"/>
       <c r="N27" s="40"/>
@@ -2389,7 +2409,7 @@
       <c r="AA27" s="42"/>
       <c r="AB27" s="34">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>199</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
@@ -2420,7 +2440,9 @@
         <v>29.0</v>
       </c>
       <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
+      <c r="K28" s="32">
+        <v>32.0</v>
+      </c>
       <c r="L28" s="31"/>
       <c r="M28" s="31"/>
       <c r="N28" s="31"/>
@@ -2439,11 +2461,11 @@
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>376</v>
+        <v>446</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36"/>
@@ -2473,7 +2495,9 @@
         <v>36.0</v>
       </c>
       <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
+      <c r="K29" s="41">
+        <v>38.0</v>
+      </c>
       <c r="L29" s="40"/>
       <c r="M29" s="40"/>
       <c r="N29" s="40"/>
@@ -2492,7 +2516,7 @@
       <c r="AA29" s="42"/>
       <c r="AB29" s="34">
         <f t="shared" si="1"/>
-        <v>195</v>
+        <v>233</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -2540,7 +2564,7 @@
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>259</v>
+        <v>290</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36"/>
@@ -2568,7 +2592,9 @@
         <v>39.0</v>
       </c>
       <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
+      <c r="K31" s="41">
+        <v>31.0</v>
+      </c>
       <c r="L31" s="40"/>
       <c r="M31" s="40"/>
       <c r="N31" s="40"/>
@@ -2587,7 +2613,7 @@
       <c r="AA31" s="51"/>
       <c r="AB31" s="52">
         <f t="shared" si="1"/>
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
@@ -4163,7 +4189,9 @@
       <c r="H5" s="80">
         <v>27.0</v>
       </c>
-      <c r="I5" s="79"/>
+      <c r="I5" s="80">
+        <v>29.0</v>
+      </c>
       <c r="J5" s="79"/>
       <c r="K5" s="79"/>
       <c r="L5" s="79"/>
@@ -4182,7 +4210,7 @@
       <c r="Y5" s="79"/>
       <c r="Z5" s="81">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="AA5" s="36"/>
     </row>
@@ -4253,7 +4281,9 @@
       <c r="H7" s="80">
         <v>26.0</v>
       </c>
-      <c r="I7" s="79"/>
+      <c r="I7" s="80">
+        <v>29.0</v>
+      </c>
       <c r="J7" s="79"/>
       <c r="K7" s="79"/>
       <c r="L7" s="79"/>
@@ -4272,7 +4302,7 @@
       <c r="Y7" s="79"/>
       <c r="Z7" s="81">
         <f t="shared" si="1"/>
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="AA7" s="36"/>
     </row>
@@ -4301,7 +4331,9 @@
       <c r="H8" s="80">
         <v>36.0</v>
       </c>
-      <c r="I8" s="79"/>
+      <c r="I8" s="80">
+        <v>33.0</v>
+      </c>
       <c r="J8" s="79"/>
       <c r="K8" s="79"/>
       <c r="L8" s="79"/>
@@ -4320,7 +4352,7 @@
       <c r="Y8" s="79"/>
       <c r="Z8" s="81">
         <f t="shared" si="1"/>
-        <v>235</v>
+        <v>268</v>
       </c>
       <c r="AA8" s="36"/>
     </row>
@@ -4483,7 +4515,9 @@
       <c r="H12" s="80">
         <v>28.0</v>
       </c>
-      <c r="I12" s="79"/>
+      <c r="I12" s="80">
+        <v>34.0</v>
+      </c>
       <c r="J12" s="79"/>
       <c r="K12" s="79"/>
       <c r="L12" s="79"/>
@@ -4502,7 +4536,7 @@
       <c r="Y12" s="79"/>
       <c r="Z12" s="81">
         <f t="shared" si="1"/>
-        <v>199</v>
+        <v>233</v>
       </c>
       <c r="AA12" s="36"/>
     </row>
@@ -4651,7 +4685,9 @@
         <v>30.0</v>
       </c>
       <c r="H16" s="79"/>
-      <c r="I16" s="79"/>
+      <c r="I16" s="80">
+        <v>27.0</v>
+      </c>
       <c r="J16" s="79"/>
       <c r="K16" s="79"/>
       <c r="L16" s="79"/>
@@ -4670,7 +4706,7 @@
       <c r="Y16" s="79"/>
       <c r="Z16" s="81">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="AA16" s="36"/>
     </row>
@@ -5397,7 +5433,7 @@
       </c>
       <c r="B2" s="98">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -5406,7 +5442,7 @@
       </c>
       <c r="B3" s="92">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -5415,7 +5451,7 @@
       </c>
       <c r="B4" s="92">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -5433,7 +5469,7 @@
       </c>
       <c r="B6" s="92">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -5442,7 +5478,7 @@
       </c>
       <c r="B7" s="92">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -5460,7 +5496,7 @@
       </c>
       <c r="B9" s="92">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -5469,7 +5505,7 @@
       </c>
       <c r="B10" s="92">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -5478,7 +5514,7 @@
       </c>
       <c r="B11" s="92">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
015 Handicap data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -5237,7 +5237,7 @@
         <v>38</v>
       </c>
       <c r="B11" s="93">
-        <v>18.0</v>
+        <v>16.0</v>
       </c>
       <c r="C11" s="95"/>
     </row>
@@ -5297,10 +5297,10 @@
         <v>44</v>
       </c>
       <c r="B17" s="93">
-        <v>27.0</v>
+        <v>25.0</v>
       </c>
       <c r="C17" s="94">
-        <v>27.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="18">

</xml_diff>

<commit_message>
016 Week 9 data update + avg fix
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="81">
   <si>
     <t>WINTER BEST PAIRS COMP(SUNDAY)</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>WINTER SINGLES (THURSDAY)</t>
+  </si>
+  <si>
+    <t>TOTAL SCORE</t>
   </si>
   <si>
     <t>STEW TAYLOR</t>
@@ -268,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -321,6 +324,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -330,7 +338,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,8 +359,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCFE2F3"/>
         <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor rgb="FFC9DAF8"/>
       </patternFill>
     </fill>
   </fills>
@@ -749,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="105">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -908,6 +928,9 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="7" fillId="0" fontId="9" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" textRotation="90" vertical="center"/>
     </xf>
@@ -924,12 +947,15 @@
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -938,7 +964,16 @@
     <xf borderId="42" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="42" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -947,7 +982,10 @@
     <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="33" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="33" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="42" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -956,7 +994,7 @@
     <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="33" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="33" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -965,22 +1003,22 @@
     <xf borderId="16" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1993,7 +2031,7 @@
       <c r="I19" s="40"/>
       <c r="J19" s="41"/>
       <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="L19" s="41"/>
       <c r="M19" s="40"/>
       <c r="N19" s="40"/>
       <c r="O19" s="40"/>
@@ -2043,7 +2081,7 @@
       <c r="K20" s="32">
         <v>37.0</v>
       </c>
-      <c r="L20" s="31"/>
+      <c r="L20" s="32"/>
       <c r="M20" s="31"/>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
@@ -2098,7 +2136,7 @@
       <c r="K21" s="41">
         <v>42.0</v>
       </c>
-      <c r="L21" s="40"/>
+      <c r="L21" s="41"/>
       <c r="M21" s="40"/>
       <c r="N21" s="40"/>
       <c r="O21" s="40"/>
@@ -2144,7 +2182,7 @@
       <c r="K22" s="32">
         <v>35.0</v>
       </c>
-      <c r="L22" s="31"/>
+      <c r="L22" s="32"/>
       <c r="M22" s="31"/>
       <c r="N22" s="31"/>
       <c r="O22" s="31"/>
@@ -2193,7 +2231,7 @@
       </c>
       <c r="J23" s="41"/>
       <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
+      <c r="L23" s="41"/>
       <c r="M23" s="40"/>
       <c r="N23" s="40"/>
       <c r="O23" s="40"/>
@@ -2235,7 +2273,7 @@
       <c r="I24" s="31"/>
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
+      <c r="L24" s="32"/>
       <c r="M24" s="31"/>
       <c r="N24" s="31"/>
       <c r="O24" s="31"/>
@@ -4009,86 +4047,86 @@
       <c r="AA2" s="70"/>
     </row>
     <row r="3" ht="79.5" customHeight="1">
-      <c r="A3" s="70"/>
-      <c r="B3" s="72">
+      <c r="A3" s="72"/>
+      <c r="B3" s="73">
         <v>45575.0</v>
       </c>
-      <c r="C3" s="72">
+      <c r="C3" s="73">
         <v>45582.0</v>
       </c>
-      <c r="D3" s="73">
+      <c r="D3" s="74">
         <v>45589.0</v>
       </c>
-      <c r="E3" s="73">
+      <c r="E3" s="74">
         <v>45596.0</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="74">
         <v>45603.0</v>
       </c>
-      <c r="G3" s="73">
+      <c r="G3" s="74">
         <v>45610.0</v>
       </c>
-      <c r="H3" s="73">
+      <c r="H3" s="74">
         <v>45617.0</v>
       </c>
-      <c r="I3" s="73">
+      <c r="I3" s="74">
         <v>45624.0</v>
       </c>
-      <c r="J3" s="73">
+      <c r="J3" s="74">
         <v>45631.0</v>
       </c>
-      <c r="K3" s="73">
+      <c r="K3" s="74">
         <v>45638.0</v>
       </c>
-      <c r="L3" s="73">
+      <c r="L3" s="74">
         <v>45645.0</v>
       </c>
-      <c r="M3" s="73">
+      <c r="M3" s="74">
         <v>45659.0</v>
       </c>
-      <c r="N3" s="73">
+      <c r="N3" s="74">
         <v>45666.0</v>
       </c>
-      <c r="O3" s="73">
+      <c r="O3" s="74">
         <v>45673.0</v>
       </c>
-      <c r="P3" s="72">
+      <c r="P3" s="73">
         <v>45680.0</v>
       </c>
-      <c r="Q3" s="72">
+      <c r="Q3" s="73">
         <v>45687.0</v>
       </c>
-      <c r="R3" s="72">
+      <c r="R3" s="73">
         <v>45694.0</v>
       </c>
-      <c r="S3" s="72">
+      <c r="S3" s="73">
         <v>45701.0</v>
       </c>
-      <c r="T3" s="72">
+      <c r="T3" s="73">
         <v>45708.0</v>
       </c>
-      <c r="U3" s="72">
+      <c r="U3" s="73">
         <v>45715.0</v>
       </c>
-      <c r="V3" s="72">
+      <c r="V3" s="73">
         <v>45722.0</v>
       </c>
-      <c r="W3" s="72">
+      <c r="W3" s="73">
         <v>45729.0</v>
       </c>
-      <c r="X3" s="72">
+      <c r="X3" s="73">
         <v>45736.0</v>
       </c>
-      <c r="Y3" s="72">
+      <c r="Y3" s="73">
         <v>45743.0</v>
       </c>
-      <c r="Z3" s="74" t="s">
+      <c r="Z3" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="75"/>
+      <c r="AA3" s="76"/>
     </row>
     <row r="4">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="77" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
@@ -4163,692 +4201,714 @@
       <c r="Y4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="77"/>
+      <c r="Z4" s="78" t="s">
+        <v>58</v>
+      </c>
       <c r="AA4" s="27"/>
     </row>
     <row r="5">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="79">
+      <c r="B5" s="80">
         <v>30.0</v>
       </c>
-      <c r="C5" s="79">
+      <c r="C5" s="80">
         <v>37.0</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79">
+      <c r="D5" s="81"/>
+      <c r="E5" s="80">
         <v>31.0</v>
       </c>
-      <c r="F5" s="79">
+      <c r="F5" s="80">
         <v>33.0</v>
       </c>
-      <c r="G5" s="80">
+      <c r="G5" s="82">
         <v>27.0</v>
       </c>
-      <c r="H5" s="80">
+      <c r="H5" s="82">
         <v>27.0</v>
       </c>
-      <c r="I5" s="80">
+      <c r="I5" s="82">
         <v>29.0</v>
       </c>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="79"/>
-      <c r="Q5" s="79"/>
-      <c r="R5" s="79"/>
-      <c r="S5" s="79"/>
-      <c r="T5" s="79"/>
-      <c r="U5" s="79"/>
-      <c r="V5" s="79"/>
-      <c r="W5" s="79"/>
-      <c r="X5" s="79"/>
-      <c r="Y5" s="79"/>
-      <c r="Z5" s="81">
+      <c r="J5" s="82">
+        <v>36.0</v>
+      </c>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="81"/>
+      <c r="Z5" s="83">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="AA5" s="36"/>
     </row>
     <row r="6">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="79">
+      <c r="B6" s="81">
         <v>36.0</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79">
+      <c r="C6" s="81"/>
+      <c r="D6" s="81">
         <v>32.0</v>
       </c>
-      <c r="E6" s="79"/>
-      <c r="F6" s="80">
+      <c r="E6" s="81"/>
+      <c r="F6" s="84">
         <v>39.0</v>
       </c>
-      <c r="G6" s="80">
+      <c r="G6" s="84">
         <v>35.0</v>
       </c>
-      <c r="H6" s="80">
+      <c r="H6" s="84">
         <v>27.0</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="79"/>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="79"/>
-      <c r="S6" s="79"/>
-      <c r="T6" s="79"/>
-      <c r="U6" s="79"/>
-      <c r="V6" s="79"/>
-      <c r="W6" s="79"/>
-      <c r="X6" s="79"/>
-      <c r="Y6" s="79"/>
-      <c r="Z6" s="81">
+      <c r="I6" s="81"/>
+      <c r="J6" s="84">
+        <v>33.0</v>
+      </c>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="81"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
+      <c r="V6" s="81"/>
+      <c r="W6" s="81"/>
+      <c r="X6" s="81"/>
+      <c r="Y6" s="81"/>
+      <c r="Z6" s="83">
         <f t="shared" si="1"/>
-        <v>169</v>
+        <v>202</v>
       </c>
       <c r="AA6" s="36"/>
     </row>
     <row r="7">
-      <c r="A7" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="79">
+      <c r="A7" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="80">
         <v>33.0</v>
       </c>
-      <c r="C7" s="79">
+      <c r="C7" s="80">
         <v>28.0</v>
       </c>
-      <c r="D7" s="79">
+      <c r="D7" s="80">
         <v>32.0</v>
       </c>
-      <c r="E7" s="79"/>
-      <c r="F7" s="80">
+      <c r="E7" s="81"/>
+      <c r="F7" s="82">
         <v>33.0</v>
       </c>
-      <c r="G7" s="80">
+      <c r="G7" s="82">
         <v>34.0</v>
       </c>
-      <c r="H7" s="80">
+      <c r="H7" s="82">
         <v>26.0</v>
       </c>
-      <c r="I7" s="80">
+      <c r="I7" s="82">
         <v>29.0</v>
       </c>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="79"/>
-      <c r="R7" s="79"/>
-      <c r="S7" s="79"/>
-      <c r="T7" s="79"/>
-      <c r="U7" s="79"/>
-      <c r="V7" s="79"/>
-      <c r="W7" s="79"/>
-      <c r="X7" s="79"/>
-      <c r="Y7" s="79"/>
-      <c r="Z7" s="81">
+      <c r="J7" s="82">
+        <v>28.0</v>
+      </c>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="81"/>
+      <c r="W7" s="81"/>
+      <c r="X7" s="81"/>
+      <c r="Y7" s="81"/>
+      <c r="Z7" s="83">
         <f t="shared" si="1"/>
-        <v>215</v>
+        <v>243</v>
       </c>
       <c r="AA7" s="36"/>
     </row>
     <row r="8">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="79">
+      <c r="B8" s="80">
         <v>37.0</v>
       </c>
-      <c r="C8" s="79">
+      <c r="C8" s="80">
         <v>35.0</v>
       </c>
-      <c r="D8" s="79">
+      <c r="D8" s="80">
         <v>32.0</v>
       </c>
-      <c r="E8" s="79">
+      <c r="E8" s="85">
         <v>31.0</v>
       </c>
-      <c r="F8" s="80">
+      <c r="F8" s="82">
         <v>31.0</v>
       </c>
-      <c r="G8" s="80">
+      <c r="G8" s="82">
         <v>33.0</v>
       </c>
-      <c r="H8" s="80">
+      <c r="H8" s="82">
         <v>36.0</v>
       </c>
-      <c r="I8" s="80">
+      <c r="I8" s="82">
         <v>33.0</v>
       </c>
-      <c r="J8" s="79"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="79"/>
-      <c r="N8" s="79"/>
-      <c r="O8" s="79"/>
-      <c r="P8" s="79"/>
-      <c r="Q8" s="79"/>
-      <c r="R8" s="79"/>
-      <c r="S8" s="79"/>
-      <c r="T8" s="79"/>
-      <c r="U8" s="79"/>
-      <c r="V8" s="79"/>
-      <c r="W8" s="79"/>
-      <c r="X8" s="79"/>
-      <c r="Y8" s="79"/>
-      <c r="Z8" s="81">
+      <c r="J8" s="86">
+        <v>36.0</v>
+      </c>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="81"/>
+      <c r="V8" s="81"/>
+      <c r="W8" s="81"/>
+      <c r="X8" s="81"/>
+      <c r="Y8" s="81"/>
+      <c r="Z8" s="83">
         <f t="shared" si="1"/>
-        <v>268</v>
+        <v>304</v>
       </c>
       <c r="AA8" s="36"/>
     </row>
     <row r="9">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="79">
+      <c r="B9" s="80">
         <v>30.0</v>
       </c>
-      <c r="C9" s="79">
+      <c r="C9" s="80">
         <v>33.0</v>
       </c>
-      <c r="D9" s="79">
+      <c r="D9" s="80">
         <v>30.0</v>
       </c>
-      <c r="E9" s="79">
+      <c r="E9" s="80">
         <v>26.0</v>
       </c>
-      <c r="F9" s="80">
+      <c r="F9" s="82">
         <v>28.0</v>
       </c>
-      <c r="G9" s="80">
+      <c r="G9" s="82">
         <v>26.0</v>
       </c>
-      <c r="H9" s="80">
+      <c r="H9" s="82">
         <v>20.0</v>
       </c>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="79"/>
-      <c r="N9" s="79"/>
-      <c r="O9" s="79"/>
-      <c r="P9" s="79"/>
-      <c r="Q9" s="79"/>
-      <c r="R9" s="79"/>
-      <c r="S9" s="79"/>
-      <c r="T9" s="79"/>
-      <c r="U9" s="79"/>
-      <c r="V9" s="79"/>
-      <c r="W9" s="79"/>
-      <c r="X9" s="79"/>
-      <c r="Y9" s="79"/>
-      <c r="Z9" s="81">
+      <c r="I9" s="81"/>
+      <c r="J9" s="82">
+        <v>34.0</v>
+      </c>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="81"/>
+      <c r="Q9" s="81"/>
+      <c r="R9" s="81"/>
+      <c r="S9" s="81"/>
+      <c r="T9" s="81"/>
+      <c r="U9" s="81"/>
+      <c r="V9" s="81"/>
+      <c r="W9" s="81"/>
+      <c r="X9" s="81"/>
+      <c r="Y9" s="81"/>
+      <c r="Z9" s="83">
         <f t="shared" si="1"/>
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="AA9" s="36"/>
     </row>
     <row r="10">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79">
+      <c r="B10" s="81"/>
+      <c r="C10" s="81">
         <v>31.0</v>
       </c>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79">
+      <c r="D10" s="81"/>
+      <c r="E10" s="81">
         <v>23.0</v>
       </c>
-      <c r="F10" s="80">
+      <c r="F10" s="84">
         <v>35.0</v>
       </c>
-      <c r="G10" s="80">
+      <c r="G10" s="84">
         <v>29.0</v>
       </c>
-      <c r="H10" s="80">
+      <c r="H10" s="84">
         <v>16.0</v>
       </c>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="79"/>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="79"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="79"/>
-      <c r="U10" s="79"/>
-      <c r="V10" s="79"/>
-      <c r="W10" s="79"/>
-      <c r="X10" s="79"/>
-      <c r="Y10" s="79"/>
-      <c r="Z10" s="81">
+      <c r="I10" s="81"/>
+      <c r="J10" s="84">
+        <v>29.0</v>
+      </c>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="81"/>
+      <c r="U10" s="81"/>
+      <c r="V10" s="81"/>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="83">
         <f t="shared" si="1"/>
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="AA10" s="36"/>
     </row>
     <row r="11">
-      <c r="A11" s="78" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="79">
+      <c r="A11" s="79" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="81">
         <v>41.0</v>
       </c>
-      <c r="C11" s="79">
+      <c r="C11" s="81">
         <v>31.0</v>
       </c>
-      <c r="D11" s="79">
+      <c r="D11" s="81">
         <v>32.0</v>
       </c>
-      <c r="E11" s="79">
+      <c r="E11" s="81">
         <v>29.0</v>
       </c>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="80">
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="84">
         <v>23.0</v>
       </c>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="79"/>
-      <c r="N11" s="79"/>
-      <c r="O11" s="79"/>
-      <c r="P11" s="79"/>
-      <c r="Q11" s="79"/>
-      <c r="R11" s="79"/>
-      <c r="S11" s="79"/>
-      <c r="T11" s="79"/>
-      <c r="U11" s="79"/>
-      <c r="V11" s="79"/>
-      <c r="W11" s="79"/>
-      <c r="X11" s="79"/>
-      <c r="Y11" s="79"/>
-      <c r="Z11" s="81">
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="81"/>
+      <c r="R11" s="81"/>
+      <c r="S11" s="81"/>
+      <c r="T11" s="81"/>
+      <c r="U11" s="81"/>
+      <c r="V11" s="81"/>
+      <c r="W11" s="81"/>
+      <c r="X11" s="81"/>
+      <c r="Y11" s="81"/>
+      <c r="Z11" s="83">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
       <c r="AA11" s="36"/>
     </row>
     <row r="12">
-      <c r="A12" s="78" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="79">
+      <c r="A12" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="80">
         <v>42.0</v>
       </c>
-      <c r="C12" s="79">
+      <c r="C12" s="80">
         <v>31.0</v>
       </c>
-      <c r="D12" s="79">
+      <c r="D12" s="80">
         <v>32.0</v>
       </c>
-      <c r="E12" s="79">
+      <c r="E12" s="80">
         <v>32.0</v>
       </c>
-      <c r="F12" s="80">
+      <c r="F12" s="82">
         <v>34.0</v>
       </c>
-      <c r="G12" s="79"/>
-      <c r="H12" s="80">
+      <c r="G12" s="81"/>
+      <c r="H12" s="82">
         <v>28.0</v>
       </c>
-      <c r="I12" s="80">
+      <c r="I12" s="82">
         <v>34.0</v>
       </c>
-      <c r="J12" s="79"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="79"/>
-      <c r="O12" s="79"/>
-      <c r="P12" s="79"/>
-      <c r="Q12" s="79"/>
-      <c r="R12" s="79"/>
-      <c r="S12" s="79"/>
-      <c r="T12" s="79"/>
-      <c r="U12" s="79"/>
-      <c r="V12" s="79"/>
-      <c r="W12" s="79"/>
-      <c r="X12" s="79"/>
-      <c r="Y12" s="79"/>
-      <c r="Z12" s="81">
+      <c r="J12" s="82">
+        <v>33.0</v>
+      </c>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="81"/>
+      <c r="R12" s="81"/>
+      <c r="S12" s="81"/>
+      <c r="T12" s="81"/>
+      <c r="U12" s="81"/>
+      <c r="V12" s="81"/>
+      <c r="W12" s="81"/>
+      <c r="X12" s="81"/>
+      <c r="Y12" s="81"/>
+      <c r="Z12" s="83">
         <f t="shared" si="1"/>
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="AA12" s="36"/>
     </row>
     <row r="13">
-      <c r="A13" s="78" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79">
+      <c r="A13" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="87"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81">
         <v>33.0</v>
       </c>
-      <c r="E13" s="79">
+      <c r="E13" s="81">
         <v>36.0</v>
       </c>
-      <c r="F13" s="80">
+      <c r="F13" s="84">
         <v>27.0</v>
       </c>
-      <c r="G13" s="80">
+      <c r="G13" s="84">
         <v>37.0</v>
       </c>
-      <c r="H13" s="80">
+      <c r="H13" s="84">
         <v>31.0</v>
       </c>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="79"/>
-      <c r="Q13" s="79"/>
-      <c r="R13" s="79"/>
-      <c r="S13" s="79"/>
-      <c r="T13" s="79"/>
-      <c r="U13" s="79"/>
-      <c r="V13" s="79"/>
-      <c r="W13" s="79"/>
-      <c r="X13" s="79"/>
-      <c r="Y13" s="79"/>
-      <c r="Z13" s="81">
+      <c r="I13" s="81"/>
+      <c r="J13" s="84">
+        <v>34.0</v>
+      </c>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+      <c r="P13" s="81"/>
+      <c r="Q13" s="81"/>
+      <c r="R13" s="81"/>
+      <c r="S13" s="81"/>
+      <c r="T13" s="81"/>
+      <c r="U13" s="81"/>
+      <c r="V13" s="81"/>
+      <c r="W13" s="81"/>
+      <c r="X13" s="81"/>
+      <c r="Y13" s="81"/>
+      <c r="Z13" s="83">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="AA13" s="36"/>
     </row>
     <row r="14">
-      <c r="A14" s="78" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79">
+      <c r="A14" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81">
         <v>22.0</v>
       </c>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="80">
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="84">
         <v>36.0</v>
       </c>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="79"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="79"/>
-      <c r="N14" s="79"/>
-      <c r="O14" s="79"/>
-      <c r="P14" s="79"/>
-      <c r="Q14" s="79"/>
-      <c r="R14" s="79"/>
-      <c r="S14" s="79"/>
-      <c r="T14" s="79"/>
-      <c r="U14" s="79"/>
-      <c r="V14" s="79"/>
-      <c r="W14" s="79"/>
-      <c r="X14" s="79"/>
-      <c r="Y14" s="79"/>
-      <c r="Z14" s="81">
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="84">
+        <v>34.0</v>
+      </c>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="81"/>
+      <c r="O14" s="81"/>
+      <c r="P14" s="81"/>
+      <c r="Q14" s="81"/>
+      <c r="R14" s="81"/>
+      <c r="S14" s="81"/>
+      <c r="T14" s="81"/>
+      <c r="U14" s="81"/>
+      <c r="V14" s="81"/>
+      <c r="W14" s="81"/>
+      <c r="X14" s="81"/>
+      <c r="Y14" s="81"/>
+      <c r="Z14" s="83">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="AA14" s="36"/>
     </row>
     <row r="15">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="79"/>
-      <c r="C15" s="79">
+      <c r="B15" s="81"/>
+      <c r="C15" s="81">
         <v>43.0</v>
       </c>
-      <c r="D15" s="79">
+      <c r="D15" s="81">
         <v>25.0</v>
       </c>
-      <c r="E15" s="79"/>
-      <c r="F15" s="80">
+      <c r="E15" s="81"/>
+      <c r="F15" s="84">
         <v>32.0</v>
       </c>
-      <c r="G15" s="80">
+      <c r="G15" s="84">
         <v>30.0</v>
       </c>
-      <c r="H15" s="80">
+      <c r="H15" s="84">
         <v>34.0</v>
       </c>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="79"/>
-      <c r="R15" s="79"/>
-      <c r="S15" s="79"/>
-      <c r="T15" s="79"/>
-      <c r="U15" s="79"/>
-      <c r="V15" s="79"/>
-      <c r="W15" s="79"/>
-      <c r="X15" s="79"/>
-      <c r="Y15" s="79"/>
-      <c r="Z15" s="81">
+      <c r="I15" s="81"/>
+      <c r="J15" s="84">
+        <v>34.0</v>
+      </c>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
+      <c r="O15" s="81"/>
+      <c r="P15" s="81"/>
+      <c r="Q15" s="81"/>
+      <c r="R15" s="81"/>
+      <c r="S15" s="81"/>
+      <c r="T15" s="81"/>
+      <c r="U15" s="81"/>
+      <c r="V15" s="81"/>
+      <c r="W15" s="81"/>
+      <c r="X15" s="81"/>
+      <c r="Y15" s="81"/>
+      <c r="Z15" s="83">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="AA15" s="36"/>
     </row>
     <row r="16">
-      <c r="A16" s="78" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79">
+      <c r="A16" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81">
         <v>29.0</v>
       </c>
-      <c r="D16" s="79">
+      <c r="D16" s="81">
         <v>28.0</v>
       </c>
-      <c r="E16" s="79"/>
-      <c r="F16" s="80">
+      <c r="E16" s="81"/>
+      <c r="F16" s="84">
         <v>23.0</v>
       </c>
-      <c r="G16" s="80">
+      <c r="G16" s="84">
         <v>30.0</v>
       </c>
-      <c r="H16" s="79"/>
-      <c r="I16" s="80">
+      <c r="H16" s="81"/>
+      <c r="I16" s="84">
         <v>27.0</v>
       </c>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="79"/>
-      <c r="R16" s="79"/>
-      <c r="S16" s="79"/>
-      <c r="T16" s="79"/>
-      <c r="U16" s="79"/>
-      <c r="V16" s="79"/>
-      <c r="W16" s="79"/>
-      <c r="X16" s="79"/>
-      <c r="Y16" s="79"/>
-      <c r="Z16" s="81">
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="81"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="81"/>
+      <c r="Q16" s="81"/>
+      <c r="R16" s="81"/>
+      <c r="S16" s="81"/>
+      <c r="T16" s="81"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="81"/>
+      <c r="W16" s="81"/>
+      <c r="X16" s="81"/>
+      <c r="Y16" s="81"/>
+      <c r="Z16" s="83">
         <f t="shared" si="1"/>
         <v>137</v>
       </c>
       <c r="AA16" s="36"/>
     </row>
     <row r="17">
-      <c r="A17" s="83" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80">
+      <c r="A17" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84">
         <v>26.0</v>
       </c>
-      <c r="H17" s="79"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="79"/>
-      <c r="R17" s="79"/>
-      <c r="S17" s="79"/>
-      <c r="T17" s="79"/>
-      <c r="U17" s="79"/>
-      <c r="V17" s="79"/>
-      <c r="W17" s="79"/>
-      <c r="X17" s="79"/>
-      <c r="Y17" s="79"/>
-      <c r="Z17" s="81">
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="81"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="81"/>
+      <c r="Y17" s="81"/>
+      <c r="Z17" s="83">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="AA17" s="36"/>
     </row>
     <row r="18">
-      <c r="A18" s="83" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80">
+      <c r="A18" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="84">
         <v>27.0</v>
       </c>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
-      <c r="K18" s="79"/>
-      <c r="L18" s="79"/>
-      <c r="M18" s="79"/>
-      <c r="N18" s="79"/>
-      <c r="O18" s="79"/>
-      <c r="P18" s="79"/>
-      <c r="Q18" s="79"/>
-      <c r="R18" s="79"/>
-      <c r="S18" s="79"/>
-      <c r="T18" s="79"/>
-      <c r="U18" s="79"/>
-      <c r="V18" s="79"/>
-      <c r="W18" s="79"/>
-      <c r="X18" s="79"/>
-      <c r="Y18" s="79"/>
-      <c r="Z18" s="81">
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
+      <c r="P18" s="81"/>
+      <c r="Q18" s="81"/>
+      <c r="R18" s="81"/>
+      <c r="S18" s="81"/>
+      <c r="T18" s="81"/>
+      <c r="U18" s="81"/>
+      <c r="V18" s="81"/>
+      <c r="W18" s="81"/>
+      <c r="X18" s="81"/>
+      <c r="Y18" s="81"/>
+      <c r="Z18" s="83">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="AA18" s="36"/>
     </row>
     <row r="19">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="79"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79">
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81">
         <v>41.0</v>
       </c>
-      <c r="E19" s="79">
+      <c r="E19" s="81">
         <v>37.0</v>
       </c>
-      <c r="F19" s="80">
+      <c r="F19" s="84">
         <v>38.0</v>
       </c>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="79"/>
-      <c r="R19" s="79"/>
-      <c r="S19" s="79"/>
-      <c r="T19" s="79"/>
-      <c r="U19" s="79"/>
-      <c r="V19" s="79"/>
-      <c r="W19" s="79"/>
-      <c r="X19" s="79"/>
-      <c r="Y19" s="79"/>
-      <c r="Z19" s="81">
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="81"/>
+      <c r="Q19" s="81"/>
+      <c r="R19" s="81"/>
+      <c r="S19" s="81"/>
+      <c r="T19" s="81"/>
+      <c r="U19" s="81"/>
+      <c r="V19" s="81"/>
+      <c r="W19" s="81"/>
+      <c r="X19" s="81"/>
+      <c r="Y19" s="81"/>
+      <c r="Z19" s="83">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="AA19" s="36"/>
     </row>
     <row r="20">
-      <c r="A20" s="84"/>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="77"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="77"/>
-      <c r="J20" s="77"/>
-      <c r="K20" s="77"/>
-      <c r="L20" s="77"/>
-      <c r="M20" s="77"/>
-      <c r="N20" s="77"/>
-      <c r="O20" s="77"/>
-      <c r="P20" s="77"/>
-      <c r="Q20" s="77"/>
-      <c r="R20" s="77"/>
-      <c r="S20" s="77"/>
-      <c r="T20" s="77"/>
-      <c r="U20" s="77"/>
-      <c r="V20" s="77"/>
-      <c r="W20" s="77"/>
-      <c r="X20" s="77"/>
-      <c r="Y20" s="77"/>
-      <c r="Z20" s="77"/>
+      <c r="A20" s="89"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="90"/>
+      <c r="L20" s="90"/>
+      <c r="M20" s="90"/>
+      <c r="N20" s="90"/>
+      <c r="O20" s="90"/>
+      <c r="P20" s="90"/>
+      <c r="Q20" s="90"/>
+      <c r="R20" s="90"/>
+      <c r="S20" s="90"/>
+      <c r="T20" s="90"/>
+      <c r="U20" s="90"/>
+      <c r="V20" s="90"/>
+      <c r="W20" s="90"/>
+      <c r="X20" s="90"/>
+      <c r="Y20" s="90"/>
+      <c r="Z20" s="90"/>
       <c r="AA20" s="36"/>
     </row>
     <row r="21">
@@ -4881,16 +4941,16 @@
       <c r="AA21" s="36"/>
     </row>
     <row r="22">
-      <c r="A22" s="85" t="s">
+      <c r="A22" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="86">
+      <c r="B22" s="92">
         <v>10.0</v>
       </c>
       <c r="C22" s="70"/>
       <c r="D22" s="70"/>
       <c r="E22" s="70"/>
-      <c r="F22" s="87" t="s">
+      <c r="F22" s="93" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="4"/>
@@ -4979,13 +5039,13 @@
       <c r="C25" s="70"/>
       <c r="D25" s="70"/>
       <c r="E25" s="70"/>
-      <c r="F25" s="88" t="s">
+      <c r="F25" s="94" t="s">
         <v>54</v>
       </c>
       <c r="G25" s="57"/>
       <c r="H25" s="55"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="89">
+      <c r="I25" s="90"/>
+      <c r="J25" s="95">
         <v>60.0</v>
       </c>
       <c r="K25" s="57"/>
@@ -5012,13 +5072,13 @@
       <c r="C26" s="70"/>
       <c r="D26" s="70"/>
       <c r="E26" s="70"/>
-      <c r="F26" s="88" t="s">
+      <c r="F26" s="94" t="s">
         <v>55</v>
       </c>
       <c r="G26" s="57"/>
       <c r="H26" s="55"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="89">
+      <c r="I26" s="90"/>
+      <c r="J26" s="95">
         <v>45.0</v>
       </c>
       <c r="K26" s="57"/>
@@ -5045,13 +5105,13 @@
       <c r="C27" s="70"/>
       <c r="D27" s="70"/>
       <c r="E27" s="70"/>
-      <c r="F27" s="88" t="s">
+      <c r="F27" s="94" t="s">
         <v>56</v>
       </c>
       <c r="G27" s="57"/>
       <c r="H27" s="55"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="89">
+      <c r="I27" s="90"/>
+      <c r="J27" s="95">
         <v>25.0</v>
       </c>
       <c r="K27" s="57"/>
@@ -5082,7 +5142,7 @@
       <c r="G28" s="70"/>
       <c r="H28" s="70"/>
       <c r="I28" s="70"/>
-      <c r="J28" s="90">
+      <c r="J28" s="96">
         <f>SUM(J25:L27)</f>
         <v>130</v>
       </c>
@@ -5135,272 +5195,272 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="98" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="97" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="99">
+        <v>12.0</v>
+      </c>
+      <c r="C2" s="100">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="99">
+        <v>5.0</v>
+      </c>
+      <c r="C3" s="101"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="97" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="99">
+        <v>11.0</v>
+      </c>
+      <c r="C4" s="101"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="97" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="99">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="101"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="99">
+        <v>17.0</v>
+      </c>
+      <c r="C6" s="100">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="97" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="99">
+        <v>12.0</v>
+      </c>
+      <c r="C7" s="100">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="97" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="99">
+        <v>-2.0</v>
+      </c>
+      <c r="C8" s="101"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="97" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="99">
+        <v>12.0</v>
+      </c>
+      <c r="C9" s="101"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="97" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="99">
+        <v>6.0</v>
+      </c>
+      <c r="C10" s="101"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="97" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="99">
+        <v>16.0</v>
+      </c>
+      <c r="C11" s="101"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="99">
+        <v>5.0</v>
+      </c>
+      <c r="C12" s="100">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="97" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="99">
+        <v>9.0</v>
+      </c>
+      <c r="C13" s="100">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="99">
+        <v>15.0</v>
+      </c>
+      <c r="C14" s="101"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="97" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="99">
+        <v>18.0</v>
+      </c>
+      <c r="C15" s="101"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="99">
+        <v>12.0</v>
+      </c>
+      <c r="C16" s="100">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="99">
+        <v>25.0</v>
+      </c>
+      <c r="C17" s="100">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="99">
+        <v>11.0</v>
+      </c>
+      <c r="C18" s="101"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="97" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="99">
+        <v>8.0</v>
+      </c>
+      <c r="C19" s="101"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="97" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="99">
+        <v>6.0</v>
+      </c>
+      <c r="C20" s="100">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="97" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="99">
+        <v>6.0</v>
+      </c>
+      <c r="C21" s="101"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="98" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="102"/>
+      <c r="C22" s="100">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="98" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="102"/>
+      <c r="C23" s="100">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="98" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="102"/>
+      <c r="C24" s="100">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="98" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="102"/>
+      <c r="C25" s="100">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="98" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="102"/>
+      <c r="C26" s="100">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="98" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="102"/>
+      <c r="C27" s="100">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="92" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="91" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="93">
-        <v>12.0</v>
-      </c>
-      <c r="C2" s="94">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="91" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="93">
-        <v>5.0</v>
-      </c>
-      <c r="C3" s="95"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="91" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="93">
-        <v>11.0</v>
-      </c>
-      <c r="C4" s="95"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="91" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="93">
-        <v>4.0</v>
-      </c>
-      <c r="C5" s="95"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="91" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="93">
-        <v>17.0</v>
-      </c>
-      <c r="C6" s="94">
-        <v>17.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="91" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="93">
-        <v>12.0</v>
-      </c>
-      <c r="C7" s="94">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="91" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="93">
-        <v>-2.0</v>
-      </c>
-      <c r="C8" s="95"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="91" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="93">
-        <v>12.0</v>
-      </c>
-      <c r="C9" s="95"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="91" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="93">
-        <v>6.0</v>
-      </c>
-      <c r="C10" s="95"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="91" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="93">
-        <v>16.0</v>
-      </c>
-      <c r="C11" s="95"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="91" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="93">
-        <v>5.0</v>
-      </c>
-      <c r="C12" s="94">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="91" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="93">
-        <v>9.0</v>
-      </c>
-      <c r="C13" s="94">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="93">
-        <v>15.0</v>
-      </c>
-      <c r="C14" s="95"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="91" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="93">
-        <v>18.0</v>
-      </c>
-      <c r="C15" s="95"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="91" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="93">
-        <v>12.0</v>
-      </c>
-      <c r="C16" s="94">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="91" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="93">
-        <v>25.0</v>
-      </c>
-      <c r="C17" s="94">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="91" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="93">
-        <v>11.0</v>
-      </c>
-      <c r="C18" s="95"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="91" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="93">
-        <v>8.0</v>
-      </c>
-      <c r="C19" s="95"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="91" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="93">
-        <v>6.0</v>
-      </c>
-      <c r="C20" s="94">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="93">
-        <v>6.0</v>
-      </c>
-      <c r="C21" s="95"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="92" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="96"/>
-      <c r="C22" s="94">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="92" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="94">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="92" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="96"/>
-      <c r="C24" s="94">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="96"/>
-      <c r="C25" s="94">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="92" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="96"/>
-      <c r="C26" s="94">
-        <v>24.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="92" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="94">
-        <v>29.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="92" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="96"/>
-      <c r="C28" s="94">
+      <c r="B28" s="102"/>
+      <c r="C28" s="100">
         <v>21.0</v>
       </c>
     </row>
@@ -5420,99 +5480,99 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="92" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="92" t="s">
+      <c r="A1" s="98" t="s">
         <v>69</v>
       </c>
+      <c r="B1" s="98" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="97" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="98">
+      <c r="A2" s="103" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="104">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
         <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="92">
+      <c r="A3" s="103" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="98">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="97" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="92">
+      <c r="A4" s="103" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="98">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
         <v>12</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="97" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="92">
+      <c r="A5" s="103" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="98">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
         <v>6</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="97" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="92">
+      <c r="A6" s="103" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="98">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
         <v>13</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="97" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="92">
+      <c r="A7" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="98">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
         <v>8</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="97" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="92">
+      <c r="A8" s="103" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="98">
         <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="97" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="92">
+      <c r="A9" s="103" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="98">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
         <v>12</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="97" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="92">
+      <c r="A10" s="103" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="98">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
         <v>14</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="97" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="92">
+      <c r="A11" s="103" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="98">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
017 Week 10 data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -271,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -304,6 +304,12 @@
     <font>
       <sz val="8.0"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -769,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -879,6 +885,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="30" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="26" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="31" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -892,7 +901,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="34" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="33" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="33" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="35" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -906,7 +915,7 @@
     </xf>
     <xf borderId="40" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="41" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -921,7 +930,7 @@
     <xf borderId="16" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -931,19 +940,19 @@
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="9" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="7" fillId="0" fontId="10" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" textRotation="90" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="9" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="0" fontId="10" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" textRotation="90" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" textRotation="90" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" textRotation="90" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -952,29 +961,32 @@
     <xf borderId="33" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="42" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="42" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="42" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="42" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="42" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="42" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="42" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="42" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="42" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -985,16 +997,16 @@
     <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="33" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="33" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="42" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="33" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="33" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1003,22 +1015,22 @@
     <xf borderId="16" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1887,8 +1899,10 @@
       <c r="K16" s="32">
         <v>23.0</v>
       </c>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32">
+        <v>29.0</v>
+      </c>
       <c r="N16" s="31"/>
       <c r="O16" s="31"/>
       <c r="P16" s="31"/>
@@ -1905,11 +1919,11 @@
       <c r="AA16" s="33"/>
       <c r="AB16" s="34">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>366</v>
+        <v>420</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36"/>
@@ -1940,8 +1954,10 @@
       <c r="K17" s="41">
         <v>31.0</v>
       </c>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41">
+        <v>25.0</v>
+      </c>
       <c r="N17" s="40"/>
       <c r="O17" s="40"/>
       <c r="P17" s="40"/>
@@ -1958,7 +1974,7 @@
       <c r="AA17" s="42"/>
       <c r="AB17" s="34">
         <f t="shared" si="1"/>
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
@@ -1986,8 +2002,10 @@
       </c>
       <c r="J18" s="32"/>
       <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32">
+        <v>28.0</v>
+      </c>
       <c r="N18" s="31"/>
       <c r="O18" s="31"/>
       <c r="P18" s="31"/>
@@ -2004,11 +2022,11 @@
       <c r="AA18" s="33"/>
       <c r="AB18" s="34">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="AC18" s="35">
         <f>SUM(AB18:AB19)</f>
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="36"/>
@@ -2032,7 +2050,7 @@
       <c r="J19" s="41"/>
       <c r="K19" s="40"/>
       <c r="L19" s="41"/>
-      <c r="M19" s="40"/>
+      <c r="M19" s="41"/>
       <c r="N19" s="40"/>
       <c r="O19" s="40"/>
       <c r="P19" s="40"/>
@@ -2082,7 +2100,9 @@
         <v>37.0</v>
       </c>
       <c r="L20" s="32"/>
-      <c r="M20" s="31"/>
+      <c r="M20" s="32">
+        <v>36.0</v>
+      </c>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
       <c r="P20" s="31"/>
@@ -2099,11 +2119,11 @@
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>213</v>
+        <v>249</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>455</v>
+        <v>522</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36"/>
@@ -2137,7 +2157,9 @@
         <v>42.0</v>
       </c>
       <c r="L21" s="41"/>
-      <c r="M21" s="40"/>
+      <c r="M21" s="41">
+        <v>31.0</v>
+      </c>
       <c r="N21" s="40"/>
       <c r="O21" s="40"/>
       <c r="P21" s="40"/>
@@ -2154,7 +2176,7 @@
       <c r="AA21" s="42"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>242</v>
+        <v>273</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
@@ -2183,7 +2205,9 @@
         <v>35.0</v>
       </c>
       <c r="L22" s="32"/>
-      <c r="M22" s="31"/>
+      <c r="M22" s="32">
+        <v>29.0</v>
+      </c>
       <c r="N22" s="31"/>
       <c r="O22" s="31"/>
       <c r="P22" s="31"/>
@@ -2200,11 +2224,11 @@
       <c r="AA22" s="33"/>
       <c r="AB22" s="34">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="AC22" s="35">
         <f>SUM(AB22:AB23)</f>
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="AD22" s="5"/>
       <c r="AE22" s="36"/>
@@ -2232,7 +2256,7 @@
       <c r="J23" s="41"/>
       <c r="K23" s="40"/>
       <c r="L23" s="41"/>
-      <c r="M23" s="40"/>
+      <c r="M23" s="41"/>
       <c r="N23" s="40"/>
       <c r="O23" s="40"/>
       <c r="P23" s="40"/>
@@ -2274,7 +2298,7 @@
       <c r="J24" s="31"/>
       <c r="K24" s="31"/>
       <c r="L24" s="32"/>
-      <c r="M24" s="31"/>
+      <c r="M24" s="32"/>
       <c r="N24" s="31"/>
       <c r="O24" s="31"/>
       <c r="P24" s="31"/>
@@ -2295,7 +2319,7 @@
       </c>
       <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
-        <v>263</v>
+        <v>291</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="36"/>
@@ -2326,8 +2350,10 @@
       <c r="K25" s="41">
         <v>31.0</v>
       </c>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41">
+        <v>28.0</v>
+      </c>
       <c r="N25" s="40"/>
       <c r="O25" s="40"/>
       <c r="P25" s="40"/>
@@ -2344,7 +2370,7 @@
       <c r="AA25" s="42"/>
       <c r="AB25" s="34">
         <f t="shared" si="1"/>
-        <v>193</v>
+        <v>221</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
@@ -2376,8 +2402,10 @@
       <c r="K26" s="32">
         <v>30.0</v>
       </c>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32">
+        <v>36.0</v>
+      </c>
       <c r="N26" s="31"/>
       <c r="O26" s="31"/>
       <c r="P26" s="31"/>
@@ -2394,11 +2422,11 @@
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>397</v>
+        <v>455</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36"/>
@@ -2429,8 +2457,10 @@
       <c r="K27" s="41">
         <v>39.0</v>
       </c>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41">
+        <v>22.0</v>
+      </c>
       <c r="N27" s="40"/>
       <c r="O27" s="40"/>
       <c r="P27" s="40"/>
@@ -2447,7 +2477,7 @@
       <c r="AA27" s="42"/>
       <c r="AB27" s="34">
         <f t="shared" si="1"/>
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
@@ -2481,8 +2511,10 @@
       <c r="K28" s="32">
         <v>32.0</v>
       </c>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32">
+        <v>33.0</v>
+      </c>
       <c r="N28" s="31"/>
       <c r="O28" s="31"/>
       <c r="P28" s="31"/>
@@ -2499,11 +2531,11 @@
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>213</v>
+        <v>246</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>446</v>
+        <v>518</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36"/>
@@ -2536,8 +2568,10 @@
       <c r="K29" s="41">
         <v>38.0</v>
       </c>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51">
+        <v>39.0</v>
+      </c>
       <c r="N29" s="40"/>
       <c r="O29" s="40"/>
       <c r="P29" s="40"/>
@@ -2554,7 +2588,7 @@
       <c r="AA29" s="42"/>
       <c r="AB29" s="34">
         <f t="shared" si="1"/>
-        <v>233</v>
+        <v>272</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -2602,7 +2636,7 @@
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>290</v>
+        <v>323</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36"/>
@@ -2633,8 +2667,10 @@
       <c r="K31" s="41">
         <v>31.0</v>
       </c>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41">
+        <v>33.0</v>
+      </c>
       <c r="N31" s="40"/>
       <c r="O31" s="40"/>
       <c r="P31" s="40"/>
@@ -2647,18 +2683,18 @@
       <c r="W31" s="40"/>
       <c r="X31" s="40"/>
       <c r="Y31" s="40"/>
-      <c r="Z31" s="51"/>
-      <c r="AA31" s="51"/>
-      <c r="AB31" s="52">
+      <c r="Z31" s="52"/>
+      <c r="AA31" s="52"/>
+      <c r="AB31" s="53">
         <f t="shared" si="1"/>
-        <v>196</v>
+        <v>229</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
       <c r="AE31" s="36"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="53"/>
+      <c r="A32" s="54"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2689,27 +2725,27 @@
       <c r="AE32" s="1"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="55"/>
-      <c r="C33" s="56" t="s">
+      <c r="B33" s="56"/>
+      <c r="C33" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="57"/>
-      <c r="E33" s="55"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="56"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="58" t="s">
+      <c r="K33" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="L33" s="59"/>
-      <c r="M33" s="59"/>
-      <c r="N33" s="59"/>
-      <c r="O33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="61"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -2728,9 +2764,9 @@
       <c r="AE33" s="1"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="53"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2761,16 +2797,16 @@
       <c r="AE34" s="1"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="53"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
+      <c r="A35" s="54"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="61" t="s">
+      <c r="E35" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="64"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2778,86 +2814,86 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="61" t="s">
+      <c r="P35" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="Q35" s="62"/>
-      <c r="R35" s="62"/>
-      <c r="S35" s="63"/>
+      <c r="Q35" s="63"/>
+      <c r="R35" s="63"/>
+      <c r="S35" s="64"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="64"/>
+      <c r="X35" s="65"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="53"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="65" t="s">
+      <c r="A36" s="54"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="66" t="s">
         <v>54</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="66">
+      <c r="E36" s="67">
         <v>80.0</v>
       </c>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="55"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="56"/>
       <c r="I36" s="36"/>
       <c r="J36" s="36"/>
       <c r="K36" s="36"/>
       <c r="L36" s="36"/>
-      <c r="M36" s="65" t="s">
+      <c r="M36" s="66" t="s">
         <v>54</v>
       </c>
       <c r="O36" s="36"/>
-      <c r="P36" s="66">
+      <c r="P36" s="67">
         <v>50.0</v>
       </c>
-      <c r="Q36" s="57"/>
-      <c r="R36" s="57"/>
-      <c r="S36" s="55"/>
+      <c r="Q36" s="58"/>
+      <c r="R36" s="58"/>
+      <c r="S36" s="56"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="67"/>
+      <c r="X36" s="68"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="53"/>
-      <c r="B37" s="53"/>
-      <c r="C37" s="65" t="s">
+      <c r="A37" s="54"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="66" t="s">
         <v>55</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="66">
+      <c r="E37" s="67">
         <v>50.0</v>
       </c>
-      <c r="F37" s="57"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="55"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="56"/>
       <c r="I37" s="36"/>
       <c r="J37" s="36"/>
       <c r="K37" s="36"/>
       <c r="L37" s="36"/>
-      <c r="M37" s="65" t="s">
+      <c r="M37" s="66" t="s">
         <v>55</v>
       </c>
       <c r="O37" s="36"/>
-      <c r="P37" s="66">
+      <c r="P37" s="67">
         <v>30.0</v>
       </c>
-      <c r="Q37" s="57"/>
-      <c r="R37" s="57"/>
-      <c r="S37" s="55"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="56"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -2872,18 +2908,18 @@
       <c r="AE37" s="1"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="53"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="65" t="s">
+      <c r="A38" s="54"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="66" t="s">
         <v>56</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="66">
+      <c r="E38" s="67">
         <v>40.0</v>
       </c>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="55"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="56"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -2891,7 +2927,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="68"/>
+      <c r="P38" s="69"/>
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="22"/>
@@ -2909,14 +2945,14 @@
       <c r="AE38" s="1"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="D39" s="69"/>
-      <c r="E39" s="68"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="69"/>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-      <c r="O39" s="69"/>
+      <c r="O39" s="70"/>
       <c r="S39" s="1"/>
       <c r="W39" s="1"/>
     </row>
@@ -3987,10 +4023,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="70"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71" t="s">
+      <c r="A1" s="71"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="72" t="s">
         <v>57</v>
       </c>
       <c r="E1" s="4"/>
@@ -4004,23 +4040,23 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
     </row>
     <row r="2">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -4033,100 +4069,100 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="8"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="70"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="71"/>
+      <c r="X2" s="71"/>
+      <c r="Y2" s="71"/>
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="71"/>
     </row>
     <row r="3" ht="79.5" customHeight="1">
-      <c r="A3" s="72"/>
-      <c r="B3" s="73">
+      <c r="A3" s="73"/>
+      <c r="B3" s="74">
         <v>45575.0</v>
       </c>
-      <c r="C3" s="73">
+      <c r="C3" s="74">
         <v>45582.0</v>
       </c>
-      <c r="D3" s="74">
+      <c r="D3" s="75">
         <v>45589.0</v>
       </c>
-      <c r="E3" s="74">
+      <c r="E3" s="75">
         <v>45596.0</v>
       </c>
-      <c r="F3" s="74">
+      <c r="F3" s="75">
         <v>45603.0</v>
       </c>
-      <c r="G3" s="74">
+      <c r="G3" s="75">
         <v>45610.0</v>
       </c>
-      <c r="H3" s="74">
+      <c r="H3" s="75">
         <v>45617.0</v>
       </c>
-      <c r="I3" s="74">
+      <c r="I3" s="75">
         <v>45624.0</v>
       </c>
-      <c r="J3" s="74">
+      <c r="J3" s="75">
         <v>45631.0</v>
       </c>
-      <c r="K3" s="74">
+      <c r="K3" s="75">
         <v>45638.0</v>
       </c>
-      <c r="L3" s="74">
+      <c r="L3" s="75">
         <v>45645.0</v>
       </c>
-      <c r="M3" s="74">
+      <c r="M3" s="75">
         <v>45659.0</v>
       </c>
-      <c r="N3" s="74">
+      <c r="N3" s="75">
         <v>45666.0</v>
       </c>
-      <c r="O3" s="74">
+      <c r="O3" s="75">
         <v>45673.0</v>
       </c>
-      <c r="P3" s="73">
+      <c r="P3" s="74">
         <v>45680.0</v>
       </c>
-      <c r="Q3" s="73">
+      <c r="Q3" s="74">
         <v>45687.0</v>
       </c>
-      <c r="R3" s="73">
+      <c r="R3" s="74">
         <v>45694.0</v>
       </c>
-      <c r="S3" s="73">
+      <c r="S3" s="74">
         <v>45701.0</v>
       </c>
-      <c r="T3" s="73">
+      <c r="T3" s="74">
         <v>45708.0</v>
       </c>
-      <c r="U3" s="73">
+      <c r="U3" s="74">
         <v>45715.0</v>
       </c>
-      <c r="V3" s="73">
+      <c r="V3" s="74">
         <v>45722.0</v>
       </c>
-      <c r="W3" s="73">
+      <c r="W3" s="74">
         <v>45729.0</v>
       </c>
-      <c r="X3" s="73">
+      <c r="X3" s="74">
         <v>45736.0</v>
       </c>
-      <c r="Y3" s="73">
+      <c r="Y3" s="74">
         <v>45743.0</v>
       </c>
-      <c r="Z3" s="75" t="s">
+      <c r="Z3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="76"/>
+      <c r="AA3" s="77"/>
     </row>
     <row r="4">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="78" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
@@ -4201,73 +4237,75 @@
       <c r="Y4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="78" t="s">
+      <c r="Z4" s="79" t="s">
         <v>58</v>
       </c>
       <c r="AA4" s="27"/>
     </row>
     <row r="5">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="80">
+      <c r="B5" s="81">
         <v>30.0</v>
       </c>
-      <c r="C5" s="80">
+      <c r="C5" s="81">
         <v>37.0</v>
       </c>
-      <c r="D5" s="81"/>
-      <c r="E5" s="80">
+      <c r="D5" s="82"/>
+      <c r="E5" s="81">
         <v>31.0</v>
       </c>
-      <c r="F5" s="80">
+      <c r="F5" s="81">
         <v>33.0</v>
       </c>
-      <c r="G5" s="82">
+      <c r="G5" s="83">
         <v>27.0</v>
       </c>
-      <c r="H5" s="82">
+      <c r="H5" s="83">
         <v>27.0</v>
       </c>
-      <c r="I5" s="82">
+      <c r="I5" s="83">
         <v>29.0</v>
       </c>
-      <c r="J5" s="82">
+      <c r="J5" s="83">
         <v>36.0</v>
       </c>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="81"/>
-      <c r="Z5" s="83">
+      <c r="K5" s="84">
+        <v>28.0</v>
+      </c>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="82"/>
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="82"/>
+      <c r="Z5" s="85">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="AA5" s="36"/>
     </row>
     <row r="6">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="81">
+      <c r="B6" s="82">
         <v>36.0</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81">
+      <c r="C6" s="82"/>
+      <c r="D6" s="82">
         <v>32.0</v>
       </c>
-      <c r="E6" s="81"/>
+      <c r="E6" s="82"/>
       <c r="F6" s="84">
         <v>39.0</v>
       </c>
@@ -4277,193 +4315,199 @@
       <c r="H6" s="84">
         <v>27.0</v>
       </c>
-      <c r="I6" s="81"/>
+      <c r="I6" s="82"/>
       <c r="J6" s="84">
         <v>33.0</v>
       </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="81"/>
-      <c r="X6" s="81"/>
-      <c r="Y6" s="81"/>
-      <c r="Z6" s="83">
+      <c r="K6" s="84">
+        <v>38.0</v>
+      </c>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82"/>
+      <c r="X6" s="82"/>
+      <c r="Y6" s="82"/>
+      <c r="Z6" s="85">
         <f t="shared" si="1"/>
-        <v>202</v>
+        <v>240</v>
       </c>
       <c r="AA6" s="36"/>
     </row>
     <row r="7">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="80">
+      <c r="B7" s="81">
         <v>33.0</v>
       </c>
-      <c r="C7" s="80">
+      <c r="C7" s="81">
         <v>28.0</v>
       </c>
-      <c r="D7" s="80">
+      <c r="D7" s="81">
         <v>32.0</v>
       </c>
-      <c r="E7" s="81"/>
-      <c r="F7" s="82">
+      <c r="E7" s="82"/>
+      <c r="F7" s="83">
         <v>33.0</v>
       </c>
-      <c r="G7" s="82">
+      <c r="G7" s="83">
         <v>34.0</v>
       </c>
-      <c r="H7" s="82">
+      <c r="H7" s="83">
         <v>26.0</v>
       </c>
-      <c r="I7" s="82">
+      <c r="I7" s="83">
         <v>29.0</v>
       </c>
-      <c r="J7" s="82">
+      <c r="J7" s="83">
         <v>28.0</v>
       </c>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="81"/>
-      <c r="U7" s="81"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="81"/>
-      <c r="Y7" s="81"/>
-      <c r="Z7" s="83">
+      <c r="K7" s="84">
+        <v>29.0</v>
+      </c>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="82"/>
+      <c r="U7" s="82"/>
+      <c r="V7" s="82"/>
+      <c r="W7" s="82"/>
+      <c r="X7" s="82"/>
+      <c r="Y7" s="82"/>
+      <c r="Z7" s="85">
         <f t="shared" si="1"/>
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="AA7" s="36"/>
     </row>
     <row r="8">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="80">
+      <c r="B8" s="81">
         <v>37.0</v>
       </c>
-      <c r="C8" s="80">
+      <c r="C8" s="81">
         <v>35.0</v>
       </c>
-      <c r="D8" s="80">
+      <c r="D8" s="81">
         <v>32.0</v>
       </c>
-      <c r="E8" s="85">
+      <c r="E8" s="86">
         <v>31.0</v>
       </c>
-      <c r="F8" s="82">
+      <c r="F8" s="83">
         <v>31.0</v>
       </c>
-      <c r="G8" s="82">
+      <c r="G8" s="83">
         <v>33.0</v>
       </c>
-      <c r="H8" s="82">
+      <c r="H8" s="83">
         <v>36.0</v>
       </c>
-      <c r="I8" s="82">
+      <c r="I8" s="83">
         <v>33.0</v>
       </c>
-      <c r="J8" s="86">
+      <c r="J8" s="87">
         <v>36.0</v>
       </c>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="81"/>
-      <c r="S8" s="81"/>
-      <c r="T8" s="81"/>
-      <c r="U8" s="81"/>
-      <c r="V8" s="81"/>
-      <c r="W8" s="81"/>
-      <c r="X8" s="81"/>
-      <c r="Y8" s="81"/>
-      <c r="Z8" s="83">
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="82"/>
+      <c r="S8" s="82"/>
+      <c r="T8" s="82"/>
+      <c r="U8" s="82"/>
+      <c r="V8" s="82"/>
+      <c r="W8" s="82"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="82"/>
+      <c r="Z8" s="85">
         <f t="shared" si="1"/>
         <v>304</v>
       </c>
       <c r="AA8" s="36"/>
     </row>
     <row r="9">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="80">
+      <c r="B9" s="81">
         <v>30.0</v>
       </c>
-      <c r="C9" s="80">
+      <c r="C9" s="81">
         <v>33.0</v>
       </c>
-      <c r="D9" s="80">
+      <c r="D9" s="81">
         <v>30.0</v>
       </c>
-      <c r="E9" s="80">
+      <c r="E9" s="81">
         <v>26.0</v>
       </c>
-      <c r="F9" s="82">
+      <c r="F9" s="83">
         <v>28.0</v>
       </c>
-      <c r="G9" s="82">
+      <c r="G9" s="83">
         <v>26.0</v>
       </c>
-      <c r="H9" s="82">
+      <c r="H9" s="83">
         <v>20.0</v>
       </c>
-      <c r="I9" s="81"/>
-      <c r="J9" s="82">
+      <c r="I9" s="82"/>
+      <c r="J9" s="83">
         <v>34.0</v>
       </c>
-      <c r="K9" s="81"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="81"/>
-      <c r="T9" s="81"/>
-      <c r="U9" s="81"/>
-      <c r="V9" s="81"/>
-      <c r="W9" s="81"/>
-      <c r="X9" s="81"/>
-      <c r="Y9" s="81"/>
-      <c r="Z9" s="83">
+      <c r="K9" s="84">
+        <v>26.0</v>
+      </c>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="82"/>
+      <c r="Q9" s="82"/>
+      <c r="R9" s="82"/>
+      <c r="S9" s="82"/>
+      <c r="T9" s="82"/>
+      <c r="U9" s="82"/>
+      <c r="V9" s="82"/>
+      <c r="W9" s="82"/>
+      <c r="X9" s="82"/>
+      <c r="Y9" s="82"/>
+      <c r="Z9" s="85">
         <f t="shared" si="1"/>
-        <v>227</v>
+        <v>253</v>
       </c>
       <c r="AA9" s="36"/>
     </row>
     <row r="10">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81">
+      <c r="B10" s="82"/>
+      <c r="C10" s="82">
         <v>31.0</v>
       </c>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81">
+      <c r="D10" s="82"/>
+      <c r="E10" s="82">
         <v>23.0</v>
       </c>
       <c r="F10" s="84">
@@ -4475,135 +4519,137 @@
       <c r="H10" s="84">
         <v>16.0</v>
       </c>
-      <c r="I10" s="81"/>
+      <c r="I10" s="82"/>
       <c r="J10" s="84">
         <v>29.0</v>
       </c>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="81"/>
-      <c r="T10" s="81"/>
-      <c r="U10" s="81"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="81"/>
-      <c r="X10" s="81"/>
-      <c r="Y10" s="81"/>
-      <c r="Z10" s="83">
+      <c r="K10" s="84">
+        <v>21.0</v>
+      </c>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="82"/>
+      <c r="S10" s="82"/>
+      <c r="T10" s="82"/>
+      <c r="U10" s="82"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="82"/>
+      <c r="X10" s="82"/>
+      <c r="Y10" s="82"/>
+      <c r="Z10" s="85">
         <f t="shared" si="1"/>
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="AA10" s="36"/>
     </row>
     <row r="11">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="81">
+      <c r="B11" s="82">
         <v>41.0</v>
       </c>
-      <c r="C11" s="81">
+      <c r="C11" s="82">
         <v>31.0</v>
       </c>
-      <c r="D11" s="81">
+      <c r="D11" s="82">
         <v>32.0</v>
       </c>
-      <c r="E11" s="81">
+      <c r="E11" s="82">
         <v>29.0</v>
       </c>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
       <c r="H11" s="84">
         <v>23.0</v>
       </c>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="81"/>
-      <c r="S11" s="81"/>
-      <c r="T11" s="81"/>
-      <c r="U11" s="81"/>
-      <c r="V11" s="81"/>
-      <c r="W11" s="81"/>
-      <c r="X11" s="81"/>
-      <c r="Y11" s="81"/>
-      <c r="Z11" s="83">
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="82"/>
+      <c r="P11" s="82"/>
+      <c r="Q11" s="82"/>
+      <c r="R11" s="82"/>
+      <c r="S11" s="82"/>
+      <c r="T11" s="82"/>
+      <c r="U11" s="82"/>
+      <c r="V11" s="82"/>
+      <c r="W11" s="82"/>
+      <c r="X11" s="82"/>
+      <c r="Y11" s="82"/>
+      <c r="Z11" s="85">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
       <c r="AA11" s="36"/>
     </row>
     <row r="12">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="80">
+      <c r="B12" s="81">
         <v>42.0</v>
       </c>
-      <c r="C12" s="80">
+      <c r="C12" s="81">
         <v>31.0</v>
       </c>
-      <c r="D12" s="80">
+      <c r="D12" s="81">
         <v>32.0</v>
       </c>
-      <c r="E12" s="80">
+      <c r="E12" s="81">
         <v>32.0</v>
       </c>
-      <c r="F12" s="82">
+      <c r="F12" s="83">
         <v>34.0</v>
       </c>
-      <c r="G12" s="81"/>
-      <c r="H12" s="82">
+      <c r="G12" s="82"/>
+      <c r="H12" s="83">
         <v>28.0</v>
       </c>
-      <c r="I12" s="82">
+      <c r="I12" s="83">
         <v>34.0</v>
       </c>
-      <c r="J12" s="82">
+      <c r="J12" s="83">
         <v>33.0</v>
       </c>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="81"/>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="81"/>
-      <c r="S12" s="81"/>
-      <c r="T12" s="81"/>
-      <c r="U12" s="81"/>
-      <c r="V12" s="81"/>
-      <c r="W12" s="81"/>
-      <c r="X12" s="81"/>
-      <c r="Y12" s="81"/>
-      <c r="Z12" s="83">
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="82"/>
+      <c r="R12" s="82"/>
+      <c r="S12" s="82"/>
+      <c r="T12" s="82"/>
+      <c r="U12" s="82"/>
+      <c r="V12" s="82"/>
+      <c r="W12" s="82"/>
+      <c r="X12" s="82"/>
+      <c r="Y12" s="82"/>
+      <c r="Z12" s="85">
         <f t="shared" si="1"/>
         <v>266</v>
       </c>
       <c r="AA12" s="36"/>
     </row>
     <row r="13">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81">
+      <c r="B13" s="88"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82">
         <v>33.0</v>
       </c>
-      <c r="E13" s="81">
+      <c r="E13" s="82">
         <v>36.0</v>
       </c>
       <c r="F13" s="84">
@@ -4615,83 +4661,87 @@
       <c r="H13" s="84">
         <v>31.0</v>
       </c>
-      <c r="I13" s="81"/>
+      <c r="I13" s="82"/>
       <c r="J13" s="84">
         <v>34.0</v>
       </c>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="81"/>
-      <c r="S13" s="81"/>
-      <c r="T13" s="81"/>
-      <c r="U13" s="81"/>
-      <c r="V13" s="81"/>
-      <c r="W13" s="81"/>
-      <c r="X13" s="81"/>
-      <c r="Y13" s="81"/>
-      <c r="Z13" s="83">
+      <c r="K13" s="89">
+        <v>40.0</v>
+      </c>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="82"/>
+      <c r="S13" s="82"/>
+      <c r="T13" s="82"/>
+      <c r="U13" s="82"/>
+      <c r="V13" s="82"/>
+      <c r="W13" s="82"/>
+      <c r="X13" s="82"/>
+      <c r="Y13" s="82"/>
+      <c r="Z13" s="85">
         <f t="shared" si="1"/>
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="AA13" s="36"/>
     </row>
     <row r="14">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="81"/>
-      <c r="C14" s="81">
+      <c r="B14" s="82"/>
+      <c r="C14" s="82">
         <v>22.0</v>
       </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
       <c r="F14" s="84">
         <v>36.0</v>
       </c>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
       <c r="J14" s="84">
         <v>34.0</v>
       </c>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="81"/>
-      <c r="Q14" s="81"/>
-      <c r="R14" s="81"/>
-      <c r="S14" s="81"/>
-      <c r="T14" s="81"/>
-      <c r="U14" s="81"/>
-      <c r="V14" s="81"/>
-      <c r="W14" s="81"/>
-      <c r="X14" s="81"/>
-      <c r="Y14" s="81"/>
-      <c r="Z14" s="83">
+      <c r="K14" s="84">
+        <v>27.0</v>
+      </c>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="82"/>
+      <c r="S14" s="82"/>
+      <c r="T14" s="82"/>
+      <c r="U14" s="82"/>
+      <c r="V14" s="82"/>
+      <c r="W14" s="82"/>
+      <c r="X14" s="82"/>
+      <c r="Y14" s="82"/>
+      <c r="Z14" s="85">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="AA14" s="36"/>
     </row>
     <row r="15">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="81"/>
-      <c r="C15" s="81">
+      <c r="B15" s="82"/>
+      <c r="C15" s="82">
         <v>43.0</v>
       </c>
-      <c r="D15" s="81">
+      <c r="D15" s="82">
         <v>25.0</v>
       </c>
-      <c r="E15" s="81"/>
+      <c r="E15" s="82"/>
       <c r="F15" s="84">
         <v>32.0</v>
       </c>
@@ -4701,256 +4751,260 @@
       <c r="H15" s="84">
         <v>34.0</v>
       </c>
-      <c r="I15" s="81"/>
+      <c r="I15" s="82"/>
       <c r="J15" s="84">
         <v>34.0</v>
       </c>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="81"/>
-      <c r="S15" s="81"/>
-      <c r="T15" s="81"/>
-      <c r="U15" s="81"/>
-      <c r="V15" s="81"/>
-      <c r="W15" s="81"/>
-      <c r="X15" s="81"/>
-      <c r="Y15" s="81"/>
-      <c r="Z15" s="83">
+      <c r="K15" s="84">
+        <v>26.0</v>
+      </c>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="82"/>
+      <c r="R15" s="82"/>
+      <c r="S15" s="82"/>
+      <c r="T15" s="82"/>
+      <c r="U15" s="82"/>
+      <c r="V15" s="82"/>
+      <c r="W15" s="82"/>
+      <c r="X15" s="82"/>
+      <c r="Y15" s="82"/>
+      <c r="Z15" s="85">
         <f t="shared" si="1"/>
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="AA15" s="36"/>
     </row>
     <row r="16">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81">
+      <c r="B16" s="82"/>
+      <c r="C16" s="82">
         <v>29.0</v>
       </c>
-      <c r="D16" s="81">
+      <c r="D16" s="82">
         <v>28.0</v>
       </c>
-      <c r="E16" s="81"/>
+      <c r="E16" s="82"/>
       <c r="F16" s="84">
         <v>23.0</v>
       </c>
       <c r="G16" s="84">
         <v>30.0</v>
       </c>
-      <c r="H16" s="81"/>
+      <c r="H16" s="82"/>
       <c r="I16" s="84">
         <v>27.0</v>
       </c>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="81"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="81"/>
-      <c r="S16" s="81"/>
-      <c r="T16" s="81"/>
-      <c r="U16" s="81"/>
-      <c r="V16" s="81"/>
-      <c r="W16" s="81"/>
-      <c r="X16" s="81"/>
-      <c r="Y16" s="81"/>
-      <c r="Z16" s="83">
+      <c r="J16" s="82"/>
+      <c r="K16" s="84">
+        <v>29.0</v>
+      </c>
+      <c r="L16" s="82"/>
+      <c r="M16" s="82"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="82"/>
+      <c r="P16" s="82"/>
+      <c r="Q16" s="82"/>
+      <c r="R16" s="82"/>
+      <c r="S16" s="82"/>
+      <c r="T16" s="82"/>
+      <c r="U16" s="82"/>
+      <c r="V16" s="82"/>
+      <c r="W16" s="82"/>
+      <c r="X16" s="82"/>
+      <c r="Y16" s="82"/>
+      <c r="Z16" s="85">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="AA16" s="36"/>
     </row>
     <row r="17">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
       <c r="F17" s="84"/>
       <c r="G17" s="84">
         <v>26.0</v>
       </c>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="81"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="81"/>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="81"/>
-      <c r="S17" s="81"/>
-      <c r="T17" s="81"/>
-      <c r="U17" s="81"/>
-      <c r="V17" s="81"/>
-      <c r="W17" s="81"/>
-      <c r="X17" s="81"/>
-      <c r="Y17" s="81"/>
-      <c r="Z17" s="83">
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="82"/>
+      <c r="S17" s="82"/>
+      <c r="T17" s="82"/>
+      <c r="U17" s="82"/>
+      <c r="V17" s="82"/>
+      <c r="W17" s="82"/>
+      <c r="X17" s="82"/>
+      <c r="Y17" s="82"/>
+      <c r="Z17" s="85">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="AA17" s="36"/>
     </row>
     <row r="18">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
       <c r="F18" s="84"/>
       <c r="G18" s="84">
         <v>27.0</v>
       </c>
-      <c r="H18" s="81"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="81"/>
-      <c r="O18" s="81"/>
-      <c r="P18" s="81"/>
-      <c r="Q18" s="81"/>
-      <c r="R18" s="81"/>
-      <c r="S18" s="81"/>
-      <c r="T18" s="81"/>
-      <c r="U18" s="81"/>
-      <c r="V18" s="81"/>
-      <c r="W18" s="81"/>
-      <c r="X18" s="81"/>
-      <c r="Y18" s="81"/>
-      <c r="Z18" s="83">
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="82"/>
+      <c r="P18" s="82"/>
+      <c r="Q18" s="82"/>
+      <c r="R18" s="82"/>
+      <c r="S18" s="82"/>
+      <c r="T18" s="82"/>
+      <c r="U18" s="82"/>
+      <c r="V18" s="82"/>
+      <c r="W18" s="82"/>
+      <c r="X18" s="82"/>
+      <c r="Y18" s="82"/>
+      <c r="Z18" s="85">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="AA18" s="36"/>
     </row>
     <row r="19">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81">
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82">
         <v>41.0</v>
       </c>
-      <c r="E19" s="81">
+      <c r="E19" s="82">
         <v>37.0</v>
       </c>
       <c r="F19" s="84">
         <v>38.0</v>
       </c>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="81"/>
-      <c r="Q19" s="81"/>
-      <c r="R19" s="81"/>
-      <c r="S19" s="81"/>
-      <c r="T19" s="81"/>
-      <c r="U19" s="81"/>
-      <c r="V19" s="81"/>
-      <c r="W19" s="81"/>
-      <c r="X19" s="81"/>
-      <c r="Y19" s="81"/>
-      <c r="Z19" s="83">
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="82"/>
+      <c r="R19" s="82"/>
+      <c r="S19" s="82"/>
+      <c r="T19" s="82"/>
+      <c r="U19" s="82"/>
+      <c r="V19" s="82"/>
+      <c r="W19" s="82"/>
+      <c r="X19" s="82"/>
+      <c r="Y19" s="82"/>
+      <c r="Z19" s="85">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="AA19" s="36"/>
     </row>
     <row r="20">
-      <c r="A20" s="89"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="90"/>
-      <c r="J20" s="90"/>
-      <c r="K20" s="90"/>
-      <c r="L20" s="90"/>
-      <c r="M20" s="90"/>
-      <c r="N20" s="90"/>
-      <c r="O20" s="90"/>
-      <c r="P20" s="90"/>
-      <c r="Q20" s="90"/>
-      <c r="R20" s="90"/>
-      <c r="S20" s="90"/>
-      <c r="T20" s="90"/>
-      <c r="U20" s="90"/>
-      <c r="V20" s="90"/>
-      <c r="W20" s="90"/>
-      <c r="X20" s="90"/>
-      <c r="Y20" s="90"/>
-      <c r="Z20" s="90"/>
+      <c r="A20" s="91"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="92"/>
+      <c r="J20" s="92"/>
+      <c r="K20" s="92"/>
+      <c r="L20" s="92"/>
+      <c r="M20" s="92"/>
+      <c r="N20" s="92"/>
+      <c r="O20" s="92"/>
+      <c r="P20" s="92"/>
+      <c r="Q20" s="92"/>
+      <c r="R20" s="92"/>
+      <c r="S20" s="92"/>
+      <c r="T20" s="92"/>
+      <c r="U20" s="92"/>
+      <c r="V20" s="92"/>
+      <c r="W20" s="92"/>
+      <c r="X20" s="92"/>
+      <c r="Y20" s="92"/>
+      <c r="Z20" s="92"/>
       <c r="AA20" s="36"/>
     </row>
     <row r="21">
-      <c r="A21" s="70"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="70"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="70"/>
-      <c r="M21" s="70"/>
-      <c r="N21" s="70"/>
-      <c r="O21" s="70"/>
-      <c r="P21" s="70"/>
-      <c r="Q21" s="70"/>
-      <c r="R21" s="70"/>
-      <c r="S21" s="70"/>
-      <c r="T21" s="70"/>
-      <c r="U21" s="70"/>
-      <c r="V21" s="70"/>
-      <c r="W21" s="70"/>
-      <c r="X21" s="70"/>
-      <c r="Y21" s="70"/>
-      <c r="Z21" s="70"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="71"/>
+      <c r="Q21" s="71"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="71"/>
+      <c r="T21" s="71"/>
+      <c r="U21" s="71"/>
+      <c r="V21" s="71"/>
+      <c r="W21" s="71"/>
+      <c r="X21" s="71"/>
+      <c r="Y21" s="71"/>
+      <c r="Z21" s="71"/>
       <c r="AA21" s="36"/>
     </row>
     <row r="22">
-      <c r="A22" s="91" t="s">
+      <c r="A22" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="92">
+      <c r="B22" s="94">
         <v>10.0</v>
       </c>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="93" t="s">
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="95" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="4"/>
@@ -4959,28 +5013,28 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="70"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="70"/>
-      <c r="P22" s="70"/>
-      <c r="Q22" s="70"/>
-      <c r="R22" s="70"/>
-      <c r="S22" s="70"/>
-      <c r="T22" s="70"/>
-      <c r="U22" s="70"/>
-      <c r="V22" s="70"/>
-      <c r="W22" s="70"/>
-      <c r="X22" s="70"/>
-      <c r="Y22" s="70"/>
-      <c r="Z22" s="70"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="71"/>
+      <c r="P22" s="71"/>
+      <c r="Q22" s="71"/>
+      <c r="R22" s="71"/>
+      <c r="S22" s="71"/>
+      <c r="T22" s="71"/>
+      <c r="U22" s="71"/>
+      <c r="V22" s="71"/>
+      <c r="W22" s="71"/>
+      <c r="X22" s="71"/>
+      <c r="Y22" s="71"/>
+      <c r="Z22" s="71"/>
       <c r="AA22" s="36"/>
     </row>
     <row r="23">
-      <c r="A23" s="70"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -4988,181 +5042,181 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="70"/>
-      <c r="N23" s="70"/>
-      <c r="O23" s="70"/>
-      <c r="P23" s="70"/>
-      <c r="Q23" s="70"/>
-      <c r="R23" s="70"/>
-      <c r="S23" s="70"/>
-      <c r="T23" s="70"/>
-      <c r="U23" s="70"/>
-      <c r="V23" s="70"/>
-      <c r="W23" s="70"/>
-      <c r="X23" s="70"/>
-      <c r="Y23" s="70"/>
-      <c r="Z23" s="70"/>
+      <c r="M23" s="71"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="71"/>
+      <c r="P23" s="71"/>
+      <c r="Q23" s="71"/>
+      <c r="R23" s="71"/>
+      <c r="S23" s="71"/>
+      <c r="T23" s="71"/>
+      <c r="U23" s="71"/>
+      <c r="V23" s="71"/>
+      <c r="W23" s="71"/>
+      <c r="X23" s="71"/>
+      <c r="Y23" s="71"/>
+      <c r="Z23" s="71"/>
       <c r="AA23" s="36"/>
     </row>
     <row r="24">
-      <c r="A24" s="70"/>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="70"/>
-      <c r="M24" s="70"/>
-      <c r="N24" s="70"/>
-      <c r="O24" s="70"/>
-      <c r="P24" s="70"/>
-      <c r="Q24" s="70"/>
-      <c r="R24" s="70"/>
-      <c r="S24" s="70"/>
-      <c r="T24" s="70"/>
-      <c r="U24" s="70"/>
-      <c r="V24" s="70"/>
-      <c r="W24" s="70"/>
-      <c r="X24" s="70"/>
-      <c r="Y24" s="70"/>
-      <c r="Z24" s="70"/>
+      <c r="A24" s="71"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+      <c r="N24" s="71"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="71"/>
+      <c r="Q24" s="71"/>
+      <c r="R24" s="71"/>
+      <c r="S24" s="71"/>
+      <c r="T24" s="71"/>
+      <c r="U24" s="71"/>
+      <c r="V24" s="71"/>
+      <c r="W24" s="71"/>
+      <c r="X24" s="71"/>
+      <c r="Y24" s="71"/>
+      <c r="Z24" s="71"/>
       <c r="AA24" s="36"/>
     </row>
     <row r="25">
-      <c r="A25" s="70"/>
-      <c r="B25" s="70"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="94" t="s">
+      <c r="A25" s="71"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="57"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="95">
+      <c r="G25" s="58"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="97">
         <v>60.0</v>
       </c>
-      <c r="K25" s="57"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="70"/>
-      <c r="N25" s="70"/>
-      <c r="O25" s="70"/>
-      <c r="P25" s="70"/>
-      <c r="Q25" s="70"/>
-      <c r="R25" s="70"/>
-      <c r="S25" s="70"/>
-      <c r="T25" s="70"/>
-      <c r="U25" s="70"/>
-      <c r="V25" s="70"/>
-      <c r="W25" s="70"/>
-      <c r="X25" s="70"/>
-      <c r="Y25" s="70"/>
-      <c r="Z25" s="70"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="71"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="71"/>
+      <c r="Q25" s="71"/>
+      <c r="R25" s="71"/>
+      <c r="S25" s="71"/>
+      <c r="T25" s="71"/>
+      <c r="U25" s="71"/>
+      <c r="V25" s="71"/>
+      <c r="W25" s="71"/>
+      <c r="X25" s="71"/>
+      <c r="Y25" s="71"/>
+      <c r="Z25" s="71"/>
       <c r="AA25" s="36"/>
     </row>
     <row r="26">
-      <c r="A26" s="70"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="94" t="s">
+      <c r="A26" s="71"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="57"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="90"/>
-      <c r="J26" s="95">
+      <c r="G26" s="58"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="97">
         <v>45.0</v>
       </c>
-      <c r="K26" s="57"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="70"/>
-      <c r="O26" s="70"/>
-      <c r="P26" s="70"/>
-      <c r="Q26" s="70"/>
-      <c r="R26" s="70"/>
-      <c r="S26" s="70"/>
-      <c r="T26" s="70"/>
-      <c r="U26" s="70"/>
-      <c r="V26" s="70"/>
-      <c r="W26" s="70"/>
-      <c r="X26" s="70"/>
-      <c r="Y26" s="70"/>
-      <c r="Z26" s="70"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="71"/>
+      <c r="N26" s="71"/>
+      <c r="O26" s="71"/>
+      <c r="P26" s="71"/>
+      <c r="Q26" s="71"/>
+      <c r="R26" s="71"/>
+      <c r="S26" s="71"/>
+      <c r="T26" s="71"/>
+      <c r="U26" s="71"/>
+      <c r="V26" s="71"/>
+      <c r="W26" s="71"/>
+      <c r="X26" s="71"/>
+      <c r="Y26" s="71"/>
+      <c r="Z26" s="71"/>
       <c r="AA26" s="36"/>
     </row>
     <row r="27">
-      <c r="A27" s="70"/>
-      <c r="B27" s="70"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="94" t="s">
+      <c r="A27" s="71"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="57"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="95">
+      <c r="G27" s="58"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="92"/>
+      <c r="J27" s="97">
         <v>25.0</v>
       </c>
-      <c r="K27" s="57"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="70"/>
-      <c r="O27" s="70"/>
-      <c r="P27" s="70"/>
-      <c r="Q27" s="70"/>
-      <c r="R27" s="70"/>
-      <c r="S27" s="70"/>
-      <c r="T27" s="70"/>
-      <c r="U27" s="70"/>
-      <c r="V27" s="70"/>
-      <c r="W27" s="70"/>
-      <c r="X27" s="70"/>
-      <c r="Y27" s="70"/>
-      <c r="Z27" s="70"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="71"/>
+      <c r="N27" s="71"/>
+      <c r="O27" s="71"/>
+      <c r="P27" s="71"/>
+      <c r="Q27" s="71"/>
+      <c r="R27" s="71"/>
+      <c r="S27" s="71"/>
+      <c r="T27" s="71"/>
+      <c r="U27" s="71"/>
+      <c r="V27" s="71"/>
+      <c r="W27" s="71"/>
+      <c r="X27" s="71"/>
+      <c r="Y27" s="71"/>
+      <c r="Z27" s="71"/>
       <c r="AA27" s="36"/>
     </row>
     <row r="28">
-      <c r="A28" s="70"/>
-      <c r="B28" s="70"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="70"/>
-      <c r="J28" s="96">
+      <c r="A28" s="71"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="98">
         <f>SUM(J25:L27)</f>
         <v>130</v>
       </c>
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
-      <c r="M28" s="70"/>
-      <c r="N28" s="70"/>
-      <c r="O28" s="70"/>
-      <c r="P28" s="70"/>
-      <c r="Q28" s="70"/>
-      <c r="R28" s="70"/>
-      <c r="S28" s="70"/>
-      <c r="T28" s="70"/>
-      <c r="U28" s="70"/>
-      <c r="V28" s="70"/>
-      <c r="W28" s="70"/>
-      <c r="X28" s="70"/>
-      <c r="Y28" s="70"/>
-      <c r="Z28" s="70"/>
-      <c r="AA28" s="70"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="71"/>
+      <c r="Q28" s="71"/>
+      <c r="R28" s="71"/>
+      <c r="S28" s="71"/>
+      <c r="T28" s="71"/>
+      <c r="U28" s="71"/>
+      <c r="V28" s="71"/>
+      <c r="W28" s="71"/>
+      <c r="X28" s="71"/>
+      <c r="Y28" s="71"/>
+      <c r="Z28" s="71"/>
+      <c r="AA28" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5195,272 +5249,272 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="100" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="99">
+      <c r="B2" s="101">
         <v>12.0</v>
       </c>
-      <c r="C2" s="100">
+      <c r="C2" s="102">
         <v>12.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="99">
+      <c r="B3" s="101">
         <v>5.0</v>
       </c>
-      <c r="C3" s="101"/>
+      <c r="C3" s="103"/>
     </row>
     <row r="4">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="99">
+      <c r="B4" s="101">
         <v>11.0</v>
       </c>
-      <c r="C4" s="101"/>
+      <c r="C4" s="103"/>
     </row>
     <row r="5">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="99">
+      <c r="B5" s="101">
         <v>4.0</v>
       </c>
-      <c r="C5" s="101"/>
+      <c r="C5" s="103"/>
     </row>
     <row r="6">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="99">
+      <c r="B6" s="101">
         <v>17.0</v>
       </c>
-      <c r="C6" s="100">
+      <c r="C6" s="102">
         <v>17.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="99">
+      <c r="B7" s="101">
         <v>12.0</v>
       </c>
-      <c r="C7" s="100">
+      <c r="C7" s="102">
         <v>12.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="99">
-        <v>-2.0</v>
-      </c>
-      <c r="C8" s="101"/>
+      <c r="B8" s="101">
+        <v>-1.0</v>
+      </c>
+      <c r="C8" s="103"/>
     </row>
     <row r="9">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="99">
+      <c r="B9" s="101">
         <v>12.0</v>
       </c>
-      <c r="C9" s="101"/>
+      <c r="C9" s="103"/>
     </row>
     <row r="10">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="99">
+      <c r="B10" s="101">
         <v>6.0</v>
       </c>
-      <c r="C10" s="101"/>
+      <c r="C10" s="103"/>
     </row>
     <row r="11">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="99">
+      <c r="B11" s="101">
         <v>16.0</v>
       </c>
-      <c r="C11" s="101"/>
+      <c r="C11" s="103"/>
     </row>
     <row r="12">
-      <c r="A12" s="97" t="s">
+      <c r="A12" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="99">
+      <c r="B12" s="101">
         <v>5.0</v>
       </c>
-      <c r="C12" s="100">
+      <c r="C12" s="102">
         <v>5.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="97" t="s">
+      <c r="A13" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="99">
+      <c r="B13" s="101">
         <v>9.0</v>
       </c>
-      <c r="C13" s="100">
+      <c r="C13" s="102">
         <v>9.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="97" t="s">
+      <c r="A14" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="99">
+      <c r="B14" s="101">
         <v>15.0</v>
       </c>
-      <c r="C14" s="101"/>
+      <c r="C14" s="103"/>
     </row>
     <row r="15">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="99">
+      <c r="B15" s="101">
         <v>18.0</v>
       </c>
-      <c r="C15" s="101"/>
+      <c r="C15" s="103"/>
     </row>
     <row r="16">
-      <c r="A16" s="97" t="s">
+      <c r="A16" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="99">
+      <c r="B16" s="101">
+        <v>11.0</v>
+      </c>
+      <c r="C16" s="102">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="99" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="101">
+        <v>26.0</v>
+      </c>
+      <c r="C17" s="102">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="101">
+        <v>11.0</v>
+      </c>
+      <c r="C18" s="103"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="101">
+        <v>7.0</v>
+      </c>
+      <c r="C19" s="103"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="99" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="101">
+        <v>6.0</v>
+      </c>
+      <c r="C20" s="102">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="99" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="101">
+        <v>7.0</v>
+      </c>
+      <c r="C21" s="103"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="100" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="104"/>
+      <c r="C22" s="102">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="100" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="104"/>
+      <c r="C23" s="102">
         <v>12.0</v>
       </c>
-      <c r="C16" s="100">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="97" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="99">
-        <v>25.0</v>
-      </c>
-      <c r="C17" s="100">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="97" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="99">
-        <v>11.0</v>
-      </c>
-      <c r="C18" s="101"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="97" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="99">
-        <v>8.0</v>
-      </c>
-      <c r="C19" s="101"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="97" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="99">
-        <v>6.0</v>
-      </c>
-      <c r="C20" s="100">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="97" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="99">
-        <v>6.0</v>
-      </c>
-      <c r="C21" s="101"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="98" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="102"/>
-      <c r="C22" s="100">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="98" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="102"/>
-      <c r="C23" s="100">
-        <v>12.0</v>
-      </c>
     </row>
     <row r="24">
-      <c r="A24" s="98" t="s">
+      <c r="A24" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="102"/>
-      <c r="C24" s="100">
+      <c r="B24" s="104"/>
+      <c r="C24" s="102">
         <v>14.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="98" t="s">
+      <c r="A25" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="102"/>
-      <c r="C25" s="100">
+      <c r="B25" s="104"/>
+      <c r="C25" s="102">
         <v>27.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="98" t="s">
+      <c r="A26" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="102"/>
-      <c r="C26" s="100">
+      <c r="B26" s="104"/>
+      <c r="C26" s="102">
         <v>24.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="98" t="s">
+      <c r="A27" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="102"/>
-      <c r="C27" s="100">
+      <c r="B27" s="104"/>
+      <c r="C27" s="102">
         <v>29.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="102"/>
-      <c r="C28" s="100">
+      <c r="B28" s="104"/>
+      <c r="C28" s="102">
         <v>21.0</v>
       </c>
     </row>
@@ -5480,101 +5534,101 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="100" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="104">
+      <c r="B2" s="106">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
         <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="105" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="98">
+      <c r="B3" s="100">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="98">
+      <c r="B4" s="100">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="98">
+      <c r="B5" s="100">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="105" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="98">
+      <c r="B6" s="100">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="98">
+      <c r="B7" s="100">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="98">
+      <c r="B8" s="100">
         <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="103" t="s">
+      <c r="A9" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="98">
+      <c r="B9" s="100">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="105" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="98">
+      <c r="B10" s="100">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="98">
+      <c r="B11" s="100">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
018 Week 11 data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -775,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -885,6 +885,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="30" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="20" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="26" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -973,6 +976,9 @@
     <xf borderId="42" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="42" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="42" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -984,9 +990,6 @@
     </xf>
     <xf borderId="0" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="42" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -1707,7 +1710,9 @@
       </c>
       <c r="L12" s="31"/>
       <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
+      <c r="N12" s="32">
+        <v>30.0</v>
+      </c>
       <c r="O12" s="31"/>
       <c r="P12" s="31"/>
       <c r="Q12" s="31"/>
@@ -1723,11 +1728,11 @@
       <c r="AA12" s="33"/>
       <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>322</v>
+        <v>386</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36"/>
@@ -1756,7 +1761,9 @@
       <c r="K13" s="40"/>
       <c r="L13" s="40"/>
       <c r="M13" s="40"/>
-      <c r="N13" s="40"/>
+      <c r="N13" s="41">
+        <v>34.0</v>
+      </c>
       <c r="O13" s="40"/>
       <c r="P13" s="40"/>
       <c r="Q13" s="40"/>
@@ -1772,7 +1779,7 @@
       <c r="AA13" s="42"/>
       <c r="AB13" s="34">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -1820,7 +1827,7 @@
       </c>
       <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
-        <v>268</v>
+        <v>300</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="36"/>
@@ -1851,7 +1858,9 @@
       </c>
       <c r="L15" s="40"/>
       <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
+      <c r="N15" s="41">
+        <v>32.0</v>
+      </c>
       <c r="O15" s="40"/>
       <c r="P15" s="40"/>
       <c r="Q15" s="40"/>
@@ -1867,7 +1876,7 @@
       <c r="AA15" s="42"/>
       <c r="AB15" s="34">
         <f t="shared" si="1"/>
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
@@ -1903,7 +1912,9 @@
       <c r="M16" s="32">
         <v>29.0</v>
       </c>
-      <c r="N16" s="31"/>
+      <c r="N16" s="32">
+        <v>29.0</v>
+      </c>
       <c r="O16" s="31"/>
       <c r="P16" s="31"/>
       <c r="Q16" s="31"/>
@@ -1919,11 +1930,11 @@
       <c r="AA16" s="33"/>
       <c r="AB16" s="34">
         <f t="shared" si="1"/>
-        <v>209</v>
+        <v>238</v>
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>420</v>
+        <v>449</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36"/>
@@ -2299,7 +2310,9 @@
       <c r="K24" s="31"/>
       <c r="L24" s="32"/>
       <c r="M24" s="32"/>
-      <c r="N24" s="31"/>
+      <c r="N24" s="32">
+        <v>28.0</v>
+      </c>
       <c r="O24" s="31"/>
       <c r="P24" s="31"/>
       <c r="Q24" s="31"/>
@@ -2315,11 +2328,11 @@
       <c r="AA24" s="33"/>
       <c r="AB24" s="34">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
-        <v>291</v>
+        <v>346</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="36"/>
@@ -2354,7 +2367,9 @@
       <c r="M25" s="41">
         <v>28.0</v>
       </c>
-      <c r="N25" s="40"/>
+      <c r="N25" s="41">
+        <v>27.0</v>
+      </c>
       <c r="O25" s="40"/>
       <c r="P25" s="40"/>
       <c r="Q25" s="40"/>
@@ -2370,7 +2385,7 @@
       <c r="AA25" s="42"/>
       <c r="AB25" s="34">
         <f t="shared" si="1"/>
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
@@ -2406,7 +2421,9 @@
       <c r="M26" s="32">
         <v>36.0</v>
       </c>
-      <c r="N26" s="31"/>
+      <c r="N26" s="32">
+        <v>27.0</v>
+      </c>
       <c r="O26" s="31"/>
       <c r="P26" s="31"/>
       <c r="Q26" s="31"/>
@@ -2422,11 +2439,11 @@
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>455</v>
+        <v>510</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36"/>
@@ -2461,7 +2478,9 @@
       <c r="M27" s="41">
         <v>22.0</v>
       </c>
-      <c r="N27" s="40"/>
+      <c r="N27" s="41">
+        <v>28.0</v>
+      </c>
       <c r="O27" s="40"/>
       <c r="P27" s="40"/>
       <c r="Q27" s="40"/>
@@ -2477,7 +2496,7 @@
       <c r="AA27" s="42"/>
       <c r="AB27" s="34">
         <f t="shared" si="1"/>
-        <v>221</v>
+        <v>249</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
@@ -2515,7 +2534,9 @@
       <c r="M28" s="32">
         <v>33.0</v>
       </c>
-      <c r="N28" s="31"/>
+      <c r="N28" s="51">
+        <v>35.0</v>
+      </c>
       <c r="O28" s="31"/>
       <c r="P28" s="31"/>
       <c r="Q28" s="31"/>
@@ -2531,11 +2552,11 @@
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>246</v>
+        <v>281</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>518</v>
+        <v>586</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36"/>
@@ -2568,11 +2589,13 @@
       <c r="K29" s="41">
         <v>38.0</v>
       </c>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51">
+      <c r="L29" s="52"/>
+      <c r="M29" s="52">
         <v>39.0</v>
       </c>
-      <c r="N29" s="40"/>
+      <c r="N29" s="41">
+        <v>33.0</v>
+      </c>
       <c r="O29" s="40"/>
       <c r="P29" s="40"/>
       <c r="Q29" s="40"/>
@@ -2588,7 +2611,7 @@
       <c r="AA29" s="42"/>
       <c r="AB29" s="34">
         <f t="shared" si="1"/>
-        <v>272</v>
+        <v>305</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -2636,7 +2659,7 @@
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>323</v>
+        <v>352</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36"/>
@@ -2671,7 +2694,9 @@
       <c r="M31" s="41">
         <v>33.0</v>
       </c>
-      <c r="N31" s="40"/>
+      <c r="N31" s="41">
+        <v>29.0</v>
+      </c>
       <c r="O31" s="40"/>
       <c r="P31" s="40"/>
       <c r="Q31" s="40"/>
@@ -2683,18 +2708,18 @@
       <c r="W31" s="40"/>
       <c r="X31" s="40"/>
       <c r="Y31" s="40"/>
-      <c r="Z31" s="52"/>
-      <c r="AA31" s="52"/>
-      <c r="AB31" s="53">
+      <c r="Z31" s="53"/>
+      <c r="AA31" s="53"/>
+      <c r="AB31" s="54">
         <f t="shared" si="1"/>
-        <v>229</v>
+        <v>258</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
       <c r="AE31" s="36"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="54"/>
+      <c r="A32" s="55"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2725,27 +2750,27 @@
       <c r="AE32" s="1"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="55" t="s">
+      <c r="A33" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="57" t="s">
+      <c r="B33" s="57"/>
+      <c r="C33" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="58"/>
-      <c r="E33" s="56"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="57"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="59" t="s">
+      <c r="K33" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="61"/>
+      <c r="L33" s="61"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="62"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -2764,9 +2789,9 @@
       <c r="AE33" s="1"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="54"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2797,16 +2822,16 @@
       <c r="AE34" s="1"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="54"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="62" t="s">
+      <c r="E35" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="65"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2814,86 +2839,86 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="62" t="s">
+      <c r="P35" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="Q35" s="63"/>
-      <c r="R35" s="63"/>
-      <c r="S35" s="64"/>
+      <c r="Q35" s="64"/>
+      <c r="R35" s="64"/>
+      <c r="S35" s="65"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="65"/>
+      <c r="X35" s="66"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="54"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="66" t="s">
+      <c r="A36" s="55"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="67" t="s">
         <v>54</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="67">
+      <c r="E36" s="68">
         <v>80.0</v>
       </c>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="56"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="59"/>
+      <c r="H36" s="57"/>
       <c r="I36" s="36"/>
       <c r="J36" s="36"/>
       <c r="K36" s="36"/>
       <c r="L36" s="36"/>
-      <c r="M36" s="66" t="s">
+      <c r="M36" s="67" t="s">
         <v>54</v>
       </c>
       <c r="O36" s="36"/>
-      <c r="P36" s="67">
+      <c r="P36" s="68">
         <v>50.0</v>
       </c>
-      <c r="Q36" s="58"/>
-      <c r="R36" s="58"/>
-      <c r="S36" s="56"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="59"/>
+      <c r="S36" s="57"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="68"/>
+      <c r="X36" s="69"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="54"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="66" t="s">
+      <c r="A37" s="55"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="67" t="s">
         <v>55</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="67">
+      <c r="E37" s="68">
         <v>50.0</v>
       </c>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="56"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="57"/>
       <c r="I37" s="36"/>
       <c r="J37" s="36"/>
       <c r="K37" s="36"/>
       <c r="L37" s="36"/>
-      <c r="M37" s="66" t="s">
+      <c r="M37" s="67" t="s">
         <v>55</v>
       </c>
       <c r="O37" s="36"/>
-      <c r="P37" s="67">
+      <c r="P37" s="68">
         <v>30.0</v>
       </c>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="56"/>
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
+      <c r="S37" s="57"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -2908,18 +2933,18 @@
       <c r="AE37" s="1"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="54"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="66" t="s">
+      <c r="A38" s="55"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="67" t="s">
         <v>56</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="67">
+      <c r="E38" s="68">
         <v>40.0</v>
       </c>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="56"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="57"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -2927,7 +2952,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="69"/>
+      <c r="P38" s="70"/>
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="22"/>
@@ -2945,14 +2970,14 @@
       <c r="AE38" s="1"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="D39" s="70"/>
-      <c r="E39" s="69"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="70"/>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-      <c r="O39" s="70"/>
+      <c r="O39" s="71"/>
       <c r="S39" s="1"/>
       <c r="W39" s="1"/>
     </row>
@@ -4023,10 +4048,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="72" t="s">
+      <c r="A1" s="72"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73" t="s">
         <v>57</v>
       </c>
       <c r="E1" s="4"/>
@@ -4040,23 +4065,23 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
-      <c r="AA1" s="71"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="72"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="72"/>
     </row>
     <row r="2">
-      <c r="A2" s="71"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
+      <c r="A2" s="72"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -4069,100 +4094,100 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="8"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="71"/>
-      <c r="AA2" s="71"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="72"/>
+      <c r="W2" s="72"/>
+      <c r="X2" s="72"/>
+      <c r="Y2" s="72"/>
+      <c r="Z2" s="72"/>
+      <c r="AA2" s="72"/>
     </row>
     <row r="3" ht="79.5" customHeight="1">
-      <c r="A3" s="73"/>
-      <c r="B3" s="74">
+      <c r="A3" s="74"/>
+      <c r="B3" s="75">
         <v>45575.0</v>
       </c>
-      <c r="C3" s="74">
+      <c r="C3" s="75">
         <v>45582.0</v>
       </c>
-      <c r="D3" s="75">
+      <c r="D3" s="76">
         <v>45589.0</v>
       </c>
-      <c r="E3" s="75">
+      <c r="E3" s="76">
         <v>45596.0</v>
       </c>
-      <c r="F3" s="75">
+      <c r="F3" s="76">
         <v>45603.0</v>
       </c>
-      <c r="G3" s="75">
+      <c r="G3" s="76">
         <v>45610.0</v>
       </c>
-      <c r="H3" s="75">
+      <c r="H3" s="76">
         <v>45617.0</v>
       </c>
-      <c r="I3" s="75">
+      <c r="I3" s="76">
         <v>45624.0</v>
       </c>
-      <c r="J3" s="75">
+      <c r="J3" s="76">
         <v>45631.0</v>
       </c>
-      <c r="K3" s="75">
+      <c r="K3" s="76">
         <v>45638.0</v>
       </c>
-      <c r="L3" s="75">
+      <c r="L3" s="76">
         <v>45645.0</v>
       </c>
-      <c r="M3" s="75">
+      <c r="M3" s="76">
         <v>45659.0</v>
       </c>
-      <c r="N3" s="75">
+      <c r="N3" s="76">
         <v>45666.0</v>
       </c>
-      <c r="O3" s="75">
+      <c r="O3" s="76">
         <v>45673.0</v>
       </c>
-      <c r="P3" s="74">
+      <c r="P3" s="75">
         <v>45680.0</v>
       </c>
-      <c r="Q3" s="74">
+      <c r="Q3" s="75">
         <v>45687.0</v>
       </c>
-      <c r="R3" s="74">
+      <c r="R3" s="75">
         <v>45694.0</v>
       </c>
-      <c r="S3" s="74">
+      <c r="S3" s="75">
         <v>45701.0</v>
       </c>
-      <c r="T3" s="74">
+      <c r="T3" s="75">
         <v>45708.0</v>
       </c>
-      <c r="U3" s="74">
+      <c r="U3" s="75">
         <v>45715.0</v>
       </c>
-      <c r="V3" s="74">
+      <c r="V3" s="75">
         <v>45722.0</v>
       </c>
-      <c r="W3" s="74">
+      <c r="W3" s="75">
         <v>45729.0</v>
       </c>
-      <c r="X3" s="74">
+      <c r="X3" s="75">
         <v>45736.0</v>
       </c>
-      <c r="Y3" s="74">
+      <c r="Y3" s="75">
         <v>45743.0</v>
       </c>
-      <c r="Z3" s="76" t="s">
+      <c r="Z3" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="77"/>
+      <c r="AA3" s="78"/>
     </row>
     <row r="4">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
@@ -4237,774 +4262,792 @@
       <c r="Y4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="79" t="s">
+      <c r="Z4" s="80" t="s">
         <v>58</v>
       </c>
       <c r="AA4" s="27"/>
     </row>
     <row r="5">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="81">
+      <c r="B5" s="82">
         <v>30.0</v>
       </c>
-      <c r="C5" s="81">
+      <c r="C5" s="82">
         <v>37.0</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="81">
+      <c r="D5" s="83"/>
+      <c r="E5" s="82">
         <v>31.0</v>
       </c>
-      <c r="F5" s="81">
+      <c r="F5" s="82">
         <v>33.0</v>
       </c>
-      <c r="G5" s="83">
+      <c r="G5" s="84">
         <v>27.0</v>
       </c>
-      <c r="H5" s="83">
+      <c r="H5" s="84">
         <v>27.0</v>
       </c>
-      <c r="I5" s="83">
+      <c r="I5" s="84">
         <v>29.0</v>
       </c>
-      <c r="J5" s="83">
+      <c r="J5" s="84">
         <v>36.0</v>
       </c>
-      <c r="K5" s="84">
+      <c r="K5" s="85">
         <v>28.0</v>
       </c>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="82"/>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="85">
+      <c r="L5" s="86">
+        <v>38.0</v>
+      </c>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="87">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>278</v>
+        <v>316</v>
       </c>
       <c r="AA5" s="36"/>
     </row>
     <row r="6">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="82">
+      <c r="B6" s="83">
         <v>36.0</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82">
+      <c r="C6" s="83"/>
+      <c r="D6" s="83">
         <v>32.0</v>
       </c>
-      <c r="E6" s="82"/>
-      <c r="F6" s="84">
+      <c r="E6" s="83"/>
+      <c r="F6" s="85">
         <v>39.0</v>
       </c>
-      <c r="G6" s="84">
+      <c r="G6" s="85">
         <v>35.0</v>
       </c>
-      <c r="H6" s="84">
+      <c r="H6" s="85">
         <v>27.0</v>
       </c>
-      <c r="I6" s="82"/>
-      <c r="J6" s="84">
+      <c r="I6" s="83"/>
+      <c r="J6" s="85">
         <v>33.0</v>
       </c>
-      <c r="K6" s="84">
+      <c r="K6" s="85">
         <v>38.0</v>
       </c>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="82"/>
-      <c r="U6" s="82"/>
-      <c r="V6" s="82"/>
-      <c r="W6" s="82"/>
-      <c r="X6" s="82"/>
-      <c r="Y6" s="82"/>
-      <c r="Z6" s="85">
+      <c r="L6" s="85">
+        <v>35.0</v>
+      </c>
+      <c r="M6" s="83"/>
+      <c r="N6" s="83"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="83"/>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="83"/>
+      <c r="S6" s="83"/>
+      <c r="T6" s="83"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="83"/>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="83"/>
+      <c r="Z6" s="87">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>275</v>
       </c>
       <c r="AA6" s="36"/>
     </row>
     <row r="7">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="81">
+      <c r="B7" s="82">
         <v>33.0</v>
       </c>
-      <c r="C7" s="81">
+      <c r="C7" s="82">
         <v>28.0</v>
       </c>
-      <c r="D7" s="81">
+      <c r="D7" s="82">
         <v>32.0</v>
       </c>
-      <c r="E7" s="82"/>
-      <c r="F7" s="83">
+      <c r="E7" s="83"/>
+      <c r="F7" s="84">
         <v>33.0</v>
       </c>
-      <c r="G7" s="83">
+      <c r="G7" s="84">
         <v>34.0</v>
       </c>
-      <c r="H7" s="83">
+      <c r="H7" s="84">
         <v>26.0</v>
       </c>
-      <c r="I7" s="83">
+      <c r="I7" s="84">
         <v>29.0</v>
       </c>
-      <c r="J7" s="83">
+      <c r="J7" s="84">
         <v>28.0</v>
       </c>
-      <c r="K7" s="84">
+      <c r="K7" s="85">
         <v>29.0</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
-      <c r="R7" s="82"/>
-      <c r="S7" s="82"/>
-      <c r="T7" s="82"/>
-      <c r="U7" s="82"/>
-      <c r="V7" s="82"/>
-      <c r="W7" s="82"/>
-      <c r="X7" s="82"/>
-      <c r="Y7" s="82"/>
-      <c r="Z7" s="85">
+      <c r="L7" s="85">
+        <v>27.0</v>
+      </c>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="83"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="83"/>
+      <c r="V7" s="83"/>
+      <c r="W7" s="83"/>
+      <c r="X7" s="83"/>
+      <c r="Y7" s="83"/>
+      <c r="Z7" s="87">
+        <f t="shared" si="1"/>
+        <v>299</v>
+      </c>
+      <c r="AA7" s="36"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="81" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="82">
+        <v>37.0</v>
+      </c>
+      <c r="C8" s="82">
+        <v>35.0</v>
+      </c>
+      <c r="D8" s="82">
+        <v>32.0</v>
+      </c>
+      <c r="E8" s="88">
+        <v>31.0</v>
+      </c>
+      <c r="F8" s="84">
+        <v>31.0</v>
+      </c>
+      <c r="G8" s="84">
+        <v>33.0</v>
+      </c>
+      <c r="H8" s="84">
+        <v>36.0</v>
+      </c>
+      <c r="I8" s="84">
+        <v>33.0</v>
+      </c>
+      <c r="J8" s="89">
+        <v>36.0</v>
+      </c>
+      <c r="K8" s="83"/>
+      <c r="L8" s="85">
+        <v>32.0</v>
+      </c>
+      <c r="M8" s="83"/>
+      <c r="N8" s="83"/>
+      <c r="O8" s="83"/>
+      <c r="P8" s="83"/>
+      <c r="Q8" s="83"/>
+      <c r="R8" s="83"/>
+      <c r="S8" s="83"/>
+      <c r="T8" s="83"/>
+      <c r="U8" s="83"/>
+      <c r="V8" s="83"/>
+      <c r="W8" s="83"/>
+      <c r="X8" s="83"/>
+      <c r="Y8" s="83"/>
+      <c r="Z8" s="87">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="AA8" s="36"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="82">
+        <v>30.0</v>
+      </c>
+      <c r="C9" s="82">
+        <v>33.0</v>
+      </c>
+      <c r="D9" s="82">
+        <v>30.0</v>
+      </c>
+      <c r="E9" s="82">
+        <v>26.0</v>
+      </c>
+      <c r="F9" s="84">
+        <v>28.0</v>
+      </c>
+      <c r="G9" s="84">
+        <v>26.0</v>
+      </c>
+      <c r="H9" s="84">
+        <v>20.0</v>
+      </c>
+      <c r="I9" s="83"/>
+      <c r="J9" s="84">
+        <v>34.0</v>
+      </c>
+      <c r="K9" s="85">
+        <v>26.0</v>
+      </c>
+      <c r="L9" s="85">
+        <v>26.0</v>
+      </c>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="83"/>
+      <c r="P9" s="83"/>
+      <c r="Q9" s="83"/>
+      <c r="R9" s="83"/>
+      <c r="S9" s="83"/>
+      <c r="T9" s="83"/>
+      <c r="U9" s="83"/>
+      <c r="V9" s="83"/>
+      <c r="W9" s="83"/>
+      <c r="X9" s="83"/>
+      <c r="Y9" s="83"/>
+      <c r="Z9" s="87">
+        <f t="shared" si="1"/>
+        <v>279</v>
+      </c>
+      <c r="AA9" s="36"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="83"/>
+      <c r="C10" s="83">
+        <v>31.0</v>
+      </c>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83">
+        <v>23.0</v>
+      </c>
+      <c r="F10" s="85">
+        <v>35.0</v>
+      </c>
+      <c r="G10" s="85">
+        <v>29.0</v>
+      </c>
+      <c r="H10" s="85">
+        <v>16.0</v>
+      </c>
+      <c r="I10" s="83"/>
+      <c r="J10" s="85">
+        <v>29.0</v>
+      </c>
+      <c r="K10" s="85">
+        <v>21.0</v>
+      </c>
+      <c r="L10" s="85">
+        <v>24.0</v>
+      </c>
+      <c r="M10" s="83"/>
+      <c r="N10" s="83"/>
+      <c r="O10" s="83"/>
+      <c r="P10" s="83"/>
+      <c r="Q10" s="83"/>
+      <c r="R10" s="83"/>
+      <c r="S10" s="83"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="83"/>
+      <c r="V10" s="83"/>
+      <c r="W10" s="83"/>
+      <c r="X10" s="83"/>
+      <c r="Y10" s="83"/>
+      <c r="Z10" s="87">
+        <f t="shared" si="1"/>
+        <v>208</v>
+      </c>
+      <c r="AA10" s="36"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="81" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="83">
+        <v>41.0</v>
+      </c>
+      <c r="C11" s="83">
+        <v>31.0</v>
+      </c>
+      <c r="D11" s="83">
+        <v>32.0</v>
+      </c>
+      <c r="E11" s="83">
+        <v>29.0</v>
+      </c>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="85">
+        <v>23.0</v>
+      </c>
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="83"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="83"/>
+      <c r="P11" s="83"/>
+      <c r="Q11" s="83"/>
+      <c r="R11" s="83"/>
+      <c r="S11" s="83"/>
+      <c r="T11" s="83"/>
+      <c r="U11" s="83"/>
+      <c r="V11" s="83"/>
+      <c r="W11" s="83"/>
+      <c r="X11" s="83"/>
+      <c r="Y11" s="83"/>
+      <c r="Z11" s="87">
+        <f t="shared" si="1"/>
+        <v>156</v>
+      </c>
+      <c r="AA11" s="36"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="82">
+        <v>42.0</v>
+      </c>
+      <c r="C12" s="82">
+        <v>31.0</v>
+      </c>
+      <c r="D12" s="82">
+        <v>32.0</v>
+      </c>
+      <c r="E12" s="82">
+        <v>32.0</v>
+      </c>
+      <c r="F12" s="84">
+        <v>34.0</v>
+      </c>
+      <c r="G12" s="83"/>
+      <c r="H12" s="84">
+        <v>28.0</v>
+      </c>
+      <c r="I12" s="84">
+        <v>34.0</v>
+      </c>
+      <c r="J12" s="84">
+        <v>33.0</v>
+      </c>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
+      <c r="P12" s="83"/>
+      <c r="Q12" s="83"/>
+      <c r="R12" s="83"/>
+      <c r="S12" s="83"/>
+      <c r="T12" s="83"/>
+      <c r="U12" s="83"/>
+      <c r="V12" s="83"/>
+      <c r="W12" s="83"/>
+      <c r="X12" s="83"/>
+      <c r="Y12" s="83"/>
+      <c r="Z12" s="87">
+        <f t="shared" si="1"/>
+        <v>266</v>
+      </c>
+      <c r="AA12" s="36"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="81" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="90"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83">
+        <v>33.0</v>
+      </c>
+      <c r="E13" s="83">
+        <v>36.0</v>
+      </c>
+      <c r="F13" s="85">
+        <v>27.0</v>
+      </c>
+      <c r="G13" s="85">
+        <v>37.0</v>
+      </c>
+      <c r="H13" s="85">
+        <v>31.0</v>
+      </c>
+      <c r="I13" s="83"/>
+      <c r="J13" s="85">
+        <v>34.0</v>
+      </c>
+      <c r="K13" s="86">
+        <v>40.0</v>
+      </c>
+      <c r="L13" s="85">
+        <v>34.0</v>
+      </c>
+      <c r="M13" s="83"/>
+      <c r="N13" s="83"/>
+      <c r="O13" s="83"/>
+      <c r="P13" s="83"/>
+      <c r="Q13" s="83"/>
+      <c r="R13" s="83"/>
+      <c r="S13" s="83"/>
+      <c r="T13" s="83"/>
+      <c r="U13" s="83"/>
+      <c r="V13" s="83"/>
+      <c r="W13" s="83"/>
+      <c r="X13" s="83"/>
+      <c r="Y13" s="83"/>
+      <c r="Z13" s="87">
         <f t="shared" si="1"/>
         <v>272</v>
       </c>
-      <c r="AA7" s="36"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="81">
+      <c r="AA13" s="36"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="81" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="83"/>
+      <c r="C14" s="83">
+        <v>22.0</v>
+      </c>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="85">
+        <v>36.0</v>
+      </c>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="85">
+        <v>34.0</v>
+      </c>
+      <c r="K14" s="85">
+        <v>27.0</v>
+      </c>
+      <c r="L14" s="85">
+        <v>35.0</v>
+      </c>
+      <c r="M14" s="83"/>
+      <c r="N14" s="83"/>
+      <c r="O14" s="83"/>
+      <c r="P14" s="83"/>
+      <c r="Q14" s="83"/>
+      <c r="R14" s="83"/>
+      <c r="S14" s="83"/>
+      <c r="T14" s="83"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="83"/>
+      <c r="W14" s="83"/>
+      <c r="X14" s="83"/>
+      <c r="Y14" s="83"/>
+      <c r="Z14" s="87">
+        <f t="shared" si="1"/>
+        <v>154</v>
+      </c>
+      <c r="AA14" s="36"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83">
+        <v>43.0</v>
+      </c>
+      <c r="D15" s="83">
+        <v>25.0</v>
+      </c>
+      <c r="E15" s="83"/>
+      <c r="F15" s="85">
+        <v>32.0</v>
+      </c>
+      <c r="G15" s="85">
+        <v>30.0</v>
+      </c>
+      <c r="H15" s="85">
+        <v>34.0</v>
+      </c>
+      <c r="I15" s="83"/>
+      <c r="J15" s="85">
+        <v>34.0</v>
+      </c>
+      <c r="K15" s="85">
+        <v>26.0</v>
+      </c>
+      <c r="L15" s="85">
         <v>37.0</v>
       </c>
-      <c r="C8" s="81">
-        <v>35.0</v>
-      </c>
-      <c r="D8" s="81">
-        <v>32.0</v>
-      </c>
-      <c r="E8" s="86">
-        <v>31.0</v>
-      </c>
-      <c r="F8" s="83">
-        <v>31.0</v>
-      </c>
-      <c r="G8" s="83">
-        <v>33.0</v>
-      </c>
-      <c r="H8" s="83">
-        <v>36.0</v>
-      </c>
-      <c r="I8" s="83">
-        <v>33.0</v>
-      </c>
-      <c r="J8" s="87">
-        <v>36.0</v>
-      </c>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="82"/>
-      <c r="N8" s="82"/>
-      <c r="O8" s="82"/>
-      <c r="P8" s="82"/>
-      <c r="Q8" s="82"/>
-      <c r="R8" s="82"/>
-      <c r="S8" s="82"/>
-      <c r="T8" s="82"/>
-      <c r="U8" s="82"/>
-      <c r="V8" s="82"/>
-      <c r="W8" s="82"/>
-      <c r="X8" s="82"/>
-      <c r="Y8" s="82"/>
-      <c r="Z8" s="85">
+      <c r="M15" s="83"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="83"/>
+      <c r="Q15" s="83"/>
+      <c r="R15" s="83"/>
+      <c r="S15" s="83"/>
+      <c r="T15" s="83"/>
+      <c r="U15" s="83"/>
+      <c r="V15" s="83"/>
+      <c r="W15" s="83"/>
+      <c r="X15" s="83"/>
+      <c r="Y15" s="83"/>
+      <c r="Z15" s="87">
         <f t="shared" si="1"/>
-        <v>304</v>
-      </c>
-      <c r="AA8" s="36"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="80" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="81">
+        <v>261</v>
+      </c>
+      <c r="AA15" s="36"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="83"/>
+      <c r="C16" s="83">
+        <v>29.0</v>
+      </c>
+      <c r="D16" s="83">
+        <v>28.0</v>
+      </c>
+      <c r="E16" s="83"/>
+      <c r="F16" s="85">
+        <v>23.0</v>
+      </c>
+      <c r="G16" s="85">
         <v>30.0</v>
       </c>
-      <c r="C9" s="81">
-        <v>33.0</v>
-      </c>
-      <c r="D9" s="81">
-        <v>30.0</v>
-      </c>
-      <c r="E9" s="81">
-        <v>26.0</v>
-      </c>
-      <c r="F9" s="83">
-        <v>28.0</v>
-      </c>
-      <c r="G9" s="83">
-        <v>26.0</v>
-      </c>
-      <c r="H9" s="83">
-        <v>20.0</v>
-      </c>
-      <c r="I9" s="82"/>
-      <c r="J9" s="83">
-        <v>34.0</v>
-      </c>
-      <c r="K9" s="84">
-        <v>26.0</v>
-      </c>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="82"/>
-      <c r="R9" s="82"/>
-      <c r="S9" s="82"/>
-      <c r="T9" s="82"/>
-      <c r="U9" s="82"/>
-      <c r="V9" s="82"/>
-      <c r="W9" s="82"/>
-      <c r="X9" s="82"/>
-      <c r="Y9" s="82"/>
-      <c r="Z9" s="85">
-        <f t="shared" si="1"/>
-        <v>253</v>
-      </c>
-      <c r="AA9" s="36"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="80" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82">
-        <v>31.0</v>
-      </c>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82">
-        <v>23.0</v>
-      </c>
-      <c r="F10" s="84">
-        <v>35.0</v>
-      </c>
-      <c r="G10" s="84">
+      <c r="H16" s="83"/>
+      <c r="I16" s="85">
+        <v>27.0</v>
+      </c>
+      <c r="J16" s="83"/>
+      <c r="K16" s="85">
         <v>29.0</v>
       </c>
-      <c r="H10" s="84">
-        <v>16.0</v>
-      </c>
-      <c r="I10" s="82"/>
-      <c r="J10" s="84">
-        <v>29.0</v>
-      </c>
-      <c r="K10" s="84">
-        <v>21.0</v>
-      </c>
-      <c r="L10" s="82"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="82"/>
-      <c r="R10" s="82"/>
-      <c r="S10" s="82"/>
-      <c r="T10" s="82"/>
-      <c r="U10" s="82"/>
-      <c r="V10" s="82"/>
-      <c r="W10" s="82"/>
-      <c r="X10" s="82"/>
-      <c r="Y10" s="82"/>
-      <c r="Z10" s="85">
-        <f t="shared" si="1"/>
-        <v>184</v>
-      </c>
-      <c r="AA10" s="36"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="82">
-        <v>41.0</v>
-      </c>
-      <c r="C11" s="82">
-        <v>31.0</v>
-      </c>
-      <c r="D11" s="82">
-        <v>32.0</v>
-      </c>
-      <c r="E11" s="82">
-        <v>29.0</v>
-      </c>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="84">
-        <v>23.0</v>
-      </c>
-      <c r="I11" s="82"/>
-      <c r="J11" s="82"/>
-      <c r="K11" s="82"/>
-      <c r="L11" s="82"/>
-      <c r="M11" s="82"/>
-      <c r="N11" s="82"/>
-      <c r="O11" s="82"/>
-      <c r="P11" s="82"/>
-      <c r="Q11" s="82"/>
-      <c r="R11" s="82"/>
-      <c r="S11" s="82"/>
-      <c r="T11" s="82"/>
-      <c r="U11" s="82"/>
-      <c r="V11" s="82"/>
-      <c r="W11" s="82"/>
-      <c r="X11" s="82"/>
-      <c r="Y11" s="82"/>
-      <c r="Z11" s="85">
-        <f t="shared" si="1"/>
-        <v>156</v>
-      </c>
-      <c r="AA11" s="36"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="80" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="81">
-        <v>42.0</v>
-      </c>
-      <c r="C12" s="81">
-        <v>31.0</v>
-      </c>
-      <c r="D12" s="81">
-        <v>32.0</v>
-      </c>
-      <c r="E12" s="81">
-        <v>32.0</v>
-      </c>
-      <c r="F12" s="83">
-        <v>34.0</v>
-      </c>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83">
-        <v>28.0</v>
-      </c>
-      <c r="I12" s="83">
-        <v>34.0</v>
-      </c>
-      <c r="J12" s="83">
-        <v>33.0</v>
-      </c>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="82"/>
-      <c r="R12" s="82"/>
-      <c r="S12" s="82"/>
-      <c r="T12" s="82"/>
-      <c r="U12" s="82"/>
-      <c r="V12" s="82"/>
-      <c r="W12" s="82"/>
-      <c r="X12" s="82"/>
-      <c r="Y12" s="82"/>
-      <c r="Z12" s="85">
-        <f t="shared" si="1"/>
-        <v>266</v>
-      </c>
-      <c r="AA12" s="36"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="80" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="88"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82">
-        <v>33.0</v>
-      </c>
-      <c r="E13" s="82">
-        <v>36.0</v>
-      </c>
-      <c r="F13" s="84">
-        <v>27.0</v>
-      </c>
-      <c r="G13" s="84">
-        <v>37.0</v>
-      </c>
-      <c r="H13" s="84">
-        <v>31.0</v>
-      </c>
-      <c r="I13" s="82"/>
-      <c r="J13" s="84">
-        <v>34.0</v>
-      </c>
-      <c r="K13" s="89">
-        <v>40.0</v>
-      </c>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="82"/>
-      <c r="O13" s="82"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="82"/>
-      <c r="S13" s="82"/>
-      <c r="T13" s="82"/>
-      <c r="U13" s="82"/>
-      <c r="V13" s="82"/>
-      <c r="W13" s="82"/>
-      <c r="X13" s="82"/>
-      <c r="Y13" s="82"/>
-      <c r="Z13" s="85">
-        <f t="shared" si="1"/>
-        <v>238</v>
-      </c>
-      <c r="AA13" s="36"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="80" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="82"/>
-      <c r="C14" s="82">
-        <v>22.0</v>
-      </c>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="84">
-        <v>36.0</v>
-      </c>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="84">
-        <v>34.0</v>
-      </c>
-      <c r="K14" s="84">
-        <v>27.0</v>
-      </c>
-      <c r="L14" s="82"/>
-      <c r="M14" s="82"/>
-      <c r="N14" s="82"/>
-      <c r="O14" s="82"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="82"/>
-      <c r="R14" s="82"/>
-      <c r="S14" s="82"/>
-      <c r="T14" s="82"/>
-      <c r="U14" s="82"/>
-      <c r="V14" s="82"/>
-      <c r="W14" s="82"/>
-      <c r="X14" s="82"/>
-      <c r="Y14" s="82"/>
-      <c r="Z14" s="85">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="AA14" s="36"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="82"/>
-      <c r="C15" s="82">
-        <v>43.0</v>
-      </c>
-      <c r="D15" s="82">
-        <v>25.0</v>
-      </c>
-      <c r="E15" s="82"/>
-      <c r="F15" s="84">
-        <v>32.0</v>
-      </c>
-      <c r="G15" s="84">
-        <v>30.0</v>
-      </c>
-      <c r="H15" s="84">
-        <v>34.0</v>
-      </c>
-      <c r="I15" s="82"/>
-      <c r="J15" s="84">
-        <v>34.0</v>
-      </c>
-      <c r="K15" s="84">
-        <v>26.0</v>
-      </c>
-      <c r="L15" s="82"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="82"/>
-      <c r="P15" s="82"/>
-      <c r="Q15" s="82"/>
-      <c r="R15" s="82"/>
-      <c r="S15" s="82"/>
-      <c r="T15" s="82"/>
-      <c r="U15" s="82"/>
-      <c r="V15" s="82"/>
-      <c r="W15" s="82"/>
-      <c r="X15" s="82"/>
-      <c r="Y15" s="82"/>
-      <c r="Z15" s="85">
-        <f t="shared" si="1"/>
-        <v>224</v>
-      </c>
-      <c r="AA15" s="36"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="80" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="82"/>
-      <c r="C16" s="82">
-        <v>29.0</v>
-      </c>
-      <c r="D16" s="82">
-        <v>28.0</v>
-      </c>
-      <c r="E16" s="82"/>
-      <c r="F16" s="84">
-        <v>23.0</v>
-      </c>
-      <c r="G16" s="84">
-        <v>30.0</v>
-      </c>
-      <c r="H16" s="82"/>
-      <c r="I16" s="84">
-        <v>27.0</v>
-      </c>
-      <c r="J16" s="82"/>
-      <c r="K16" s="84">
-        <v>29.0</v>
-      </c>
-      <c r="L16" s="82"/>
-      <c r="M16" s="82"/>
-      <c r="N16" s="82"/>
-      <c r="O16" s="82"/>
-      <c r="P16" s="82"/>
-      <c r="Q16" s="82"/>
-      <c r="R16" s="82"/>
-      <c r="S16" s="82"/>
-      <c r="T16" s="82"/>
-      <c r="U16" s="82"/>
-      <c r="V16" s="82"/>
-      <c r="W16" s="82"/>
-      <c r="X16" s="82"/>
-      <c r="Y16" s="82"/>
-      <c r="Z16" s="85">
+      <c r="L16" s="83"/>
+      <c r="M16" s="83"/>
+      <c r="N16" s="83"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="83"/>
+      <c r="Q16" s="83"/>
+      <c r="R16" s="83"/>
+      <c r="S16" s="83"/>
+      <c r="T16" s="83"/>
+      <c r="U16" s="83"/>
+      <c r="V16" s="83"/>
+      <c r="W16" s="83"/>
+      <c r="X16" s="83"/>
+      <c r="Y16" s="83"/>
+      <c r="Z16" s="87">
         <f t="shared" si="1"/>
         <v>166</v>
       </c>
       <c r="AA16" s="36"/>
     </row>
     <row r="17">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84">
+      <c r="B17" s="83"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="85"/>
+      <c r="G17" s="85">
         <v>26.0</v>
       </c>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="82"/>
-      <c r="O17" s="82"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="82"/>
-      <c r="R17" s="82"/>
-      <c r="S17" s="82"/>
-      <c r="T17" s="82"/>
-      <c r="U17" s="82"/>
-      <c r="V17" s="82"/>
-      <c r="W17" s="82"/>
-      <c r="X17" s="82"/>
-      <c r="Y17" s="82"/>
-      <c r="Z17" s="85">
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="83"/>
+      <c r="N17" s="83"/>
+      <c r="O17" s="83"/>
+      <c r="P17" s="83"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="83"/>
+      <c r="S17" s="83"/>
+      <c r="T17" s="83"/>
+      <c r="U17" s="83"/>
+      <c r="V17" s="83"/>
+      <c r="W17" s="83"/>
+      <c r="X17" s="83"/>
+      <c r="Y17" s="83"/>
+      <c r="Z17" s="87">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="AA17" s="36"/>
     </row>
     <row r="18">
-      <c r="A18" s="90" t="s">
+      <c r="A18" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84">
+      <c r="B18" s="83"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85">
         <v>27.0</v>
       </c>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="82"/>
-      <c r="P18" s="82"/>
-      <c r="Q18" s="82"/>
-      <c r="R18" s="82"/>
-      <c r="S18" s="82"/>
-      <c r="T18" s="82"/>
-      <c r="U18" s="82"/>
-      <c r="V18" s="82"/>
-      <c r="W18" s="82"/>
-      <c r="X18" s="82"/>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="85">
+      <c r="H18" s="83"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="83"/>
+      <c r="K18" s="83"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="83"/>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="83"/>
+      <c r="S18" s="83"/>
+      <c r="T18" s="83"/>
+      <c r="U18" s="83"/>
+      <c r="V18" s="83"/>
+      <c r="W18" s="83"/>
+      <c r="X18" s="83"/>
+      <c r="Y18" s="83"/>
+      <c r="Z18" s="87">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="AA18" s="36"/>
     </row>
     <row r="19">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82">
+      <c r="B19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83">
         <v>41.0</v>
       </c>
-      <c r="E19" s="82">
+      <c r="E19" s="83">
         <v>37.0</v>
       </c>
-      <c r="F19" s="84">
+      <c r="F19" s="85">
         <v>38.0</v>
       </c>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="82"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="82"/>
-      <c r="R19" s="82"/>
-      <c r="S19" s="82"/>
-      <c r="T19" s="82"/>
-      <c r="U19" s="82"/>
-      <c r="V19" s="82"/>
-      <c r="W19" s="82"/>
-      <c r="X19" s="82"/>
-      <c r="Y19" s="82"/>
-      <c r="Z19" s="85">
+      <c r="G19" s="83"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="83"/>
+      <c r="J19" s="83"/>
+      <c r="K19" s="83"/>
+      <c r="L19" s="83"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="83"/>
+      <c r="P19" s="83"/>
+      <c r="Q19" s="83"/>
+      <c r="R19" s="83"/>
+      <c r="S19" s="83"/>
+      <c r="T19" s="83"/>
+      <c r="U19" s="83"/>
+      <c r="V19" s="83"/>
+      <c r="W19" s="83"/>
+      <c r="X19" s="83"/>
+      <c r="Y19" s="83"/>
+      <c r="Z19" s="87">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="AA19" s="36"/>
     </row>
     <row r="20">
-      <c r="A20" s="91"/>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="92"/>
-      <c r="M20" s="92"/>
-      <c r="N20" s="92"/>
-      <c r="O20" s="92"/>
-      <c r="P20" s="92"/>
-      <c r="Q20" s="92"/>
-      <c r="R20" s="92"/>
-      <c r="S20" s="92"/>
-      <c r="T20" s="92"/>
-      <c r="U20" s="92"/>
-      <c r="V20" s="92"/>
-      <c r="W20" s="92"/>
-      <c r="X20" s="92"/>
-      <c r="Y20" s="92"/>
-      <c r="Z20" s="92"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="93"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="93"/>
+      <c r="L20" s="93"/>
+      <c r="M20" s="93"/>
+      <c r="N20" s="93"/>
+      <c r="O20" s="93"/>
+      <c r="P20" s="93"/>
+      <c r="Q20" s="93"/>
+      <c r="R20" s="93"/>
+      <c r="S20" s="93"/>
+      <c r="T20" s="93"/>
+      <c r="U20" s="93"/>
+      <c r="V20" s="93"/>
+      <c r="W20" s="93"/>
+      <c r="X20" s="93"/>
+      <c r="Y20" s="93"/>
+      <c r="Z20" s="93"/>
       <c r="AA20" s="36"/>
     </row>
     <row r="21">
-      <c r="A21" s="71"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="71"/>
-      <c r="M21" s="71"/>
-      <c r="N21" s="71"/>
-      <c r="O21" s="71"/>
-      <c r="P21" s="71"/>
-      <c r="Q21" s="71"/>
-      <c r="R21" s="71"/>
-      <c r="S21" s="71"/>
-      <c r="T21" s="71"/>
-      <c r="U21" s="71"/>
-      <c r="V21" s="71"/>
-      <c r="W21" s="71"/>
-      <c r="X21" s="71"/>
-      <c r="Y21" s="71"/>
-      <c r="Z21" s="71"/>
+      <c r="A21" s="72"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="72"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="72"/>
+      <c r="Q21" s="72"/>
+      <c r="R21" s="72"/>
+      <c r="S21" s="72"/>
+      <c r="T21" s="72"/>
+      <c r="U21" s="72"/>
+      <c r="V21" s="72"/>
+      <c r="W21" s="72"/>
+      <c r="X21" s="72"/>
+      <c r="Y21" s="72"/>
+      <c r="Z21" s="72"/>
       <c r="AA21" s="36"/>
     </row>
     <row r="22">
-      <c r="A22" s="93" t="s">
+      <c r="A22" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="94">
+      <c r="B22" s="95">
         <v>10.0</v>
       </c>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="95" t="s">
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="96" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="4"/>
@@ -5013,28 +5056,28 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="71"/>
-      <c r="P22" s="71"/>
-      <c r="Q22" s="71"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="71"/>
-      <c r="T22" s="71"/>
-      <c r="U22" s="71"/>
-      <c r="V22" s="71"/>
-      <c r="W22" s="71"/>
-      <c r="X22" s="71"/>
-      <c r="Y22" s="71"/>
-      <c r="Z22" s="71"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="72"/>
+      <c r="Q22" s="72"/>
+      <c r="R22" s="72"/>
+      <c r="S22" s="72"/>
+      <c r="T22" s="72"/>
+      <c r="U22" s="72"/>
+      <c r="V22" s="72"/>
+      <c r="W22" s="72"/>
+      <c r="X22" s="72"/>
+      <c r="Y22" s="72"/>
+      <c r="Z22" s="72"/>
       <c r="AA22" s="36"/>
     </row>
     <row r="23">
-      <c r="A23" s="71"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
+      <c r="A23" s="72"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -5042,181 +5085,181 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="71"/>
-      <c r="N23" s="71"/>
-      <c r="O23" s="71"/>
-      <c r="P23" s="71"/>
-      <c r="Q23" s="71"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="71"/>
-      <c r="T23" s="71"/>
-      <c r="U23" s="71"/>
-      <c r="V23" s="71"/>
-      <c r="W23" s="71"/>
-      <c r="X23" s="71"/>
-      <c r="Y23" s="71"/>
-      <c r="Z23" s="71"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="72"/>
+      <c r="R23" s="72"/>
+      <c r="S23" s="72"/>
+      <c r="T23" s="72"/>
+      <c r="U23" s="72"/>
+      <c r="V23" s="72"/>
+      <c r="W23" s="72"/>
+      <c r="X23" s="72"/>
+      <c r="Y23" s="72"/>
+      <c r="Z23" s="72"/>
       <c r="AA23" s="36"/>
     </row>
     <row r="24">
-      <c r="A24" s="71"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="71"/>
-      <c r="N24" s="71"/>
-      <c r="O24" s="71"/>
-      <c r="P24" s="71"/>
-      <c r="Q24" s="71"/>
-      <c r="R24" s="71"/>
-      <c r="S24" s="71"/>
-      <c r="T24" s="71"/>
-      <c r="U24" s="71"/>
-      <c r="V24" s="71"/>
-      <c r="W24" s="71"/>
-      <c r="X24" s="71"/>
-      <c r="Y24" s="71"/>
-      <c r="Z24" s="71"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="72"/>
+      <c r="K24" s="72"/>
+      <c r="L24" s="72"/>
+      <c r="M24" s="72"/>
+      <c r="N24" s="72"/>
+      <c r="O24" s="72"/>
+      <c r="P24" s="72"/>
+      <c r="Q24" s="72"/>
+      <c r="R24" s="72"/>
+      <c r="S24" s="72"/>
+      <c r="T24" s="72"/>
+      <c r="U24" s="72"/>
+      <c r="V24" s="72"/>
+      <c r="W24" s="72"/>
+      <c r="X24" s="72"/>
+      <c r="Y24" s="72"/>
+      <c r="Z24" s="72"/>
       <c r="AA24" s="36"/>
     </row>
     <row r="25">
-      <c r="A25" s="71"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="96" t="s">
+      <c r="A25" s="72"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="58"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="92"/>
-      <c r="J25" s="97">
+      <c r="G25" s="59"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="93"/>
+      <c r="J25" s="98">
         <v>60.0</v>
       </c>
-      <c r="K25" s="58"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="71"/>
-      <c r="N25" s="71"/>
-      <c r="O25" s="71"/>
-      <c r="P25" s="71"/>
-      <c r="Q25" s="71"/>
-      <c r="R25" s="71"/>
-      <c r="S25" s="71"/>
-      <c r="T25" s="71"/>
-      <c r="U25" s="71"/>
-      <c r="V25" s="71"/>
-      <c r="W25" s="71"/>
-      <c r="X25" s="71"/>
-      <c r="Y25" s="71"/>
-      <c r="Z25" s="71"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="72"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="72"/>
+      <c r="P25" s="72"/>
+      <c r="Q25" s="72"/>
+      <c r="R25" s="72"/>
+      <c r="S25" s="72"/>
+      <c r="T25" s="72"/>
+      <c r="U25" s="72"/>
+      <c r="V25" s="72"/>
+      <c r="W25" s="72"/>
+      <c r="X25" s="72"/>
+      <c r="Y25" s="72"/>
+      <c r="Z25" s="72"/>
       <c r="AA25" s="36"/>
     </row>
     <row r="26">
-      <c r="A26" s="71"/>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="96" t="s">
+      <c r="A26" s="72"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="58"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="92"/>
-      <c r="J26" s="97">
+      <c r="G26" s="59"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="93"/>
+      <c r="J26" s="98">
         <v>45.0</v>
       </c>
-      <c r="K26" s="58"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="71"/>
-      <c r="N26" s="71"/>
-      <c r="O26" s="71"/>
-      <c r="P26" s="71"/>
-      <c r="Q26" s="71"/>
-      <c r="R26" s="71"/>
-      <c r="S26" s="71"/>
-      <c r="T26" s="71"/>
-      <c r="U26" s="71"/>
-      <c r="V26" s="71"/>
-      <c r="W26" s="71"/>
-      <c r="X26" s="71"/>
-      <c r="Y26" s="71"/>
-      <c r="Z26" s="71"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
+      <c r="O26" s="72"/>
+      <c r="P26" s="72"/>
+      <c r="Q26" s="72"/>
+      <c r="R26" s="72"/>
+      <c r="S26" s="72"/>
+      <c r="T26" s="72"/>
+      <c r="U26" s="72"/>
+      <c r="V26" s="72"/>
+      <c r="W26" s="72"/>
+      <c r="X26" s="72"/>
+      <c r="Y26" s="72"/>
+      <c r="Z26" s="72"/>
       <c r="AA26" s="36"/>
     </row>
     <row r="27">
-      <c r="A27" s="71"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="96" t="s">
+      <c r="A27" s="72"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="58"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="92"/>
-      <c r="J27" s="97">
+      <c r="G27" s="59"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="98">
         <v>25.0</v>
       </c>
-      <c r="K27" s="58"/>
-      <c r="L27" s="56"/>
-      <c r="M27" s="71"/>
-      <c r="N27" s="71"/>
-      <c r="O27" s="71"/>
-      <c r="P27" s="71"/>
-      <c r="Q27" s="71"/>
-      <c r="R27" s="71"/>
-      <c r="S27" s="71"/>
-      <c r="T27" s="71"/>
-      <c r="U27" s="71"/>
-      <c r="V27" s="71"/>
-      <c r="W27" s="71"/>
-      <c r="X27" s="71"/>
-      <c r="Y27" s="71"/>
-      <c r="Z27" s="71"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="57"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="72"/>
+      <c r="Q27" s="72"/>
+      <c r="R27" s="72"/>
+      <c r="S27" s="72"/>
+      <c r="T27" s="72"/>
+      <c r="U27" s="72"/>
+      <c r="V27" s="72"/>
+      <c r="W27" s="72"/>
+      <c r="X27" s="72"/>
+      <c r="Y27" s="72"/>
+      <c r="Z27" s="72"/>
       <c r="AA27" s="36"/>
     </row>
     <row r="28">
-      <c r="A28" s="71"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="98">
+      <c r="A28" s="72"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="99">
         <f>SUM(J25:L27)</f>
         <v>130</v>
       </c>
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
-      <c r="M28" s="71"/>
-      <c r="N28" s="71"/>
-      <c r="O28" s="71"/>
-      <c r="P28" s="71"/>
-      <c r="Q28" s="71"/>
-      <c r="R28" s="71"/>
-      <c r="S28" s="71"/>
-      <c r="T28" s="71"/>
-      <c r="U28" s="71"/>
-      <c r="V28" s="71"/>
-      <c r="W28" s="71"/>
-      <c r="X28" s="71"/>
-      <c r="Y28" s="71"/>
-      <c r="Z28" s="71"/>
-      <c r="AA28" s="71"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
+      <c r="O28" s="72"/>
+      <c r="P28" s="72"/>
+      <c r="Q28" s="72"/>
+      <c r="R28" s="72"/>
+      <c r="S28" s="72"/>
+      <c r="T28" s="72"/>
+      <c r="U28" s="72"/>
+      <c r="V28" s="72"/>
+      <c r="W28" s="72"/>
+      <c r="X28" s="72"/>
+      <c r="Y28" s="72"/>
+      <c r="Z28" s="72"/>
+      <c r="AA28" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5249,272 +5292,272 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="101" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="101" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="101">
+      <c r="B2" s="102">
+        <v>11.0</v>
+      </c>
+      <c r="C2" s="103">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="100" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="102">
+        <v>5.0</v>
+      </c>
+      <c r="C3" s="104"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="100" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="102">
+        <v>11.0</v>
+      </c>
+      <c r="C4" s="104"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="100" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="102">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="104"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="100" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="102">
+        <v>17.0</v>
+      </c>
+      <c r="C6" s="103">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="102">
         <v>12.0</v>
       </c>
-      <c r="C2" s="102">
+      <c r="C7" s="103">
         <v>12.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="99" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="101">
+    <row r="8">
+      <c r="A8" s="100" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="102">
+        <v>-1.0</v>
+      </c>
+      <c r="C8" s="104"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="102">
+        <v>12.0</v>
+      </c>
+      <c r="C9" s="104"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="100" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="102">
+        <v>6.0</v>
+      </c>
+      <c r="C10" s="104"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="100" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="102">
+        <v>16.0</v>
+      </c>
+      <c r="C11" s="104"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="100" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="102">
         <v>5.0</v>
       </c>
-      <c r="C3" s="103"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="99" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="101">
+      <c r="C12" s="103">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="100" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="102">
+        <v>9.0</v>
+      </c>
+      <c r="C13" s="103">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="100" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="102">
+        <v>15.0</v>
+      </c>
+      <c r="C14" s="104"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="100" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="102">
+        <v>18.0</v>
+      </c>
+      <c r="C15" s="104"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="100" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="102">
         <v>11.0</v>
       </c>
-      <c r="C4" s="103"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="99" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="101">
-        <v>4.0</v>
-      </c>
-      <c r="C5" s="103"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="99" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="101">
-        <v>17.0</v>
-      </c>
-      <c r="C6" s="102">
-        <v>17.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="101">
+      <c r="C16" s="103">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="100" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="102">
+        <v>26.0</v>
+      </c>
+      <c r="C17" s="103">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="100" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="102">
+        <v>11.0</v>
+      </c>
+      <c r="C18" s="104"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="102">
+        <v>7.0</v>
+      </c>
+      <c r="C19" s="104"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="102">
+        <v>6.0</v>
+      </c>
+      <c r="C20" s="103">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="100" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="102">
+        <v>7.0</v>
+      </c>
+      <c r="C21" s="104"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="101" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="105"/>
+      <c r="C22" s="103">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="101" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="105"/>
+      <c r="C23" s="103">
         <v>12.0</v>
       </c>
-      <c r="C7" s="102">
+    </row>
+    <row r="24">
+      <c r="A24" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="105"/>
+      <c r="C24" s="103">
         <v>12.0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="99" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="101">
-        <v>-1.0</v>
-      </c>
-      <c r="C8" s="103"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="99" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="101">
-        <v>12.0</v>
-      </c>
-      <c r="C9" s="103"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="99" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="101">
-        <v>6.0</v>
-      </c>
-      <c r="C10" s="103"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="99" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="101">
-        <v>16.0</v>
-      </c>
-      <c r="C11" s="103"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="99" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="101">
-        <v>5.0</v>
-      </c>
-      <c r="C12" s="102">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="99" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="101">
-        <v>9.0</v>
-      </c>
-      <c r="C13" s="102">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="99" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="101">
-        <v>15.0</v>
-      </c>
-      <c r="C14" s="103"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="99" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="101">
-        <v>18.0</v>
-      </c>
-      <c r="C15" s="103"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="99" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="101">
-        <v>11.0</v>
-      </c>
-      <c r="C16" s="102">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="99" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="101">
-        <v>26.0</v>
-      </c>
-      <c r="C17" s="102">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="99" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="101">
-        <v>11.0</v>
-      </c>
-      <c r="C18" s="103"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="99" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="101">
-        <v>7.0</v>
-      </c>
-      <c r="C19" s="103"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="99" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="101">
-        <v>6.0</v>
-      </c>
-      <c r="C20" s="102">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="99" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="101">
-        <v>7.0</v>
-      </c>
-      <c r="C21" s="103"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="104"/>
-      <c r="C22" s="102">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="100" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="104"/>
-      <c r="C23" s="102">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="100" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="104"/>
-      <c r="C24" s="102">
-        <v>14.0</v>
-      </c>
-    </row>
     <row r="25">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="104"/>
-      <c r="C25" s="102">
+      <c r="B25" s="105"/>
+      <c r="C25" s="103">
         <v>27.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="100" t="s">
+      <c r="A26" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="104"/>
-      <c r="C26" s="102">
+      <c r="B26" s="105"/>
+      <c r="C26" s="103">
         <v>24.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="100" t="s">
+      <c r="A27" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="104"/>
-      <c r="C27" s="102">
+      <c r="B27" s="105"/>
+      <c r="C27" s="103">
         <v>29.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="100" t="s">
+      <c r="A28" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="104"/>
-      <c r="C28" s="102">
+      <c r="B28" s="105"/>
+      <c r="C28" s="103">
         <v>21.0</v>
       </c>
     </row>
@@ -5534,101 +5577,101 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="101" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="106">
+      <c r="B2" s="107">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="100">
+      <c r="B3" s="101">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="100">
+      <c r="B4" s="101">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="100">
+      <c r="B5" s="101">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
         <v>7</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="105" t="s">
+      <c r="A6" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="100">
+      <c r="B6" s="101">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
         <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="105" t="s">
+      <c r="A7" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="100">
+      <c r="B7" s="101">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
         <v>9</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="105" t="s">
+      <c r="A8" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="100">
+      <c r="B8" s="101">
         <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="105" t="s">
+      <c r="A9" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="100">
+      <c r="B9" s="101">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="105" t="s">
+      <c r="A10" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="100">
+      <c r="B10" s="101">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="105" t="s">
+      <c r="A11" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="100">
+      <c r="B11" s="101">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 12 (Thurs) update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -2052,7 +2052,7 @@
       <c r="O18" s="35">
         <v>38.0</v>
       </c>
-      <c r="P18" s="34"/>
+      <c r="P18" s="35"/>
       <c r="Q18" s="34"/>
       <c r="R18" s="34"/>
       <c r="S18" s="34"/>
@@ -2097,7 +2097,7 @@
       <c r="M19" s="44"/>
       <c r="N19" s="43"/>
       <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
+      <c r="P19" s="44"/>
       <c r="Q19" s="43"/>
       <c r="R19" s="43"/>
       <c r="S19" s="43"/>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="N20" s="34"/>
       <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
+      <c r="P20" s="35"/>
       <c r="Q20" s="34"/>
       <c r="R20" s="34"/>
       <c r="S20" s="34"/>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="N21" s="43"/>
       <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
+      <c r="P21" s="44"/>
       <c r="Q21" s="43"/>
       <c r="R21" s="43"/>
       <c r="S21" s="43"/>
@@ -2256,7 +2256,7 @@
       <c r="O22" s="35">
         <v>30.0</v>
       </c>
-      <c r="P22" s="34"/>
+      <c r="P22" s="35"/>
       <c r="Q22" s="34"/>
       <c r="R22" s="34"/>
       <c r="S22" s="34"/>
@@ -2307,7 +2307,7 @@
       <c r="O23" s="44">
         <v>34.0</v>
       </c>
-      <c r="P23" s="43"/>
+      <c r="P23" s="44"/>
       <c r="Q23" s="43"/>
       <c r="R23" s="43"/>
       <c r="S23" s="43"/>
@@ -4353,7 +4353,9 @@
       <c r="L5" s="90">
         <v>38.0</v>
       </c>
-      <c r="M5" s="87"/>
+      <c r="M5" s="89">
+        <v>38.0</v>
+      </c>
       <c r="N5" s="87"/>
       <c r="O5" s="87"/>
       <c r="P5" s="87"/>
@@ -4368,7 +4370,7 @@
       <c r="Y5" s="87"/>
       <c r="Z5" s="91">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>316</v>
+        <v>354</v>
       </c>
       <c r="AA5" s="39"/>
     </row>
@@ -4403,7 +4405,9 @@
       <c r="L6" s="89">
         <v>35.0</v>
       </c>
-      <c r="M6" s="87"/>
+      <c r="M6" s="89">
+        <v>32.0</v>
+      </c>
       <c r="N6" s="87"/>
       <c r="O6" s="87"/>
       <c r="P6" s="87"/>
@@ -4418,7 +4422,7 @@
       <c r="Y6" s="87"/>
       <c r="Z6" s="91">
         <f t="shared" si="1"/>
-        <v>275</v>
+        <v>307</v>
       </c>
       <c r="AA6" s="39"/>
     </row>
@@ -4457,7 +4461,9 @@
       <c r="L7" s="89">
         <v>27.0</v>
       </c>
-      <c r="M7" s="87"/>
+      <c r="M7" s="90">
+        <v>38.0</v>
+      </c>
       <c r="N7" s="87"/>
       <c r="O7" s="87"/>
       <c r="P7" s="87"/>
@@ -4472,7 +4478,7 @@
       <c r="Y7" s="87"/>
       <c r="Z7" s="91">
         <f t="shared" si="1"/>
-        <v>299</v>
+        <v>337</v>
       </c>
       <c r="AA7" s="39"/>
     </row>
@@ -4511,7 +4517,9 @@
       <c r="L8" s="89">
         <v>32.0</v>
       </c>
-      <c r="M8" s="87"/>
+      <c r="M8" s="89">
+        <v>33.0</v>
+      </c>
       <c r="N8" s="87"/>
       <c r="O8" s="87"/>
       <c r="P8" s="87"/>
@@ -4526,7 +4534,7 @@
       <c r="Y8" s="87"/>
       <c r="Z8" s="91">
         <f t="shared" si="1"/>
-        <v>336</v>
+        <v>369</v>
       </c>
       <c r="AA8" s="39"/>
     </row>
@@ -4565,7 +4573,9 @@
       <c r="L9" s="89">
         <v>26.0</v>
       </c>
-      <c r="M9" s="87"/>
+      <c r="M9" s="89">
+        <v>24.0</v>
+      </c>
       <c r="N9" s="87"/>
       <c r="O9" s="87"/>
       <c r="P9" s="87"/>
@@ -4580,7 +4590,7 @@
       <c r="Y9" s="87"/>
       <c r="Z9" s="91">
         <f t="shared" si="1"/>
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="AA9" s="39"/>
     </row>
@@ -4615,7 +4625,9 @@
       <c r="L10" s="89">
         <v>24.0</v>
       </c>
-      <c r="M10" s="87"/>
+      <c r="M10" s="89">
+        <v>28.0</v>
+      </c>
       <c r="N10" s="87"/>
       <c r="O10" s="87"/>
       <c r="P10" s="87"/>
@@ -4630,7 +4642,7 @@
       <c r="Y10" s="87"/>
       <c r="Z10" s="91">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>236</v>
       </c>
       <c r="AA10" s="39"/>
     </row>
@@ -4759,7 +4771,9 @@
       <c r="L13" s="89">
         <v>34.0</v>
       </c>
-      <c r="M13" s="87"/>
+      <c r="M13" s="89">
+        <v>31.0</v>
+      </c>
       <c r="N13" s="87"/>
       <c r="O13" s="87"/>
       <c r="P13" s="87"/>
@@ -4774,7 +4788,7 @@
       <c r="Y13" s="87"/>
       <c r="Z13" s="91">
         <f t="shared" si="1"/>
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="AA13" s="39"/>
     </row>
@@ -4853,7 +4867,9 @@
       <c r="L15" s="89">
         <v>37.0</v>
       </c>
-      <c r="M15" s="87"/>
+      <c r="M15" s="89">
+        <v>32.0</v>
+      </c>
       <c r="N15" s="87"/>
       <c r="O15" s="87"/>
       <c r="P15" s="87"/>
@@ -4868,7 +4884,7 @@
       <c r="Y15" s="87"/>
       <c r="Z15" s="91">
         <f t="shared" si="1"/>
-        <v>261</v>
+        <v>293</v>
       </c>
       <c r="AA15" s="39"/>
     </row>

</xml_diff>

<commit_message>
023 Week 13/14 update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -1736,7 +1736,9 @@
         <v>31.0</v>
       </c>
       <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
+      <c r="Q12" s="35">
+        <v>32.0</v>
+      </c>
       <c r="R12" s="34"/>
       <c r="S12" s="34"/>
       <c r="T12" s="34"/>
@@ -1749,11 +1751,11 @@
       <c r="AA12" s="36"/>
       <c r="AB12" s="37">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="AC12" s="38">
         <f>SUM(AB12:AB13)</f>
-        <v>453</v>
+        <v>517</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="39"/>
@@ -1789,7 +1791,9 @@
         <v>36.0</v>
       </c>
       <c r="P13" s="43"/>
-      <c r="Q13" s="43"/>
+      <c r="Q13" s="44">
+        <v>32.0</v>
+      </c>
       <c r="R13" s="43"/>
       <c r="S13" s="43"/>
       <c r="T13" s="43"/>
@@ -1802,7 +1806,7 @@
       <c r="AA13" s="45"/>
       <c r="AB13" s="37">
         <f t="shared" si="1"/>
-        <v>203</v>
+        <v>235</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -1946,7 +1950,9 @@
         <v>23.0</v>
       </c>
       <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
+      <c r="Q16" s="35">
+        <v>25.0</v>
+      </c>
       <c r="R16" s="34"/>
       <c r="S16" s="34"/>
       <c r="T16" s="34"/>
@@ -1959,11 +1965,11 @@
       <c r="AA16" s="36"/>
       <c r="AB16" s="37">
         <f t="shared" si="1"/>
-        <v>261</v>
+        <v>286</v>
       </c>
       <c r="AC16" s="38">
         <f>SUM(AB16:AB17)</f>
-        <v>507</v>
+        <v>532</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="39"/>
@@ -2053,7 +2059,9 @@
         <v>38.0</v>
       </c>
       <c r="P18" s="35"/>
-      <c r="Q18" s="34"/>
+      <c r="Q18" s="35">
+        <v>28.0</v>
+      </c>
       <c r="R18" s="34"/>
       <c r="S18" s="34"/>
       <c r="T18" s="34"/>
@@ -2066,11 +2074,11 @@
       <c r="AA18" s="36"/>
       <c r="AB18" s="37">
         <f t="shared" si="1"/>
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="AC18" s="38">
         <f>SUM(AB18:AB19)</f>
-        <v>260</v>
+        <v>288</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="39"/>
@@ -2150,7 +2158,9 @@
       <c r="N20" s="34"/>
       <c r="O20" s="34"/>
       <c r="P20" s="35"/>
-      <c r="Q20" s="34"/>
+      <c r="Q20" s="35">
+        <v>28.0</v>
+      </c>
       <c r="R20" s="34"/>
       <c r="S20" s="34"/>
       <c r="T20" s="34"/>
@@ -2163,11 +2173,11 @@
       <c r="AA20" s="36"/>
       <c r="AB20" s="37">
         <f t="shared" si="1"/>
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="AC20" s="38">
         <f>SUM(AB20:AB21)</f>
-        <v>522</v>
+        <v>578</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="39"/>
@@ -2207,7 +2217,9 @@
       <c r="N21" s="43"/>
       <c r="O21" s="43"/>
       <c r="P21" s="44"/>
-      <c r="Q21" s="43"/>
+      <c r="Q21" s="44">
+        <v>28.0</v>
+      </c>
       <c r="R21" s="43"/>
       <c r="S21" s="43"/>
       <c r="T21" s="43"/>
@@ -2220,7 +2232,7 @@
       <c r="AA21" s="45"/>
       <c r="AB21" s="37">
         <f t="shared" si="1"/>
-        <v>273</v>
+        <v>301</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
@@ -2257,7 +2269,9 @@
         <v>30.0</v>
       </c>
       <c r="P22" s="35"/>
-      <c r="Q22" s="34"/>
+      <c r="Q22" s="35">
+        <v>26.0</v>
+      </c>
       <c r="R22" s="34"/>
       <c r="S22" s="34"/>
       <c r="T22" s="34"/>
@@ -2270,11 +2284,11 @@
       <c r="AA22" s="36"/>
       <c r="AB22" s="37">
         <f t="shared" si="1"/>
-        <v>187</v>
+        <v>213</v>
       </c>
       <c r="AC22" s="38">
         <f>SUM(AB22:AB23)</f>
-        <v>331</v>
+        <v>357</v>
       </c>
       <c r="AD22" s="5"/>
       <c r="AE22" s="39"/>
@@ -2352,7 +2366,9 @@
       </c>
       <c r="O24" s="34"/>
       <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
+      <c r="Q24" s="55">
+        <v>38.0</v>
+      </c>
       <c r="R24" s="34"/>
       <c r="S24" s="34"/>
       <c r="T24" s="34"/>
@@ -2365,11 +2381,11 @@
       <c r="AA24" s="36"/>
       <c r="AB24" s="37">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="AC24" s="38">
         <f>SUM(AB24:AB25)</f>
-        <v>378</v>
+        <v>416</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="39"/>
@@ -2467,7 +2483,9 @@
         <v>33.0</v>
       </c>
       <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
+      <c r="Q26" s="35">
+        <v>34.0</v>
+      </c>
       <c r="R26" s="34"/>
       <c r="S26" s="34"/>
       <c r="T26" s="34"/>
@@ -2480,11 +2498,11 @@
       <c r="AA26" s="36"/>
       <c r="AB26" s="37">
         <f t="shared" si="1"/>
-        <v>294</v>
+        <v>328</v>
       </c>
       <c r="AC26" s="38">
         <f>SUM(AB26:AB27)</f>
-        <v>575</v>
+        <v>638</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="39"/>
@@ -2526,7 +2544,9 @@
         <v>32.0</v>
       </c>
       <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
+      <c r="Q27" s="44">
+        <v>29.0</v>
+      </c>
       <c r="R27" s="43"/>
       <c r="S27" s="43"/>
       <c r="T27" s="43"/>
@@ -2539,7 +2559,7 @@
       <c r="AA27" s="45"/>
       <c r="AB27" s="37">
         <f t="shared" si="1"/>
-        <v>281</v>
+        <v>310</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
@@ -2601,7 +2621,7 @@
       </c>
       <c r="AC28" s="38">
         <f>SUM(AB28:AB29)</f>
-        <v>653</v>
+        <v>687</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="39"/>
@@ -2645,7 +2665,9 @@
         <v>33.0</v>
       </c>
       <c r="P29" s="43"/>
-      <c r="Q29" s="43"/>
+      <c r="Q29" s="44">
+        <v>34.0</v>
+      </c>
       <c r="R29" s="43"/>
       <c r="S29" s="43"/>
       <c r="T29" s="43"/>
@@ -2658,7 +2680,7 @@
       <c r="AA29" s="45"/>
       <c r="AB29" s="37">
         <f t="shared" si="1"/>
-        <v>338</v>
+        <v>372</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -2708,7 +2730,7 @@
       </c>
       <c r="AC30" s="38">
         <f>SUM(AB30:AB31)</f>
-        <v>409</v>
+        <v>437</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="39"/>
@@ -2750,7 +2772,9 @@
         <v>29.0</v>
       </c>
       <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
+      <c r="Q31" s="44">
+        <v>28.0</v>
+      </c>
       <c r="R31" s="43"/>
       <c r="S31" s="43"/>
       <c r="T31" s="43"/>
@@ -2763,7 +2787,7 @@
       <c r="AA31" s="57"/>
       <c r="AB31" s="58">
         <f t="shared" si="1"/>
-        <v>287</v>
+        <v>315</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
@@ -4408,7 +4432,9 @@
       <c r="M6" s="89">
         <v>32.0</v>
       </c>
-      <c r="N6" s="87"/>
+      <c r="N6" s="90">
+        <v>33.0</v>
+      </c>
       <c r="O6" s="87"/>
       <c r="P6" s="87"/>
       <c r="Q6" s="87"/>
@@ -4422,7 +4448,7 @@
       <c r="Y6" s="87"/>
       <c r="Z6" s="91">
         <f t="shared" si="1"/>
-        <v>307</v>
+        <v>340</v>
       </c>
       <c r="AA6" s="39"/>
     </row>
@@ -4576,7 +4602,9 @@
       <c r="M9" s="89">
         <v>24.0</v>
       </c>
-      <c r="N9" s="87"/>
+      <c r="N9" s="89">
+        <v>28.0</v>
+      </c>
       <c r="O9" s="87"/>
       <c r="P9" s="87"/>
       <c r="Q9" s="87"/>
@@ -4590,7 +4618,7 @@
       <c r="Y9" s="87"/>
       <c r="Z9" s="91">
         <f t="shared" si="1"/>
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="AA9" s="39"/>
     </row>
@@ -4774,7 +4802,9 @@
       <c r="M13" s="89">
         <v>31.0</v>
       </c>
-      <c r="N13" s="87"/>
+      <c r="N13" s="89">
+        <v>29.0</v>
+      </c>
       <c r="O13" s="87"/>
       <c r="P13" s="87"/>
       <c r="Q13" s="87"/>
@@ -4788,7 +4818,7 @@
       <c r="Y13" s="87"/>
       <c r="Z13" s="91">
         <f t="shared" si="1"/>
-        <v>303</v>
+        <v>332</v>
       </c>
       <c r="AA13" s="39"/>
     </row>
@@ -4870,7 +4900,9 @@
       <c r="M15" s="89">
         <v>32.0</v>
       </c>
-      <c r="N15" s="87"/>
+      <c r="N15" s="89">
+        <v>27.0</v>
+      </c>
       <c r="O15" s="87"/>
       <c r="P15" s="87"/>
       <c r="Q15" s="87"/>
@@ -4884,7 +4916,7 @@
       <c r="Y15" s="87"/>
       <c r="Z15" s="91">
         <f t="shared" si="1"/>
-        <v>293</v>
+        <v>320</v>
       </c>
       <c r="AA15" s="39"/>
     </row>
@@ -5385,7 +5417,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="106">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C3" s="108"/>
     </row>
@@ -5657,7 +5689,7 @@
       </c>
       <c r="B2" s="111">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -5675,7 +5707,7 @@
       </c>
       <c r="B4" s="105">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -5684,7 +5716,7 @@
       </c>
       <c r="B5" s="105">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -5693,7 +5725,7 @@
       </c>
       <c r="B6" s="105">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -5702,7 +5734,7 @@
       </c>
       <c r="B7" s="105">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -5720,7 +5752,7 @@
       </c>
       <c r="B9" s="105">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -5729,7 +5761,7 @@
       </c>
       <c r="B10" s="105">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -5738,7 +5770,7 @@
       </c>
       <c r="B11" s="105">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
025 Week 14/15 update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -1739,7 +1739,9 @@
       <c r="Q12" s="35">
         <v>32.0</v>
       </c>
-      <c r="R12" s="34"/>
+      <c r="R12" s="35">
+        <v>32.0</v>
+      </c>
       <c r="S12" s="34"/>
       <c r="T12" s="34"/>
       <c r="U12" s="34"/>
@@ -1751,11 +1753,11 @@
       <c r="AA12" s="36"/>
       <c r="AB12" s="37">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>282</v>
+        <v>314</v>
       </c>
       <c r="AC12" s="38">
         <f>SUM(AB12:AB13)</f>
-        <v>517</v>
+        <v>585</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="39"/>
@@ -1794,7 +1796,9 @@
       <c r="Q13" s="44">
         <v>32.0</v>
       </c>
-      <c r="R13" s="43"/>
+      <c r="R13" s="44">
+        <v>36.0</v>
+      </c>
       <c r="S13" s="43"/>
       <c r="T13" s="43"/>
       <c r="U13" s="43"/>
@@ -1806,7 +1810,7 @@
       <c r="AA13" s="45"/>
       <c r="AB13" s="37">
         <f t="shared" si="1"/>
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -1856,7 +1860,7 @@
       </c>
       <c r="AC14" s="38">
         <f>SUM(AB14:AB15)</f>
-        <v>371</v>
+        <v>399</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="39"/>
@@ -1895,7 +1899,9 @@
       </c>
       <c r="P15" s="43"/>
       <c r="Q15" s="43"/>
-      <c r="R15" s="43"/>
+      <c r="R15" s="44">
+        <v>28.0</v>
+      </c>
       <c r="S15" s="43"/>
       <c r="T15" s="43"/>
       <c r="U15" s="43"/>
@@ -1907,7 +1913,7 @@
       <c r="AA15" s="45"/>
       <c r="AB15" s="37">
         <f t="shared" si="1"/>
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
@@ -1953,7 +1959,9 @@
       <c r="Q16" s="35">
         <v>25.0</v>
       </c>
-      <c r="R16" s="34"/>
+      <c r="R16" s="35">
+        <v>30.0</v>
+      </c>
       <c r="S16" s="34"/>
       <c r="T16" s="34"/>
       <c r="U16" s="34"/>
@@ -1965,11 +1973,11 @@
       <c r="AA16" s="36"/>
       <c r="AB16" s="37">
         <f t="shared" si="1"/>
-        <v>286</v>
+        <v>316</v>
       </c>
       <c r="AC16" s="38">
         <f>SUM(AB16:AB17)</f>
-        <v>532</v>
+        <v>562</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="39"/>
@@ -2062,7 +2070,9 @@
       <c r="Q18" s="35">
         <v>28.0</v>
       </c>
-      <c r="R18" s="34"/>
+      <c r="R18" s="35">
+        <v>31.0</v>
+      </c>
       <c r="S18" s="34"/>
       <c r="T18" s="34"/>
       <c r="U18" s="34"/>
@@ -2074,11 +2084,11 @@
       <c r="AA18" s="36"/>
       <c r="AB18" s="37">
         <f t="shared" si="1"/>
-        <v>227</v>
+        <v>258</v>
       </c>
       <c r="AC18" s="38">
         <f>SUM(AB18:AB19)</f>
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="39"/>
@@ -2161,7 +2171,9 @@
       <c r="Q20" s="35">
         <v>28.0</v>
       </c>
-      <c r="R20" s="34"/>
+      <c r="R20" s="35">
+        <v>35.0</v>
+      </c>
       <c r="S20" s="34"/>
       <c r="T20" s="34"/>
       <c r="U20" s="34"/>
@@ -2173,11 +2185,11 @@
       <c r="AA20" s="36"/>
       <c r="AB20" s="37">
         <f t="shared" si="1"/>
-        <v>277</v>
+        <v>312</v>
       </c>
       <c r="AC20" s="38">
         <f>SUM(AB20:AB21)</f>
-        <v>578</v>
+        <v>639</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="39"/>
@@ -2220,7 +2232,9 @@
       <c r="Q21" s="44">
         <v>28.0</v>
       </c>
-      <c r="R21" s="43"/>
+      <c r="R21" s="44">
+        <v>26.0</v>
+      </c>
       <c r="S21" s="43"/>
       <c r="T21" s="43"/>
       <c r="U21" s="43"/>
@@ -2232,7 +2246,7 @@
       <c r="AA21" s="45"/>
       <c r="AB21" s="37">
         <f t="shared" si="1"/>
-        <v>301</v>
+        <v>327</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
@@ -2486,7 +2500,9 @@
       <c r="Q26" s="35">
         <v>34.0</v>
       </c>
-      <c r="R26" s="34"/>
+      <c r="R26" s="55">
+        <v>37.0</v>
+      </c>
       <c r="S26" s="34"/>
       <c r="T26" s="34"/>
       <c r="U26" s="34"/>
@@ -2498,11 +2514,11 @@
       <c r="AA26" s="36"/>
       <c r="AB26" s="37">
         <f t="shared" si="1"/>
-        <v>328</v>
+        <v>365</v>
       </c>
       <c r="AC26" s="38">
         <f>SUM(AB26:AB27)</f>
-        <v>638</v>
+        <v>675</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="39"/>
@@ -2605,7 +2621,9 @@
       </c>
       <c r="P28" s="34"/>
       <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
+      <c r="R28" s="35">
+        <v>35.0</v>
+      </c>
       <c r="S28" s="34"/>
       <c r="T28" s="34"/>
       <c r="U28" s="34"/>
@@ -2617,11 +2635,11 @@
       <c r="AA28" s="36"/>
       <c r="AB28" s="37">
         <f t="shared" si="1"/>
-        <v>315</v>
+        <v>350</v>
       </c>
       <c r="AC28" s="38">
         <f>SUM(AB28:AB29)</f>
-        <v>687</v>
+        <v>754</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="39"/>
@@ -2668,7 +2686,9 @@
       <c r="Q29" s="44">
         <v>34.0</v>
       </c>
-      <c r="R29" s="43"/>
+      <c r="R29" s="44">
+        <v>32.0</v>
+      </c>
       <c r="S29" s="43"/>
       <c r="T29" s="43"/>
       <c r="U29" s="43"/>
@@ -2680,7 +2700,7 @@
       <c r="AA29" s="45"/>
       <c r="AB29" s="37">
         <f t="shared" si="1"/>
-        <v>372</v>
+        <v>404</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -4381,7 +4401,9 @@
         <v>38.0</v>
       </c>
       <c r="N5" s="87"/>
-      <c r="O5" s="87"/>
+      <c r="O5" s="90">
+        <v>36.0</v>
+      </c>
       <c r="P5" s="87"/>
       <c r="Q5" s="87"/>
       <c r="R5" s="87"/>
@@ -4394,7 +4416,7 @@
       <c r="Y5" s="87"/>
       <c r="Z5" s="91">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>354</v>
+        <v>390</v>
       </c>
       <c r="AA5" s="39"/>
     </row>
@@ -4435,7 +4457,9 @@
       <c r="N6" s="90">
         <v>33.0</v>
       </c>
-      <c r="O6" s="87"/>
+      <c r="O6" s="89">
+        <v>34.0</v>
+      </c>
       <c r="P6" s="87"/>
       <c r="Q6" s="87"/>
       <c r="R6" s="87"/>
@@ -4448,7 +4472,7 @@
       <c r="Y6" s="87"/>
       <c r="Z6" s="91">
         <f t="shared" si="1"/>
-        <v>340</v>
+        <v>374</v>
       </c>
       <c r="AA6" s="39"/>
     </row>
@@ -4491,7 +4515,9 @@
         <v>38.0</v>
       </c>
       <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
+      <c r="O7" s="89">
+        <v>32.0</v>
+      </c>
       <c r="P7" s="87"/>
       <c r="Q7" s="87"/>
       <c r="R7" s="87"/>
@@ -4504,7 +4530,7 @@
       <c r="Y7" s="87"/>
       <c r="Z7" s="91">
         <f t="shared" si="1"/>
-        <v>337</v>
+        <v>369</v>
       </c>
       <c r="AA7" s="39"/>
     </row>
@@ -4605,7 +4631,9 @@
       <c r="N9" s="89">
         <v>28.0</v>
       </c>
-      <c r="O9" s="87"/>
+      <c r="O9" s="89">
+        <v>28.0</v>
+      </c>
       <c r="P9" s="87"/>
       <c r="Q9" s="87"/>
       <c r="R9" s="87"/>
@@ -4618,7 +4646,7 @@
       <c r="Y9" s="87"/>
       <c r="Z9" s="91">
         <f t="shared" si="1"/>
-        <v>331</v>
+        <v>359</v>
       </c>
       <c r="AA9" s="39"/>
     </row>
@@ -4657,7 +4685,9 @@
         <v>28.0</v>
       </c>
       <c r="N10" s="87"/>
-      <c r="O10" s="87"/>
+      <c r="O10" s="89">
+        <v>14.0</v>
+      </c>
       <c r="P10" s="87"/>
       <c r="Q10" s="87"/>
       <c r="R10" s="87"/>
@@ -4670,7 +4700,7 @@
       <c r="Y10" s="87"/>
       <c r="Z10" s="91">
         <f t="shared" si="1"/>
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="AA10" s="39"/>
     </row>
@@ -4751,7 +4781,9 @@
       <c r="L12" s="87"/>
       <c r="M12" s="87"/>
       <c r="N12" s="87"/>
-      <c r="O12" s="87"/>
+      <c r="O12" s="89">
+        <v>30.0</v>
+      </c>
       <c r="P12" s="87"/>
       <c r="Q12" s="87"/>
       <c r="R12" s="87"/>
@@ -4764,7 +4796,7 @@
       <c r="Y12" s="87"/>
       <c r="Z12" s="91">
         <f t="shared" si="1"/>
-        <v>266</v>
+        <v>296</v>
       </c>
       <c r="AA12" s="39"/>
     </row>
@@ -4849,7 +4881,9 @@
       </c>
       <c r="M14" s="87"/>
       <c r="N14" s="87"/>
-      <c r="O14" s="87"/>
+      <c r="O14" s="89">
+        <v>32.0</v>
+      </c>
       <c r="P14" s="87"/>
       <c r="Q14" s="87"/>
       <c r="R14" s="87"/>
@@ -4862,7 +4896,7 @@
       <c r="Y14" s="87"/>
       <c r="Z14" s="91">
         <f t="shared" si="1"/>
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="AA14" s="39"/>
     </row>
@@ -4949,7 +4983,9 @@
       <c r="L16" s="87"/>
       <c r="M16" s="87"/>
       <c r="N16" s="87"/>
-      <c r="O16" s="87"/>
+      <c r="O16" s="89">
+        <v>35.0</v>
+      </c>
       <c r="P16" s="87"/>
       <c r="Q16" s="87"/>
       <c r="R16" s="87"/>
@@ -4962,7 +4998,7 @@
       <c r="Y16" s="87"/>
       <c r="Z16" s="91">
         <f t="shared" si="1"/>
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="AA16" s="39"/>
     </row>
@@ -5417,7 +5453,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="106">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C3" s="108"/>
     </row>
@@ -5435,7 +5471,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="106">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C5" s="108"/>
     </row>
@@ -5444,10 +5480,10 @@
         <v>33</v>
       </c>
       <c r="B6" s="106">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="C6" s="107">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="7">
@@ -5466,7 +5502,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="106">
-        <v>-2.0</v>
+        <v>-1.0</v>
       </c>
       <c r="C8" s="108"/>
     </row>
@@ -5689,7 +5725,7 @@
       </c>
       <c r="B2" s="111">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -5698,7 +5734,7 @@
       </c>
       <c r="B3" s="105">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -5707,7 +5743,7 @@
       </c>
       <c r="B4" s="105">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -5716,7 +5752,7 @@
       </c>
       <c r="B5" s="105">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -5725,7 +5761,7 @@
       </c>
       <c r="B6" s="105">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
@@ -5752,7 +5788,7 @@
       </c>
       <c r="B9" s="105">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
@@ -5761,7 +5797,7 @@
       </c>
       <c r="B10" s="105">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
027 Week 15/16 update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -1742,7 +1742,9 @@
       <c r="R12" s="35">
         <v>32.0</v>
       </c>
-      <c r="S12" s="34"/>
+      <c r="S12" s="35">
+        <v>31.0</v>
+      </c>
       <c r="T12" s="34"/>
       <c r="U12" s="34"/>
       <c r="V12" s="34"/>
@@ -1753,11 +1755,11 @@
       <c r="AA12" s="36"/>
       <c r="AB12" s="37">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>314</v>
+        <v>345</v>
       </c>
       <c r="AC12" s="38">
         <f>SUM(AB12:AB13)</f>
-        <v>585</v>
+        <v>651</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="39"/>
@@ -1799,7 +1801,9 @@
       <c r="R13" s="44">
         <v>36.0</v>
       </c>
-      <c r="S13" s="43"/>
+      <c r="S13" s="44">
+        <v>35.0</v>
+      </c>
       <c r="T13" s="43"/>
       <c r="U13" s="43"/>
       <c r="V13" s="43"/>
@@ -1810,7 +1814,7 @@
       <c r="AA13" s="45"/>
       <c r="AB13" s="37">
         <f t="shared" si="1"/>
-        <v>271</v>
+        <v>306</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -1962,7 +1966,9 @@
       <c r="R16" s="35">
         <v>30.0</v>
       </c>
-      <c r="S16" s="34"/>
+      <c r="S16" s="35">
+        <v>31.0</v>
+      </c>
       <c r="T16" s="34"/>
       <c r="U16" s="34"/>
       <c r="V16" s="34"/>
@@ -1973,11 +1979,11 @@
       <c r="AA16" s="36"/>
       <c r="AB16" s="37">
         <f t="shared" si="1"/>
-        <v>316</v>
+        <v>347</v>
       </c>
       <c r="AC16" s="38">
         <f>SUM(AB16:AB17)</f>
-        <v>562</v>
+        <v>616</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="39"/>
@@ -2019,7 +2025,9 @@
       <c r="P17" s="43"/>
       <c r="Q17" s="43"/>
       <c r="R17" s="43"/>
-      <c r="S17" s="43"/>
+      <c r="S17" s="44">
+        <v>23.0</v>
+      </c>
       <c r="T17" s="43"/>
       <c r="U17" s="43"/>
       <c r="V17" s="43"/>
@@ -2030,7 +2038,7 @@
       <c r="AA17" s="45"/>
       <c r="AB17" s="37">
         <f t="shared" si="1"/>
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
@@ -2073,7 +2081,9 @@
       <c r="R18" s="35">
         <v>31.0</v>
       </c>
-      <c r="S18" s="34"/>
+      <c r="S18" s="35">
+        <v>28.0</v>
+      </c>
       <c r="T18" s="34"/>
       <c r="U18" s="34"/>
       <c r="V18" s="34"/>
@@ -2084,11 +2094,11 @@
       <c r="AA18" s="36"/>
       <c r="AB18" s="37">
         <f t="shared" si="1"/>
-        <v>258</v>
+        <v>286</v>
       </c>
       <c r="AC18" s="38">
         <f>SUM(AB18:AB19)</f>
-        <v>319</v>
+        <v>347</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="39"/>
@@ -2174,7 +2184,9 @@
       <c r="R20" s="35">
         <v>35.0</v>
       </c>
-      <c r="S20" s="34"/>
+      <c r="S20" s="35">
+        <v>28.0</v>
+      </c>
       <c r="T20" s="34"/>
       <c r="U20" s="34"/>
       <c r="V20" s="34"/>
@@ -2185,11 +2197,11 @@
       <c r="AA20" s="36"/>
       <c r="AB20" s="37">
         <f t="shared" si="1"/>
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="AC20" s="38">
         <f>SUM(AB20:AB21)</f>
-        <v>639</v>
+        <v>667</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="39"/>
@@ -2503,7 +2515,9 @@
       <c r="R26" s="55">
         <v>37.0</v>
       </c>
-      <c r="S26" s="34"/>
+      <c r="S26" s="35">
+        <v>30.0</v>
+      </c>
       <c r="T26" s="34"/>
       <c r="U26" s="34"/>
       <c r="V26" s="34"/>
@@ -2514,11 +2528,11 @@
       <c r="AA26" s="36"/>
       <c r="AB26" s="37">
         <f t="shared" si="1"/>
-        <v>365</v>
+        <v>395</v>
       </c>
       <c r="AC26" s="38">
         <f>SUM(AB26:AB27)</f>
-        <v>675</v>
+        <v>705</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="39"/>
@@ -2624,7 +2638,9 @@
       <c r="R28" s="35">
         <v>35.0</v>
       </c>
-      <c r="S28" s="34"/>
+      <c r="S28" s="35">
+        <v>31.0</v>
+      </c>
       <c r="T28" s="34"/>
       <c r="U28" s="34"/>
       <c r="V28" s="34"/>
@@ -2635,11 +2651,11 @@
       <c r="AA28" s="36"/>
       <c r="AB28" s="37">
         <f t="shared" si="1"/>
-        <v>350</v>
+        <v>381</v>
       </c>
       <c r="AC28" s="38">
         <f>SUM(AB28:AB29)</f>
-        <v>754</v>
+        <v>823</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="39"/>
@@ -2689,7 +2705,9 @@
       <c r="R29" s="44">
         <v>32.0</v>
       </c>
-      <c r="S29" s="43"/>
+      <c r="S29" s="56">
+        <v>38.0</v>
+      </c>
       <c r="T29" s="43"/>
       <c r="U29" s="43"/>
       <c r="V29" s="43"/>
@@ -2700,7 +2718,7 @@
       <c r="AA29" s="45"/>
       <c r="AB29" s="37">
         <f t="shared" si="1"/>
-        <v>404</v>
+        <v>442</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -2750,7 +2768,7 @@
       </c>
       <c r="AC30" s="38">
         <f>SUM(AB30:AB31)</f>
-        <v>437</v>
+        <v>467</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="39"/>
@@ -2796,7 +2814,9 @@
         <v>28.0</v>
       </c>
       <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
+      <c r="S31" s="44">
+        <v>30.0</v>
+      </c>
       <c r="T31" s="43"/>
       <c r="U31" s="43"/>
       <c r="V31" s="43"/>
@@ -2807,7 +2827,7 @@
       <c r="AA31" s="57"/>
       <c r="AB31" s="58">
         <f t="shared" si="1"/>
-        <v>315</v>
+        <v>345</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
@@ -5727,7 +5747,7 @@
       </c>
       <c r="B2" s="111">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -5745,7 +5765,7 @@
       </c>
       <c r="B4" s="105">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -5754,7 +5774,7 @@
       </c>
       <c r="B5" s="105">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -5763,7 +5783,7 @@
       </c>
       <c r="B6" s="105">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -5790,7 +5810,7 @@
       </c>
       <c r="B9" s="105">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
@@ -5799,7 +5819,7 @@
       </c>
       <c r="B10" s="105">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -5808,7 +5828,7 @@
       </c>
       <c r="B11" s="105">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 17/18 data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -781,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -878,6 +878,9 @@
     <xf borderId="20" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="20" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="26" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -988,6 +991,9 @@
     <xf borderId="42" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="42" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="42" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -999,9 +1005,6 @@
     </xf>
     <xf borderId="0" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="42" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="33" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -1028,6 +1031,9 @@
     <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1728,7 +1734,9 @@
       <c r="T12" s="32">
         <v>30.0</v>
       </c>
-      <c r="U12" s="31"/>
+      <c r="U12" s="32">
+        <v>29.0</v>
+      </c>
       <c r="V12" s="31"/>
       <c r="W12" s="31"/>
       <c r="X12" s="31"/>
@@ -1737,11 +1745,11 @@
       <c r="AA12" s="33"/>
       <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>375</v>
+        <v>404</v>
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>715</v>
+        <v>778</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36"/>
@@ -1789,7 +1797,9 @@
       <c r="T13" s="41">
         <v>34.0</v>
       </c>
-      <c r="U13" s="40"/>
+      <c r="U13" s="41">
+        <v>34.0</v>
+      </c>
       <c r="V13" s="40"/>
       <c r="W13" s="40"/>
       <c r="X13" s="40"/>
@@ -1798,7 +1808,7 @@
       <c r="AA13" s="42"/>
       <c r="AB13" s="34">
         <f t="shared" si="1"/>
-        <v>340</v>
+        <v>374</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -1835,7 +1845,9 @@
       <c r="R14" s="31"/>
       <c r="S14" s="31"/>
       <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
+      <c r="U14" s="44">
+        <v>38.0</v>
+      </c>
       <c r="V14" s="31"/>
       <c r="W14" s="31"/>
       <c r="X14" s="31"/>
@@ -1844,11 +1856,11 @@
       <c r="AA14" s="33"/>
       <c r="AB14" s="34">
         <f t="shared" si="1"/>
-        <v>134</v>
+        <v>172</v>
       </c>
       <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
-        <v>399</v>
+        <v>469</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="36"/>
@@ -1892,7 +1904,9 @@
       </c>
       <c r="S15" s="40"/>
       <c r="T15" s="40"/>
-      <c r="U15" s="40"/>
+      <c r="U15" s="41">
+        <v>32.0</v>
+      </c>
       <c r="V15" s="40"/>
       <c r="W15" s="40"/>
       <c r="X15" s="40"/>
@@ -1901,7 +1915,7 @@
       <c r="AA15" s="42"/>
       <c r="AB15" s="34">
         <f t="shared" si="1"/>
-        <v>265</v>
+        <v>297</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
@@ -1956,7 +1970,9 @@
       <c r="T16" s="32">
         <v>34.0</v>
       </c>
-      <c r="U16" s="31"/>
+      <c r="U16" s="32">
+        <v>25.0</v>
+      </c>
       <c r="V16" s="31"/>
       <c r="W16" s="31"/>
       <c r="X16" s="31"/>
@@ -1965,11 +1981,11 @@
       <c r="AA16" s="33"/>
       <c r="AB16" s="34">
         <f t="shared" si="1"/>
-        <v>381</v>
+        <v>406</v>
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>689</v>
+        <v>714</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36"/>
@@ -2014,7 +2030,7 @@
       <c r="S17" s="40">
         <v>23.0</v>
       </c>
-      <c r="T17" s="44">
+      <c r="T17" s="45">
         <v>39.0</v>
       </c>
       <c r="U17" s="40"/>
@@ -2075,7 +2091,9 @@
       <c r="T18" s="32">
         <v>30.0</v>
       </c>
-      <c r="U18" s="31"/>
+      <c r="U18" s="32">
+        <v>30.0</v>
+      </c>
       <c r="V18" s="31"/>
       <c r="W18" s="31"/>
       <c r="X18" s="31"/>
@@ -2084,11 +2102,11 @@
       <c r="AA18" s="33"/>
       <c r="AB18" s="34">
         <f t="shared" si="1"/>
-        <v>316</v>
+        <v>346</v>
       </c>
       <c r="AC18" s="35">
         <f>SUM(AB18:AB19)</f>
-        <v>377</v>
+        <v>407</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="36"/>
@@ -2140,8 +2158,8 @@
         <v>37</v>
       </c>
       <c r="B20" s="29"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="31">
         <v>32.0</v>
       </c>
@@ -2180,7 +2198,9 @@
       <c r="T20" s="32">
         <v>31.0</v>
       </c>
-      <c r="U20" s="31"/>
+      <c r="U20" s="32">
+        <v>32.0</v>
+      </c>
       <c r="V20" s="31"/>
       <c r="W20" s="31"/>
       <c r="X20" s="31"/>
@@ -2189,11 +2209,11 @@
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>371</v>
+        <v>403</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>698</v>
+        <v>760</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36"/>
@@ -2203,8 +2223,8 @@
         <v>38</v>
       </c>
       <c r="B21" s="38"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="48">
+      <c r="C21" s="48"/>
+      <c r="D21" s="49">
         <v>36.0</v>
       </c>
       <c r="E21" s="40">
@@ -2241,7 +2261,9 @@
       </c>
       <c r="S21" s="40"/>
       <c r="T21" s="40"/>
-      <c r="U21" s="40"/>
+      <c r="U21" s="41">
+        <v>30.0</v>
+      </c>
       <c r="V21" s="40"/>
       <c r="W21" s="40"/>
       <c r="X21" s="40"/>
@@ -2250,17 +2272,17 @@
       <c r="AA21" s="42"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>327</v>
+        <v>357</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
       <c r="AE21" s="36"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="50"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="21"/>
       <c r="D22" s="31">
         <v>33.0</v>
@@ -2312,11 +2334,11 @@
       <c r="AE22" s="36"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="52" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="52"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="40">
         <v>25.0</v>
       </c>
@@ -2386,7 +2408,7 @@
       </c>
       <c r="O24" s="31"/>
       <c r="P24" s="31"/>
-      <c r="Q24" s="53">
+      <c r="Q24" s="54">
         <v>38.0</v>
       </c>
       <c r="R24" s="31"/>
@@ -2394,7 +2416,9 @@
       <c r="T24" s="32">
         <v>31.0</v>
       </c>
-      <c r="U24" s="31"/>
+      <c r="U24" s="32">
+        <v>33.0</v>
+      </c>
       <c r="V24" s="31"/>
       <c r="W24" s="31"/>
       <c r="X24" s="31"/>
@@ -2403,11 +2427,11 @@
       <c r="AA24" s="33"/>
       <c r="AB24" s="34">
         <f t="shared" si="1"/>
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
-        <v>473</v>
+        <v>541</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="36"/>
@@ -2455,7 +2479,9 @@
       <c r="T25" s="41">
         <v>26.0</v>
       </c>
-      <c r="U25" s="40"/>
+      <c r="U25" s="41">
+        <v>35.0</v>
+      </c>
       <c r="V25" s="40"/>
       <c r="W25" s="40"/>
       <c r="X25" s="40"/>
@@ -2464,7 +2490,7 @@
       <c r="AA25" s="42"/>
       <c r="AB25" s="34">
         <f t="shared" si="1"/>
-        <v>306</v>
+        <v>341</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
@@ -2510,7 +2536,7 @@
       <c r="Q26" s="31">
         <v>34.0</v>
       </c>
-      <c r="R26" s="53">
+      <c r="R26" s="54">
         <v>37.0</v>
       </c>
       <c r="S26" s="31">
@@ -2519,7 +2545,9 @@
       <c r="T26" s="32">
         <v>32.0</v>
       </c>
-      <c r="U26" s="31"/>
+      <c r="U26" s="32">
+        <v>22.0</v>
+      </c>
       <c r="V26" s="31"/>
       <c r="W26" s="31"/>
       <c r="X26" s="31"/>
@@ -2528,11 +2556,11 @@
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>427</v>
+        <v>449</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>757</v>
+        <v>779</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36"/>
@@ -2629,7 +2657,7 @@
       <c r="M28" s="31">
         <v>33.0</v>
       </c>
-      <c r="N28" s="53">
+      <c r="N28" s="54">
         <v>35.0</v>
       </c>
       <c r="O28" s="31">
@@ -2646,7 +2674,9 @@
       <c r="T28" s="32">
         <v>29.0</v>
       </c>
-      <c r="U28" s="31"/>
+      <c r="U28" s="32">
+        <v>33.0</v>
+      </c>
       <c r="V28" s="31"/>
       <c r="W28" s="31"/>
       <c r="X28" s="31"/>
@@ -2655,11 +2685,11 @@
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>410</v>
+        <v>443</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>886</v>
+        <v>955</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36"/>
@@ -2692,8 +2722,8 @@
       <c r="K29" s="40">
         <v>38.0</v>
       </c>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54">
+      <c r="L29" s="55"/>
+      <c r="M29" s="55">
         <v>39.0</v>
       </c>
       <c r="N29" s="40">
@@ -2709,13 +2739,15 @@
       <c r="R29" s="40">
         <v>32.0</v>
       </c>
-      <c r="S29" s="54">
+      <c r="S29" s="55">
         <v>38.0</v>
       </c>
       <c r="T29" s="41">
         <v>34.0</v>
       </c>
-      <c r="U29" s="40"/>
+      <c r="U29" s="41">
+        <v>36.0</v>
+      </c>
       <c r="V29" s="40"/>
       <c r="W29" s="40"/>
       <c r="X29" s="40"/>
@@ -2724,7 +2756,7 @@
       <c r="AA29" s="42"/>
       <c r="AB29" s="34">
         <f t="shared" si="1"/>
-        <v>476</v>
+        <v>512</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -2763,7 +2795,9 @@
       <c r="T30" s="32">
         <v>24.0</v>
       </c>
-      <c r="U30" s="31"/>
+      <c r="U30" s="32">
+        <v>35.0</v>
+      </c>
       <c r="V30" s="31"/>
       <c r="W30" s="31"/>
       <c r="X30" s="31"/>
@@ -2772,11 +2806,11 @@
       <c r="AA30" s="33"/>
       <c r="AB30" s="34">
         <f t="shared" si="1"/>
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>491</v>
+        <v>553</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36"/>
@@ -2826,23 +2860,25 @@
         <v>30.0</v>
       </c>
       <c r="T31" s="40"/>
-      <c r="U31" s="40"/>
+      <c r="U31" s="41">
+        <v>27.0</v>
+      </c>
       <c r="V31" s="40"/>
       <c r="W31" s="40"/>
       <c r="X31" s="40"/>
       <c r="Y31" s="40"/>
-      <c r="Z31" s="55"/>
-      <c r="AA31" s="55"/>
-      <c r="AB31" s="56">
+      <c r="Z31" s="56"/>
+      <c r="AA31" s="56"/>
+      <c r="AB31" s="57">
         <f t="shared" si="1"/>
-        <v>345</v>
+        <v>372</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
       <c r="AE31" s="36"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="57"/>
+      <c r="A32" s="58"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2873,27 +2909,27 @@
       <c r="AE32" s="1"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="58" t="s">
+      <c r="A33" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="59"/>
-      <c r="C33" s="60" t="s">
+      <c r="B33" s="60"/>
+      <c r="C33" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="61"/>
-      <c r="E33" s="59"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="60"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="62" t="s">
+      <c r="K33" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="L33" s="63"/>
-      <c r="M33" s="63"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="64"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="64"/>
+      <c r="N33" s="64"/>
+      <c r="O33" s="65"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -2912,9 +2948,9 @@
       <c r="AE33" s="1"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="57"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="58"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2945,16 +2981,16 @@
       <c r="AE34" s="1"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="57"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="58"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="65" t="s">
+      <c r="E35" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="66"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="67"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="68"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2962,86 +2998,86 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="65" t="s">
+      <c r="P35" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="Q35" s="66"/>
-      <c r="R35" s="66"/>
-      <c r="S35" s="67"/>
+      <c r="Q35" s="67"/>
+      <c r="R35" s="67"/>
+      <c r="S35" s="68"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="68"/>
+      <c r="X35" s="69"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="57"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="69" t="s">
+      <c r="A36" s="58"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="70" t="s">
         <v>54</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="70">
+      <c r="E36" s="71">
         <v>80.0</v>
       </c>
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="59"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="60"/>
       <c r="I36" s="36"/>
       <c r="J36" s="36"/>
       <c r="K36" s="36"/>
       <c r="L36" s="36"/>
-      <c r="M36" s="69" t="s">
+      <c r="M36" s="70" t="s">
         <v>54</v>
       </c>
       <c r="O36" s="36"/>
-      <c r="P36" s="70">
+      <c r="P36" s="71">
         <v>50.0</v>
       </c>
-      <c r="Q36" s="61"/>
-      <c r="R36" s="61"/>
-      <c r="S36" s="59"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="60"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="71"/>
+      <c r="X36" s="72"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="57"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="69" t="s">
+      <c r="A37" s="58"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="70" t="s">
         <v>55</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="70">
+      <c r="E37" s="71">
         <v>50.0</v>
       </c>
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="59"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="60"/>
       <c r="I37" s="36"/>
       <c r="J37" s="36"/>
       <c r="K37" s="36"/>
       <c r="L37" s="36"/>
-      <c r="M37" s="69" t="s">
+      <c r="M37" s="70" t="s">
         <v>55</v>
       </c>
       <c r="O37" s="36"/>
-      <c r="P37" s="70">
+      <c r="P37" s="71">
         <v>30.0</v>
       </c>
-      <c r="Q37" s="61"/>
-      <c r="R37" s="61"/>
-      <c r="S37" s="59"/>
+      <c r="Q37" s="62"/>
+      <c r="R37" s="62"/>
+      <c r="S37" s="60"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -3056,18 +3092,18 @@
       <c r="AE37" s="1"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="57"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="69" t="s">
+      <c r="A38" s="58"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="70" t="s">
         <v>56</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="70">
+      <c r="E38" s="71">
         <v>40.0</v>
       </c>
-      <c r="F38" s="61"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="59"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="60"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -3075,7 +3111,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="72"/>
+      <c r="P38" s="73"/>
       <c r="Q38" s="23"/>
       <c r="R38" s="23"/>
       <c r="S38" s="23"/>
@@ -3093,14 +3129,14 @@
       <c r="AE38" s="1"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="D39" s="73"/>
-      <c r="E39" s="72"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="73"/>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-      <c r="O39" s="73"/>
+      <c r="O39" s="74"/>
       <c r="S39" s="1"/>
       <c r="W39" s="1"/>
     </row>
@@ -4171,10 +4207,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="75" t="s">
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="76" t="s">
         <v>57</v>
       </c>
       <c r="E1" s="4"/>
@@ -4188,23 +4224,23 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="74"/>
-      <c r="Z1" s="74"/>
-      <c r="AA1" s="74"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
     </row>
     <row r="2">
-      <c r="A2" s="74"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -4217,100 +4253,100 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="8"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="74"/>
-      <c r="U2" s="74"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="74"/>
-      <c r="X2" s="74"/>
-      <c r="Y2" s="74"/>
-      <c r="Z2" s="74"/>
-      <c r="AA2" s="74"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="75"/>
     </row>
     <row r="3" ht="79.5" customHeight="1">
-      <c r="A3" s="76"/>
-      <c r="B3" s="77">
+      <c r="A3" s="77"/>
+      <c r="B3" s="78">
         <v>45575.0</v>
       </c>
-      <c r="C3" s="77">
+      <c r="C3" s="78">
         <v>45582.0</v>
       </c>
-      <c r="D3" s="78">
+      <c r="D3" s="79">
         <v>45589.0</v>
       </c>
-      <c r="E3" s="78">
+      <c r="E3" s="79">
         <v>45596.0</v>
       </c>
-      <c r="F3" s="78">
+      <c r="F3" s="79">
         <v>45603.0</v>
       </c>
-      <c r="G3" s="78">
+      <c r="G3" s="79">
         <v>45610.0</v>
       </c>
-      <c r="H3" s="78">
+      <c r="H3" s="79">
         <v>45617.0</v>
       </c>
-      <c r="I3" s="78">
+      <c r="I3" s="79">
         <v>45624.0</v>
       </c>
-      <c r="J3" s="78">
+      <c r="J3" s="79">
         <v>45631.0</v>
       </c>
-      <c r="K3" s="78">
+      <c r="K3" s="79">
         <v>45638.0</v>
       </c>
-      <c r="L3" s="78">
+      <c r="L3" s="79">
         <v>45645.0</v>
       </c>
-      <c r="M3" s="78">
+      <c r="M3" s="79">
         <v>45659.0</v>
       </c>
-      <c r="N3" s="78">
+      <c r="N3" s="79">
         <v>45666.0</v>
       </c>
-      <c r="O3" s="78">
+      <c r="O3" s="79">
         <v>45673.0</v>
       </c>
-      <c r="P3" s="77">
+      <c r="P3" s="78">
         <v>45680.0</v>
       </c>
-      <c r="Q3" s="77">
+      <c r="Q3" s="78">
         <v>45687.0</v>
       </c>
-      <c r="R3" s="77">
+      <c r="R3" s="78">
         <v>45694.0</v>
       </c>
-      <c r="S3" s="77">
+      <c r="S3" s="78">
         <v>45701.0</v>
       </c>
-      <c r="T3" s="77">
+      <c r="T3" s="78">
         <v>45708.0</v>
       </c>
-      <c r="U3" s="77">
+      <c r="U3" s="78">
         <v>45715.0</v>
       </c>
-      <c r="V3" s="77">
+      <c r="V3" s="78">
         <v>45722.0</v>
       </c>
-      <c r="W3" s="77">
+      <c r="W3" s="78">
         <v>45729.0</v>
       </c>
-      <c r="X3" s="77">
+      <c r="X3" s="78">
         <v>45736.0</v>
       </c>
-      <c r="Y3" s="77">
+      <c r="Y3" s="78">
         <v>45743.0</v>
       </c>
-      <c r="Z3" s="79" t="s">
+      <c r="Z3" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="80"/>
+      <c r="AA3" s="81"/>
     </row>
     <row r="4">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="82" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
@@ -4385,856 +4421,880 @@
       <c r="Y4" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="82" t="s">
+      <c r="Z4" s="83" t="s">
         <v>58</v>
       </c>
       <c r="AA4" s="27"/>
     </row>
     <row r="5">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="84">
+      <c r="B5" s="85">
         <v>30.0</v>
       </c>
-      <c r="C5" s="84">
+      <c r="C5" s="85">
         <v>37.0</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="84">
+      <c r="D5" s="86"/>
+      <c r="E5" s="85">
         <v>31.0</v>
       </c>
-      <c r="F5" s="84">
+      <c r="F5" s="85">
         <v>33.0</v>
       </c>
-      <c r="G5" s="84">
+      <c r="G5" s="85">
         <v>27.0</v>
       </c>
-      <c r="H5" s="84">
+      <c r="H5" s="85">
         <v>27.0</v>
       </c>
-      <c r="I5" s="84">
+      <c r="I5" s="85">
         <v>29.0</v>
       </c>
-      <c r="J5" s="84">
+      <c r="J5" s="85">
         <v>36.0</v>
       </c>
-      <c r="K5" s="85">
+      <c r="K5" s="86">
         <v>28.0</v>
       </c>
-      <c r="L5" s="86">
+      <c r="L5" s="87">
         <v>38.0</v>
       </c>
-      <c r="M5" s="85">
+      <c r="M5" s="86">
         <v>38.0</v>
       </c>
-      <c r="N5" s="85"/>
-      <c r="O5" s="86">
+      <c r="N5" s="86"/>
+      <c r="O5" s="87">
         <v>36.0</v>
       </c>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="87">
+      <c r="P5" s="88"/>
+      <c r="Q5" s="88">
         <v>27.0</v>
       </c>
-      <c r="R5" s="85"/>
-      <c r="S5" s="87"/>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="85"/>
-      <c r="Z5" s="88">
+      <c r="R5" s="89">
+        <v>35.0</v>
+      </c>
+      <c r="S5" s="88"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="86"/>
+      <c r="X5" s="86"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="90">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>417</v>
+        <v>452</v>
       </c>
       <c r="AA5" s="36"/>
     </row>
     <row r="6">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="85">
+      <c r="B6" s="86">
         <v>36.0</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85">
+      <c r="C6" s="86"/>
+      <c r="D6" s="86">
         <v>32.0</v>
       </c>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85">
+      <c r="E6" s="86"/>
+      <c r="F6" s="86">
         <v>39.0</v>
       </c>
-      <c r="G6" s="85">
+      <c r="G6" s="86">
         <v>35.0</v>
       </c>
-      <c r="H6" s="85">
+      <c r="H6" s="86">
         <v>27.0</v>
       </c>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85">
+      <c r="I6" s="86"/>
+      <c r="J6" s="86">
         <v>33.0</v>
       </c>
-      <c r="K6" s="85">
+      <c r="K6" s="86">
         <v>38.0</v>
       </c>
-      <c r="L6" s="85">
+      <c r="L6" s="86">
         <v>35.0</v>
       </c>
-      <c r="M6" s="85">
+      <c r="M6" s="86">
         <v>32.0</v>
       </c>
-      <c r="N6" s="86">
+      <c r="N6" s="87">
         <v>33.0</v>
       </c>
-      <c r="O6" s="85">
+      <c r="O6" s="86">
         <v>34.0</v>
       </c>
-      <c r="P6" s="87"/>
-      <c r="Q6" s="87">
+      <c r="P6" s="88"/>
+      <c r="Q6" s="88">
         <v>30.0</v>
       </c>
-      <c r="R6" s="85"/>
-      <c r="S6" s="87"/>
-      <c r="T6" s="85"/>
-      <c r="U6" s="85"/>
-      <c r="V6" s="85"/>
-      <c r="W6" s="85"/>
-      <c r="X6" s="85"/>
-      <c r="Y6" s="85"/>
-      <c r="Z6" s="88">
+      <c r="R6" s="88">
+        <v>25.0</v>
+      </c>
+      <c r="S6" s="88"/>
+      <c r="T6" s="86"/>
+      <c r="U6" s="86"/>
+      <c r="V6" s="86"/>
+      <c r="W6" s="86"/>
+      <c r="X6" s="86"/>
+      <c r="Y6" s="86"/>
+      <c r="Z6" s="90">
         <f t="shared" si="1"/>
-        <v>404</v>
+        <v>429</v>
       </c>
       <c r="AA6" s="36"/>
     </row>
     <row r="7">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="84">
+      <c r="B7" s="85">
         <v>33.0</v>
       </c>
-      <c r="C7" s="84">
+      <c r="C7" s="85">
         <v>28.0</v>
       </c>
-      <c r="D7" s="84">
+      <c r="D7" s="85">
         <v>32.0</v>
       </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="84">
+      <c r="E7" s="86"/>
+      <c r="F7" s="85">
         <v>33.0</v>
       </c>
-      <c r="G7" s="84">
+      <c r="G7" s="85">
         <v>34.0</v>
       </c>
-      <c r="H7" s="84">
+      <c r="H7" s="85">
         <v>26.0</v>
       </c>
-      <c r="I7" s="84">
+      <c r="I7" s="85">
         <v>29.0</v>
       </c>
-      <c r="J7" s="84">
+      <c r="J7" s="85">
         <v>28.0</v>
       </c>
-      <c r="K7" s="85">
+      <c r="K7" s="86">
         <v>29.0</v>
       </c>
-      <c r="L7" s="85">
+      <c r="L7" s="86">
         <v>27.0</v>
       </c>
-      <c r="M7" s="86">
+      <c r="M7" s="87">
         <v>38.0</v>
       </c>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85">
+      <c r="N7" s="86"/>
+      <c r="O7" s="86">
         <v>32.0</v>
       </c>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="87">
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88">
         <v>24.0</v>
       </c>
-      <c r="R7" s="85"/>
-      <c r="S7" s="87"/>
-      <c r="T7" s="85"/>
-      <c r="U7" s="85"/>
-      <c r="V7" s="85"/>
-      <c r="W7" s="85"/>
-      <c r="X7" s="85"/>
-      <c r="Y7" s="85"/>
-      <c r="Z7" s="88">
+      <c r="R7" s="88">
+        <v>28.0</v>
+      </c>
+      <c r="S7" s="88"/>
+      <c r="T7" s="86"/>
+      <c r="U7" s="86"/>
+      <c r="V7" s="86"/>
+      <c r="W7" s="86"/>
+      <c r="X7" s="86"/>
+      <c r="Y7" s="86"/>
+      <c r="Z7" s="90">
         <f t="shared" si="1"/>
-        <v>393</v>
+        <v>421</v>
       </c>
       <c r="AA7" s="36"/>
     </row>
     <row r="8">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="84">
+      <c r="B8" s="85">
         <v>37.0</v>
       </c>
-      <c r="C8" s="84">
+      <c r="C8" s="85">
         <v>35.0</v>
       </c>
-      <c r="D8" s="84">
+      <c r="D8" s="85">
         <v>32.0</v>
       </c>
-      <c r="E8" s="89">
+      <c r="E8" s="91">
         <v>31.0</v>
       </c>
-      <c r="F8" s="84">
+      <c r="F8" s="85">
         <v>31.0</v>
       </c>
-      <c r="G8" s="84">
+      <c r="G8" s="85">
         <v>33.0</v>
       </c>
-      <c r="H8" s="84">
+      <c r="H8" s="85">
         <v>36.0</v>
       </c>
-      <c r="I8" s="84">
+      <c r="I8" s="85">
         <v>33.0</v>
       </c>
-      <c r="J8" s="90">
+      <c r="J8" s="92">
         <v>36.0</v>
       </c>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85">
+      <c r="K8" s="86"/>
+      <c r="L8" s="86">
         <v>32.0</v>
       </c>
-      <c r="M8" s="85">
+      <c r="M8" s="86">
         <v>33.0</v>
       </c>
-      <c r="N8" s="85"/>
-      <c r="O8" s="85"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="87">
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88">
         <v>22.0</v>
       </c>
-      <c r="R8" s="85"/>
-      <c r="S8" s="87"/>
-      <c r="T8" s="85"/>
-      <c r="U8" s="85"/>
-      <c r="V8" s="85"/>
-      <c r="W8" s="85"/>
-      <c r="X8" s="85"/>
-      <c r="Y8" s="85"/>
-      <c r="Z8" s="88">
+      <c r="R8" s="88">
+        <v>34.0</v>
+      </c>
+      <c r="S8" s="88"/>
+      <c r="T8" s="86"/>
+      <c r="U8" s="86"/>
+      <c r="V8" s="86"/>
+      <c r="W8" s="86"/>
+      <c r="X8" s="86"/>
+      <c r="Y8" s="86"/>
+      <c r="Z8" s="90">
         <f t="shared" si="1"/>
-        <v>391</v>
+        <v>425</v>
       </c>
       <c r="AA8" s="36"/>
     </row>
     <row r="9">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="84">
+      <c r="B9" s="85">
         <v>30.0</v>
       </c>
-      <c r="C9" s="84">
+      <c r="C9" s="85">
         <v>33.0</v>
       </c>
-      <c r="D9" s="84">
+      <c r="D9" s="85">
         <v>30.0</v>
       </c>
-      <c r="E9" s="84">
+      <c r="E9" s="85">
         <v>26.0</v>
       </c>
-      <c r="F9" s="84">
+      <c r="F9" s="85">
         <v>28.0</v>
       </c>
-      <c r="G9" s="84">
+      <c r="G9" s="85">
         <v>26.0</v>
       </c>
-      <c r="H9" s="84">
+      <c r="H9" s="85">
         <v>20.0</v>
       </c>
-      <c r="I9" s="85"/>
-      <c r="J9" s="84">
+      <c r="I9" s="86"/>
+      <c r="J9" s="85">
         <v>34.0</v>
       </c>
-      <c r="K9" s="85">
+      <c r="K9" s="86">
         <v>26.0</v>
       </c>
-      <c r="L9" s="85">
+      <c r="L9" s="86">
         <v>26.0</v>
       </c>
-      <c r="M9" s="85">
+      <c r="M9" s="86">
         <v>24.0</v>
       </c>
-      <c r="N9" s="85">
+      <c r="N9" s="86">
         <v>28.0</v>
       </c>
-      <c r="O9" s="85">
+      <c r="O9" s="86">
         <v>28.0</v>
       </c>
-      <c r="P9" s="87"/>
-      <c r="Q9" s="87">
+      <c r="P9" s="88"/>
+      <c r="Q9" s="88">
         <v>31.0</v>
       </c>
-      <c r="R9" s="85"/>
-      <c r="S9" s="87"/>
-      <c r="T9" s="85"/>
-      <c r="U9" s="85"/>
-      <c r="V9" s="85"/>
-      <c r="W9" s="85"/>
-      <c r="X9" s="85"/>
-      <c r="Y9" s="85"/>
-      <c r="Z9" s="88">
+      <c r="R9" s="88">
+        <v>30.0</v>
+      </c>
+      <c r="S9" s="88"/>
+      <c r="T9" s="86"/>
+      <c r="U9" s="86"/>
+      <c r="V9" s="86"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="86"/>
+      <c r="Y9" s="86"/>
+      <c r="Z9" s="90">
         <f t="shared" si="1"/>
-        <v>390</v>
+        <v>420</v>
       </c>
       <c r="AA9" s="36"/>
     </row>
     <row r="10">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85">
+      <c r="B10" s="86"/>
+      <c r="C10" s="86">
         <v>31.0</v>
       </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85">
+      <c r="D10" s="86"/>
+      <c r="E10" s="86">
         <v>23.0</v>
       </c>
-      <c r="F10" s="85">
+      <c r="F10" s="86">
         <v>35.0</v>
       </c>
-      <c r="G10" s="85">
+      <c r="G10" s="86">
         <v>29.0</v>
       </c>
-      <c r="H10" s="85">
+      <c r="H10" s="86">
         <v>16.0</v>
       </c>
-      <c r="I10" s="85"/>
-      <c r="J10" s="85">
+      <c r="I10" s="86"/>
+      <c r="J10" s="86">
         <v>29.0</v>
       </c>
-      <c r="K10" s="85">
+      <c r="K10" s="86">
         <v>21.0</v>
       </c>
-      <c r="L10" s="85">
+      <c r="L10" s="86">
         <v>24.0</v>
       </c>
-      <c r="M10" s="85">
+      <c r="M10" s="86">
         <v>28.0</v>
       </c>
-      <c r="N10" s="85"/>
-      <c r="O10" s="85">
+      <c r="N10" s="86"/>
+      <c r="O10" s="86">
         <v>14.0</v>
       </c>
-      <c r="P10" s="87"/>
-      <c r="Q10" s="87">
+      <c r="P10" s="88"/>
+      <c r="Q10" s="88">
         <v>22.0</v>
       </c>
-      <c r="R10" s="85"/>
-      <c r="S10" s="87"/>
-      <c r="T10" s="85"/>
-      <c r="U10" s="85"/>
-      <c r="V10" s="85"/>
-      <c r="W10" s="85"/>
-      <c r="X10" s="85"/>
-      <c r="Y10" s="85"/>
-      <c r="Z10" s="88">
+      <c r="R10" s="88">
+        <v>20.0</v>
+      </c>
+      <c r="S10" s="88"/>
+      <c r="T10" s="86"/>
+      <c r="U10" s="86"/>
+      <c r="V10" s="86"/>
+      <c r="W10" s="86"/>
+      <c r="X10" s="86"/>
+      <c r="Y10" s="86"/>
+      <c r="Z10" s="90">
         <f t="shared" si="1"/>
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="AA10" s="36"/>
     </row>
     <row r="11">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="85">
+      <c r="B11" s="86">
         <v>41.0</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="86">
         <v>31.0</v>
       </c>
-      <c r="D11" s="85">
+      <c r="D11" s="86">
         <v>32.0</v>
       </c>
-      <c r="E11" s="85">
+      <c r="E11" s="86">
         <v>29.0</v>
       </c>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85"/>
-      <c r="H11" s="85">
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86">
         <v>23.0</v>
       </c>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="85"/>
-      <c r="L11" s="85"/>
-      <c r="M11" s="85"/>
-      <c r="N11" s="85"/>
-      <c r="O11" s="85"/>
-      <c r="P11" s="85"/>
-      <c r="Q11" s="85"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="85"/>
-      <c r="T11" s="85"/>
-      <c r="U11" s="85"/>
-      <c r="V11" s="85"/>
-      <c r="W11" s="85"/>
-      <c r="X11" s="85"/>
-      <c r="Y11" s="85"/>
-      <c r="Z11" s="88">
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
+      <c r="T11" s="86"/>
+      <c r="U11" s="86"/>
+      <c r="V11" s="86"/>
+      <c r="W11" s="86"/>
+      <c r="X11" s="86"/>
+      <c r="Y11" s="86"/>
+      <c r="Z11" s="90">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
       <c r="AA11" s="36"/>
     </row>
     <row r="12">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="84">
+      <c r="B12" s="85">
         <v>42.0</v>
       </c>
-      <c r="C12" s="84">
+      <c r="C12" s="85">
         <v>31.0</v>
       </c>
-      <c r="D12" s="84">
+      <c r="D12" s="85">
         <v>32.0</v>
       </c>
-      <c r="E12" s="84">
+      <c r="E12" s="85">
         <v>32.0</v>
       </c>
-      <c r="F12" s="84">
+      <c r="F12" s="85">
         <v>34.0</v>
       </c>
-      <c r="G12" s="85"/>
-      <c r="H12" s="84">
+      <c r="G12" s="86"/>
+      <c r="H12" s="85">
         <v>28.0</v>
       </c>
-      <c r="I12" s="84">
+      <c r="I12" s="85">
         <v>34.0</v>
       </c>
-      <c r="J12" s="84">
+      <c r="J12" s="85">
         <v>33.0</v>
       </c>
-      <c r="K12" s="85"/>
-      <c r="L12" s="85"/>
-      <c r="M12" s="85"/>
-      <c r="N12" s="85"/>
-      <c r="O12" s="85">
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86">
         <v>30.0</v>
       </c>
-      <c r="P12" s="87"/>
-      <c r="Q12" s="87">
+      <c r="P12" s="88"/>
+      <c r="Q12" s="88">
         <v>27.0</v>
       </c>
-      <c r="R12" s="85"/>
-      <c r="S12" s="85"/>
-      <c r="T12" s="85"/>
-      <c r="U12" s="85"/>
-      <c r="V12" s="85"/>
-      <c r="W12" s="85"/>
-      <c r="X12" s="85"/>
-      <c r="Y12" s="85"/>
-      <c r="Z12" s="88">
+      <c r="R12" s="88">
+        <v>26.0</v>
+      </c>
+      <c r="S12" s="86"/>
+      <c r="T12" s="86"/>
+      <c r="U12" s="86"/>
+      <c r="V12" s="86"/>
+      <c r="W12" s="86"/>
+      <c r="X12" s="86"/>
+      <c r="Y12" s="86"/>
+      <c r="Z12" s="90">
         <f t="shared" si="1"/>
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="AA12" s="36"/>
     </row>
     <row r="13">
-      <c r="A13" s="83" t="s">
+      <c r="A13" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85">
+      <c r="B13" s="93"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86">
         <v>33.0</v>
       </c>
-      <c r="E13" s="85">
+      <c r="E13" s="86">
         <v>36.0</v>
       </c>
-      <c r="F13" s="85">
+      <c r="F13" s="86">
         <v>27.0</v>
       </c>
-      <c r="G13" s="85">
+      <c r="G13" s="86">
         <v>37.0</v>
       </c>
-      <c r="H13" s="85">
+      <c r="H13" s="86">
         <v>31.0</v>
       </c>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85">
+      <c r="I13" s="86"/>
+      <c r="J13" s="86">
         <v>34.0</v>
       </c>
-      <c r="K13" s="86">
+      <c r="K13" s="87">
         <v>40.0</v>
       </c>
-      <c r="L13" s="85">
+      <c r="L13" s="86">
         <v>34.0</v>
       </c>
-      <c r="M13" s="85">
+      <c r="M13" s="86">
         <v>31.0</v>
       </c>
-      <c r="N13" s="85">
+      <c r="N13" s="86">
         <v>29.0</v>
       </c>
-      <c r="O13" s="85">
+      <c r="O13" s="86">
         <v>34.0</v>
       </c>
-      <c r="P13" s="92"/>
-      <c r="Q13" s="92">
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89">
         <v>38.0</v>
       </c>
-      <c r="R13" s="85"/>
-      <c r="S13" s="85"/>
-      <c r="T13" s="85"/>
-      <c r="U13" s="85"/>
-      <c r="V13" s="85"/>
-      <c r="W13" s="85"/>
-      <c r="X13" s="85"/>
-      <c r="Y13" s="85"/>
-      <c r="Z13" s="88">
+      <c r="R13" s="88">
+        <v>28.0</v>
+      </c>
+      <c r="S13" s="86"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="86"/>
+      <c r="V13" s="86"/>
+      <c r="W13" s="86"/>
+      <c r="X13" s="86"/>
+      <c r="Y13" s="86"/>
+      <c r="Z13" s="90">
         <f t="shared" si="1"/>
-        <v>404</v>
+        <v>432</v>
       </c>
       <c r="AA13" s="36"/>
     </row>
     <row r="14">
-      <c r="A14" s="83" t="s">
+      <c r="A14" s="84" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="85"/>
-      <c r="C14" s="85">
+      <c r="B14" s="86"/>
+      <c r="C14" s="86">
         <v>22.0</v>
       </c>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85">
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86">
         <v>36.0</v>
       </c>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85">
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86">
         <v>34.0</v>
       </c>
-      <c r="K14" s="85">
+      <c r="K14" s="86">
         <v>27.0</v>
       </c>
-      <c r="L14" s="85">
+      <c r="L14" s="86">
         <v>35.0</v>
       </c>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85">
+      <c r="M14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86">
         <v>32.0</v>
       </c>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="85"/>
-      <c r="X14" s="85"/>
-      <c r="Y14" s="85"/>
-      <c r="Z14" s="88">
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
+      <c r="R14" s="88">
+        <v>31.0</v>
+      </c>
+      <c r="S14" s="86"/>
+      <c r="T14" s="86"/>
+      <c r="U14" s="86"/>
+      <c r="V14" s="86"/>
+      <c r="W14" s="86"/>
+      <c r="X14" s="86"/>
+      <c r="Y14" s="86"/>
+      <c r="Z14" s="90">
         <f t="shared" si="1"/>
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="AA14" s="36"/>
     </row>
     <row r="15">
-      <c r="A15" s="83" t="s">
+      <c r="A15" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="85"/>
-      <c r="C15" s="85">
+      <c r="B15" s="86"/>
+      <c r="C15" s="86">
         <v>43.0</v>
       </c>
-      <c r="D15" s="85">
+      <c r="D15" s="86">
         <v>25.0</v>
       </c>
-      <c r="E15" s="85"/>
-      <c r="F15" s="85">
+      <c r="E15" s="86"/>
+      <c r="F15" s="86">
         <v>32.0</v>
       </c>
-      <c r="G15" s="85">
+      <c r="G15" s="86">
         <v>30.0</v>
       </c>
-      <c r="H15" s="85">
+      <c r="H15" s="86">
         <v>34.0</v>
       </c>
-      <c r="I15" s="85"/>
-      <c r="J15" s="85">
+      <c r="I15" s="86"/>
+      <c r="J15" s="86">
         <v>34.0</v>
       </c>
-      <c r="K15" s="85">
+      <c r="K15" s="86">
         <v>26.0</v>
       </c>
-      <c r="L15" s="85">
+      <c r="L15" s="86">
         <v>37.0</v>
       </c>
-      <c r="M15" s="85">
+      <c r="M15" s="86">
         <v>32.0</v>
       </c>
-      <c r="N15" s="85">
+      <c r="N15" s="86">
         <v>27.0</v>
       </c>
-      <c r="O15" s="85"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="87">
+      <c r="O15" s="86"/>
+      <c r="P15" s="88"/>
+      <c r="Q15" s="88">
         <v>27.0</v>
       </c>
-      <c r="R15" s="85"/>
-      <c r="S15" s="85"/>
-      <c r="T15" s="85"/>
-      <c r="U15" s="85"/>
-      <c r="V15" s="85"/>
-      <c r="W15" s="85"/>
-      <c r="X15" s="85"/>
-      <c r="Y15" s="85"/>
-      <c r="Z15" s="88">
+      <c r="R15" s="88">
+        <v>28.0</v>
+      </c>
+      <c r="S15" s="86"/>
+      <c r="T15" s="86"/>
+      <c r="U15" s="86"/>
+      <c r="V15" s="86"/>
+      <c r="W15" s="86"/>
+      <c r="X15" s="86"/>
+      <c r="Y15" s="86"/>
+      <c r="Z15" s="90">
         <f t="shared" si="1"/>
-        <v>347</v>
+        <v>375</v>
       </c>
       <c r="AA15" s="36"/>
     </row>
     <row r="16">
-      <c r="A16" s="83" t="s">
+      <c r="A16" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85">
+      <c r="B16" s="86"/>
+      <c r="C16" s="86">
         <v>29.0</v>
       </c>
-      <c r="D16" s="85">
+      <c r="D16" s="86">
         <v>28.0</v>
       </c>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85">
+      <c r="E16" s="86"/>
+      <c r="F16" s="86">
         <v>23.0</v>
       </c>
-      <c r="G16" s="85">
+      <c r="G16" s="86">
         <v>30.0</v>
       </c>
-      <c r="H16" s="85"/>
-      <c r="I16" s="85">
+      <c r="H16" s="86"/>
+      <c r="I16" s="86">
         <v>27.0</v>
       </c>
-      <c r="J16" s="85"/>
-      <c r="K16" s="85">
+      <c r="J16" s="86"/>
+      <c r="K16" s="86">
         <v>29.0</v>
       </c>
-      <c r="L16" s="85"/>
-      <c r="M16" s="85"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="85">
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
+      <c r="N16" s="86"/>
+      <c r="O16" s="86">
         <v>35.0</v>
       </c>
-      <c r="P16" s="87"/>
-      <c r="Q16" s="87">
+      <c r="P16" s="88"/>
+      <c r="Q16" s="88">
         <v>33.0</v>
       </c>
-      <c r="R16" s="85"/>
-      <c r="S16" s="85"/>
-      <c r="T16" s="85"/>
-      <c r="U16" s="85"/>
-      <c r="V16" s="85"/>
-      <c r="W16" s="85"/>
-      <c r="X16" s="85"/>
-      <c r="Y16" s="85"/>
-      <c r="Z16" s="88">
+      <c r="R16" s="88">
+        <v>27.0</v>
+      </c>
+      <c r="S16" s="86"/>
+      <c r="T16" s="86"/>
+      <c r="U16" s="86"/>
+      <c r="V16" s="86"/>
+      <c r="W16" s="86"/>
+      <c r="X16" s="86"/>
+      <c r="Y16" s="86"/>
+      <c r="Z16" s="90">
         <f t="shared" si="1"/>
-        <v>234</v>
+        <v>261</v>
       </c>
       <c r="AA16" s="36"/>
     </row>
     <row r="17">
-      <c r="A17" s="83" t="s">
+      <c r="A17" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="85">
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86">
         <v>26.0</v>
       </c>
-      <c r="H17" s="85"/>
-      <c r="I17" s="85"/>
-      <c r="J17" s="85"/>
-      <c r="K17" s="85"/>
-      <c r="L17" s="85"/>
-      <c r="M17" s="85"/>
-      <c r="N17" s="85"/>
-      <c r="O17" s="85"/>
-      <c r="P17" s="85"/>
-      <c r="Q17" s="85"/>
-      <c r="R17" s="85"/>
-      <c r="S17" s="85"/>
-      <c r="T17" s="85"/>
-      <c r="U17" s="85"/>
-      <c r="V17" s="85"/>
-      <c r="W17" s="85"/>
-      <c r="X17" s="85"/>
-      <c r="Y17" s="85"/>
-      <c r="Z17" s="88">
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="86"/>
+      <c r="Q17" s="86"/>
+      <c r="R17" s="86"/>
+      <c r="S17" s="86"/>
+      <c r="T17" s="86"/>
+      <c r="U17" s="86"/>
+      <c r="V17" s="86"/>
+      <c r="W17" s="86"/>
+      <c r="X17" s="86"/>
+      <c r="Y17" s="86"/>
+      <c r="Z17" s="90">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="AA17" s="36"/>
     </row>
     <row r="18">
-      <c r="A18" s="83" t="s">
+      <c r="A18" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="85"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="85">
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86">
         <v>27.0</v>
       </c>
-      <c r="H18" s="85"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="85"/>
-      <c r="K18" s="85"/>
-      <c r="L18" s="85"/>
-      <c r="M18" s="85"/>
-      <c r="N18" s="85"/>
-      <c r="O18" s="85"/>
-      <c r="P18" s="85"/>
-      <c r="Q18" s="85"/>
-      <c r="R18" s="85"/>
-      <c r="S18" s="85"/>
-      <c r="T18" s="85"/>
-      <c r="U18" s="85"/>
-      <c r="V18" s="85"/>
-      <c r="W18" s="85"/>
-      <c r="X18" s="85"/>
-      <c r="Y18" s="85"/>
-      <c r="Z18" s="88">
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="86"/>
+      <c r="P18" s="86"/>
+      <c r="Q18" s="86"/>
+      <c r="R18" s="86"/>
+      <c r="S18" s="86"/>
+      <c r="T18" s="86"/>
+      <c r="U18" s="86"/>
+      <c r="V18" s="86"/>
+      <c r="W18" s="86"/>
+      <c r="X18" s="86"/>
+      <c r="Y18" s="86"/>
+      <c r="Z18" s="90">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="AA18" s="36"/>
     </row>
     <row r="19">
-      <c r="A19" s="83" t="s">
+      <c r="A19" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="85"/>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85">
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86">
         <v>41.0</v>
       </c>
-      <c r="E19" s="85">
+      <c r="E19" s="86">
         <v>37.0</v>
       </c>
-      <c r="F19" s="85">
+      <c r="F19" s="86">
         <v>38.0</v>
       </c>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="87"/>
-      <c r="Q19" s="87">
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
+      <c r="N19" s="86"/>
+      <c r="O19" s="86"/>
+      <c r="P19" s="88"/>
+      <c r="Q19" s="88">
         <v>32.0</v>
       </c>
-      <c r="R19" s="85"/>
-      <c r="S19" s="85"/>
-      <c r="T19" s="85"/>
-      <c r="U19" s="85"/>
-      <c r="V19" s="85"/>
-      <c r="W19" s="85"/>
-      <c r="X19" s="85"/>
-      <c r="Y19" s="85"/>
-      <c r="Z19" s="88">
+      <c r="R19" s="88">
+        <v>24.0</v>
+      </c>
+      <c r="S19" s="86"/>
+      <c r="T19" s="86"/>
+      <c r="U19" s="86"/>
+      <c r="V19" s="86"/>
+      <c r="W19" s="86"/>
+      <c r="X19" s="86"/>
+      <c r="Y19" s="86"/>
+      <c r="Z19" s="90">
         <f t="shared" si="1"/>
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="AA19" s="36"/>
     </row>
     <row r="20">
-      <c r="A20" s="93"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="82"/>
-      <c r="O20" s="82"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="82"/>
-      <c r="R20" s="82"/>
-      <c r="S20" s="82"/>
-      <c r="T20" s="82"/>
-      <c r="U20" s="82"/>
-      <c r="V20" s="82"/>
-      <c r="W20" s="82"/>
-      <c r="X20" s="82"/>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="82"/>
+      <c r="A20" s="94"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="83"/>
+      <c r="K20" s="83"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="83"/>
+      <c r="P20" s="83"/>
+      <c r="Q20" s="83"/>
+      <c r="R20" s="83"/>
+      <c r="S20" s="83"/>
+      <c r="T20" s="83"/>
+      <c r="U20" s="83"/>
+      <c r="V20" s="83"/>
+      <c r="W20" s="83"/>
+      <c r="X20" s="83"/>
+      <c r="Y20" s="83"/>
+      <c r="Z20" s="83"/>
       <c r="AA20" s="36"/>
     </row>
     <row r="21">
-      <c r="A21" s="74"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="74"/>
-      <c r="Q21" s="74"/>
-      <c r="R21" s="74"/>
-      <c r="S21" s="74"/>
-      <c r="T21" s="74"/>
-      <c r="U21" s="74"/>
-      <c r="V21" s="74"/>
-      <c r="W21" s="74"/>
-      <c r="X21" s="74"/>
-      <c r="Y21" s="74"/>
-      <c r="Z21" s="74"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="75"/>
+      <c r="M21" s="75"/>
+      <c r="N21" s="75"/>
+      <c r="O21" s="75"/>
+      <c r="P21" s="75"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="75"/>
+      <c r="T21" s="75"/>
+      <c r="U21" s="75"/>
+      <c r="V21" s="75"/>
+      <c r="W21" s="75"/>
+      <c r="X21" s="75"/>
+      <c r="Y21" s="75"/>
+      <c r="Z21" s="75"/>
       <c r="AA21" s="36"/>
     </row>
     <row r="22">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="95">
+      <c r="B22" s="96">
         <v>10.0</v>
       </c>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="96" t="s">
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="97" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="4"/>
@@ -5243,28 +5303,28 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="74"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-      <c r="S22" s="74"/>
-      <c r="T22" s="74"/>
-      <c r="U22" s="74"/>
-      <c r="V22" s="74"/>
-      <c r="W22" s="74"/>
-      <c r="X22" s="74"/>
-      <c r="Y22" s="74"/>
-      <c r="Z22" s="74"/>
+      <c r="M22" s="75"/>
+      <c r="N22" s="75"/>
+      <c r="O22" s="75"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="75"/>
+      <c r="S22" s="75"/>
+      <c r="T22" s="75"/>
+      <c r="U22" s="75"/>
+      <c r="V22" s="75"/>
+      <c r="W22" s="75"/>
+      <c r="X22" s="75"/>
+      <c r="Y22" s="75"/>
+      <c r="Z22" s="75"/>
       <c r="AA22" s="36"/>
     </row>
     <row r="23">
-      <c r="A23" s="74"/>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
+      <c r="A23" s="75"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -5272,181 +5332,181 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="74"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="74"/>
-      <c r="R23" s="74"/>
-      <c r="S23" s="74"/>
-      <c r="T23" s="74"/>
-      <c r="U23" s="74"/>
-      <c r="V23" s="74"/>
-      <c r="W23" s="74"/>
-      <c r="X23" s="74"/>
-      <c r="Y23" s="74"/>
-      <c r="Z23" s="74"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="75"/>
+      <c r="O23" s="75"/>
+      <c r="P23" s="75"/>
+      <c r="Q23" s="75"/>
+      <c r="R23" s="75"/>
+      <c r="S23" s="75"/>
+      <c r="T23" s="75"/>
+      <c r="U23" s="75"/>
+      <c r="V23" s="75"/>
+      <c r="W23" s="75"/>
+      <c r="X23" s="75"/>
+      <c r="Y23" s="75"/>
+      <c r="Z23" s="75"/>
       <c r="AA23" s="36"/>
     </row>
     <row r="24">
-      <c r="A24" s="74"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="74"/>
-      <c r="L24" s="74"/>
-      <c r="M24" s="74"/>
-      <c r="N24" s="74"/>
-      <c r="O24" s="74"/>
-      <c r="P24" s="74"/>
-      <c r="Q24" s="74"/>
-      <c r="R24" s="74"/>
-      <c r="S24" s="74"/>
-      <c r="T24" s="74"/>
-      <c r="U24" s="74"/>
-      <c r="V24" s="74"/>
-      <c r="W24" s="74"/>
-      <c r="X24" s="74"/>
-      <c r="Y24" s="74"/>
-      <c r="Z24" s="74"/>
+      <c r="A24" s="75"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="75"/>
+      <c r="P24" s="75"/>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="75"/>
+      <c r="S24" s="75"/>
+      <c r="T24" s="75"/>
+      <c r="U24" s="75"/>
+      <c r="V24" s="75"/>
+      <c r="W24" s="75"/>
+      <c r="X24" s="75"/>
+      <c r="Y24" s="75"/>
+      <c r="Z24" s="75"/>
       <c r="AA24" s="36"/>
     </row>
     <row r="25">
-      <c r="A25" s="74"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="97" t="s">
+      <c r="A25" s="75"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="61"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="98">
+      <c r="G25" s="62"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="99">
         <v>60.0</v>
       </c>
-      <c r="K25" s="61"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="74"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
-      <c r="S25" s="74"/>
-      <c r="T25" s="74"/>
-      <c r="U25" s="74"/>
-      <c r="V25" s="74"/>
-      <c r="W25" s="74"/>
-      <c r="X25" s="74"/>
-      <c r="Y25" s="74"/>
-      <c r="Z25" s="74"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="75"/>
+      <c r="O25" s="75"/>
+      <c r="P25" s="75"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="75"/>
+      <c r="S25" s="75"/>
+      <c r="T25" s="75"/>
+      <c r="U25" s="75"/>
+      <c r="V25" s="75"/>
+      <c r="W25" s="75"/>
+      <c r="X25" s="75"/>
+      <c r="Y25" s="75"/>
+      <c r="Z25" s="75"/>
       <c r="AA25" s="36"/>
     </row>
     <row r="26">
-      <c r="A26" s="74"/>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="97" t="s">
+      <c r="A26" s="75"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="61"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="98">
+      <c r="G26" s="62"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="83"/>
+      <c r="J26" s="99">
         <v>45.0</v>
       </c>
-      <c r="K26" s="61"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="74"/>
-      <c r="N26" s="74"/>
-      <c r="O26" s="74"/>
-      <c r="P26" s="74"/>
-      <c r="Q26" s="74"/>
-      <c r="R26" s="74"/>
-      <c r="S26" s="74"/>
-      <c r="T26" s="74"/>
-      <c r="U26" s="74"/>
-      <c r="V26" s="74"/>
-      <c r="W26" s="74"/>
-      <c r="X26" s="74"/>
-      <c r="Y26" s="74"/>
-      <c r="Z26" s="74"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="75"/>
+      <c r="O26" s="75"/>
+      <c r="P26" s="75"/>
+      <c r="Q26" s="75"/>
+      <c r="R26" s="75"/>
+      <c r="S26" s="75"/>
+      <c r="T26" s="75"/>
+      <c r="U26" s="75"/>
+      <c r="V26" s="75"/>
+      <c r="W26" s="75"/>
+      <c r="X26" s="75"/>
+      <c r="Y26" s="75"/>
+      <c r="Z26" s="75"/>
       <c r="AA26" s="36"/>
     </row>
     <row r="27">
-      <c r="A27" s="74"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="97" t="s">
+      <c r="A27" s="75"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="61"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="82"/>
-      <c r="J27" s="98">
+      <c r="G27" s="62"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="83"/>
+      <c r="J27" s="99">
         <v>25.0</v>
       </c>
-      <c r="K27" s="61"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="74"/>
-      <c r="N27" s="74"/>
-      <c r="O27" s="74"/>
-      <c r="P27" s="74"/>
-      <c r="Q27" s="74"/>
-      <c r="R27" s="74"/>
-      <c r="S27" s="74"/>
-      <c r="T27" s="74"/>
-      <c r="U27" s="74"/>
-      <c r="V27" s="74"/>
-      <c r="W27" s="74"/>
-      <c r="X27" s="74"/>
-      <c r="Y27" s="74"/>
-      <c r="Z27" s="74"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="75"/>
+      <c r="O27" s="75"/>
+      <c r="P27" s="75"/>
+      <c r="Q27" s="75"/>
+      <c r="R27" s="75"/>
+      <c r="S27" s="75"/>
+      <c r="T27" s="75"/>
+      <c r="U27" s="75"/>
+      <c r="V27" s="75"/>
+      <c r="W27" s="75"/>
+      <c r="X27" s="75"/>
+      <c r="Y27" s="75"/>
+      <c r="Z27" s="75"/>
       <c r="AA27" s="36"/>
     </row>
     <row r="28">
-      <c r="A28" s="74"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="99">
+      <c r="A28" s="75"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="100">
         <f>SUM(J25:L27)</f>
         <v>130</v>
       </c>
       <c r="K28" s="23"/>
       <c r="L28" s="23"/>
-      <c r="M28" s="74"/>
-      <c r="N28" s="74"/>
-      <c r="O28" s="74"/>
-      <c r="P28" s="74"/>
-      <c r="Q28" s="74"/>
-      <c r="R28" s="74"/>
-      <c r="S28" s="74"/>
-      <c r="T28" s="74"/>
-      <c r="U28" s="74"/>
-      <c r="V28" s="74"/>
-      <c r="W28" s="74"/>
-      <c r="X28" s="74"/>
-      <c r="Y28" s="74"/>
-      <c r="Z28" s="74"/>
-      <c r="AA28" s="74"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="75"/>
+      <c r="O28" s="75"/>
+      <c r="P28" s="75"/>
+      <c r="Q28" s="75"/>
+      <c r="R28" s="75"/>
+      <c r="S28" s="75"/>
+      <c r="T28" s="75"/>
+      <c r="U28" s="75"/>
+      <c r="V28" s="75"/>
+      <c r="W28" s="75"/>
+      <c r="X28" s="75"/>
+      <c r="Y28" s="75"/>
+      <c r="Z28" s="75"/>
+      <c r="AA28" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5479,272 +5539,272 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="101" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="101" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="101">
+      <c r="B2" s="102">
         <v>11.0</v>
       </c>
-      <c r="C2" s="102">
+      <c r="C2" s="103">
         <v>11.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="101">
+      <c r="B3" s="102">
         <v>5.0</v>
       </c>
-      <c r="C3" s="102"/>
+      <c r="C3" s="103"/>
     </row>
     <row r="4">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="101">
+      <c r="B4" s="102">
         <v>10.0</v>
       </c>
-      <c r="C4" s="102"/>
+      <c r="C4" s="103"/>
     </row>
     <row r="5">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="101">
+      <c r="B5" s="102">
         <v>5.0</v>
       </c>
-      <c r="C5" s="102"/>
+      <c r="C5" s="103"/>
     </row>
     <row r="6">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="101">
+      <c r="B6" s="102">
         <v>18.0</v>
       </c>
-      <c r="C6" s="102">
+      <c r="C6" s="103">
         <v>18.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="100" t="s">
+      <c r="A7" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="103">
+      <c r="B7" s="104">
         <v>11.0</v>
       </c>
-      <c r="C7" s="102">
+      <c r="C7" s="105">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="102">
+        <v>-1.0</v>
+      </c>
+      <c r="C8" s="103"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="101" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="102">
         <v>12.0</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="100" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="101">
-        <v>-1.0</v>
-      </c>
-      <c r="C8" s="102"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="100" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="101">
+      <c r="C9" s="103"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="101" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="102">
+        <v>6.0</v>
+      </c>
+      <c r="C10" s="103"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="102">
+        <v>16.0</v>
+      </c>
+      <c r="C11" s="103"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="101" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="104">
+        <v>6.0</v>
+      </c>
+      <c r="C12" s="105">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="101" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="104">
+        <v>10.0</v>
+      </c>
+      <c r="C13" s="105">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="101" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="104">
+        <v>14.0</v>
+      </c>
+      <c r="C14" s="103"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="101" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="104">
+        <v>19.0</v>
+      </c>
+      <c r="C15" s="103"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="101" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="102">
+        <v>11.0</v>
+      </c>
+      <c r="C16" s="103">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="104">
+        <v>27.0</v>
+      </c>
+      <c r="C17" s="105">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="101" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="104">
         <v>12.0</v>
       </c>
-      <c r="C9" s="102"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="100" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="101">
-        <v>6.0</v>
-      </c>
-      <c r="C10" s="102"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="100" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="101">
-        <v>16.0</v>
-      </c>
-      <c r="C11" s="102"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="100" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="101">
-        <v>5.0</v>
-      </c>
-      <c r="C12" s="102">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="100" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="101">
-        <v>9.0</v>
-      </c>
-      <c r="C13" s="102">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="100" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="101">
-        <v>15.0</v>
-      </c>
-      <c r="C14" s="102"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="100" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="101">
-        <v>18.0</v>
-      </c>
-      <c r="C15" s="102"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="100" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="101">
+      <c r="C18" s="103"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="101" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="102">
+        <v>7.0</v>
+      </c>
+      <c r="C19" s="103"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="101" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="104">
+        <v>7.0</v>
+      </c>
+      <c r="C20" s="105">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="101" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="102">
+        <v>7.0</v>
+      </c>
+      <c r="C21" s="103"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="101" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="102"/>
+      <c r="C22" s="103">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="101" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="102"/>
+      <c r="C23" s="103">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="102"/>
+      <c r="C24" s="105">
         <v>11.0</v>
       </c>
-      <c r="C16" s="102">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="100" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="101">
+    </row>
+    <row r="25">
+      <c r="A25" s="101" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="102"/>
+      <c r="C25" s="105">
         <v>26.0</v>
       </c>
-      <c r="C17" s="102">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="100" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="103">
-        <v>12.0</v>
-      </c>
-      <c r="C18" s="102"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="100" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="101">
-        <v>7.0</v>
-      </c>
-      <c r="C19" s="102"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="100" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="101">
-        <v>6.0</v>
-      </c>
-      <c r="C20" s="102">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="100" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="101">
-        <v>7.0</v>
-      </c>
-      <c r="C21" s="102"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="101"/>
-      <c r="C22" s="102">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="100" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="101"/>
-      <c r="C23" s="102">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="100" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="101"/>
-      <c r="C24" s="102">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="100" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="101"/>
-      <c r="C25" s="102">
-        <v>27.0</v>
-      </c>
     </row>
     <row r="26">
-      <c r="A26" s="100" t="s">
+      <c r="A26" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="101"/>
-      <c r="C26" s="102">
+      <c r="B26" s="102"/>
+      <c r="C26" s="103">
         <v>24.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="100" t="s">
+      <c r="A27" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="101"/>
-      <c r="C27" s="102">
+      <c r="B27" s="102"/>
+      <c r="C27" s="103">
         <v>29.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="100" t="s">
+      <c r="A28" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="101"/>
-      <c r="C28" s="102">
+      <c r="B28" s="102"/>
+      <c r="C28" s="103">
         <v>21.0</v>
       </c>
     </row>
@@ -5764,101 +5824,101 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="101" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="100">
+      <c r="B2" s="101">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="100">
+      <c r="B3" s="101">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="100">
+      <c r="B4" s="101">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="101">
+        <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="106" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="101">
+        <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
         <v>23</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="104" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="100">
-        <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="104" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="100">
-        <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>21</v>
-      </c>
-    </row>
     <row r="7">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="100">
+      <c r="B7" s="101">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
         <v>13</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="100">
+      <c r="B8" s="101">
         <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="100">
+      <c r="B9" s="101">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="100">
+      <c r="B10" s="101">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="100">
+      <c r="B11" s="101">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
032 Week 18/19 update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -310,13 +310,13 @@
     <font>
       <b/>
       <sz val="10.0"/>
-      <color rgb="FFFF9900"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <sz val="10.0"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFF9900"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -872,16 +872,16 @@
     <xf borderId="26" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="26" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="20" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="20" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="20" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="26" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -900,10 +900,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="30" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="20" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="26" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="26" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="31" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1028,14 +1028,14 @@
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1737,7 +1737,9 @@
       <c r="U12" s="32">
         <v>29.0</v>
       </c>
-      <c r="V12" s="31"/>
+      <c r="V12" s="32">
+        <v>30.0</v>
+      </c>
       <c r="W12" s="31"/>
       <c r="X12" s="31"/>
       <c r="Y12" s="31"/>
@@ -1745,11 +1747,11 @@
       <c r="AA12" s="33"/>
       <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>404</v>
+        <v>434</v>
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>778</v>
+        <v>849</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36"/>
@@ -1800,15 +1802,17 @@
       <c r="U13" s="41">
         <v>34.0</v>
       </c>
-      <c r="V13" s="40"/>
+      <c r="V13" s="42">
+        <v>41.0</v>
+      </c>
       <c r="W13" s="40"/>
       <c r="X13" s="40"/>
       <c r="Y13" s="40"/>
-      <c r="Z13" s="42"/>
-      <c r="AA13" s="42"/>
+      <c r="Z13" s="43"/>
+      <c r="AA13" s="43"/>
       <c r="AB13" s="34">
         <f t="shared" si="1"/>
-        <v>374</v>
+        <v>415</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -1837,7 +1841,7 @@
       <c r="L14" s="31"/>
       <c r="M14" s="31"/>
       <c r="N14" s="31"/>
-      <c r="O14" s="43">
+      <c r="O14" s="44">
         <v>38.0</v>
       </c>
       <c r="P14" s="31"/>
@@ -1845,7 +1849,7 @@
       <c r="R14" s="31"/>
       <c r="S14" s="31"/>
       <c r="T14" s="31"/>
-      <c r="U14" s="44">
+      <c r="U14" s="45">
         <v>38.0</v>
       </c>
       <c r="V14" s="31"/>
@@ -1860,7 +1864,7 @@
       </c>
       <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
-        <v>469</v>
+        <v>504</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="36"/>
@@ -1907,15 +1911,17 @@
       <c r="U15" s="41">
         <v>32.0</v>
       </c>
-      <c r="V15" s="40"/>
+      <c r="V15" s="41">
+        <v>35.0</v>
+      </c>
       <c r="W15" s="40"/>
       <c r="X15" s="40"/>
       <c r="Y15" s="40"/>
-      <c r="Z15" s="42"/>
-      <c r="AA15" s="42"/>
+      <c r="Z15" s="43"/>
+      <c r="AA15" s="43"/>
       <c r="AB15" s="34">
         <f t="shared" si="1"/>
-        <v>297</v>
+        <v>332</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
@@ -1973,7 +1979,9 @@
       <c r="U16" s="32">
         <v>25.0</v>
       </c>
-      <c r="V16" s="31"/>
+      <c r="V16" s="32">
+        <v>30.0</v>
+      </c>
       <c r="W16" s="31"/>
       <c r="X16" s="31"/>
       <c r="Y16" s="31"/>
@@ -1981,11 +1989,11 @@
       <c r="AA16" s="33"/>
       <c r="AB16" s="34">
         <f t="shared" si="1"/>
-        <v>406</v>
+        <v>436</v>
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>714</v>
+        <v>744</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36"/>
@@ -2030,7 +2038,7 @@
       <c r="S17" s="40">
         <v>23.0</v>
       </c>
-      <c r="T17" s="45">
+      <c r="T17" s="42">
         <v>39.0</v>
       </c>
       <c r="U17" s="40"/>
@@ -2038,8 +2046,8 @@
       <c r="W17" s="40"/>
       <c r="X17" s="40"/>
       <c r="Y17" s="40"/>
-      <c r="Z17" s="42"/>
-      <c r="AA17" s="42"/>
+      <c r="Z17" s="43"/>
+      <c r="AA17" s="43"/>
       <c r="AB17" s="34">
         <f t="shared" si="1"/>
         <v>308</v>
@@ -2143,8 +2151,8 @@
       <c r="W19" s="40"/>
       <c r="X19" s="40"/>
       <c r="Y19" s="40"/>
-      <c r="Z19" s="42"/>
-      <c r="AA19" s="42"/>
+      <c r="Z19" s="43"/>
+      <c r="AA19" s="43"/>
       <c r="AB19" s="34">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -2201,7 +2209,9 @@
       <c r="U20" s="32">
         <v>32.0</v>
       </c>
-      <c r="V20" s="31"/>
+      <c r="V20" s="32">
+        <v>36.0</v>
+      </c>
       <c r="W20" s="31"/>
       <c r="X20" s="31"/>
       <c r="Y20" s="31"/>
@@ -2209,11 +2219,11 @@
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>403</v>
+        <v>439</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>760</v>
+        <v>826</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36"/>
@@ -2264,15 +2274,17 @@
       <c r="U21" s="41">
         <v>30.0</v>
       </c>
-      <c r="V21" s="40"/>
+      <c r="V21" s="41">
+        <v>30.0</v>
+      </c>
       <c r="W21" s="40"/>
       <c r="X21" s="40"/>
       <c r="Y21" s="40"/>
-      <c r="Z21" s="42"/>
-      <c r="AA21" s="42"/>
+      <c r="Z21" s="43"/>
+      <c r="AA21" s="43"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>357</v>
+        <v>387</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
@@ -2373,8 +2385,8 @@
       <c r="W23" s="40"/>
       <c r="X23" s="40"/>
       <c r="Y23" s="40"/>
-      <c r="Z23" s="42"/>
-      <c r="AA23" s="42"/>
+      <c r="Z23" s="43"/>
+      <c r="AA23" s="43"/>
       <c r="AB23" s="34">
         <f t="shared" si="1"/>
         <v>170</v>
@@ -2431,7 +2443,7 @@
       </c>
       <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
-        <v>541</v>
+        <v>574</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="36"/>
@@ -2482,15 +2494,17 @@
       <c r="U25" s="41">
         <v>35.0</v>
       </c>
-      <c r="V25" s="40"/>
+      <c r="V25" s="41">
+        <v>33.0</v>
+      </c>
       <c r="W25" s="40"/>
       <c r="X25" s="40"/>
       <c r="Y25" s="40"/>
-      <c r="Z25" s="42"/>
-      <c r="AA25" s="42"/>
+      <c r="Z25" s="43"/>
+      <c r="AA25" s="43"/>
       <c r="AB25" s="34">
         <f t="shared" si="1"/>
-        <v>341</v>
+        <v>374</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
@@ -2548,7 +2562,9 @@
       <c r="U26" s="32">
         <v>22.0</v>
       </c>
-      <c r="V26" s="31"/>
+      <c r="V26" s="32">
+        <v>31.0</v>
+      </c>
       <c r="W26" s="31"/>
       <c r="X26" s="31"/>
       <c r="Y26" s="31"/>
@@ -2556,11 +2572,11 @@
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>449</v>
+        <v>480</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>779</v>
+        <v>834</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36"/>
@@ -2611,15 +2627,17 @@
         <v>20.0</v>
       </c>
       <c r="U27" s="40"/>
-      <c r="V27" s="40"/>
+      <c r="V27" s="41">
+        <v>24.0</v>
+      </c>
       <c r="W27" s="40"/>
       <c r="X27" s="40"/>
       <c r="Y27" s="40"/>
-      <c r="Z27" s="42"/>
-      <c r="AA27" s="42"/>
+      <c r="Z27" s="43"/>
+      <c r="AA27" s="43"/>
       <c r="AB27" s="34">
         <f t="shared" si="1"/>
-        <v>330</v>
+        <v>354</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
@@ -2677,7 +2695,9 @@
       <c r="U28" s="32">
         <v>33.0</v>
       </c>
-      <c r="V28" s="31"/>
+      <c r="V28" s="32">
+        <v>32.0</v>
+      </c>
       <c r="W28" s="31"/>
       <c r="X28" s="31"/>
       <c r="Y28" s="31"/>
@@ -2685,11 +2705,11 @@
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>443</v>
+        <v>475</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>955</v>
+        <v>1018</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36"/>
@@ -2748,15 +2768,17 @@
       <c r="U29" s="41">
         <v>36.0</v>
       </c>
-      <c r="V29" s="40"/>
+      <c r="V29" s="41">
+        <v>31.0</v>
+      </c>
       <c r="W29" s="40"/>
       <c r="X29" s="40"/>
       <c r="Y29" s="40"/>
-      <c r="Z29" s="42"/>
-      <c r="AA29" s="42"/>
+      <c r="Z29" s="43"/>
+      <c r="AA29" s="43"/>
       <c r="AB29" s="34">
         <f t="shared" si="1"/>
-        <v>512</v>
+        <v>543</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -2798,7 +2820,9 @@
       <c r="U30" s="32">
         <v>35.0</v>
       </c>
-      <c r="V30" s="31"/>
+      <c r="V30" s="32">
+        <v>33.0</v>
+      </c>
       <c r="W30" s="31"/>
       <c r="X30" s="31"/>
       <c r="Y30" s="31"/>
@@ -2806,11 +2830,11 @@
       <c r="AA30" s="33"/>
       <c r="AB30" s="34">
         <f t="shared" si="1"/>
-        <v>181</v>
+        <v>214</v>
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>553</v>
+        <v>586</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36"/>
@@ -4475,7 +4499,9 @@
       <c r="R5" s="89">
         <v>35.0</v>
       </c>
-      <c r="S5" s="88"/>
+      <c r="S5" s="88">
+        <v>32.0</v>
+      </c>
       <c r="T5" s="86"/>
       <c r="U5" s="86"/>
       <c r="V5" s="86"/>
@@ -4484,7 +4510,7 @@
       <c r="Y5" s="86"/>
       <c r="Z5" s="90">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>452</v>
+        <v>484</v>
       </c>
       <c r="AA5" s="36"/>
     </row>
@@ -4535,7 +4561,9 @@
       <c r="R6" s="88">
         <v>25.0</v>
       </c>
-      <c r="S6" s="88"/>
+      <c r="S6" s="88">
+        <v>31.0</v>
+      </c>
       <c r="T6" s="86"/>
       <c r="U6" s="86"/>
       <c r="V6" s="86"/>
@@ -4544,7 +4572,7 @@
       <c r="Y6" s="86"/>
       <c r="Z6" s="90">
         <f t="shared" si="1"/>
-        <v>429</v>
+        <v>460</v>
       </c>
       <c r="AA6" s="36"/>
     </row>
@@ -4597,7 +4625,9 @@
       <c r="R7" s="88">
         <v>28.0</v>
       </c>
-      <c r="S7" s="88"/>
+      <c r="S7" s="88">
+        <v>30.0</v>
+      </c>
       <c r="T7" s="86"/>
       <c r="U7" s="86"/>
       <c r="V7" s="86"/>
@@ -4606,7 +4636,7 @@
       <c r="Y7" s="86"/>
       <c r="Z7" s="90">
         <f t="shared" si="1"/>
-        <v>421</v>
+        <v>451</v>
       </c>
       <c r="AA7" s="36"/>
     </row>
@@ -4721,7 +4751,9 @@
       <c r="R9" s="88">
         <v>30.0</v>
       </c>
-      <c r="S9" s="88"/>
+      <c r="S9" s="88">
+        <v>29.0</v>
+      </c>
       <c r="T9" s="86"/>
       <c r="U9" s="86"/>
       <c r="V9" s="86"/>
@@ -4730,7 +4762,7 @@
       <c r="Y9" s="86"/>
       <c r="Z9" s="90">
         <f t="shared" si="1"/>
-        <v>420</v>
+        <v>449</v>
       </c>
       <c r="AA9" s="36"/>
     </row>
@@ -4779,7 +4811,9 @@
       <c r="R10" s="88">
         <v>20.0</v>
       </c>
-      <c r="S10" s="88"/>
+      <c r="S10" s="88">
+        <v>26.0</v>
+      </c>
       <c r="T10" s="86"/>
       <c r="U10" s="86"/>
       <c r="V10" s="86"/>
@@ -4788,7 +4822,7 @@
       <c r="Y10" s="86"/>
       <c r="Z10" s="90">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>318</v>
       </c>
       <c r="AA10" s="36"/>
     </row>
@@ -4939,7 +4973,9 @@
       <c r="R13" s="88">
         <v>28.0</v>
       </c>
-      <c r="S13" s="86"/>
+      <c r="S13" s="88">
+        <v>32.0</v>
+      </c>
       <c r="T13" s="86"/>
       <c r="U13" s="86"/>
       <c r="V13" s="86"/>
@@ -4948,7 +4984,7 @@
       <c r="Y13" s="86"/>
       <c r="Z13" s="90">
         <f t="shared" si="1"/>
-        <v>432</v>
+        <v>464</v>
       </c>
       <c r="AA13" s="36"/>
     </row>
@@ -4987,7 +5023,9 @@
       <c r="R14" s="88">
         <v>31.0</v>
       </c>
-      <c r="S14" s="86"/>
+      <c r="S14" s="88">
+        <v>29.0</v>
+      </c>
       <c r="T14" s="86"/>
       <c r="U14" s="86"/>
       <c r="V14" s="86"/>
@@ -4996,7 +5034,7 @@
       <c r="Y14" s="86"/>
       <c r="Z14" s="90">
         <f t="shared" si="1"/>
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="AA14" s="36"/>
     </row>
@@ -5213,7 +5251,9 @@
       <c r="R19" s="88">
         <v>24.0</v>
       </c>
-      <c r="S19" s="86"/>
+      <c r="S19" s="89">
+        <v>40.0</v>
+      </c>
       <c r="T19" s="86"/>
       <c r="U19" s="86"/>
       <c r="V19" s="86"/>
@@ -5222,7 +5262,7 @@
       <c r="Y19" s="86"/>
       <c r="Z19" s="90">
         <f t="shared" si="1"/>
-        <v>172</v>
+        <v>212</v>
       </c>
       <c r="AA19" s="36"/>
     </row>
@@ -5554,10 +5594,10 @@
         <v>29</v>
       </c>
       <c r="B2" s="102">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="C2" s="103">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="3">
@@ -5565,36 +5605,36 @@
         <v>30</v>
       </c>
       <c r="B3" s="102">
-        <v>5.0</v>
-      </c>
-      <c r="C3" s="103"/>
+        <v>4.0</v>
+      </c>
+      <c r="C3" s="104"/>
     </row>
     <row r="4">
       <c r="A4" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="102">
+      <c r="B4" s="105">
         <v>10.0</v>
       </c>
-      <c r="C4" s="103"/>
+      <c r="C4" s="104"/>
     </row>
     <row r="5">
       <c r="A5" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="102">
+      <c r="B5" s="105">
         <v>5.0</v>
       </c>
-      <c r="C5" s="103"/>
+      <c r="C5" s="104"/>
     </row>
     <row r="6">
       <c r="A6" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="102">
+      <c r="B6" s="105">
         <v>18.0</v>
       </c>
-      <c r="C6" s="103">
+      <c r="C6" s="104">
         <v>18.0</v>
       </c>
     </row>
@@ -5602,10 +5642,10 @@
       <c r="A7" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="104">
+      <c r="B7" s="102">
         <v>11.0</v>
       </c>
-      <c r="C7" s="105">
+      <c r="C7" s="103">
         <v>11.0</v>
       </c>
     </row>
@@ -5613,46 +5653,46 @@
       <c r="A8" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="102">
+      <c r="B8" s="105">
         <v>-1.0</v>
       </c>
-      <c r="C8" s="103"/>
+      <c r="C8" s="104"/>
     </row>
     <row r="9">
       <c r="A9" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="102">
+      <c r="B9" s="105">
         <v>12.0</v>
       </c>
-      <c r="C9" s="103"/>
+      <c r="C9" s="104"/>
     </row>
     <row r="10">
       <c r="A10" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="102">
+      <c r="B10" s="105">
         <v>6.0</v>
       </c>
-      <c r="C10" s="103"/>
+      <c r="C10" s="104"/>
     </row>
     <row r="11">
       <c r="A11" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="102">
+      <c r="B11" s="105">
         <v>16.0</v>
       </c>
-      <c r="C11" s="103"/>
+      <c r="C11" s="104"/>
     </row>
     <row r="12">
       <c r="A12" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="104">
+      <c r="B12" s="102">
         <v>6.0</v>
       </c>
-      <c r="C12" s="105">
+      <c r="C12" s="103">
         <v>6.0</v>
       </c>
     </row>
@@ -5660,10 +5700,10 @@
       <c r="A13" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="104">
+      <c r="B13" s="102">
         <v>10.0</v>
       </c>
-      <c r="C13" s="105">
+      <c r="C13" s="103">
         <v>10.0</v>
       </c>
     </row>
@@ -5671,39 +5711,39 @@
       <c r="A14" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="104">
+      <c r="B14" s="102">
         <v>14.0</v>
       </c>
-      <c r="C14" s="103"/>
+      <c r="C14" s="104"/>
     </row>
     <row r="15">
       <c r="A15" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="104">
+      <c r="B15" s="102">
         <v>19.0</v>
       </c>
-      <c r="C15" s="103"/>
+      <c r="C15" s="104"/>
     </row>
     <row r="16">
       <c r="A16" s="101" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="102">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="C16" s="103">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="104">
+      <c r="B17" s="102">
         <v>27.0</v>
       </c>
-      <c r="C17" s="105">
+      <c r="C17" s="103">
         <v>27.0</v>
       </c>
     </row>
@@ -5711,46 +5751,46 @@
       <c r="A18" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="104">
+      <c r="B18" s="102">
         <v>12.0</v>
       </c>
-      <c r="C18" s="103"/>
+      <c r="C18" s="104"/>
     </row>
     <row r="19">
       <c r="A19" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="102">
+      <c r="B19" s="105">
         <v>7.0</v>
       </c>
-      <c r="C19" s="103"/>
+      <c r="C19" s="104"/>
     </row>
     <row r="20">
       <c r="A20" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="104">
-        <v>7.0</v>
-      </c>
-      <c r="C20" s="105">
-        <v>7.0</v>
+      <c r="B20" s="102">
+        <v>6.0</v>
+      </c>
+      <c r="C20" s="103">
+        <v>6.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="102">
+      <c r="B21" s="105">
         <v>7.0</v>
       </c>
-      <c r="C21" s="103"/>
+      <c r="C21" s="104"/>
     </row>
     <row r="22">
       <c r="A22" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="102"/>
-      <c r="C22" s="103">
+      <c r="B22" s="105"/>
+      <c r="C22" s="104">
         <v>13.0</v>
       </c>
     </row>
@@ -5758,8 +5798,8 @@
       <c r="A23" s="101" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="102"/>
-      <c r="C23" s="103">
+      <c r="B23" s="105"/>
+      <c r="C23" s="104">
         <v>12.0</v>
       </c>
     </row>
@@ -5767,8 +5807,8 @@
       <c r="A24" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="102"/>
-      <c r="C24" s="105">
+      <c r="B24" s="105"/>
+      <c r="C24" s="103">
         <v>11.0</v>
       </c>
     </row>
@@ -5776,8 +5816,8 @@
       <c r="A25" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="102"/>
-      <c r="C25" s="105">
+      <c r="B25" s="105"/>
+      <c r="C25" s="103">
         <v>26.0</v>
       </c>
     </row>
@@ -5785,8 +5825,8 @@
       <c r="A26" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="102"/>
-      <c r="C26" s="103">
+      <c r="B26" s="105"/>
+      <c r="C26" s="104">
         <v>24.0</v>
       </c>
     </row>
@@ -5794,8 +5834,8 @@
       <c r="A27" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="102"/>
-      <c r="C27" s="103">
+      <c r="B27" s="105"/>
+      <c r="C27" s="104">
         <v>29.0</v>
       </c>
     </row>
@@ -5803,8 +5843,8 @@
       <c r="A28" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="102"/>
-      <c r="C28" s="103">
+      <c r="B28" s="105"/>
+      <c r="C28" s="104">
         <v>21.0</v>
       </c>
     </row>
@@ -5837,7 +5877,7 @@
       </c>
       <c r="B2" s="101">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
@@ -5846,7 +5886,7 @@
       </c>
       <c r="B3" s="101">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -5855,7 +5895,7 @@
       </c>
       <c r="B4" s="101">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -5873,7 +5913,7 @@
       </c>
       <c r="B6" s="101">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -5891,7 +5931,7 @@
       </c>
       <c r="B8" s="101">
         <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -5900,7 +5940,7 @@
       </c>
       <c r="B9" s="101">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
@@ -5909,7 +5949,7 @@
       </c>
       <c r="B10" s="101">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -5918,7 +5958,7 @@
       </c>
       <c r="B11" s="101">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
035 Week 19/20 update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -1740,18 +1740,20 @@
       <c r="V12" s="32">
         <v>30.0</v>
       </c>
-      <c r="W12" s="31"/>
+      <c r="W12" s="32">
+        <v>33.0</v>
+      </c>
       <c r="X12" s="31"/>
       <c r="Y12" s="31"/>
       <c r="Z12" s="33"/>
       <c r="AA12" s="33"/>
       <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>434</v>
+        <v>467</v>
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>849</v>
+        <v>910</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36"/>
@@ -1805,14 +1807,16 @@
       <c r="V13" s="42">
         <v>41.0</v>
       </c>
-      <c r="W13" s="40"/>
+      <c r="W13" s="41">
+        <v>28.0</v>
+      </c>
       <c r="X13" s="40"/>
       <c r="Y13" s="40"/>
       <c r="Z13" s="43"/>
       <c r="AA13" s="43"/>
       <c r="AB13" s="34">
         <f t="shared" si="1"/>
-        <v>415</v>
+        <v>443</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -1853,18 +1857,20 @@
         <v>38.0</v>
       </c>
       <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
+      <c r="W14" s="32">
+        <v>31.0</v>
+      </c>
       <c r="X14" s="31"/>
       <c r="Y14" s="31"/>
       <c r="Z14" s="33"/>
       <c r="AA14" s="33"/>
       <c r="AB14" s="34">
         <f t="shared" si="1"/>
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
-        <v>504</v>
+        <v>535</v>
       </c>
       <c r="AD14" s="5"/>
       <c r="AE14" s="36"/>
@@ -1982,18 +1988,20 @@
       <c r="V16" s="32">
         <v>30.0</v>
       </c>
-      <c r="W16" s="31"/>
+      <c r="W16" s="32">
+        <v>33.0</v>
+      </c>
       <c r="X16" s="31"/>
       <c r="Y16" s="31"/>
       <c r="Z16" s="33"/>
       <c r="AA16" s="33"/>
       <c r="AB16" s="34">
         <f t="shared" si="1"/>
-        <v>436</v>
+        <v>469</v>
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>744</v>
+        <v>811</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36"/>
@@ -2043,14 +2051,16 @@
       </c>
       <c r="U17" s="40"/>
       <c r="V17" s="40"/>
-      <c r="W17" s="40"/>
+      <c r="W17" s="41">
+        <v>34.0</v>
+      </c>
       <c r="X17" s="40"/>
       <c r="Y17" s="40"/>
       <c r="Z17" s="43"/>
       <c r="AA17" s="43"/>
       <c r="AB17" s="34">
         <f t="shared" si="1"/>
-        <v>308</v>
+        <v>342</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
@@ -2103,18 +2113,20 @@
         <v>30.0</v>
       </c>
       <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
+      <c r="W18" s="32">
+        <v>33.0</v>
+      </c>
       <c r="X18" s="31"/>
       <c r="Y18" s="31"/>
       <c r="Z18" s="33"/>
       <c r="AA18" s="33"/>
       <c r="AB18" s="34">
         <f t="shared" si="1"/>
-        <v>346</v>
+        <v>379</v>
       </c>
       <c r="AC18" s="35">
         <f>SUM(AB18:AB19)</f>
-        <v>407</v>
+        <v>440</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="36"/>
@@ -2212,18 +2224,20 @@
       <c r="V20" s="32">
         <v>36.0</v>
       </c>
-      <c r="W20" s="31"/>
+      <c r="W20" s="32">
+        <v>31.0</v>
+      </c>
       <c r="X20" s="31"/>
       <c r="Y20" s="31"/>
       <c r="Z20" s="33"/>
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>439</v>
+        <v>470</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>826</v>
+        <v>893</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36"/>
@@ -2277,14 +2291,16 @@
       <c r="V21" s="41">
         <v>30.0</v>
       </c>
-      <c r="W21" s="40"/>
+      <c r="W21" s="41">
+        <v>36.0</v>
+      </c>
       <c r="X21" s="40"/>
       <c r="Y21" s="40"/>
       <c r="Z21" s="43"/>
       <c r="AA21" s="43"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>387</v>
+        <v>423</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
@@ -2329,18 +2345,20 @@
       <c r="T22" s="31"/>
       <c r="U22" s="31"/>
       <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
+      <c r="W22" s="32">
+        <v>32.0</v>
+      </c>
       <c r="X22" s="31"/>
       <c r="Y22" s="31"/>
       <c r="Z22" s="33"/>
       <c r="AA22" s="33"/>
       <c r="AB22" s="34">
         <f t="shared" si="1"/>
-        <v>213</v>
+        <v>245</v>
       </c>
       <c r="AC22" s="35">
         <f>SUM(AB22:AB23)</f>
-        <v>383</v>
+        <v>449</v>
       </c>
       <c r="AD22" s="5"/>
       <c r="AE22" s="36"/>
@@ -2382,14 +2400,16 @@
       </c>
       <c r="U23" s="40"/>
       <c r="V23" s="40"/>
-      <c r="W23" s="40"/>
+      <c r="W23" s="41">
+        <v>34.0</v>
+      </c>
       <c r="X23" s="40"/>
       <c r="Y23" s="40"/>
       <c r="Z23" s="43"/>
       <c r="AA23" s="43"/>
       <c r="AB23" s="34">
         <f t="shared" si="1"/>
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="AC23" s="6"/>
       <c r="AD23" s="8"/>
@@ -2432,18 +2452,20 @@
         <v>33.0</v>
       </c>
       <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
+      <c r="W24" s="32">
+        <v>31.0</v>
+      </c>
       <c r="X24" s="31"/>
       <c r="Y24" s="31"/>
       <c r="Z24" s="33"/>
       <c r="AA24" s="33"/>
       <c r="AB24" s="34">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>231</v>
       </c>
       <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
-        <v>574</v>
+        <v>635</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="36"/>
@@ -2497,14 +2519,16 @@
       <c r="V25" s="41">
         <v>33.0</v>
       </c>
-      <c r="W25" s="40"/>
+      <c r="W25" s="41">
+        <v>30.0</v>
+      </c>
       <c r="X25" s="40"/>
       <c r="Y25" s="40"/>
       <c r="Z25" s="43"/>
       <c r="AA25" s="43"/>
       <c r="AB25" s="34">
         <f t="shared" si="1"/>
-        <v>374</v>
+        <v>404</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
@@ -2565,18 +2589,20 @@
       <c r="V26" s="32">
         <v>31.0</v>
       </c>
-      <c r="W26" s="31"/>
+      <c r="W26" s="32">
+        <v>30.0</v>
+      </c>
       <c r="X26" s="31"/>
       <c r="Y26" s="31"/>
       <c r="Z26" s="33"/>
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>510</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>834</v>
+        <v>864</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36"/>
@@ -2709,7 +2735,7 @@
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>1018</v>
+        <v>1054</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36"/>
@@ -2771,14 +2797,16 @@
       <c r="V29" s="41">
         <v>31.0</v>
       </c>
-      <c r="W29" s="40"/>
+      <c r="W29" s="42">
+        <v>36.0</v>
+      </c>
       <c r="X29" s="40"/>
       <c r="Y29" s="40"/>
       <c r="Z29" s="43"/>
       <c r="AA29" s="43"/>
       <c r="AB29" s="34">
         <f t="shared" si="1"/>
-        <v>543</v>
+        <v>579</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
@@ -4564,7 +4592,9 @@
       <c r="S6" s="88">
         <v>31.0</v>
       </c>
-      <c r="T6" s="86"/>
+      <c r="T6" s="89">
+        <v>34.0</v>
+      </c>
       <c r="U6" s="86"/>
       <c r="V6" s="86"/>
       <c r="W6" s="86"/>
@@ -4572,7 +4602,7 @@
       <c r="Y6" s="86"/>
       <c r="Z6" s="90">
         <f t="shared" si="1"/>
-        <v>460</v>
+        <v>494</v>
       </c>
       <c r="AA6" s="36"/>
     </row>
@@ -4754,7 +4784,9 @@
       <c r="S9" s="88">
         <v>29.0</v>
       </c>
-      <c r="T9" s="86"/>
+      <c r="T9" s="88">
+        <v>22.0</v>
+      </c>
       <c r="U9" s="86"/>
       <c r="V9" s="86"/>
       <c r="W9" s="86"/>
@@ -4762,7 +4794,7 @@
       <c r="Y9" s="86"/>
       <c r="Z9" s="90">
         <f t="shared" si="1"/>
-        <v>449</v>
+        <v>471</v>
       </c>
       <c r="AA9" s="36"/>
     </row>
@@ -5084,7 +5116,9 @@
         <v>28.0</v>
       </c>
       <c r="S15" s="86"/>
-      <c r="T15" s="86"/>
+      <c r="T15" s="88">
+        <v>25.0</v>
+      </c>
       <c r="U15" s="86"/>
       <c r="V15" s="86"/>
       <c r="W15" s="86"/>
@@ -5092,7 +5126,7 @@
       <c r="Y15" s="86"/>
       <c r="Z15" s="90">
         <f t="shared" si="1"/>
-        <v>375</v>
+        <v>400</v>
       </c>
       <c r="AA15" s="36"/>
     </row>
@@ -5671,8 +5705,8 @@
       <c r="A10" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="105">
-        <v>6.0</v>
+      <c r="B10" s="102">
+        <v>7.0</v>
       </c>
       <c r="C10" s="104"/>
     </row>
@@ -5877,7 +5911,7 @@
       </c>
       <c r="B2" s="101">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -5886,7 +5920,7 @@
       </c>
       <c r="B3" s="101">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -5895,7 +5929,7 @@
       </c>
       <c r="B4" s="101">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -5904,7 +5938,7 @@
       </c>
       <c r="B5" s="101">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -5913,7 +5947,7 @@
       </c>
       <c r="B6" s="101">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -5922,7 +5956,7 @@
       </c>
       <c r="B7" s="101">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -5931,7 +5965,7 @@
       </c>
       <c r="B8" s="101">
         <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -5940,7 +5974,7 @@
       </c>
       <c r="B9" s="101">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -5949,7 +5983,7 @@
       </c>
       <c r="B10" s="101">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
036 Week 20/21 Update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -1743,17 +1743,19 @@
       <c r="W12" s="32">
         <v>33.0</v>
       </c>
-      <c r="X12" s="31"/>
+      <c r="X12" s="32">
+        <v>33.0</v>
+      </c>
       <c r="Y12" s="31"/>
       <c r="Z12" s="33"/>
       <c r="AA12" s="33"/>
       <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
-        <v>467</v>
+        <v>500</v>
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>910</v>
+        <v>974</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36"/>
@@ -1810,13 +1812,15 @@
       <c r="W13" s="41">
         <v>28.0</v>
       </c>
-      <c r="X13" s="40"/>
+      <c r="X13" s="41">
+        <v>31.0</v>
+      </c>
       <c r="Y13" s="40"/>
       <c r="Z13" s="43"/>
       <c r="AA13" s="43"/>
       <c r="AB13" s="34">
         <f t="shared" si="1"/>
-        <v>443</v>
+        <v>474</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -2227,17 +2231,19 @@
       <c r="W20" s="32">
         <v>31.0</v>
       </c>
-      <c r="X20" s="31"/>
+      <c r="X20" s="32">
+        <v>29.0</v>
+      </c>
       <c r="Y20" s="31"/>
       <c r="Z20" s="33"/>
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>470</v>
+        <v>499</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>893</v>
+        <v>955</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36"/>
@@ -2294,13 +2300,15 @@
       <c r="W21" s="41">
         <v>36.0</v>
       </c>
-      <c r="X21" s="40"/>
+      <c r="X21" s="41">
+        <v>33.0</v>
+      </c>
       <c r="Y21" s="40"/>
       <c r="Z21" s="43"/>
       <c r="AA21" s="43"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>423</v>
+        <v>456</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
@@ -2348,17 +2356,19 @@
       <c r="W22" s="32">
         <v>32.0</v>
       </c>
-      <c r="X22" s="31"/>
+      <c r="X22" s="32">
+        <v>32.0</v>
+      </c>
       <c r="Y22" s="31"/>
       <c r="Z22" s="33"/>
       <c r="AA22" s="33"/>
       <c r="AB22" s="34">
         <f t="shared" si="1"/>
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="AC22" s="35">
         <f>SUM(AB22:AB23)</f>
-        <v>449</v>
+        <v>481</v>
       </c>
       <c r="AD22" s="5"/>
       <c r="AE22" s="36"/>
@@ -2592,17 +2602,19 @@
       <c r="W26" s="32">
         <v>30.0</v>
       </c>
-      <c r="X26" s="31"/>
+      <c r="X26" s="32">
+        <v>35.0</v>
+      </c>
       <c r="Y26" s="31"/>
       <c r="Z26" s="33"/>
       <c r="AA26" s="33"/>
       <c r="AB26" s="34">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>545</v>
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>864</v>
+        <v>934</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36"/>
@@ -2657,13 +2669,15 @@
         <v>24.0</v>
       </c>
       <c r="W27" s="40"/>
-      <c r="X27" s="40"/>
+      <c r="X27" s="41">
+        <v>35.0</v>
+      </c>
       <c r="Y27" s="40"/>
       <c r="Z27" s="43"/>
       <c r="AA27" s="43"/>
       <c r="AB27" s="34">
         <f t="shared" si="1"/>
-        <v>354</v>
+        <v>389</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
@@ -2725,17 +2739,19 @@
         <v>32.0</v>
       </c>
       <c r="W28" s="31"/>
-      <c r="X28" s="31"/>
+      <c r="X28" s="45">
+        <v>35.0</v>
+      </c>
       <c r="Y28" s="31"/>
       <c r="Z28" s="33"/>
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>475</v>
+        <v>510</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>1054</v>
+        <v>1089</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36"/>
@@ -2862,7 +2878,7 @@
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>586</v>
+        <v>615</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36"/>
@@ -2917,13 +2933,15 @@
       </c>
       <c r="V31" s="40"/>
       <c r="W31" s="40"/>
-      <c r="X31" s="40"/>
+      <c r="X31" s="41">
+        <v>29.0</v>
+      </c>
       <c r="Y31" s="40"/>
       <c r="Z31" s="56"/>
       <c r="AA31" s="56"/>
       <c r="AB31" s="57">
         <f t="shared" si="1"/>
-        <v>372</v>
+        <v>401</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
@@ -4531,14 +4549,16 @@
         <v>33.0</v>
       </c>
       <c r="T5" s="86"/>
-      <c r="U5" s="86"/>
+      <c r="U5" s="89">
+        <v>37.0</v>
+      </c>
       <c r="V5" s="86"/>
       <c r="W5" s="86"/>
       <c r="X5" s="86"/>
       <c r="Y5" s="86"/>
       <c r="Z5" s="90">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>485</v>
+        <v>522</v>
       </c>
       <c r="AA5" s="36"/>
     </row>
@@ -4595,14 +4615,16 @@
       <c r="T6" s="89">
         <v>34.0</v>
       </c>
-      <c r="U6" s="86"/>
+      <c r="U6" s="88">
+        <v>32.0</v>
+      </c>
       <c r="V6" s="86"/>
       <c r="W6" s="86"/>
       <c r="X6" s="86"/>
       <c r="Y6" s="86"/>
       <c r="Z6" s="90">
         <f t="shared" si="1"/>
-        <v>494</v>
+        <v>526</v>
       </c>
       <c r="AA6" s="36"/>
     </row>
@@ -4659,14 +4681,16 @@
         <v>30.0</v>
       </c>
       <c r="T7" s="86"/>
-      <c r="U7" s="86"/>
+      <c r="U7" s="88">
+        <v>27.0</v>
+      </c>
       <c r="V7" s="86"/>
       <c r="W7" s="86"/>
       <c r="X7" s="86"/>
       <c r="Y7" s="86"/>
       <c r="Z7" s="90">
         <f t="shared" si="1"/>
-        <v>451</v>
+        <v>478</v>
       </c>
       <c r="AA7" s="36"/>
     </row>
@@ -4947,14 +4971,16 @@
       </c>
       <c r="S12" s="86"/>
       <c r="T12" s="86"/>
-      <c r="U12" s="86"/>
+      <c r="U12" s="88">
+        <v>32.0</v>
+      </c>
       <c r="V12" s="86"/>
       <c r="W12" s="86"/>
       <c r="X12" s="86"/>
       <c r="Y12" s="86"/>
       <c r="Z12" s="90">
         <f t="shared" si="1"/>
-        <v>349</v>
+        <v>381</v>
       </c>
       <c r="AA12" s="36"/>
     </row>
@@ -5009,14 +5035,16 @@
         <v>32.0</v>
       </c>
       <c r="T13" s="86"/>
-      <c r="U13" s="86"/>
+      <c r="U13" s="88">
+        <v>34.0</v>
+      </c>
       <c r="V13" s="86"/>
       <c r="W13" s="86"/>
       <c r="X13" s="86"/>
       <c r="Y13" s="86"/>
       <c r="Z13" s="90">
         <f t="shared" si="1"/>
-        <v>464</v>
+        <v>498</v>
       </c>
       <c r="AA13" s="36"/>
     </row>
@@ -5119,14 +5147,16 @@
       <c r="T15" s="88">
         <v>25.0</v>
       </c>
-      <c r="U15" s="86"/>
+      <c r="U15" s="88">
+        <v>23.0</v>
+      </c>
       <c r="V15" s="86"/>
       <c r="W15" s="86"/>
       <c r="X15" s="86"/>
       <c r="Y15" s="86"/>
       <c r="Z15" s="90">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="AA15" s="36"/>
     </row>
@@ -5171,14 +5201,16 @@
       </c>
       <c r="S16" s="86"/>
       <c r="T16" s="86"/>
-      <c r="U16" s="86"/>
+      <c r="U16" s="88">
+        <v>27.0</v>
+      </c>
       <c r="V16" s="86"/>
       <c r="W16" s="86"/>
       <c r="X16" s="86"/>
       <c r="Y16" s="86"/>
       <c r="Z16" s="90">
         <f t="shared" si="1"/>
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="AA16" s="36"/>
     </row>
@@ -5677,10 +5709,10 @@
         <v>34</v>
       </c>
       <c r="B7" s="102">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="C7" s="103">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="8">
@@ -5911,7 +5943,7 @@
       </c>
       <c r="B2" s="101">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -5947,7 +5979,7 @@
       </c>
       <c r="B6" s="101">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -5956,7 +5988,7 @@
       </c>
       <c r="B7" s="101">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -5974,7 +6006,7 @@
       </c>
       <c r="B9" s="101">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -5983,7 +6015,7 @@
       </c>
       <c r="B10" s="101">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
@@ -5992,7 +6024,7 @@
       </c>
       <c r="B11" s="101">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
037 Week 21/22 Update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -1755,7 +1755,7 @@
       </c>
       <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
-        <v>974</v>
+        <v>1010</v>
       </c>
       <c r="AD12" s="5"/>
       <c r="AE12" s="36"/>
@@ -1815,12 +1815,14 @@
       <c r="X13" s="41">
         <v>31.0</v>
       </c>
-      <c r="Y13" s="40"/>
+      <c r="Y13" s="42">
+        <v>36.0</v>
+      </c>
       <c r="Z13" s="43"/>
       <c r="AA13" s="43"/>
       <c r="AB13" s="34">
         <f t="shared" si="1"/>
-        <v>474</v>
+        <v>510</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
@@ -2005,7 +2007,7 @@
       </c>
       <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
-        <v>811</v>
+        <v>841</v>
       </c>
       <c r="AD16" s="5"/>
       <c r="AE16" s="36"/>
@@ -2059,12 +2061,14 @@
         <v>34.0</v>
       </c>
       <c r="X17" s="40"/>
-      <c r="Y17" s="40"/>
+      <c r="Y17" s="41">
+        <v>30.0</v>
+      </c>
       <c r="Z17" s="43"/>
       <c r="AA17" s="43"/>
       <c r="AB17" s="34">
         <f t="shared" si="1"/>
-        <v>342</v>
+        <v>372</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
@@ -2121,16 +2125,18 @@
         <v>33.0</v>
       </c>
       <c r="X18" s="31"/>
-      <c r="Y18" s="31"/>
+      <c r="Y18" s="32">
+        <v>31.0</v>
+      </c>
       <c r="Z18" s="33"/>
       <c r="AA18" s="33"/>
       <c r="AB18" s="34">
         <f t="shared" si="1"/>
-        <v>379</v>
+        <v>410</v>
       </c>
       <c r="AC18" s="35">
         <f>SUM(AB18:AB19)</f>
-        <v>440</v>
+        <v>499</v>
       </c>
       <c r="AD18" s="5"/>
       <c r="AE18" s="36"/>
@@ -2166,12 +2172,14 @@
       <c r="V19" s="40"/>
       <c r="W19" s="40"/>
       <c r="X19" s="40"/>
-      <c r="Y19" s="40"/>
+      <c r="Y19" s="41">
+        <v>28.0</v>
+      </c>
       <c r="Z19" s="43"/>
       <c r="AA19" s="43"/>
       <c r="AB19" s="34">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="AC19" s="6"/>
       <c r="AD19" s="8"/>
@@ -2234,16 +2242,18 @@
       <c r="X20" s="32">
         <v>29.0</v>
       </c>
-      <c r="Y20" s="31"/>
+      <c r="Y20" s="32">
+        <v>32.0</v>
+      </c>
       <c r="Z20" s="33"/>
       <c r="AA20" s="33"/>
       <c r="AB20" s="34">
         <f t="shared" si="1"/>
-        <v>499</v>
+        <v>531</v>
       </c>
       <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
-        <v>955</v>
+        <v>1022</v>
       </c>
       <c r="AD20" s="5"/>
       <c r="AE20" s="36"/>
@@ -2303,12 +2313,14 @@
       <c r="X21" s="41">
         <v>33.0</v>
       </c>
-      <c r="Y21" s="40"/>
+      <c r="Y21" s="41">
+        <v>35.0</v>
+      </c>
       <c r="Z21" s="43"/>
       <c r="AA21" s="43"/>
       <c r="AB21" s="34">
         <f t="shared" si="1"/>
-        <v>456</v>
+        <v>491</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
@@ -2614,7 +2626,7 @@
       </c>
       <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
-        <v>934</v>
+        <v>959</v>
       </c>
       <c r="AD26" s="5"/>
       <c r="AE26" s="36"/>
@@ -2672,12 +2684,14 @@
       <c r="X27" s="41">
         <v>35.0</v>
       </c>
-      <c r="Y27" s="40"/>
+      <c r="Y27" s="41">
+        <v>25.0</v>
+      </c>
       <c r="Z27" s="43"/>
       <c r="AA27" s="43"/>
       <c r="AB27" s="34">
         <f t="shared" si="1"/>
-        <v>389</v>
+        <v>414</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
@@ -2742,16 +2756,18 @@
       <c r="X28" s="45">
         <v>35.0</v>
       </c>
-      <c r="Y28" s="31"/>
+      <c r="Y28" s="32">
+        <v>35.0</v>
+      </c>
       <c r="Z28" s="33"/>
       <c r="AA28" s="33"/>
       <c r="AB28" s="34">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>545</v>
       </c>
       <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
-        <v>1089</v>
+        <v>1124</v>
       </c>
       <c r="AD28" s="5"/>
       <c r="AE28" s="36"/>
@@ -2878,7 +2894,7 @@
       </c>
       <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
-        <v>615</v>
+        <v>648</v>
       </c>
       <c r="AD30" s="5"/>
       <c r="AE30" s="36"/>
@@ -2936,12 +2952,14 @@
       <c r="X31" s="41">
         <v>29.0</v>
       </c>
-      <c r="Y31" s="40"/>
+      <c r="Y31" s="41">
+        <v>33.0</v>
+      </c>
       <c r="Z31" s="56"/>
       <c r="AA31" s="56"/>
       <c r="AB31" s="57">
         <f t="shared" si="1"/>
-        <v>401</v>
+        <v>434</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
@@ -4684,13 +4702,15 @@
       <c r="U7" s="88">
         <v>27.0</v>
       </c>
-      <c r="V7" s="86"/>
+      <c r="V7" s="89">
+        <v>35.0</v>
+      </c>
       <c r="W7" s="86"/>
       <c r="X7" s="86"/>
       <c r="Y7" s="86"/>
       <c r="Z7" s="90">
         <f t="shared" si="1"/>
-        <v>478</v>
+        <v>513</v>
       </c>
       <c r="AA7" s="36"/>
     </row>
@@ -4872,13 +4892,15 @@
       </c>
       <c r="T10" s="86"/>
       <c r="U10" s="86"/>
-      <c r="V10" s="86"/>
+      <c r="V10" s="88">
+        <v>30.0</v>
+      </c>
       <c r="W10" s="86"/>
       <c r="X10" s="86"/>
       <c r="Y10" s="86"/>
       <c r="Z10" s="90">
         <f t="shared" si="1"/>
-        <v>318</v>
+        <v>348</v>
       </c>
       <c r="AA10" s="36"/>
     </row>
@@ -4974,13 +4996,15 @@
       <c r="U12" s="88">
         <v>32.0</v>
       </c>
-      <c r="V12" s="86"/>
+      <c r="V12" s="88">
+        <v>27.0</v>
+      </c>
       <c r="W12" s="86"/>
       <c r="X12" s="86"/>
       <c r="Y12" s="86"/>
       <c r="Z12" s="90">
         <f t="shared" si="1"/>
-        <v>381</v>
+        <v>408</v>
       </c>
       <c r="AA12" s="36"/>
     </row>
@@ -5204,13 +5228,15 @@
       <c r="U16" s="88">
         <v>27.0</v>
       </c>
-      <c r="V16" s="86"/>
+      <c r="V16" s="88">
+        <v>27.0</v>
+      </c>
       <c r="W16" s="86"/>
       <c r="X16" s="86"/>
       <c r="Y16" s="86"/>
       <c r="Z16" s="90">
         <f t="shared" si="1"/>
-        <v>288</v>
+        <v>315</v>
       </c>
       <c r="AA16" s="36"/>
     </row>
@@ -5660,10 +5686,10 @@
         <v>29</v>
       </c>
       <c r="B2" s="102">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="C2" s="103">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="3">
@@ -5943,7 +5969,7 @@
       </c>
       <c r="B2" s="101">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -5961,7 +5987,7 @@
       </c>
       <c r="B4" s="101">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -5970,7 +5996,7 @@
       </c>
       <c r="B5" s="101">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
@@ -5979,7 +6005,7 @@
       </c>
       <c r="B6" s="101">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
@@ -6006,7 +6032,7 @@
       </c>
       <c r="B9" s="101">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
@@ -6015,7 +6041,7 @@
       </c>
       <c r="B10" s="101">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -6024,7 +6050,7 @@
       </c>
       <c r="B11" s="101">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
038 Week 22/23 data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -781,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="111">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -850,6 +850,9 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="21" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="21" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -875,6 +878,9 @@
     <xf borderId="26" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="11" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -882,6 +888,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="20" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -905,6 +914,9 @@
     </xf>
     <xf borderId="26" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="31" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="31" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -1747,86 +1759,90 @@
         <v>33.0</v>
       </c>
       <c r="Y12" s="31"/>
-      <c r="Z12" s="33"/>
-      <c r="AA12" s="33"/>
-      <c r="AB12" s="34">
+      <c r="Z12" s="33">
+        <v>35.0</v>
+      </c>
+      <c r="AA12" s="34"/>
+      <c r="AB12" s="35">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
         <v>500</v>
       </c>
-      <c r="AC12" s="35">
+      <c r="AC12" s="36">
         <f>SUM(AB12:AB13)</f>
         <v>1010</v>
       </c>
       <c r="AD12" s="5"/>
-      <c r="AE12" s="36"/>
+      <c r="AE12" s="37"/>
     </row>
     <row r="13">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40">
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41">
         <v>32.0</v>
       </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40">
+      <c r="E13" s="41"/>
+      <c r="F13" s="41">
         <v>35.0</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="41">
         <v>35.0</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="41">
         <v>31.0</v>
       </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="40">
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41">
         <v>34.0</v>
       </c>
-      <c r="O13" s="40">
+      <c r="O13" s="41">
         <v>36.0</v>
       </c>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40">
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41">
         <v>32.0</v>
       </c>
-      <c r="R13" s="40">
+      <c r="R13" s="41">
         <v>36.0</v>
       </c>
-      <c r="S13" s="40">
+      <c r="S13" s="41">
         <v>35.0</v>
       </c>
-      <c r="T13" s="41">
+      <c r="T13" s="42">
         <v>34.0</v>
       </c>
-      <c r="U13" s="41">
+      <c r="U13" s="42">
         <v>34.0</v>
       </c>
-      <c r="V13" s="42">
+      <c r="V13" s="43">
         <v>41.0</v>
       </c>
-      <c r="W13" s="41">
+      <c r="W13" s="42">
         <v>28.0</v>
       </c>
-      <c r="X13" s="41">
+      <c r="X13" s="42">
         <v>31.0</v>
       </c>
-      <c r="Y13" s="42">
+      <c r="Y13" s="43">
         <v>36.0</v>
       </c>
-      <c r="Z13" s="43"/>
-      <c r="AA13" s="43"/>
-      <c r="AB13" s="34">
+      <c r="Z13" s="44">
+        <v>39.0</v>
+      </c>
+      <c r="AA13" s="45"/>
+      <c r="AB13" s="35">
         <f t="shared" si="1"/>
         <v>510</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
-      <c r="AE13" s="36"/>
+      <c r="AE13" s="37"/>
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
@@ -1851,7 +1867,7 @@
       <c r="L14" s="31"/>
       <c r="M14" s="31"/>
       <c r="N14" s="31"/>
-      <c r="O14" s="44">
+      <c r="O14" s="46">
         <v>38.0</v>
       </c>
       <c r="P14" s="31"/>
@@ -1859,7 +1875,7 @@
       <c r="R14" s="31"/>
       <c r="S14" s="31"/>
       <c r="T14" s="31"/>
-      <c r="U14" s="45">
+      <c r="U14" s="47">
         <v>38.0</v>
       </c>
       <c r="V14" s="31"/>
@@ -1868,76 +1884,76 @@
       </c>
       <c r="X14" s="31"/>
       <c r="Y14" s="31"/>
-      <c r="Z14" s="33"/>
-      <c r="AA14" s="33"/>
-      <c r="AB14" s="34">
+      <c r="Z14" s="34"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="35">
         <f t="shared" si="1"/>
         <v>203</v>
       </c>
-      <c r="AC14" s="35">
+      <c r="AC14" s="36">
         <f>SUM(AB14:AB15)</f>
         <v>535</v>
       </c>
       <c r="AD14" s="5"/>
-      <c r="AE14" s="36"/>
+      <c r="AE14" s="37"/>
     </row>
     <row r="15">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40">
+      <c r="B15" s="39"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="41">
         <v>37.0</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40">
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41">
         <v>31.0</v>
       </c>
-      <c r="H15" s="40">
+      <c r="H15" s="41">
         <v>38.0</v>
       </c>
-      <c r="I15" s="40">
+      <c r="I15" s="41">
         <v>30.0</v>
       </c>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40">
+      <c r="J15" s="41"/>
+      <c r="K15" s="41">
         <v>36.0</v>
       </c>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40">
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41">
         <v>32.0</v>
       </c>
-      <c r="O15" s="40">
+      <c r="O15" s="41">
         <v>33.0</v>
       </c>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40">
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41">
         <v>28.0</v>
       </c>
-      <c r="S15" s="40"/>
-      <c r="T15" s="40"/>
-      <c r="U15" s="41">
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="42">
         <v>32.0</v>
       </c>
-      <c r="V15" s="41">
+      <c r="V15" s="42">
         <v>35.0</v>
       </c>
-      <c r="W15" s="40"/>
-      <c r="X15" s="40"/>
-      <c r="Y15" s="40"/>
-      <c r="Z15" s="43"/>
-      <c r="AA15" s="43"/>
-      <c r="AB15" s="34">
+      <c r="W15" s="41"/>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="45"/>
+      <c r="AA15" s="45"/>
+      <c r="AB15" s="35">
         <f t="shared" si="1"/>
         <v>332</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
-      <c r="AE15" s="36"/>
+      <c r="AE15" s="37"/>
     </row>
     <row r="16">
       <c r="A16" s="28" t="s">
@@ -1999,80 +2015,84 @@
       </c>
       <c r="X16" s="31"/>
       <c r="Y16" s="31"/>
-      <c r="Z16" s="33"/>
-      <c r="AA16" s="33"/>
-      <c r="AB16" s="34">
+      <c r="Z16" s="33">
+        <v>33.0</v>
+      </c>
+      <c r="AA16" s="34"/>
+      <c r="AB16" s="35">
         <f t="shared" si="1"/>
         <v>469</v>
       </c>
-      <c r="AC16" s="35">
+      <c r="AC16" s="36">
         <f>SUM(AB16:AB17)</f>
         <v>841</v>
       </c>
       <c r="AD16" s="5"/>
-      <c r="AE16" s="36"/>
+      <c r="AE16" s="37"/>
     </row>
     <row r="17">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40">
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41">
         <v>31.0</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40">
+      <c r="E17" s="41"/>
+      <c r="F17" s="41">
         <v>32.0</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="41">
         <v>26.0</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17" s="41">
         <v>32.0</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I17" s="41">
         <v>34.0</v>
       </c>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40">
+      <c r="J17" s="41"/>
+      <c r="K17" s="41">
         <v>31.0</v>
       </c>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40">
+      <c r="L17" s="41"/>
+      <c r="M17" s="41">
         <v>25.0</v>
       </c>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40">
+      <c r="N17" s="41"/>
+      <c r="O17" s="41">
         <v>35.0</v>
       </c>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="40">
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41">
         <v>23.0</v>
       </c>
-      <c r="T17" s="42">
+      <c r="T17" s="43">
         <v>39.0</v>
       </c>
-      <c r="U17" s="40"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="41">
+      <c r="U17" s="41"/>
+      <c r="V17" s="41"/>
+      <c r="W17" s="42">
         <v>34.0</v>
       </c>
-      <c r="X17" s="40"/>
-      <c r="Y17" s="41">
+      <c r="X17" s="41"/>
+      <c r="Y17" s="42">
         <v>30.0</v>
       </c>
-      <c r="Z17" s="43"/>
-      <c r="AA17" s="43"/>
-      <c r="AB17" s="34">
+      <c r="Z17" s="48">
+        <v>29.0</v>
+      </c>
+      <c r="AA17" s="45"/>
+      <c r="AB17" s="35">
         <f t="shared" si="1"/>
         <v>372</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
-      <c r="AE17" s="36"/>
+      <c r="AE17" s="37"/>
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
@@ -2128,70 +2148,74 @@
       <c r="Y18" s="32">
         <v>31.0</v>
       </c>
-      <c r="Z18" s="33"/>
-      <c r="AA18" s="33"/>
-      <c r="AB18" s="34">
+      <c r="Z18" s="33">
+        <v>36.0</v>
+      </c>
+      <c r="AA18" s="34"/>
+      <c r="AB18" s="35">
         <f t="shared" si="1"/>
         <v>410</v>
       </c>
-      <c r="AC18" s="35">
+      <c r="AC18" s="36">
         <f>SUM(AB18:AB19)</f>
         <v>499</v>
       </c>
       <c r="AD18" s="5"/>
-      <c r="AE18" s="36"/>
+      <c r="AE18" s="37"/>
     </row>
     <row r="19">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40">
+      <c r="B19" s="39"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41">
         <v>28.0</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40">
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41">
         <v>33.0</v>
       </c>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="40"/>
-      <c r="T19" s="40"/>
-      <c r="U19" s="40"/>
-      <c r="V19" s="40"/>
-      <c r="W19" s="40"/>
-      <c r="X19" s="40"/>
-      <c r="Y19" s="41">
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="41"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="42">
         <v>28.0</v>
       </c>
-      <c r="Z19" s="43"/>
-      <c r="AA19" s="43"/>
-      <c r="AB19" s="34">
+      <c r="Z19" s="48">
+        <v>24.0</v>
+      </c>
+      <c r="AA19" s="45"/>
+      <c r="AB19" s="35">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="AC19" s="6"/>
       <c r="AD19" s="8"/>
-      <c r="AE19" s="36"/>
+      <c r="AE19" s="37"/>
     </row>
     <row r="20">
       <c r="A20" s="28" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="29"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="31">
         <v>32.0</v>
       </c>
@@ -2245,92 +2269,96 @@
       <c r="Y20" s="32">
         <v>32.0</v>
       </c>
-      <c r="Z20" s="33"/>
-      <c r="AA20" s="33"/>
-      <c r="AB20" s="34">
+      <c r="Z20" s="33">
+        <v>28.0</v>
+      </c>
+      <c r="AA20" s="34"/>
+      <c r="AB20" s="35">
         <f t="shared" si="1"/>
         <v>531</v>
       </c>
-      <c r="AC20" s="35">
+      <c r="AC20" s="36">
         <f>SUM(AB20:AB21)</f>
         <v>1022</v>
       </c>
       <c r="AD20" s="5"/>
-      <c r="AE20" s="36"/>
+      <c r="AE20" s="37"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49">
+      <c r="B21" s="39"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52">
         <v>36.0</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="41">
         <v>39.0</v>
       </c>
-      <c r="F21" s="40">
+      <c r="F21" s="41">
         <v>33.0</v>
       </c>
-      <c r="G21" s="40">
+      <c r="G21" s="41">
         <v>29.0</v>
       </c>
-      <c r="H21" s="40">
+      <c r="H21" s="41">
         <v>32.0</v>
       </c>
-      <c r="I21" s="40">
+      <c r="I21" s="41">
         <v>31.0</v>
       </c>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40">
+      <c r="J21" s="41"/>
+      <c r="K21" s="41">
         <v>42.0</v>
       </c>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40">
+      <c r="L21" s="41"/>
+      <c r="M21" s="41">
         <v>31.0</v>
       </c>
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="40">
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41">
         <v>28.0</v>
       </c>
-      <c r="R21" s="40">
+      <c r="R21" s="41">
         <v>26.0</v>
       </c>
-      <c r="S21" s="40"/>
-      <c r="T21" s="40"/>
-      <c r="U21" s="41">
+      <c r="S21" s="41"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="42">
         <v>30.0</v>
       </c>
-      <c r="V21" s="41">
+      <c r="V21" s="42">
         <v>30.0</v>
       </c>
-      <c r="W21" s="41">
+      <c r="W21" s="42">
         <v>36.0</v>
       </c>
-      <c r="X21" s="41">
+      <c r="X21" s="42">
         <v>33.0</v>
       </c>
-      <c r="Y21" s="41">
+      <c r="Y21" s="42">
         <v>35.0</v>
       </c>
-      <c r="Z21" s="43"/>
-      <c r="AA21" s="43"/>
-      <c r="AB21" s="34">
+      <c r="Z21" s="48">
+        <v>38.0</v>
+      </c>
+      <c r="AA21" s="45"/>
+      <c r="AB21" s="35">
         <f t="shared" si="1"/>
         <v>491</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
-      <c r="AE21" s="36"/>
+      <c r="AE21" s="37"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="51"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="21"/>
       <c r="D22" s="31">
         <v>33.0</v>
@@ -2372,70 +2400,70 @@
         <v>32.0</v>
       </c>
       <c r="Y22" s="31"/>
-      <c r="Z22" s="33"/>
-      <c r="AA22" s="33"/>
-      <c r="AB22" s="34">
+      <c r="Z22" s="34"/>
+      <c r="AA22" s="34"/>
+      <c r="AB22" s="35">
         <f t="shared" si="1"/>
         <v>277</v>
       </c>
-      <c r="AC22" s="35">
+      <c r="AC22" s="36">
         <f>SUM(AB22:AB23)</f>
         <v>481</v>
       </c>
       <c r="AD22" s="5"/>
-      <c r="AE22" s="36"/>
+      <c r="AE22" s="37"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="55" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="40">
+      <c r="C23" s="56"/>
+      <c r="D23" s="41">
         <v>25.0</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40">
+      <c r="E23" s="41"/>
+      <c r="F23" s="41">
         <v>30.0</v>
       </c>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40">
+      <c r="G23" s="41"/>
+      <c r="H23" s="41">
         <v>28.0</v>
       </c>
-      <c r="I23" s="40">
+      <c r="I23" s="41">
         <v>27.0</v>
       </c>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40">
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41">
         <v>34.0</v>
       </c>
-      <c r="P23" s="40"/>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="40"/>
-      <c r="S23" s="40"/>
-      <c r="T23" s="41">
+      <c r="P23" s="41"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="42">
         <v>26.0</v>
       </c>
-      <c r="U23" s="40"/>
-      <c r="V23" s="40"/>
-      <c r="W23" s="41">
+      <c r="U23" s="41"/>
+      <c r="V23" s="41"/>
+      <c r="W23" s="42">
         <v>34.0</v>
       </c>
-      <c r="X23" s="40"/>
-      <c r="Y23" s="40"/>
-      <c r="Z23" s="43"/>
-      <c r="AA23" s="43"/>
-      <c r="AB23" s="34">
+      <c r="X23" s="41"/>
+      <c r="Y23" s="41"/>
+      <c r="Z23" s="45"/>
+      <c r="AA23" s="45"/>
+      <c r="AB23" s="35">
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
       <c r="AC23" s="6"/>
       <c r="AD23" s="8"/>
-      <c r="AE23" s="36"/>
+      <c r="AE23" s="37"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="28" t="s">
@@ -2462,7 +2490,7 @@
       </c>
       <c r="O24" s="31"/>
       <c r="P24" s="31"/>
-      <c r="Q24" s="54">
+      <c r="Q24" s="57">
         <v>38.0</v>
       </c>
       <c r="R24" s="31"/>
@@ -2479,82 +2507,84 @@
       </c>
       <c r="X24" s="31"/>
       <c r="Y24" s="31"/>
-      <c r="Z24" s="33"/>
-      <c r="AA24" s="33"/>
-      <c r="AB24" s="34">
+      <c r="Z24" s="34"/>
+      <c r="AA24" s="34"/>
+      <c r="AB24" s="35">
         <f t="shared" si="1"/>
         <v>231</v>
       </c>
-      <c r="AC24" s="35">
+      <c r="AC24" s="36">
         <f>SUM(AB24:AB25)</f>
         <v>635</v>
       </c>
       <c r="AD24" s="5"/>
-      <c r="AE24" s="36"/>
+      <c r="AE24" s="37"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40">
+      <c r="B25" s="39"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41">
         <v>36.0</v>
       </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40">
+      <c r="E25" s="41"/>
+      <c r="F25" s="41">
         <v>33.0</v>
       </c>
-      <c r="G25" s="40">
+      <c r="G25" s="41">
         <v>33.0</v>
       </c>
-      <c r="H25" s="40">
+      <c r="H25" s="41">
         <v>34.0</v>
       </c>
-      <c r="I25" s="40">
+      <c r="I25" s="41">
         <v>26.0</v>
       </c>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40">
+      <c r="J25" s="41"/>
+      <c r="K25" s="41">
         <v>31.0</v>
       </c>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40">
+      <c r="L25" s="41"/>
+      <c r="M25" s="41">
         <v>28.0</v>
       </c>
-      <c r="N25" s="40">
+      <c r="N25" s="41">
         <v>27.0</v>
       </c>
-      <c r="O25" s="40">
+      <c r="O25" s="41">
         <v>32.0</v>
       </c>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="40"/>
-      <c r="S25" s="40"/>
-      <c r="T25" s="41">
+      <c r="P25" s="41"/>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="42">
         <v>26.0</v>
       </c>
-      <c r="U25" s="41">
+      <c r="U25" s="42">
         <v>35.0</v>
       </c>
-      <c r="V25" s="41">
+      <c r="V25" s="42">
         <v>33.0</v>
       </c>
-      <c r="W25" s="41">
+      <c r="W25" s="42">
         <v>30.0</v>
       </c>
-      <c r="X25" s="40"/>
-      <c r="Y25" s="40"/>
-      <c r="Z25" s="43"/>
-      <c r="AA25" s="43"/>
-      <c r="AB25" s="34">
+      <c r="X25" s="41"/>
+      <c r="Y25" s="41"/>
+      <c r="Z25" s="48">
+        <v>26.0</v>
+      </c>
+      <c r="AA25" s="45"/>
+      <c r="AB25" s="35">
         <f t="shared" si="1"/>
         <v>404</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
-      <c r="AE25" s="36"/>
+      <c r="AE25" s="37"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="28" t="s">
@@ -2596,7 +2626,7 @@
       <c r="Q26" s="31">
         <v>34.0</v>
       </c>
-      <c r="R26" s="54">
+      <c r="R26" s="57">
         <v>37.0</v>
       </c>
       <c r="S26" s="31">
@@ -2618,84 +2648,86 @@
         <v>35.0</v>
       </c>
       <c r="Y26" s="31"/>
-      <c r="Z26" s="33"/>
-      <c r="AA26" s="33"/>
-      <c r="AB26" s="34">
+      <c r="Z26" s="34"/>
+      <c r="AA26" s="34"/>
+      <c r="AB26" s="35">
         <f t="shared" si="1"/>
         <v>545</v>
       </c>
-      <c r="AC26" s="35">
+      <c r="AC26" s="36">
         <f>SUM(AB26:AB27)</f>
         <v>959</v>
       </c>
       <c r="AD26" s="5"/>
-      <c r="AE26" s="36"/>
+      <c r="AE26" s="37"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="40">
+      <c r="B27" s="39"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41">
         <v>42.0</v>
       </c>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40">
+      <c r="E27" s="41"/>
+      <c r="F27" s="41">
         <v>29.0</v>
       </c>
-      <c r="G27" s="40">
+      <c r="G27" s="41">
         <v>40.0</v>
       </c>
-      <c r="H27" s="40">
+      <c r="H27" s="41">
         <v>28.0</v>
       </c>
-      <c r="I27" s="40">
+      <c r="I27" s="41">
         <v>21.0</v>
       </c>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40">
+      <c r="J27" s="41"/>
+      <c r="K27" s="41">
         <v>39.0</v>
       </c>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40">
+      <c r="L27" s="41"/>
+      <c r="M27" s="41">
         <v>22.0</v>
       </c>
-      <c r="N27" s="40">
+      <c r="N27" s="41">
         <v>28.0</v>
       </c>
-      <c r="O27" s="40">
+      <c r="O27" s="41">
         <v>32.0</v>
       </c>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="40">
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41">
         <v>29.0</v>
       </c>
-      <c r="R27" s="40"/>
-      <c r="S27" s="40"/>
-      <c r="T27" s="41">
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="42">
         <v>20.0</v>
       </c>
-      <c r="U27" s="40"/>
-      <c r="V27" s="41">
+      <c r="U27" s="41"/>
+      <c r="V27" s="42">
         <v>24.0</v>
       </c>
-      <c r="W27" s="40"/>
-      <c r="X27" s="41">
+      <c r="W27" s="41"/>
+      <c r="X27" s="42">
         <v>35.0</v>
       </c>
-      <c r="Y27" s="41">
+      <c r="Y27" s="42">
         <v>25.0</v>
       </c>
-      <c r="Z27" s="43"/>
-      <c r="AA27" s="43"/>
-      <c r="AB27" s="34">
+      <c r="Z27" s="48">
+        <v>29.0</v>
+      </c>
+      <c r="AA27" s="45"/>
+      <c r="AB27" s="35">
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
-      <c r="AE27" s="36"/>
+      <c r="AE27" s="37"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="28" t="s">
@@ -2729,7 +2761,7 @@
       <c r="M28" s="31">
         <v>33.0</v>
       </c>
-      <c r="N28" s="54">
+      <c r="N28" s="57">
         <v>35.0</v>
       </c>
       <c r="O28" s="31">
@@ -2753,96 +2785,98 @@
         <v>32.0</v>
       </c>
       <c r="W28" s="31"/>
-      <c r="X28" s="45">
+      <c r="X28" s="47">
         <v>35.0</v>
       </c>
       <c r="Y28" s="32">
         <v>35.0</v>
       </c>
-      <c r="Z28" s="33"/>
-      <c r="AA28" s="33"/>
-      <c r="AB28" s="34">
+      <c r="Z28" s="34"/>
+      <c r="AA28" s="34"/>
+      <c r="AB28" s="35">
         <f t="shared" si="1"/>
         <v>545</v>
       </c>
-      <c r="AC28" s="35">
+      <c r="AC28" s="36">
         <f>SUM(AB28:AB29)</f>
         <v>1124</v>
       </c>
       <c r="AD28" s="5"/>
-      <c r="AE28" s="36"/>
+      <c r="AE28" s="37"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="40">
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41">
         <v>24.0</v>
       </c>
-      <c r="E29" s="40">
+      <c r="E29" s="41">
         <v>30.0</v>
       </c>
-      <c r="F29" s="40">
+      <c r="F29" s="41">
         <v>32.0</v>
       </c>
-      <c r="G29" s="40">
+      <c r="G29" s="41">
         <v>37.0</v>
       </c>
-      <c r="H29" s="40">
+      <c r="H29" s="41">
         <v>36.0</v>
       </c>
-      <c r="I29" s="40">
+      <c r="I29" s="41">
         <v>36.0</v>
       </c>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40">
+      <c r="J29" s="41"/>
+      <c r="K29" s="41">
         <v>38.0</v>
       </c>
-      <c r="L29" s="55"/>
-      <c r="M29" s="55">
+      <c r="L29" s="58"/>
+      <c r="M29" s="58">
         <v>39.0</v>
       </c>
-      <c r="N29" s="40">
+      <c r="N29" s="41">
         <v>33.0</v>
       </c>
-      <c r="O29" s="40">
+      <c r="O29" s="41">
         <v>33.0</v>
       </c>
-      <c r="P29" s="40"/>
-      <c r="Q29" s="40">
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41">
         <v>34.0</v>
       </c>
-      <c r="R29" s="40">
+      <c r="R29" s="41">
         <v>32.0</v>
       </c>
-      <c r="S29" s="55">
+      <c r="S29" s="58">
         <v>38.0</v>
       </c>
-      <c r="T29" s="41">
+      <c r="T29" s="42">
         <v>34.0</v>
       </c>
-      <c r="U29" s="41">
+      <c r="U29" s="42">
         <v>36.0</v>
       </c>
-      <c r="V29" s="41">
+      <c r="V29" s="42">
         <v>31.0</v>
       </c>
-      <c r="W29" s="42">
+      <c r="W29" s="43">
         <v>36.0</v>
       </c>
-      <c r="X29" s="40"/>
-      <c r="Y29" s="40"/>
-      <c r="Z29" s="43"/>
-      <c r="AA29" s="43"/>
-      <c r="AB29" s="34">
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41"/>
+      <c r="Z29" s="48">
+        <v>33.0</v>
+      </c>
+      <c r="AA29" s="45"/>
+      <c r="AB29" s="35">
         <f t="shared" si="1"/>
         <v>579</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
-      <c r="AE29" s="36"/>
+      <c r="AE29" s="37"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="28" t="s">
@@ -2886,87 +2920,91 @@
       <c r="W30" s="31"/>
       <c r="X30" s="31"/>
       <c r="Y30" s="31"/>
-      <c r="Z30" s="33"/>
-      <c r="AA30" s="33"/>
-      <c r="AB30" s="34">
+      <c r="Z30" s="33">
+        <v>31.0</v>
+      </c>
+      <c r="AA30" s="34"/>
+      <c r="AB30" s="35">
         <f t="shared" si="1"/>
         <v>214</v>
       </c>
-      <c r="AC30" s="35">
+      <c r="AC30" s="36">
         <f>SUM(AB30:AB31)</f>
         <v>648</v>
       </c>
       <c r="AD30" s="5"/>
-      <c r="AE30" s="36"/>
+      <c r="AE30" s="37"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="40">
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="41">
         <v>33.0</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40">
+      <c r="E31" s="41"/>
+      <c r="F31" s="41">
         <v>34.0</v>
       </c>
-      <c r="G31" s="40">
+      <c r="G31" s="41">
         <v>30.0</v>
       </c>
-      <c r="H31" s="40">
+      <c r="H31" s="41">
         <v>29.0</v>
       </c>
-      <c r="I31" s="40">
+      <c r="I31" s="41">
         <v>39.0</v>
       </c>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40">
+      <c r="J31" s="41"/>
+      <c r="K31" s="41">
         <v>31.0</v>
       </c>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40">
+      <c r="L31" s="41"/>
+      <c r="M31" s="41">
         <v>33.0</v>
       </c>
-      <c r="N31" s="40">
+      <c r="N31" s="41">
         <v>29.0</v>
       </c>
-      <c r="O31" s="40">
+      <c r="O31" s="41">
         <v>29.0</v>
       </c>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40">
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41">
         <v>28.0</v>
       </c>
-      <c r="R31" s="40"/>
-      <c r="S31" s="40">
+      <c r="R31" s="41"/>
+      <c r="S31" s="41">
         <v>30.0</v>
       </c>
-      <c r="T31" s="40"/>
-      <c r="U31" s="41">
+      <c r="T31" s="41"/>
+      <c r="U31" s="42">
         <v>27.0</v>
       </c>
-      <c r="V31" s="40"/>
-      <c r="W31" s="40"/>
-      <c r="X31" s="41">
+      <c r="V31" s="41"/>
+      <c r="W31" s="41"/>
+      <c r="X31" s="42">
         <v>29.0</v>
       </c>
-      <c r="Y31" s="41">
+      <c r="Y31" s="42">
         <v>33.0</v>
       </c>
-      <c r="Z31" s="56"/>
-      <c r="AA31" s="56"/>
-      <c r="AB31" s="57">
+      <c r="Z31" s="59">
+        <v>33.0</v>
+      </c>
+      <c r="AA31" s="60"/>
+      <c r="AB31" s="61">
         <f t="shared" si="1"/>
         <v>434</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
-      <c r="AE31" s="36"/>
+      <c r="AE31" s="37"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="58"/>
+      <c r="A32" s="62"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2997,27 +3035,27 @@
       <c r="AE32" s="1"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="60"/>
-      <c r="C33" s="61" t="s">
+      <c r="B33" s="64"/>
+      <c r="C33" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="62"/>
-      <c r="E33" s="60"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="64"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="63" t="s">
+      <c r="K33" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="65"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="69"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -3036,9 +3074,9 @@
       <c r="AE33" s="1"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="58"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
+      <c r="A34" s="62"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -3069,16 +3107,16 @@
       <c r="AE34" s="1"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="58"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
+      <c r="A35" s="62"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="66" t="s">
+      <c r="E35" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="68"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="72"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -3086,86 +3124,86 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="66" t="s">
+      <c r="P35" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="Q35" s="67"/>
-      <c r="R35" s="67"/>
-      <c r="S35" s="68"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="71"/>
+      <c r="S35" s="72"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="69"/>
+      <c r="X35" s="73"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="1"/>
       <c r="AE35" s="1"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="58"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="70" t="s">
+      <c r="A36" s="62"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="74" t="s">
         <v>54</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="71">
+      <c r="E36" s="75">
         <v>80.0</v>
       </c>
-      <c r="F36" s="62"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="70" t="s">
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="O36" s="36"/>
-      <c r="P36" s="71">
+      <c r="O36" s="37"/>
+      <c r="P36" s="75">
         <v>50.0</v>
       </c>
-      <c r="Q36" s="62"/>
-      <c r="R36" s="62"/>
-      <c r="S36" s="60"/>
+      <c r="Q36" s="66"/>
+      <c r="R36" s="66"/>
+      <c r="S36" s="64"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="72"/>
+      <c r="X36" s="76"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
       <c r="AE36" s="1"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="58"/>
-      <c r="B37" s="58"/>
-      <c r="C37" s="70" t="s">
+      <c r="A37" s="62"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="74" t="s">
         <v>55</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="71">
+      <c r="E37" s="75">
         <v>50.0</v>
       </c>
-      <c r="F37" s="62"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="70" t="s">
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="O37" s="36"/>
-      <c r="P37" s="71">
+      <c r="O37" s="37"/>
+      <c r="P37" s="75">
         <v>30.0</v>
       </c>
-      <c r="Q37" s="62"/>
-      <c r="R37" s="62"/>
-      <c r="S37" s="60"/>
+      <c r="Q37" s="66"/>
+      <c r="R37" s="66"/>
+      <c r="S37" s="64"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -3180,18 +3218,18 @@
       <c r="AE37" s="1"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="58"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="70" t="s">
+      <c r="A38" s="62"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="74" t="s">
         <v>56</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="71">
+      <c r="E38" s="75">
         <v>40.0</v>
       </c>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="60"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="64"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -3199,7 +3237,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="73"/>
+      <c r="P38" s="77"/>
       <c r="Q38" s="23"/>
       <c r="R38" s="23"/>
       <c r="S38" s="23"/>
@@ -3217,14 +3255,14 @@
       <c r="AE38" s="1"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="D39" s="74"/>
-      <c r="E39" s="73"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="77"/>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
       <c r="H39" s="23"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
-      <c r="O39" s="74"/>
+      <c r="O39" s="78"/>
       <c r="S39" s="1"/>
       <c r="W39" s="1"/>
     </row>
@@ -4295,10 +4333,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="75"/>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="76" t="s">
+      <c r="A1" s="79"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="80" t="s">
         <v>57</v>
       </c>
       <c r="E1" s="4"/>
@@ -4312,23 +4350,23 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="5"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
     </row>
     <row r="2">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -4341,100 +4379,100 @@
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="8"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="75"/>
-      <c r="AA2" s="75"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="79"/>
     </row>
     <row r="3" ht="79.5" customHeight="1">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78">
+      <c r="A3" s="81"/>
+      <c r="B3" s="82">
         <v>45575.0</v>
       </c>
-      <c r="C3" s="78">
+      <c r="C3" s="82">
         <v>45582.0</v>
       </c>
-      <c r="D3" s="79">
+      <c r="D3" s="83">
         <v>45589.0</v>
       </c>
-      <c r="E3" s="79">
+      <c r="E3" s="83">
         <v>45596.0</v>
       </c>
-      <c r="F3" s="79">
+      <c r="F3" s="83">
         <v>45603.0</v>
       </c>
-      <c r="G3" s="79">
+      <c r="G3" s="83">
         <v>45610.0</v>
       </c>
-      <c r="H3" s="79">
+      <c r="H3" s="83">
         <v>45617.0</v>
       </c>
-      <c r="I3" s="79">
+      <c r="I3" s="83">
         <v>45624.0</v>
       </c>
-      <c r="J3" s="79">
+      <c r="J3" s="83">
         <v>45631.0</v>
       </c>
-      <c r="K3" s="79">
+      <c r="K3" s="83">
         <v>45638.0</v>
       </c>
-      <c r="L3" s="79">
+      <c r="L3" s="83">
         <v>45645.0</v>
       </c>
-      <c r="M3" s="79">
+      <c r="M3" s="83">
         <v>45659.0</v>
       </c>
-      <c r="N3" s="79">
+      <c r="N3" s="83">
         <v>45666.0</v>
       </c>
-      <c r="O3" s="79">
+      <c r="O3" s="83">
         <v>45673.0</v>
       </c>
-      <c r="P3" s="78">
+      <c r="P3" s="82">
         <v>45680.0</v>
       </c>
-      <c r="Q3" s="78">
+      <c r="Q3" s="82">
         <v>45687.0</v>
       </c>
-      <c r="R3" s="78">
+      <c r="R3" s="82">
         <v>45694.0</v>
       </c>
-      <c r="S3" s="78">
+      <c r="S3" s="82">
         <v>45701.0</v>
       </c>
-      <c r="T3" s="78">
+      <c r="T3" s="82">
         <v>45708.0</v>
       </c>
-      <c r="U3" s="78">
+      <c r="U3" s="82">
         <v>45715.0</v>
       </c>
-      <c r="V3" s="78">
+      <c r="V3" s="82">
         <v>45722.0</v>
       </c>
-      <c r="W3" s="78">
+      <c r="W3" s="82">
         <v>45729.0</v>
       </c>
-      <c r="X3" s="78">
+      <c r="X3" s="82">
         <v>45736.0</v>
       </c>
-      <c r="Y3" s="78">
+      <c r="Y3" s="82">
         <v>45743.0</v>
       </c>
-      <c r="Z3" s="80" t="s">
+      <c r="Z3" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="81"/>
+      <c r="AA3" s="85"/>
     </row>
     <row r="4">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="86" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
@@ -4509,924 +4547,940 @@
       <c r="Y4" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="Z4" s="83" t="s">
+      <c r="Z4" s="87" t="s">
         <v>58</v>
       </c>
       <c r="AA4" s="27"/>
     </row>
     <row r="5">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="85">
+      <c r="B5" s="89">
         <v>30.0</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="89">
         <v>37.0</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="85">
+      <c r="D5" s="90"/>
+      <c r="E5" s="89">
         <v>31.0</v>
       </c>
-      <c r="F5" s="85">
+      <c r="F5" s="89">
         <v>33.0</v>
       </c>
-      <c r="G5" s="85">
+      <c r="G5" s="89">
         <v>27.0</v>
       </c>
-      <c r="H5" s="85">
+      <c r="H5" s="89">
         <v>27.0</v>
       </c>
-      <c r="I5" s="85">
+      <c r="I5" s="89">
         <v>29.0</v>
       </c>
-      <c r="J5" s="85">
+      <c r="J5" s="89">
         <v>36.0</v>
       </c>
-      <c r="K5" s="86">
+      <c r="K5" s="90">
         <v>28.0</v>
       </c>
-      <c r="L5" s="87">
+      <c r="L5" s="91">
         <v>38.0</v>
       </c>
-      <c r="M5" s="86">
+      <c r="M5" s="90">
         <v>38.0</v>
       </c>
-      <c r="N5" s="86"/>
-      <c r="O5" s="87">
+      <c r="N5" s="90"/>
+      <c r="O5" s="91">
         <v>36.0</v>
       </c>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88">
+      <c r="P5" s="92"/>
+      <c r="Q5" s="92">
         <v>27.0</v>
       </c>
-      <c r="R5" s="89">
+      <c r="R5" s="93">
         <v>35.0</v>
       </c>
-      <c r="S5" s="88">
+      <c r="S5" s="92">
         <v>33.0</v>
       </c>
-      <c r="T5" s="86"/>
-      <c r="U5" s="89">
+      <c r="T5" s="90"/>
+      <c r="U5" s="93">
         <v>37.0</v>
       </c>
-      <c r="V5" s="86"/>
-      <c r="W5" s="86"/>
-      <c r="X5" s="86"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="90">
+      <c r="V5" s="90"/>
+      <c r="W5" s="92">
+        <v>26.0</v>
+      </c>
+      <c r="X5" s="90"/>
+      <c r="Y5" s="90"/>
+      <c r="Z5" s="94">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
-        <v>522</v>
-      </c>
-      <c r="AA5" s="36"/>
+        <v>548</v>
+      </c>
+      <c r="AA5" s="37"/>
     </row>
     <row r="6">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="86">
+      <c r="B6" s="90">
         <v>36.0</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86">
+      <c r="C6" s="90"/>
+      <c r="D6" s="90">
         <v>32.0</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86">
+      <c r="E6" s="90"/>
+      <c r="F6" s="90">
         <v>39.0</v>
       </c>
-      <c r="G6" s="86">
+      <c r="G6" s="90">
         <v>35.0</v>
       </c>
-      <c r="H6" s="86">
+      <c r="H6" s="90">
         <v>27.0</v>
       </c>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86">
+      <c r="I6" s="90"/>
+      <c r="J6" s="90">
         <v>33.0</v>
       </c>
-      <c r="K6" s="86">
+      <c r="K6" s="90">
         <v>38.0</v>
       </c>
-      <c r="L6" s="86">
+      <c r="L6" s="90">
         <v>35.0</v>
       </c>
-      <c r="M6" s="86">
+      <c r="M6" s="90">
         <v>32.0</v>
       </c>
-      <c r="N6" s="87">
+      <c r="N6" s="91">
         <v>33.0</v>
       </c>
-      <c r="O6" s="86">
+      <c r="O6" s="90">
         <v>34.0</v>
       </c>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="88">
+      <c r="P6" s="92"/>
+      <c r="Q6" s="92">
         <v>30.0</v>
       </c>
-      <c r="R6" s="88">
+      <c r="R6" s="92">
         <v>25.0</v>
       </c>
-      <c r="S6" s="88">
+      <c r="S6" s="92">
         <v>31.0</v>
       </c>
-      <c r="T6" s="89">
+      <c r="T6" s="93">
         <v>34.0</v>
       </c>
-      <c r="U6" s="88">
+      <c r="U6" s="92">
         <v>32.0</v>
       </c>
-      <c r="V6" s="86"/>
-      <c r="W6" s="86"/>
-      <c r="X6" s="86"/>
-      <c r="Y6" s="86"/>
-      <c r="Z6" s="90">
+      <c r="V6" s="90"/>
+      <c r="W6" s="90"/>
+      <c r="X6" s="90"/>
+      <c r="Y6" s="90"/>
+      <c r="Z6" s="94">
         <f t="shared" si="1"/>
         <v>526</v>
       </c>
-      <c r="AA6" s="36"/>
+      <c r="AA6" s="37"/>
     </row>
     <row r="7">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="85">
+      <c r="B7" s="89">
         <v>33.0</v>
       </c>
-      <c r="C7" s="85">
+      <c r="C7" s="89">
         <v>28.0</v>
       </c>
-      <c r="D7" s="85">
+      <c r="D7" s="89">
         <v>32.0</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="85">
+      <c r="E7" s="90"/>
+      <c r="F7" s="89">
         <v>33.0</v>
       </c>
-      <c r="G7" s="85">
+      <c r="G7" s="89">
         <v>34.0</v>
       </c>
-      <c r="H7" s="85">
+      <c r="H7" s="89">
         <v>26.0</v>
       </c>
-      <c r="I7" s="85">
+      <c r="I7" s="89">
         <v>29.0</v>
       </c>
-      <c r="J7" s="85">
+      <c r="J7" s="89">
         <v>28.0</v>
       </c>
-      <c r="K7" s="86">
+      <c r="K7" s="90">
         <v>29.0</v>
       </c>
-      <c r="L7" s="86">
+      <c r="L7" s="90">
         <v>27.0</v>
       </c>
-      <c r="M7" s="87">
+      <c r="M7" s="91">
         <v>38.0</v>
       </c>
-      <c r="N7" s="86"/>
-      <c r="O7" s="86">
+      <c r="N7" s="90"/>
+      <c r="O7" s="90">
         <v>32.0</v>
       </c>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="88">
+      <c r="P7" s="92"/>
+      <c r="Q7" s="92">
         <v>24.0</v>
       </c>
-      <c r="R7" s="88">
+      <c r="R7" s="92">
         <v>28.0</v>
       </c>
-      <c r="S7" s="88">
+      <c r="S7" s="92">
         <v>30.0</v>
       </c>
-      <c r="T7" s="86"/>
-      <c r="U7" s="88">
+      <c r="T7" s="90"/>
+      <c r="U7" s="92">
         <v>27.0</v>
       </c>
-      <c r="V7" s="89">
+      <c r="V7" s="93">
         <v>35.0</v>
       </c>
-      <c r="W7" s="86"/>
-      <c r="X7" s="86"/>
-      <c r="Y7" s="86"/>
-      <c r="Z7" s="90">
+      <c r="W7" s="92">
+        <v>28.0</v>
+      </c>
+      <c r="X7" s="90"/>
+      <c r="Y7" s="90"/>
+      <c r="Z7" s="94">
         <f t="shared" si="1"/>
-        <v>513</v>
-      </c>
-      <c r="AA7" s="36"/>
+        <v>541</v>
+      </c>
+      <c r="AA7" s="37"/>
     </row>
     <row r="8">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="85">
+      <c r="B8" s="89">
         <v>37.0</v>
       </c>
-      <c r="C8" s="85">
+      <c r="C8" s="89">
         <v>35.0</v>
       </c>
-      <c r="D8" s="85">
+      <c r="D8" s="89">
         <v>32.0</v>
       </c>
-      <c r="E8" s="91">
+      <c r="E8" s="95">
         <v>31.0</v>
       </c>
-      <c r="F8" s="85">
+      <c r="F8" s="89">
         <v>31.0</v>
       </c>
-      <c r="G8" s="85">
+      <c r="G8" s="89">
         <v>33.0</v>
       </c>
-      <c r="H8" s="85">
+      <c r="H8" s="89">
         <v>36.0</v>
       </c>
-      <c r="I8" s="85">
+      <c r="I8" s="89">
         <v>33.0</v>
       </c>
-      <c r="J8" s="92">
+      <c r="J8" s="96">
         <v>36.0</v>
       </c>
-      <c r="K8" s="86"/>
-      <c r="L8" s="86">
+      <c r="K8" s="90"/>
+      <c r="L8" s="90">
         <v>32.0</v>
       </c>
-      <c r="M8" s="86">
+      <c r="M8" s="90">
         <v>33.0</v>
       </c>
-      <c r="N8" s="86"/>
-      <c r="O8" s="86"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="88">
+      <c r="N8" s="90"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="92"/>
+      <c r="Q8" s="92">
         <v>22.0</v>
       </c>
-      <c r="R8" s="88">
+      <c r="R8" s="92">
         <v>34.0</v>
       </c>
-      <c r="S8" s="88"/>
-      <c r="T8" s="86"/>
-      <c r="U8" s="86"/>
-      <c r="V8" s="86"/>
-      <c r="W8" s="86"/>
-      <c r="X8" s="86"/>
-      <c r="Y8" s="86"/>
-      <c r="Z8" s="90">
+      <c r="S8" s="92"/>
+      <c r="T8" s="90"/>
+      <c r="U8" s="90"/>
+      <c r="V8" s="90"/>
+      <c r="W8" s="93">
+        <v>35.0</v>
+      </c>
+      <c r="X8" s="90"/>
+      <c r="Y8" s="90"/>
+      <c r="Z8" s="94">
         <f t="shared" si="1"/>
-        <v>425</v>
-      </c>
-      <c r="AA8" s="36"/>
+        <v>460</v>
+      </c>
+      <c r="AA8" s="37"/>
     </row>
     <row r="9">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="85">
+      <c r="B9" s="89">
         <v>30.0</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="89">
         <v>33.0</v>
       </c>
-      <c r="D9" s="85">
+      <c r="D9" s="89">
         <v>30.0</v>
       </c>
-      <c r="E9" s="85">
+      <c r="E9" s="89">
         <v>26.0</v>
       </c>
-      <c r="F9" s="85">
+      <c r="F9" s="89">
         <v>28.0</v>
       </c>
-      <c r="G9" s="85">
+      <c r="G9" s="89">
         <v>26.0</v>
       </c>
-      <c r="H9" s="85">
+      <c r="H9" s="89">
         <v>20.0</v>
       </c>
-      <c r="I9" s="86"/>
-      <c r="J9" s="85">
+      <c r="I9" s="90"/>
+      <c r="J9" s="89">
         <v>34.0</v>
       </c>
-      <c r="K9" s="86">
+      <c r="K9" s="90">
         <v>26.0</v>
       </c>
-      <c r="L9" s="86">
+      <c r="L9" s="90">
         <v>26.0</v>
       </c>
-      <c r="M9" s="86">
+      <c r="M9" s="90">
         <v>24.0</v>
       </c>
-      <c r="N9" s="86">
+      <c r="N9" s="90">
         <v>28.0</v>
       </c>
-      <c r="O9" s="86">
+      <c r="O9" s="90">
         <v>28.0</v>
       </c>
-      <c r="P9" s="88"/>
-      <c r="Q9" s="88">
+      <c r="P9" s="92"/>
+      <c r="Q9" s="92">
         <v>31.0</v>
       </c>
-      <c r="R9" s="88">
+      <c r="R9" s="92">
         <v>30.0</v>
       </c>
-      <c r="S9" s="88">
+      <c r="S9" s="92">
         <v>29.0</v>
       </c>
-      <c r="T9" s="88">
+      <c r="T9" s="92">
         <v>22.0</v>
       </c>
-      <c r="U9" s="86"/>
-      <c r="V9" s="86"/>
-      <c r="W9" s="86"/>
-      <c r="X9" s="86"/>
-      <c r="Y9" s="86"/>
-      <c r="Z9" s="90">
+      <c r="U9" s="90"/>
+      <c r="V9" s="90"/>
+      <c r="W9" s="92">
+        <v>29.0</v>
+      </c>
+      <c r="X9" s="90"/>
+      <c r="Y9" s="90"/>
+      <c r="Z9" s="94">
         <f t="shared" si="1"/>
-        <v>471</v>
-      </c>
-      <c r="AA9" s="36"/>
+        <v>500</v>
+      </c>
+      <c r="AA9" s="37"/>
     </row>
     <row r="10">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86">
+      <c r="B10" s="90"/>
+      <c r="C10" s="90">
         <v>31.0</v>
       </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86">
+      <c r="D10" s="90"/>
+      <c r="E10" s="90">
         <v>23.0</v>
       </c>
-      <c r="F10" s="86">
+      <c r="F10" s="90">
         <v>35.0</v>
       </c>
-      <c r="G10" s="86">
+      <c r="G10" s="90">
         <v>29.0</v>
       </c>
-      <c r="H10" s="86">
+      <c r="H10" s="90">
         <v>16.0</v>
       </c>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86">
+      <c r="I10" s="90"/>
+      <c r="J10" s="90">
         <v>29.0</v>
       </c>
-      <c r="K10" s="86">
+      <c r="K10" s="90">
         <v>21.0</v>
       </c>
-      <c r="L10" s="86">
+      <c r="L10" s="90">
         <v>24.0</v>
       </c>
-      <c r="M10" s="86">
+      <c r="M10" s="90">
         <v>28.0</v>
       </c>
-      <c r="N10" s="86"/>
-      <c r="O10" s="86">
+      <c r="N10" s="90"/>
+      <c r="O10" s="90">
         <v>14.0</v>
       </c>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88">
+      <c r="P10" s="92"/>
+      <c r="Q10" s="92">
         <v>22.0</v>
       </c>
-      <c r="R10" s="88">
+      <c r="R10" s="92">
         <v>20.0</v>
       </c>
-      <c r="S10" s="88">
+      <c r="S10" s="92">
         <v>26.0</v>
       </c>
-      <c r="T10" s="86"/>
-      <c r="U10" s="86"/>
-      <c r="V10" s="88">
+      <c r="T10" s="90"/>
+      <c r="U10" s="90"/>
+      <c r="V10" s="92">
         <v>30.0</v>
       </c>
-      <c r="W10" s="86"/>
-      <c r="X10" s="86"/>
-      <c r="Y10" s="86"/>
-      <c r="Z10" s="90">
+      <c r="W10" s="92">
+        <v>28.0</v>
+      </c>
+      <c r="X10" s="90"/>
+      <c r="Y10" s="90"/>
+      <c r="Z10" s="94">
         <f t="shared" si="1"/>
-        <v>348</v>
-      </c>
-      <c r="AA10" s="36"/>
+        <v>376</v>
+      </c>
+      <c r="AA10" s="37"/>
     </row>
     <row r="11">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="86">
+      <c r="B11" s="90">
         <v>41.0</v>
       </c>
-      <c r="C11" s="86">
+      <c r="C11" s="90">
         <v>31.0</v>
       </c>
-      <c r="D11" s="86">
+      <c r="D11" s="90">
         <v>32.0</v>
       </c>
-      <c r="E11" s="86">
+      <c r="E11" s="90">
         <v>29.0</v>
       </c>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86">
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90">
         <v>23.0</v>
       </c>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="86"/>
-      <c r="S11" s="86"/>
-      <c r="T11" s="86"/>
-      <c r="U11" s="86"/>
-      <c r="V11" s="86"/>
-      <c r="W11" s="86"/>
-      <c r="X11" s="86"/>
-      <c r="Y11" s="86"/>
-      <c r="Z11" s="90">
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="90"/>
+      <c r="P11" s="90"/>
+      <c r="Q11" s="90"/>
+      <c r="R11" s="90"/>
+      <c r="S11" s="90"/>
+      <c r="T11" s="90"/>
+      <c r="U11" s="90"/>
+      <c r="V11" s="90"/>
+      <c r="W11" s="90"/>
+      <c r="X11" s="90"/>
+      <c r="Y11" s="90"/>
+      <c r="Z11" s="94">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
-      <c r="AA11" s="36"/>
+      <c r="AA11" s="37"/>
     </row>
     <row r="12">
-      <c r="A12" s="84" t="s">
+      <c r="A12" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="85">
+      <c r="B12" s="89">
         <v>42.0</v>
       </c>
-      <c r="C12" s="85">
+      <c r="C12" s="89">
         <v>31.0</v>
       </c>
-      <c r="D12" s="85">
+      <c r="D12" s="89">
         <v>32.0</v>
       </c>
-      <c r="E12" s="85">
+      <c r="E12" s="89">
         <v>32.0</v>
       </c>
-      <c r="F12" s="85">
+      <c r="F12" s="89">
         <v>34.0</v>
       </c>
-      <c r="G12" s="86"/>
-      <c r="H12" s="85">
+      <c r="G12" s="90"/>
+      <c r="H12" s="89">
         <v>28.0</v>
       </c>
-      <c r="I12" s="85">
+      <c r="I12" s="89">
         <v>34.0</v>
       </c>
-      <c r="J12" s="85">
+      <c r="J12" s="89">
         <v>33.0</v>
       </c>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86">
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="90"/>
+      <c r="O12" s="90">
         <v>30.0</v>
       </c>
-      <c r="P12" s="88"/>
-      <c r="Q12" s="88">
+      <c r="P12" s="92"/>
+      <c r="Q12" s="92">
         <v>27.0</v>
       </c>
-      <c r="R12" s="88">
+      <c r="R12" s="92">
         <v>26.0</v>
       </c>
-      <c r="S12" s="86"/>
-      <c r="T12" s="86"/>
-      <c r="U12" s="88">
+      <c r="S12" s="90"/>
+      <c r="T12" s="90"/>
+      <c r="U12" s="92">
         <v>32.0</v>
       </c>
-      <c r="V12" s="88">
+      <c r="V12" s="92">
         <v>27.0</v>
       </c>
-      <c r="W12" s="86"/>
-      <c r="X12" s="86"/>
-      <c r="Y12" s="86"/>
-      <c r="Z12" s="90">
+      <c r="W12" s="92">
+        <v>24.0</v>
+      </c>
+      <c r="X12" s="90"/>
+      <c r="Y12" s="90"/>
+      <c r="Z12" s="94">
         <f t="shared" si="1"/>
-        <v>408</v>
-      </c>
-      <c r="AA12" s="36"/>
+        <v>432</v>
+      </c>
+      <c r="AA12" s="37"/>
     </row>
     <row r="13">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86">
+      <c r="B13" s="97"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90">
         <v>33.0</v>
       </c>
-      <c r="E13" s="86">
+      <c r="E13" s="90">
         <v>36.0</v>
       </c>
-      <c r="F13" s="86">
+      <c r="F13" s="90">
         <v>27.0</v>
       </c>
-      <c r="G13" s="86">
+      <c r="G13" s="90">
         <v>37.0</v>
       </c>
-      <c r="H13" s="86">
+      <c r="H13" s="90">
         <v>31.0</v>
       </c>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86">
+      <c r="I13" s="90"/>
+      <c r="J13" s="90">
         <v>34.0</v>
       </c>
-      <c r="K13" s="87">
+      <c r="K13" s="91">
         <v>40.0</v>
       </c>
-      <c r="L13" s="86">
+      <c r="L13" s="90">
         <v>34.0</v>
       </c>
-      <c r="M13" s="86">
+      <c r="M13" s="90">
         <v>31.0</v>
       </c>
-      <c r="N13" s="86">
+      <c r="N13" s="90">
         <v>29.0</v>
       </c>
-      <c r="O13" s="86">
+      <c r="O13" s="90">
         <v>34.0</v>
       </c>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89">
+      <c r="P13" s="93"/>
+      <c r="Q13" s="93">
         <v>38.0</v>
       </c>
-      <c r="R13" s="88">
+      <c r="R13" s="92">
         <v>28.0</v>
       </c>
-      <c r="S13" s="88">
+      <c r="S13" s="92">
         <v>32.0</v>
       </c>
-      <c r="T13" s="86"/>
-      <c r="U13" s="88">
+      <c r="T13" s="90"/>
+      <c r="U13" s="92">
         <v>34.0</v>
       </c>
-      <c r="V13" s="86"/>
-      <c r="W13" s="86"/>
-      <c r="X13" s="86"/>
-      <c r="Y13" s="86"/>
-      <c r="Z13" s="90">
+      <c r="V13" s="90"/>
+      <c r="W13" s="92">
+        <v>28.0</v>
+      </c>
+      <c r="X13" s="90"/>
+      <c r="Y13" s="90"/>
+      <c r="Z13" s="94">
         <f t="shared" si="1"/>
-        <v>498</v>
-      </c>
-      <c r="AA13" s="36"/>
+        <v>526</v>
+      </c>
+      <c r="AA13" s="37"/>
     </row>
     <row r="14">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86">
+      <c r="B14" s="90"/>
+      <c r="C14" s="90">
         <v>22.0</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86">
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90">
         <v>36.0</v>
       </c>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86">
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90">
         <v>34.0</v>
       </c>
-      <c r="K14" s="86">
+      <c r="K14" s="90">
         <v>27.0</v>
       </c>
-      <c r="L14" s="86">
+      <c r="L14" s="90">
         <v>35.0</v>
       </c>
-      <c r="M14" s="86"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86">
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="90">
         <v>32.0</v>
       </c>
-      <c r="P14" s="86"/>
-      <c r="Q14" s="86"/>
-      <c r="R14" s="88">
+      <c r="P14" s="90"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="92">
         <v>31.0</v>
       </c>
-      <c r="S14" s="88">
+      <c r="S14" s="92">
         <v>29.0</v>
       </c>
-      <c r="T14" s="86"/>
-      <c r="U14" s="86"/>
-      <c r="V14" s="86"/>
-      <c r="W14" s="86"/>
-      <c r="X14" s="86"/>
-      <c r="Y14" s="86"/>
-      <c r="Z14" s="90">
+      <c r="T14" s="90"/>
+      <c r="U14" s="90"/>
+      <c r="V14" s="90"/>
+      <c r="W14" s="90"/>
+      <c r="X14" s="90"/>
+      <c r="Y14" s="90"/>
+      <c r="Z14" s="94">
         <f t="shared" si="1"/>
         <v>246</v>
       </c>
-      <c r="AA14" s="36"/>
+      <c r="AA14" s="37"/>
     </row>
     <row r="15">
-      <c r="A15" s="84" t="s">
+      <c r="A15" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86">
+      <c r="B15" s="90"/>
+      <c r="C15" s="90">
         <v>43.0</v>
       </c>
-      <c r="D15" s="86">
+      <c r="D15" s="90">
         <v>25.0</v>
       </c>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86">
+      <c r="E15" s="90"/>
+      <c r="F15" s="90">
         <v>32.0</v>
       </c>
-      <c r="G15" s="86">
+      <c r="G15" s="90">
         <v>30.0</v>
       </c>
-      <c r="H15" s="86">
+      <c r="H15" s="90">
         <v>34.0</v>
       </c>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86">
+      <c r="I15" s="90"/>
+      <c r="J15" s="90">
         <v>34.0</v>
       </c>
-      <c r="K15" s="86">
+      <c r="K15" s="90">
         <v>26.0</v>
       </c>
-      <c r="L15" s="86">
+      <c r="L15" s="90">
         <v>37.0</v>
       </c>
-      <c r="M15" s="86">
+      <c r="M15" s="90">
         <v>32.0</v>
       </c>
-      <c r="N15" s="86">
+      <c r="N15" s="90">
         <v>27.0</v>
       </c>
-      <c r="O15" s="86"/>
-      <c r="P15" s="88"/>
-      <c r="Q15" s="88">
+      <c r="O15" s="90"/>
+      <c r="P15" s="92"/>
+      <c r="Q15" s="92">
         <v>27.0</v>
       </c>
-      <c r="R15" s="88">
+      <c r="R15" s="92">
         <v>28.0</v>
       </c>
-      <c r="S15" s="86"/>
-      <c r="T15" s="88">
+      <c r="S15" s="90"/>
+      <c r="T15" s="92">
         <v>25.0</v>
       </c>
-      <c r="U15" s="88">
+      <c r="U15" s="92">
         <v>23.0</v>
       </c>
-      <c r="V15" s="86"/>
-      <c r="W15" s="86"/>
-      <c r="X15" s="86"/>
-      <c r="Y15" s="86"/>
-      <c r="Z15" s="90">
+      <c r="V15" s="90"/>
+      <c r="W15" s="90"/>
+      <c r="X15" s="90"/>
+      <c r="Y15" s="90"/>
+      <c r="Z15" s="94">
         <f t="shared" si="1"/>
         <v>423</v>
       </c>
-      <c r="AA15" s="36"/>
+      <c r="AA15" s="37"/>
     </row>
     <row r="16">
-      <c r="A16" s="84" t="s">
+      <c r="A16" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86">
+      <c r="B16" s="90"/>
+      <c r="C16" s="90">
         <v>29.0</v>
       </c>
-      <c r="D16" s="86">
+      <c r="D16" s="90">
         <v>28.0</v>
       </c>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86">
+      <c r="E16" s="90"/>
+      <c r="F16" s="90">
         <v>23.0</v>
       </c>
-      <c r="G16" s="86">
+      <c r="G16" s="90">
         <v>30.0</v>
       </c>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86">
+      <c r="H16" s="90"/>
+      <c r="I16" s="90">
         <v>27.0</v>
       </c>
-      <c r="J16" s="86"/>
-      <c r="K16" s="86">
+      <c r="J16" s="90"/>
+      <c r="K16" s="90">
         <v>29.0</v>
       </c>
-      <c r="L16" s="86"/>
-      <c r="M16" s="86"/>
-      <c r="N16" s="86"/>
-      <c r="O16" s="86">
+      <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90"/>
+      <c r="O16" s="90">
         <v>35.0</v>
       </c>
-      <c r="P16" s="88"/>
-      <c r="Q16" s="88">
+      <c r="P16" s="92"/>
+      <c r="Q16" s="92">
         <v>33.0</v>
       </c>
-      <c r="R16" s="88">
+      <c r="R16" s="92">
         <v>27.0</v>
       </c>
-      <c r="S16" s="86"/>
-      <c r="T16" s="86"/>
-      <c r="U16" s="88">
+      <c r="S16" s="90"/>
+      <c r="T16" s="90"/>
+      <c r="U16" s="92">
         <v>27.0</v>
       </c>
-      <c r="V16" s="88">
+      <c r="V16" s="92">
         <v>27.0</v>
       </c>
-      <c r="W16" s="86"/>
-      <c r="X16" s="86"/>
-      <c r="Y16" s="86"/>
-      <c r="Z16" s="90">
+      <c r="W16" s="92">
+        <v>30.0</v>
+      </c>
+      <c r="X16" s="90"/>
+      <c r="Y16" s="90"/>
+      <c r="Z16" s="94">
         <f t="shared" si="1"/>
-        <v>315</v>
-      </c>
-      <c r="AA16" s="36"/>
+        <v>345</v>
+      </c>
+      <c r="AA16" s="37"/>
     </row>
     <row r="17">
-      <c r="A17" s="84" t="s">
+      <c r="A17" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86">
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90">
         <v>26.0</v>
       </c>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
-      <c r="L17" s="86"/>
-      <c r="M17" s="86"/>
-      <c r="N17" s="86"/>
-      <c r="O17" s="86"/>
-      <c r="P17" s="86"/>
-      <c r="Q17" s="86"/>
-      <c r="R17" s="86"/>
-      <c r="S17" s="86"/>
-      <c r="T17" s="86"/>
-      <c r="U17" s="86"/>
-      <c r="V17" s="86"/>
-      <c r="W17" s="86"/>
-      <c r="X17" s="86"/>
-      <c r="Y17" s="86"/>
-      <c r="Z17" s="90">
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="90"/>
+      <c r="N17" s="90"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="90"/>
+      <c r="Q17" s="90"/>
+      <c r="R17" s="90"/>
+      <c r="S17" s="90"/>
+      <c r="T17" s="90"/>
+      <c r="U17" s="90"/>
+      <c r="V17" s="90"/>
+      <c r="W17" s="90"/>
+      <c r="X17" s="90"/>
+      <c r="Y17" s="90"/>
+      <c r="Z17" s="94">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="AA17" s="36"/>
+      <c r="AA17" s="37"/>
     </row>
     <row r="18">
-      <c r="A18" s="84" t="s">
+      <c r="A18" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86">
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90">
         <v>27.0</v>
       </c>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="86"/>
-      <c r="N18" s="86"/>
-      <c r="O18" s="86"/>
-      <c r="P18" s="86"/>
-      <c r="Q18" s="86"/>
-      <c r="R18" s="86"/>
-      <c r="S18" s="86"/>
-      <c r="T18" s="86"/>
-      <c r="U18" s="86"/>
-      <c r="V18" s="86"/>
-      <c r="W18" s="86"/>
-      <c r="X18" s="86"/>
-      <c r="Y18" s="86"/>
-      <c r="Z18" s="90">
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="90"/>
+      <c r="R18" s="90"/>
+      <c r="S18" s="90"/>
+      <c r="T18" s="90"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="90"/>
+      <c r="X18" s="90"/>
+      <c r="Y18" s="90"/>
+      <c r="Z18" s="94">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="AA18" s="36"/>
+      <c r="AA18" s="37"/>
     </row>
     <row r="19">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86">
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90">
         <v>41.0</v>
       </c>
-      <c r="E19" s="86">
+      <c r="E19" s="90">
         <v>37.0</v>
       </c>
-      <c r="F19" s="86">
+      <c r="F19" s="90">
         <v>38.0</v>
       </c>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="86"/>
-      <c r="J19" s="86"/>
-      <c r="K19" s="86"/>
-      <c r="L19" s="86"/>
-      <c r="M19" s="86"/>
-      <c r="N19" s="86"/>
-      <c r="O19" s="86"/>
-      <c r="P19" s="88"/>
-      <c r="Q19" s="88">
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="90"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="90"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="90"/>
+      <c r="P19" s="92"/>
+      <c r="Q19" s="92">
         <v>32.0</v>
       </c>
-      <c r="R19" s="88">
+      <c r="R19" s="92">
         <v>24.0</v>
       </c>
-      <c r="S19" s="89">
+      <c r="S19" s="93">
         <v>40.0</v>
       </c>
-      <c r="T19" s="86"/>
-      <c r="U19" s="86"/>
-      <c r="V19" s="86"/>
-      <c r="W19" s="86"/>
-      <c r="X19" s="86"/>
-      <c r="Y19" s="86"/>
-      <c r="Z19" s="90">
+      <c r="T19" s="90"/>
+      <c r="U19" s="90"/>
+      <c r="V19" s="90"/>
+      <c r="W19" s="90"/>
+      <c r="X19" s="90"/>
+      <c r="Y19" s="90"/>
+      <c r="Z19" s="94">
         <f t="shared" si="1"/>
         <v>212</v>
       </c>
-      <c r="AA19" s="36"/>
+      <c r="AA19" s="37"/>
     </row>
     <row r="20">
-      <c r="A20" s="94"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="83"/>
-      <c r="N20" s="83"/>
-      <c r="O20" s="83"/>
-      <c r="P20" s="83"/>
-      <c r="Q20" s="83"/>
-      <c r="R20" s="83"/>
-      <c r="S20" s="83"/>
-      <c r="T20" s="83"/>
-      <c r="U20" s="83"/>
-      <c r="V20" s="83"/>
-      <c r="W20" s="83"/>
-      <c r="X20" s="83"/>
-      <c r="Y20" s="83"/>
-      <c r="Z20" s="83"/>
-      <c r="AA20" s="36"/>
+      <c r="A20" s="98"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="87"/>
+      <c r="N20" s="87"/>
+      <c r="O20" s="87"/>
+      <c r="P20" s="87"/>
+      <c r="Q20" s="87"/>
+      <c r="R20" s="87"/>
+      <c r="S20" s="87"/>
+      <c r="T20" s="87"/>
+      <c r="U20" s="87"/>
+      <c r="V20" s="87"/>
+      <c r="W20" s="87"/>
+      <c r="X20" s="87"/>
+      <c r="Y20" s="87"/>
+      <c r="Z20" s="87"/>
+      <c r="AA20" s="37"/>
     </row>
     <row r="21">
-      <c r="A21" s="75"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="75"/>
-      <c r="N21" s="75"/>
-      <c r="O21" s="75"/>
-      <c r="P21" s="75"/>
-      <c r="Q21" s="75"/>
-      <c r="R21" s="75"/>
-      <c r="S21" s="75"/>
-      <c r="T21" s="75"/>
-      <c r="U21" s="75"/>
-      <c r="V21" s="75"/>
-      <c r="W21" s="75"/>
-      <c r="X21" s="75"/>
-      <c r="Y21" s="75"/>
-      <c r="Z21" s="75"/>
-      <c r="AA21" s="36"/>
+      <c r="A21" s="79"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="79"/>
+      <c r="P21" s="79"/>
+      <c r="Q21" s="79"/>
+      <c r="R21" s="79"/>
+      <c r="S21" s="79"/>
+      <c r="T21" s="79"/>
+      <c r="U21" s="79"/>
+      <c r="V21" s="79"/>
+      <c r="W21" s="79"/>
+      <c r="X21" s="79"/>
+      <c r="Y21" s="79"/>
+      <c r="Z21" s="79"/>
+      <c r="AA21" s="37"/>
     </row>
     <row r="22">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="96">
+      <c r="B22" s="100">
         <v>10.0</v>
       </c>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="97" t="s">
+      <c r="C22" s="79"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="101" t="s">
         <v>51</v>
       </c>
       <c r="G22" s="4"/>
@@ -5435,28 +5489,28 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="75"/>
-      <c r="N22" s="75"/>
-      <c r="O22" s="75"/>
-      <c r="P22" s="75"/>
-      <c r="Q22" s="75"/>
-      <c r="R22" s="75"/>
-      <c r="S22" s="75"/>
-      <c r="T22" s="75"/>
-      <c r="U22" s="75"/>
-      <c r="V22" s="75"/>
-      <c r="W22" s="75"/>
-      <c r="X22" s="75"/>
-      <c r="Y22" s="75"/>
-      <c r="Z22" s="75"/>
-      <c r="AA22" s="36"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="79"/>
+      <c r="P22" s="79"/>
+      <c r="Q22" s="79"/>
+      <c r="R22" s="79"/>
+      <c r="S22" s="79"/>
+      <c r="T22" s="79"/>
+      <c r="U22" s="79"/>
+      <c r="V22" s="79"/>
+      <c r="W22" s="79"/>
+      <c r="X22" s="79"/>
+      <c r="Y22" s="79"/>
+      <c r="Z22" s="79"/>
+      <c r="AA22" s="37"/>
     </row>
     <row r="23">
-      <c r="A23" s="75"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
+      <c r="A23" s="79"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
       <c r="F23" s="6"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
@@ -5464,181 +5518,181 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="75"/>
-      <c r="O23" s="75"/>
-      <c r="P23" s="75"/>
-      <c r="Q23" s="75"/>
-      <c r="R23" s="75"/>
-      <c r="S23" s="75"/>
-      <c r="T23" s="75"/>
-      <c r="U23" s="75"/>
-      <c r="V23" s="75"/>
-      <c r="W23" s="75"/>
-      <c r="X23" s="75"/>
-      <c r="Y23" s="75"/>
-      <c r="Z23" s="75"/>
-      <c r="AA23" s="36"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="79"/>
+      <c r="P23" s="79"/>
+      <c r="Q23" s="79"/>
+      <c r="R23" s="79"/>
+      <c r="S23" s="79"/>
+      <c r="T23" s="79"/>
+      <c r="U23" s="79"/>
+      <c r="V23" s="79"/>
+      <c r="W23" s="79"/>
+      <c r="X23" s="79"/>
+      <c r="Y23" s="79"/>
+      <c r="Z23" s="79"/>
+      <c r="AA23" s="37"/>
     </row>
     <row r="24">
-      <c r="A24" s="75"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="75"/>
-      <c r="O24" s="75"/>
-      <c r="P24" s="75"/>
-      <c r="Q24" s="75"/>
-      <c r="R24" s="75"/>
-      <c r="S24" s="75"/>
-      <c r="T24" s="75"/>
-      <c r="U24" s="75"/>
-      <c r="V24" s="75"/>
-      <c r="W24" s="75"/>
-      <c r="X24" s="75"/>
-      <c r="Y24" s="75"/>
-      <c r="Z24" s="75"/>
-      <c r="AA24" s="36"/>
+      <c r="A24" s="79"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="79"/>
+      <c r="S24" s="79"/>
+      <c r="T24" s="79"/>
+      <c r="U24" s="79"/>
+      <c r="V24" s="79"/>
+      <c r="W24" s="79"/>
+      <c r="X24" s="79"/>
+      <c r="Y24" s="79"/>
+      <c r="Z24" s="79"/>
+      <c r="AA24" s="37"/>
     </row>
     <row r="25">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="98" t="s">
+      <c r="A25" s="79"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="62"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="99">
+      <c r="G25" s="66"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="87"/>
+      <c r="J25" s="103">
         <v>60.0</v>
       </c>
-      <c r="K25" s="62"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="75"/>
-      <c r="N25" s="75"/>
-      <c r="O25" s="75"/>
-      <c r="P25" s="75"/>
-      <c r="Q25" s="75"/>
-      <c r="R25" s="75"/>
-      <c r="S25" s="75"/>
-      <c r="T25" s="75"/>
-      <c r="U25" s="75"/>
-      <c r="V25" s="75"/>
-      <c r="W25" s="75"/>
-      <c r="X25" s="75"/>
-      <c r="Y25" s="75"/>
-      <c r="Z25" s="75"/>
-      <c r="AA25" s="36"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="79"/>
+      <c r="P25" s="79"/>
+      <c r="Q25" s="79"/>
+      <c r="R25" s="79"/>
+      <c r="S25" s="79"/>
+      <c r="T25" s="79"/>
+      <c r="U25" s="79"/>
+      <c r="V25" s="79"/>
+      <c r="W25" s="79"/>
+      <c r="X25" s="79"/>
+      <c r="Y25" s="79"/>
+      <c r="Z25" s="79"/>
+      <c r="AA25" s="37"/>
     </row>
     <row r="26">
-      <c r="A26" s="75"/>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="98" t="s">
+      <c r="A26" s="79"/>
+      <c r="B26" s="79"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="62"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="83"/>
-      <c r="J26" s="99">
+      <c r="G26" s="66"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="87"/>
+      <c r="J26" s="103">
         <v>45.0</v>
       </c>
-      <c r="K26" s="62"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="75"/>
-      <c r="N26" s="75"/>
-      <c r="O26" s="75"/>
-      <c r="P26" s="75"/>
-      <c r="Q26" s="75"/>
-      <c r="R26" s="75"/>
-      <c r="S26" s="75"/>
-      <c r="T26" s="75"/>
-      <c r="U26" s="75"/>
-      <c r="V26" s="75"/>
-      <c r="W26" s="75"/>
-      <c r="X26" s="75"/>
-      <c r="Y26" s="75"/>
-      <c r="Z26" s="75"/>
-      <c r="AA26" s="36"/>
+      <c r="K26" s="66"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="79"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="79"/>
+      <c r="P26" s="79"/>
+      <c r="Q26" s="79"/>
+      <c r="R26" s="79"/>
+      <c r="S26" s="79"/>
+      <c r="T26" s="79"/>
+      <c r="U26" s="79"/>
+      <c r="V26" s="79"/>
+      <c r="W26" s="79"/>
+      <c r="X26" s="79"/>
+      <c r="Y26" s="79"/>
+      <c r="Z26" s="79"/>
+      <c r="AA26" s="37"/>
     </row>
     <row r="27">
-      <c r="A27" s="75"/>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="98" t="s">
+      <c r="A27" s="79"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="62"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="83"/>
-      <c r="J27" s="99">
+      <c r="G27" s="66"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="103">
         <v>25.0</v>
       </c>
-      <c r="K27" s="62"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="75"/>
-      <c r="N27" s="75"/>
-      <c r="O27" s="75"/>
-      <c r="P27" s="75"/>
-      <c r="Q27" s="75"/>
-      <c r="R27" s="75"/>
-      <c r="S27" s="75"/>
-      <c r="T27" s="75"/>
-      <c r="U27" s="75"/>
-      <c r="V27" s="75"/>
-      <c r="W27" s="75"/>
-      <c r="X27" s="75"/>
-      <c r="Y27" s="75"/>
-      <c r="Z27" s="75"/>
-      <c r="AA27" s="36"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="79"/>
+      <c r="N27" s="79"/>
+      <c r="O27" s="79"/>
+      <c r="P27" s="79"/>
+      <c r="Q27" s="79"/>
+      <c r="R27" s="79"/>
+      <c r="S27" s="79"/>
+      <c r="T27" s="79"/>
+      <c r="U27" s="79"/>
+      <c r="V27" s="79"/>
+      <c r="W27" s="79"/>
+      <c r="X27" s="79"/>
+      <c r="Y27" s="79"/>
+      <c r="Z27" s="79"/>
+      <c r="AA27" s="37"/>
     </row>
     <row r="28">
-      <c r="A28" s="75"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="100">
+      <c r="A28" s="79"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="104">
         <f>SUM(J25:L27)</f>
         <v>130</v>
       </c>
       <c r="K28" s="23"/>
       <c r="L28" s="23"/>
-      <c r="M28" s="75"/>
-      <c r="N28" s="75"/>
-      <c r="O28" s="75"/>
-      <c r="P28" s="75"/>
-      <c r="Q28" s="75"/>
-      <c r="R28" s="75"/>
-      <c r="S28" s="75"/>
-      <c r="T28" s="75"/>
-      <c r="U28" s="75"/>
-      <c r="V28" s="75"/>
-      <c r="W28" s="75"/>
-      <c r="X28" s="75"/>
-      <c r="Y28" s="75"/>
-      <c r="Z28" s="75"/>
-      <c r="AA28" s="75"/>
+      <c r="M28" s="79"/>
+      <c r="N28" s="79"/>
+      <c r="O28" s="79"/>
+      <c r="P28" s="79"/>
+      <c r="Q28" s="79"/>
+      <c r="R28" s="79"/>
+      <c r="S28" s="79"/>
+      <c r="T28" s="79"/>
+      <c r="U28" s="79"/>
+      <c r="V28" s="79"/>
+      <c r="W28" s="79"/>
+      <c r="X28" s="79"/>
+      <c r="Y28" s="79"/>
+      <c r="Z28" s="79"/>
+      <c r="AA28" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5671,272 +5725,272 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="101" t="s">
+      <c r="C1" s="105" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="105" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="102">
+      <c r="B2" s="106">
         <v>11.0</v>
       </c>
-      <c r="C2" s="103">
+      <c r="C2" s="107">
         <v>11.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="102">
+      <c r="B3" s="106">
         <v>4.0</v>
       </c>
-      <c r="C3" s="104"/>
+      <c r="C3" s="108"/>
     </row>
     <row r="4">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="105">
+      <c r="B4" s="109">
         <v>10.0</v>
       </c>
-      <c r="C4" s="104"/>
+      <c r="C4" s="108"/>
     </row>
     <row r="5">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="105">
+      <c r="B5" s="109">
         <v>5.0</v>
       </c>
-      <c r="C5" s="104"/>
+      <c r="C5" s="108"/>
     </row>
     <row r="6">
-      <c r="A6" s="101" t="s">
+      <c r="A6" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="105">
+      <c r="B6" s="109">
         <v>18.0</v>
       </c>
-      <c r="C6" s="104">
+      <c r="C6" s="108">
         <v>18.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="102">
+      <c r="B7" s="106">
         <v>12.0</v>
       </c>
-      <c r="C7" s="103">
+      <c r="C7" s="107">
         <v>12.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="101" t="s">
+      <c r="A8" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="105">
+      <c r="B8" s="109">
         <v>-1.0</v>
       </c>
-      <c r="C8" s="104"/>
+      <c r="C8" s="108"/>
     </row>
     <row r="9">
-      <c r="A9" s="101" t="s">
+      <c r="A9" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="105">
+      <c r="B9" s="109">
         <v>12.0</v>
       </c>
-      <c r="C9" s="104"/>
+      <c r="C9" s="108"/>
     </row>
     <row r="10">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="102">
+      <c r="B10" s="106">
         <v>7.0</v>
       </c>
-      <c r="C10" s="104"/>
+      <c r="C10" s="108"/>
     </row>
     <row r="11">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="105">
+      <c r="B11" s="109">
         <v>16.0</v>
       </c>
-      <c r="C11" s="104"/>
+      <c r="C11" s="108"/>
     </row>
     <row r="12">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="102">
+      <c r="B12" s="106">
         <v>6.0</v>
       </c>
-      <c r="C12" s="103">
+      <c r="C12" s="107">
         <v>6.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="101" t="s">
+      <c r="A13" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="102">
+      <c r="B13" s="106">
         <v>10.0</v>
       </c>
-      <c r="C13" s="103">
+      <c r="C13" s="107">
         <v>10.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="101" t="s">
+      <c r="A14" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="102">
+      <c r="B14" s="106">
         <v>14.0</v>
       </c>
-      <c r="C14" s="104"/>
+      <c r="C14" s="108"/>
     </row>
     <row r="15">
-      <c r="A15" s="101" t="s">
+      <c r="A15" s="105" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="102">
+      <c r="B15" s="106">
         <v>19.0</v>
       </c>
-      <c r="C15" s="104"/>
+      <c r="C15" s="108"/>
     </row>
     <row r="16">
-      <c r="A16" s="101" t="s">
+      <c r="A16" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="102">
+      <c r="B16" s="106">
         <v>12.0</v>
       </c>
-      <c r="C16" s="103">
+      <c r="C16" s="107">
         <v>12.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="102">
+      <c r="B17" s="106">
         <v>27.0</v>
       </c>
-      <c r="C17" s="103">
+      <c r="C17" s="107">
         <v>27.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="101" t="s">
+      <c r="A18" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="102">
+      <c r="B18" s="106">
         <v>12.0</v>
       </c>
-      <c r="C18" s="104"/>
+      <c r="C18" s="108"/>
     </row>
     <row r="19">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="105">
+      <c r="B19" s="109">
         <v>7.0</v>
       </c>
-      <c r="C19" s="104"/>
+      <c r="C19" s="108"/>
     </row>
     <row r="20">
-      <c r="A20" s="101" t="s">
+      <c r="A20" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="102">
+      <c r="B20" s="106">
         <v>6.0</v>
       </c>
-      <c r="C20" s="103">
+      <c r="C20" s="107">
         <v>6.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="101" t="s">
+      <c r="A21" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="105">
+      <c r="B21" s="109">
         <v>7.0</v>
       </c>
-      <c r="C21" s="104"/>
+      <c r="C21" s="108"/>
     </row>
     <row r="22">
-      <c r="A22" s="101" t="s">
+      <c r="A22" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="105"/>
-      <c r="C22" s="104">
+      <c r="B22" s="109"/>
+      <c r="C22" s="108">
         <v>13.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="101" t="s">
+      <c r="A23" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="105"/>
-      <c r="C23" s="104">
+      <c r="B23" s="109"/>
+      <c r="C23" s="108">
         <v>12.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="101" t="s">
+      <c r="A24" s="105" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="105"/>
-      <c r="C24" s="103">
+      <c r="B24" s="109"/>
+      <c r="C24" s="107">
         <v>11.0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="101" t="s">
+      <c r="A25" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="105"/>
-      <c r="C25" s="103">
+      <c r="B25" s="109"/>
+      <c r="C25" s="107">
         <v>26.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="101" t="s">
+      <c r="A26" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="105"/>
-      <c r="C26" s="104">
+      <c r="B26" s="109"/>
+      <c r="C26" s="108">
         <v>24.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="101" t="s">
+      <c r="A27" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="105"/>
-      <c r="C27" s="104">
+      <c r="B27" s="109"/>
+      <c r="C27" s="108">
         <v>29.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="101" t="s">
+      <c r="A28" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="104">
+      <c r="B28" s="109"/>
+      <c r="C28" s="108">
         <v>21.0</v>
       </c>
     </row>
@@ -5956,101 +6010,101 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="105" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="101">
+      <c r="B2" s="105">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="110" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="101">
+      <c r="B3" s="105">
         <f>COUNTIF(Sheet1!D14:AA15,"&lt;&gt;"&amp;"")</f>
         <v>16</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="110" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="101">
+      <c r="B4" s="105">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="106" t="s">
+      <c r="A5" s="110" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="101">
+      <c r="B5" s="105">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="110" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="101">
+      <c r="B6" s="105">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="110" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="101">
+      <c r="B7" s="105">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
         <v>16</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="101">
+      <c r="B8" s="105">
         <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="106" t="s">
+      <c r="A9" s="110" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="101">
+      <c r="B9" s="105">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="106" t="s">
+      <c r="A10" s="110" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="101">
+      <c r="B10" s="105">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="110" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="101">
+      <c r="B11" s="105">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
039 Week 23/24 data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -852,9 +852,6 @@
     <xf borderId="21" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="21" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="22" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -882,7 +879,7 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="20" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -890,8 +887,11 @@
     <xf borderId="20" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="21" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="27" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="19" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -912,14 +912,14 @@
     <xf borderId="20" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="21" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="26" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="31" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="31" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf borderId="32" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -1762,87 +1762,91 @@
       <c r="Z12" s="33">
         <v>35.0</v>
       </c>
-      <c r="AA12" s="34"/>
-      <c r="AB12" s="35">
+      <c r="AA12" s="33">
+        <v>29.0</v>
+      </c>
+      <c r="AB12" s="34">
         <f t="shared" ref="AB12:AB31" si="1">SUM(D12:Y12)</f>
         <v>500</v>
       </c>
-      <c r="AC12" s="36">
+      <c r="AC12" s="35">
         <f>SUM(AB12:AB13)</f>
         <v>1010</v>
       </c>
       <c r="AD12" s="5"/>
-      <c r="AE12" s="37"/>
+      <c r="AE12" s="36"/>
     </row>
     <row r="13">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41">
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40">
         <v>32.0</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41">
+      <c r="E13" s="40"/>
+      <c r="F13" s="40">
         <v>35.0</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="40">
         <v>35.0</v>
       </c>
-      <c r="H13" s="41">
+      <c r="H13" s="40">
         <v>31.0</v>
       </c>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41">
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40">
         <v>34.0</v>
       </c>
-      <c r="O13" s="41">
+      <c r="O13" s="40">
         <v>36.0</v>
       </c>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41">
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40">
         <v>32.0</v>
       </c>
-      <c r="R13" s="41">
+      <c r="R13" s="40">
         <v>36.0</v>
       </c>
-      <c r="S13" s="41">
+      <c r="S13" s="40">
         <v>35.0</v>
       </c>
-      <c r="T13" s="42">
+      <c r="T13" s="41">
         <v>34.0</v>
       </c>
-      <c r="U13" s="42">
+      <c r="U13" s="41">
         <v>34.0</v>
       </c>
-      <c r="V13" s="43">
+      <c r="V13" s="42">
         <v>41.0</v>
       </c>
-      <c r="W13" s="42">
+      <c r="W13" s="41">
         <v>28.0</v>
       </c>
-      <c r="X13" s="42">
+      <c r="X13" s="41">
         <v>31.0</v>
       </c>
-      <c r="Y13" s="43">
+      <c r="Y13" s="42">
         <v>36.0</v>
       </c>
-      <c r="Z13" s="44">
+      <c r="Z13" s="43">
         <v>39.0</v>
       </c>
-      <c r="AA13" s="45"/>
-      <c r="AB13" s="35">
+      <c r="AA13" s="44">
+        <v>35.0</v>
+      </c>
+      <c r="AB13" s="34">
         <f t="shared" si="1"/>
         <v>510</v>
       </c>
       <c r="AC13" s="6"/>
       <c r="AD13" s="8"/>
-      <c r="AE13" s="37"/>
+      <c r="AE13" s="36"/>
     </row>
     <row r="14">
       <c r="A14" s="28" t="s">
@@ -1867,7 +1871,7 @@
       <c r="L14" s="31"/>
       <c r="M14" s="31"/>
       <c r="N14" s="31"/>
-      <c r="O14" s="46">
+      <c r="O14" s="45">
         <v>38.0</v>
       </c>
       <c r="P14" s="31"/>
@@ -1875,7 +1879,7 @@
       <c r="R14" s="31"/>
       <c r="S14" s="31"/>
       <c r="T14" s="31"/>
-      <c r="U14" s="47">
+      <c r="U14" s="46">
         <v>38.0</v>
       </c>
       <c r="V14" s="31"/>
@@ -1884,76 +1888,76 @@
       </c>
       <c r="X14" s="31"/>
       <c r="Y14" s="31"/>
-      <c r="Z14" s="34"/>
-      <c r="AA14" s="34"/>
-      <c r="AB14" s="35">
+      <c r="Z14" s="47"/>
+      <c r="AA14" s="47"/>
+      <c r="AB14" s="34">
         <f t="shared" si="1"/>
         <v>203</v>
       </c>
-      <c r="AC14" s="36">
+      <c r="AC14" s="35">
         <f>SUM(AB14:AB15)</f>
         <v>535</v>
       </c>
       <c r="AD14" s="5"/>
-      <c r="AE14" s="37"/>
+      <c r="AE14" s="36"/>
     </row>
     <row r="15">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="41">
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40">
         <v>37.0</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41">
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40">
         <v>31.0</v>
       </c>
-      <c r="H15" s="41">
+      <c r="H15" s="40">
         <v>38.0</v>
       </c>
-      <c r="I15" s="41">
+      <c r="I15" s="40">
         <v>30.0</v>
       </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41">
+      <c r="J15" s="40"/>
+      <c r="K15" s="40">
         <v>36.0</v>
       </c>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41">
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40">
         <v>32.0</v>
       </c>
-      <c r="O15" s="41">
+      <c r="O15" s="40">
         <v>33.0</v>
       </c>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41">
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40">
         <v>28.0</v>
       </c>
-      <c r="S15" s="41"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="42">
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="41">
         <v>32.0</v>
       </c>
-      <c r="V15" s="42">
+      <c r="V15" s="41">
         <v>35.0</v>
       </c>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="45"/>
-      <c r="AA15" s="45"/>
-      <c r="AB15" s="35">
+      <c r="W15" s="40"/>
+      <c r="X15" s="40"/>
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="48"/>
+      <c r="AA15" s="48"/>
+      <c r="AB15" s="34">
         <f t="shared" si="1"/>
         <v>332</v>
       </c>
       <c r="AC15" s="6"/>
       <c r="AD15" s="8"/>
-      <c r="AE15" s="37"/>
+      <c r="AE15" s="36"/>
     </row>
     <row r="16">
       <c r="A16" s="28" t="s">
@@ -2018,81 +2022,85 @@
       <c r="Z16" s="33">
         <v>33.0</v>
       </c>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="35">
+      <c r="AA16" s="33">
+        <v>37.0</v>
+      </c>
+      <c r="AB16" s="34">
         <f t="shared" si="1"/>
         <v>469</v>
       </c>
-      <c r="AC16" s="36">
+      <c r="AC16" s="35">
         <f>SUM(AB16:AB17)</f>
         <v>841</v>
       </c>
       <c r="AD16" s="5"/>
-      <c r="AE16" s="37"/>
+      <c r="AE16" s="36"/>
     </row>
     <row r="17">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41">
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40">
         <v>31.0</v>
       </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41">
+      <c r="E17" s="40"/>
+      <c r="F17" s="40">
         <v>32.0</v>
       </c>
-      <c r="G17" s="41">
+      <c r="G17" s="40">
         <v>26.0</v>
       </c>
-      <c r="H17" s="41">
+      <c r="H17" s="40">
         <v>32.0</v>
       </c>
-      <c r="I17" s="41">
+      <c r="I17" s="40">
         <v>34.0</v>
       </c>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41">
+      <c r="J17" s="40"/>
+      <c r="K17" s="40">
         <v>31.0</v>
       </c>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41">
+      <c r="L17" s="40"/>
+      <c r="M17" s="40">
         <v>25.0</v>
       </c>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41">
+      <c r="N17" s="40"/>
+      <c r="O17" s="40">
         <v>35.0</v>
       </c>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
-      <c r="S17" s="41">
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40">
         <v>23.0</v>
       </c>
-      <c r="T17" s="43">
+      <c r="T17" s="42">
         <v>39.0</v>
       </c>
-      <c r="U17" s="41"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="42">
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="41">
         <v>34.0</v>
       </c>
-      <c r="X17" s="41"/>
-      <c r="Y17" s="42">
+      <c r="X17" s="40"/>
+      <c r="Y17" s="41">
         <v>30.0</v>
       </c>
-      <c r="Z17" s="48">
+      <c r="Z17" s="44">
         <v>29.0</v>
       </c>
-      <c r="AA17" s="45"/>
-      <c r="AB17" s="35">
+      <c r="AA17" s="44">
+        <v>33.0</v>
+      </c>
+      <c r="AB17" s="34">
         <f t="shared" si="1"/>
         <v>372</v>
       </c>
       <c r="AC17" s="6"/>
       <c r="AD17" s="8"/>
-      <c r="AE17" s="37"/>
+      <c r="AE17" s="36"/>
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
@@ -2151,63 +2159,65 @@
       <c r="Z18" s="33">
         <v>36.0</v>
       </c>
-      <c r="AA18" s="34"/>
-      <c r="AB18" s="35">
+      <c r="AA18" s="47"/>
+      <c r="AB18" s="34">
         <f t="shared" si="1"/>
         <v>410</v>
       </c>
-      <c r="AC18" s="36">
+      <c r="AC18" s="35">
         <f>SUM(AB18:AB19)</f>
         <v>499</v>
       </c>
       <c r="AD18" s="5"/>
-      <c r="AE18" s="37"/>
+      <c r="AE18" s="36"/>
     </row>
     <row r="19">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41">
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40">
         <v>28.0</v>
       </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41">
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40">
         <v>33.0</v>
       </c>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="41"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="41"/>
-      <c r="U19" s="41"/>
-      <c r="V19" s="41"/>
-      <c r="W19" s="41"/>
-      <c r="X19" s="41"/>
-      <c r="Y19" s="42">
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="40"/>
+      <c r="W19" s="40"/>
+      <c r="X19" s="40"/>
+      <c r="Y19" s="41">
         <v>28.0</v>
       </c>
-      <c r="Z19" s="48">
+      <c r="Z19" s="44">
         <v>24.0</v>
       </c>
-      <c r="AA19" s="45"/>
-      <c r="AB19" s="35">
+      <c r="AA19" s="44">
+        <v>35.0</v>
+      </c>
+      <c r="AB19" s="34">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="AC19" s="6"/>
       <c r="AD19" s="8"/>
-      <c r="AE19" s="37"/>
+      <c r="AE19" s="36"/>
     </row>
     <row r="20">
       <c r="A20" s="28" t="s">
@@ -2272,87 +2282,91 @@
       <c r="Z20" s="33">
         <v>28.0</v>
       </c>
-      <c r="AA20" s="34"/>
-      <c r="AB20" s="35">
+      <c r="AA20" s="33">
+        <v>36.0</v>
+      </c>
+      <c r="AB20" s="34">
         <f t="shared" si="1"/>
         <v>531</v>
       </c>
-      <c r="AC20" s="36">
+      <c r="AC20" s="35">
         <f>SUM(AB20:AB21)</f>
         <v>1022</v>
       </c>
       <c r="AD20" s="5"/>
-      <c r="AE20" s="37"/>
+      <c r="AE20" s="36"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="39"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="51"/>
       <c r="D21" s="52">
         <v>36.0</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="40">
         <v>39.0</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F21" s="40">
         <v>33.0</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G21" s="40">
         <v>29.0</v>
       </c>
-      <c r="H21" s="41">
+      <c r="H21" s="40">
         <v>32.0</v>
       </c>
-      <c r="I21" s="41">
+      <c r="I21" s="40">
         <v>31.0</v>
       </c>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41">
+      <c r="J21" s="40"/>
+      <c r="K21" s="40">
         <v>42.0</v>
       </c>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41">
+      <c r="L21" s="40"/>
+      <c r="M21" s="40">
         <v>31.0</v>
       </c>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41">
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40">
         <v>28.0</v>
       </c>
-      <c r="R21" s="41">
+      <c r="R21" s="40">
         <v>26.0</v>
       </c>
-      <c r="S21" s="41"/>
-      <c r="T21" s="41"/>
-      <c r="U21" s="42">
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="41">
         <v>30.0</v>
       </c>
-      <c r="V21" s="42">
+      <c r="V21" s="41">
         <v>30.0</v>
       </c>
-      <c r="W21" s="42">
+      <c r="W21" s="41">
         <v>36.0</v>
       </c>
-      <c r="X21" s="42">
+      <c r="X21" s="41">
         <v>33.0</v>
       </c>
-      <c r="Y21" s="42">
+      <c r="Y21" s="41">
         <v>35.0</v>
       </c>
-      <c r="Z21" s="48">
+      <c r="Z21" s="44">
         <v>38.0</v>
       </c>
-      <c r="AA21" s="45"/>
-      <c r="AB21" s="35">
+      <c r="AA21" s="44">
+        <v>32.0</v>
+      </c>
+      <c r="AB21" s="34">
         <f t="shared" si="1"/>
         <v>491</v>
       </c>
       <c r="AC21" s="6"/>
       <c r="AD21" s="8"/>
-      <c r="AE21" s="37"/>
+      <c r="AE21" s="36"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="53" t="s">
@@ -2400,18 +2414,20 @@
         <v>32.0</v>
       </c>
       <c r="Y22" s="31"/>
-      <c r="Z22" s="34"/>
-      <c r="AA22" s="34"/>
-      <c r="AB22" s="35">
+      <c r="Z22" s="47"/>
+      <c r="AA22" s="33">
+        <v>34.0</v>
+      </c>
+      <c r="AB22" s="34">
         <f t="shared" si="1"/>
         <v>277</v>
       </c>
-      <c r="AC22" s="36">
+      <c r="AC22" s="35">
         <f>SUM(AB22:AB23)</f>
         <v>481</v>
       </c>
       <c r="AD22" s="5"/>
-      <c r="AE22" s="37"/>
+      <c r="AE22" s="36"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="55" t="s">
@@ -2419,51 +2435,53 @@
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="56"/>
-      <c r="D23" s="41">
+      <c r="D23" s="40">
         <v>25.0</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41">
+      <c r="E23" s="40"/>
+      <c r="F23" s="40">
         <v>30.0</v>
       </c>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41">
+      <c r="G23" s="40"/>
+      <c r="H23" s="40">
         <v>28.0</v>
       </c>
-      <c r="I23" s="41">
+      <c r="I23" s="40">
         <v>27.0</v>
       </c>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41">
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40">
         <v>34.0</v>
       </c>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="41"/>
-      <c r="T23" s="42">
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="41">
         <v>26.0</v>
       </c>
-      <c r="U23" s="41"/>
-      <c r="V23" s="41"/>
-      <c r="W23" s="42">
+      <c r="U23" s="40"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="41">
         <v>34.0</v>
       </c>
-      <c r="X23" s="41"/>
-      <c r="Y23" s="41"/>
-      <c r="Z23" s="45"/>
-      <c r="AA23" s="45"/>
-      <c r="AB23" s="35">
+      <c r="X23" s="40"/>
+      <c r="Y23" s="40"/>
+      <c r="Z23" s="48"/>
+      <c r="AA23" s="44">
+        <v>37.0</v>
+      </c>
+      <c r="AB23" s="34">
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
       <c r="AC23" s="6"/>
       <c r="AD23" s="8"/>
-      <c r="AE23" s="37"/>
+      <c r="AE23" s="36"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="28" t="s">
@@ -2507,84 +2525,88 @@
       </c>
       <c r="X24" s="31"/>
       <c r="Y24" s="31"/>
-      <c r="Z24" s="34"/>
-      <c r="AA24" s="34"/>
-      <c r="AB24" s="35">
+      <c r="Z24" s="47"/>
+      <c r="AA24" s="58">
+        <v>39.0</v>
+      </c>
+      <c r="AB24" s="34">
         <f t="shared" si="1"/>
         <v>231</v>
       </c>
-      <c r="AC24" s="36">
+      <c r="AC24" s="35">
         <f>SUM(AB24:AB25)</f>
         <v>635</v>
       </c>
       <c r="AD24" s="5"/>
-      <c r="AE24" s="37"/>
+      <c r="AE24" s="36"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="41">
+      <c r="B25" s="38"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40">
         <v>36.0</v>
       </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41">
+      <c r="E25" s="40"/>
+      <c r="F25" s="40">
         <v>33.0</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="40">
         <v>33.0</v>
       </c>
-      <c r="H25" s="41">
+      <c r="H25" s="40">
         <v>34.0</v>
       </c>
-      <c r="I25" s="41">
+      <c r="I25" s="40">
         <v>26.0</v>
       </c>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41">
+      <c r="J25" s="40"/>
+      <c r="K25" s="40">
         <v>31.0</v>
       </c>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41">
+      <c r="L25" s="40"/>
+      <c r="M25" s="40">
         <v>28.0</v>
       </c>
-      <c r="N25" s="41">
+      <c r="N25" s="40">
         <v>27.0</v>
       </c>
-      <c r="O25" s="41">
+      <c r="O25" s="40">
         <v>32.0</v>
       </c>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="41"/>
-      <c r="S25" s="41"/>
-      <c r="T25" s="42">
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="41">
         <v>26.0</v>
       </c>
-      <c r="U25" s="42">
+      <c r="U25" s="41">
         <v>35.0</v>
       </c>
-      <c r="V25" s="42">
+      <c r="V25" s="41">
         <v>33.0</v>
       </c>
-      <c r="W25" s="42">
+      <c r="W25" s="41">
         <v>30.0</v>
       </c>
-      <c r="X25" s="41"/>
-      <c r="Y25" s="41"/>
-      <c r="Z25" s="48">
+      <c r="X25" s="40"/>
+      <c r="Y25" s="40"/>
+      <c r="Z25" s="44">
         <v>26.0</v>
       </c>
-      <c r="AA25" s="45"/>
-      <c r="AB25" s="35">
+      <c r="AA25" s="44">
+        <v>36.0</v>
+      </c>
+      <c r="AB25" s="34">
         <f t="shared" si="1"/>
         <v>404</v>
       </c>
       <c r="AC25" s="6"/>
       <c r="AD25" s="8"/>
-      <c r="AE25" s="37"/>
+      <c r="AE25" s="36"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="28" t="s">
@@ -2648,86 +2670,90 @@
         <v>35.0</v>
       </c>
       <c r="Y26" s="31"/>
-      <c r="Z26" s="34"/>
-      <c r="AA26" s="34"/>
-      <c r="AB26" s="35">
+      <c r="Z26" s="47"/>
+      <c r="AA26" s="33">
+        <v>35.0</v>
+      </c>
+      <c r="AB26" s="34">
         <f t="shared" si="1"/>
         <v>545</v>
       </c>
-      <c r="AC26" s="36">
+      <c r="AC26" s="35">
         <f>SUM(AB26:AB27)</f>
         <v>959</v>
       </c>
       <c r="AD26" s="5"/>
-      <c r="AE26" s="37"/>
+      <c r="AE26" s="36"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="41">
+      <c r="B27" s="38"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40">
         <v>42.0</v>
       </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41">
+      <c r="E27" s="40"/>
+      <c r="F27" s="40">
         <v>29.0</v>
       </c>
-      <c r="G27" s="41">
+      <c r="G27" s="40">
         <v>40.0</v>
       </c>
-      <c r="H27" s="41">
+      <c r="H27" s="40">
         <v>28.0</v>
       </c>
-      <c r="I27" s="41">
+      <c r="I27" s="40">
         <v>21.0</v>
       </c>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41">
+      <c r="J27" s="40"/>
+      <c r="K27" s="40">
         <v>39.0</v>
       </c>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41">
+      <c r="L27" s="40"/>
+      <c r="M27" s="40">
         <v>22.0</v>
       </c>
-      <c r="N27" s="41">
+      <c r="N27" s="40">
         <v>28.0</v>
       </c>
-      <c r="O27" s="41">
+      <c r="O27" s="40">
         <v>32.0</v>
       </c>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="41">
+      <c r="P27" s="40"/>
+      <c r="Q27" s="40">
         <v>29.0</v>
       </c>
-      <c r="R27" s="41"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="42">
+      <c r="R27" s="40"/>
+      <c r="S27" s="40"/>
+      <c r="T27" s="41">
         <v>20.0</v>
       </c>
-      <c r="U27" s="41"/>
-      <c r="V27" s="42">
+      <c r="U27" s="40"/>
+      <c r="V27" s="41">
         <v>24.0</v>
       </c>
-      <c r="W27" s="41"/>
-      <c r="X27" s="42">
+      <c r="W27" s="40"/>
+      <c r="X27" s="41">
         <v>35.0</v>
       </c>
-      <c r="Y27" s="42">
+      <c r="Y27" s="41">
         <v>25.0</v>
       </c>
-      <c r="Z27" s="48">
+      <c r="Z27" s="44">
         <v>29.0</v>
       </c>
-      <c r="AA27" s="45"/>
-      <c r="AB27" s="35">
+      <c r="AA27" s="44">
+        <v>33.0</v>
+      </c>
+      <c r="AB27" s="34">
         <f t="shared" si="1"/>
         <v>414</v>
       </c>
       <c r="AC27" s="6"/>
       <c r="AD27" s="8"/>
-      <c r="AE27" s="37"/>
+      <c r="AE27" s="36"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="28" t="s">
@@ -2785,98 +2811,100 @@
         <v>32.0</v>
       </c>
       <c r="W28" s="31"/>
-      <c r="X28" s="47">
+      <c r="X28" s="46">
         <v>35.0</v>
       </c>
       <c r="Y28" s="32">
         <v>35.0</v>
       </c>
-      <c r="Z28" s="34"/>
-      <c r="AA28" s="34"/>
-      <c r="AB28" s="35">
+      <c r="Z28" s="47"/>
+      <c r="AA28" s="47"/>
+      <c r="AB28" s="34">
         <f t="shared" si="1"/>
         <v>545</v>
       </c>
-      <c r="AC28" s="36">
+      <c r="AC28" s="35">
         <f>SUM(AB28:AB29)</f>
         <v>1124</v>
       </c>
       <c r="AD28" s="5"/>
-      <c r="AE28" s="37"/>
+      <c r="AE28" s="36"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="41">
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40">
         <v>24.0</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="40">
         <v>30.0</v>
       </c>
-      <c r="F29" s="41">
+      <c r="F29" s="40">
         <v>32.0</v>
       </c>
-      <c r="G29" s="41">
+      <c r="G29" s="40">
         <v>37.0</v>
       </c>
-      <c r="H29" s="41">
+      <c r="H29" s="40">
         <v>36.0</v>
       </c>
-      <c r="I29" s="41">
+      <c r="I29" s="40">
         <v>36.0</v>
       </c>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41">
+      <c r="J29" s="40"/>
+      <c r="K29" s="40">
         <v>38.0</v>
       </c>
-      <c r="L29" s="58"/>
-      <c r="M29" s="58">
+      <c r="L29" s="59"/>
+      <c r="M29" s="59">
         <v>39.0</v>
       </c>
-      <c r="N29" s="41">
+      <c r="N29" s="40">
         <v>33.0</v>
       </c>
-      <c r="O29" s="41">
+      <c r="O29" s="40">
         <v>33.0</v>
       </c>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41">
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40">
         <v>34.0</v>
       </c>
-      <c r="R29" s="41">
+      <c r="R29" s="40">
         <v>32.0</v>
       </c>
-      <c r="S29" s="58">
+      <c r="S29" s="59">
         <v>38.0</v>
       </c>
-      <c r="T29" s="42">
+      <c r="T29" s="41">
         <v>34.0</v>
       </c>
-      <c r="U29" s="42">
+      <c r="U29" s="41">
         <v>36.0</v>
       </c>
-      <c r="V29" s="42">
+      <c r="V29" s="41">
         <v>31.0</v>
       </c>
-      <c r="W29" s="43">
+      <c r="W29" s="42">
         <v>36.0</v>
       </c>
-      <c r="X29" s="41"/>
-      <c r="Y29" s="41"/>
-      <c r="Z29" s="48">
+      <c r="X29" s="40"/>
+      <c r="Y29" s="40"/>
+      <c r="Z29" s="44">
         <v>33.0</v>
       </c>
-      <c r="AA29" s="45"/>
-      <c r="AB29" s="35">
+      <c r="AA29" s="44">
+        <v>38.0</v>
+      </c>
+      <c r="AB29" s="34">
         <f t="shared" si="1"/>
         <v>579</v>
       </c>
       <c r="AC29" s="6"/>
       <c r="AD29" s="8"/>
-      <c r="AE29" s="37"/>
+      <c r="AE29" s="36"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="28" t="s">
@@ -2923,85 +2951,89 @@
       <c r="Z30" s="33">
         <v>31.0</v>
       </c>
-      <c r="AA30" s="34"/>
-      <c r="AB30" s="35">
+      <c r="AA30" s="33">
+        <v>37.0</v>
+      </c>
+      <c r="AB30" s="34">
         <f t="shared" si="1"/>
         <v>214</v>
       </c>
-      <c r="AC30" s="36">
+      <c r="AC30" s="35">
         <f>SUM(AB30:AB31)</f>
         <v>648</v>
       </c>
       <c r="AD30" s="5"/>
-      <c r="AE30" s="37"/>
+      <c r="AE30" s="36"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="41">
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="40">
         <v>33.0</v>
       </c>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41">
+      <c r="E31" s="40"/>
+      <c r="F31" s="40">
         <v>34.0</v>
       </c>
-      <c r="G31" s="41">
+      <c r="G31" s="40">
         <v>30.0</v>
       </c>
-      <c r="H31" s="41">
+      <c r="H31" s="40">
         <v>29.0</v>
       </c>
-      <c r="I31" s="41">
+      <c r="I31" s="40">
         <v>39.0</v>
       </c>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41">
+      <c r="J31" s="40"/>
+      <c r="K31" s="40">
         <v>31.0</v>
       </c>
-      <c r="L31" s="41"/>
-      <c r="M31" s="41">
+      <c r="L31" s="40"/>
+      <c r="M31" s="40">
         <v>33.0</v>
       </c>
-      <c r="N31" s="41">
+      <c r="N31" s="40">
         <v>29.0</v>
       </c>
-      <c r="O31" s="41">
+      <c r="O31" s="40">
         <v>29.0</v>
       </c>
-      <c r="P31" s="41"/>
-      <c r="Q31" s="41">
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40">
         <v>28.0</v>
       </c>
-      <c r="R31" s="41"/>
-      <c r="S31" s="41">
+      <c r="R31" s="40"/>
+      <c r="S31" s="40">
         <v>30.0</v>
       </c>
-      <c r="T31" s="41"/>
-      <c r="U31" s="42">
+      <c r="T31" s="40"/>
+      <c r="U31" s="41">
         <v>27.0</v>
       </c>
-      <c r="V31" s="41"/>
-      <c r="W31" s="41"/>
-      <c r="X31" s="42">
+      <c r="V31" s="40"/>
+      <c r="W31" s="40"/>
+      <c r="X31" s="41">
         <v>29.0</v>
       </c>
-      <c r="Y31" s="42">
+      <c r="Y31" s="41">
         <v>33.0</v>
       </c>
-      <c r="Z31" s="59">
+      <c r="Z31" s="60">
         <v>33.0</v>
       </c>
-      <c r="AA31" s="60"/>
+      <c r="AA31" s="60">
+        <v>33.0</v>
+      </c>
       <c r="AB31" s="61">
         <f t="shared" si="1"/>
         <v>434</v>
       </c>
       <c r="AC31" s="6"/>
       <c r="AD31" s="8"/>
-      <c r="AE31" s="37"/>
+      <c r="AE31" s="36"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="62"/>
@@ -3153,14 +3185,14 @@
       <c r="F36" s="66"/>
       <c r="G36" s="66"/>
       <c r="H36" s="64"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="37"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
       <c r="M36" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="O36" s="37"/>
+      <c r="O36" s="36"/>
       <c r="P36" s="75">
         <v>50.0</v>
       </c>
@@ -3190,14 +3222,14 @@
       <c r="F37" s="66"/>
       <c r="G37" s="66"/>
       <c r="H37" s="64"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="36"/>
+      <c r="L37" s="36"/>
       <c r="M37" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="O37" s="37"/>
+      <c r="O37" s="36"/>
       <c r="P37" s="75">
         <v>30.0</v>
       </c>
@@ -4612,13 +4644,15 @@
       <c r="W5" s="92">
         <v>26.0</v>
       </c>
-      <c r="X5" s="90"/>
+      <c r="X5" s="92">
+        <v>34.0</v>
+      </c>
       <c r="Y5" s="90"/>
       <c r="Z5" s="94">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
         <v>548</v>
       </c>
-      <c r="AA5" s="37"/>
+      <c r="AA5" s="36"/>
     </row>
     <row r="6">
       <c r="A6" s="88" t="s">
@@ -4678,13 +4712,15 @@
       </c>
       <c r="V6" s="90"/>
       <c r="W6" s="90"/>
-      <c r="X6" s="90"/>
+      <c r="X6" s="92">
+        <v>34.0</v>
+      </c>
       <c r="Y6" s="90"/>
       <c r="Z6" s="94">
         <f t="shared" si="1"/>
         <v>526</v>
       </c>
-      <c r="AA6" s="37"/>
+      <c r="AA6" s="36"/>
     </row>
     <row r="7">
       <c r="A7" s="88" t="s">
@@ -4748,13 +4784,15 @@
       <c r="W7" s="92">
         <v>28.0</v>
       </c>
-      <c r="X7" s="90"/>
+      <c r="X7" s="92">
+        <v>25.0</v>
+      </c>
       <c r="Y7" s="90"/>
       <c r="Z7" s="94">
         <f t="shared" si="1"/>
         <v>541</v>
       </c>
-      <c r="AA7" s="37"/>
+      <c r="AA7" s="36"/>
     </row>
     <row r="8">
       <c r="A8" s="88" t="s">
@@ -4810,13 +4848,15 @@
       <c r="W8" s="93">
         <v>35.0</v>
       </c>
-      <c r="X8" s="90"/>
+      <c r="X8" s="92">
+        <v>32.0</v>
+      </c>
       <c r="Y8" s="90"/>
       <c r="Z8" s="94">
         <f t="shared" si="1"/>
         <v>460</v>
       </c>
-      <c r="AA8" s="37"/>
+      <c r="AA8" s="36"/>
     </row>
     <row r="9">
       <c r="A9" s="88" t="s">
@@ -4880,13 +4920,15 @@
       <c r="W9" s="92">
         <v>29.0</v>
       </c>
-      <c r="X9" s="90"/>
+      <c r="X9" s="92">
+        <v>32.0</v>
+      </c>
       <c r="Y9" s="90"/>
       <c r="Z9" s="94">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="AA9" s="37"/>
+      <c r="AA9" s="36"/>
     </row>
     <row r="10">
       <c r="A10" s="88" t="s">
@@ -4944,13 +4986,15 @@
       <c r="W10" s="92">
         <v>28.0</v>
       </c>
-      <c r="X10" s="90"/>
+      <c r="X10" s="92">
+        <v>26.0</v>
+      </c>
       <c r="Y10" s="90"/>
       <c r="Z10" s="94">
         <f t="shared" si="1"/>
         <v>376</v>
       </c>
-      <c r="AA10" s="37"/>
+      <c r="AA10" s="36"/>
     </row>
     <row r="11">
       <c r="A11" s="88" t="s">
@@ -4994,7 +5038,7 @@
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
-      <c r="AA11" s="37"/>
+      <c r="AA11" s="36"/>
     </row>
     <row r="12">
       <c r="A12" s="88" t="s">
@@ -5050,13 +5094,15 @@
       <c r="W12" s="92">
         <v>24.0</v>
       </c>
-      <c r="X12" s="90"/>
+      <c r="X12" s="92">
+        <v>32.0</v>
+      </c>
       <c r="Y12" s="90"/>
       <c r="Z12" s="94">
         <f t="shared" si="1"/>
         <v>432</v>
       </c>
-      <c r="AA12" s="37"/>
+      <c r="AA12" s="36"/>
     </row>
     <row r="13">
       <c r="A13" s="88" t="s">
@@ -5122,7 +5168,7 @@
         <f t="shared" si="1"/>
         <v>526</v>
       </c>
-      <c r="AA13" s="37"/>
+      <c r="AA13" s="36"/>
     </row>
     <row r="14">
       <c r="A14" s="88" t="s">
@@ -5172,7 +5218,7 @@
         <f t="shared" si="1"/>
         <v>246</v>
       </c>
-      <c r="AA14" s="37"/>
+      <c r="AA14" s="36"/>
     </row>
     <row r="15">
       <c r="A15" s="88" t="s">
@@ -5228,13 +5274,15 @@
       </c>
       <c r="V15" s="90"/>
       <c r="W15" s="90"/>
-      <c r="X15" s="90"/>
+      <c r="X15" s="92">
+        <v>35.0</v>
+      </c>
       <c r="Y15" s="90"/>
       <c r="Z15" s="94">
         <f t="shared" si="1"/>
         <v>423</v>
       </c>
-      <c r="AA15" s="37"/>
+      <c r="AA15" s="36"/>
     </row>
     <row r="16">
       <c r="A16" s="88" t="s">
@@ -5286,13 +5334,15 @@
       <c r="W16" s="92">
         <v>30.0</v>
       </c>
-      <c r="X16" s="90"/>
+      <c r="X16" s="93">
+        <v>40.0</v>
+      </c>
       <c r="Y16" s="90"/>
       <c r="Z16" s="94">
         <f t="shared" si="1"/>
         <v>345</v>
       </c>
-      <c r="AA16" s="37"/>
+      <c r="AA16" s="36"/>
     </row>
     <row r="17">
       <c r="A17" s="88" t="s">
@@ -5328,7 +5378,7 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="AA17" s="37"/>
+      <c r="AA17" s="36"/>
     </row>
     <row r="18">
       <c r="A18" s="88" t="s">
@@ -5364,7 +5414,7 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="AA18" s="37"/>
+      <c r="AA18" s="36"/>
     </row>
     <row r="19">
       <c r="A19" s="88" t="s">
@@ -5404,13 +5454,15 @@
       <c r="U19" s="90"/>
       <c r="V19" s="90"/>
       <c r="W19" s="90"/>
-      <c r="X19" s="90"/>
+      <c r="X19" s="92">
+        <v>34.0</v>
+      </c>
       <c r="Y19" s="90"/>
       <c r="Z19" s="94">
         <f t="shared" si="1"/>
         <v>212</v>
       </c>
-      <c r="AA19" s="37"/>
+      <c r="AA19" s="36"/>
     </row>
     <row r="20">
       <c r="A20" s="98"/>
@@ -5439,7 +5491,7 @@
       <c r="X20" s="87"/>
       <c r="Y20" s="87"/>
       <c r="Z20" s="87"/>
-      <c r="AA20" s="37"/>
+      <c r="AA20" s="36"/>
     </row>
     <row r="21">
       <c r="A21" s="79"/>
@@ -5468,7 +5520,7 @@
       <c r="X21" s="79"/>
       <c r="Y21" s="79"/>
       <c r="Z21" s="79"/>
-      <c r="AA21" s="37"/>
+      <c r="AA21" s="36"/>
     </row>
     <row r="22">
       <c r="A22" s="99" t="s">
@@ -5503,7 +5555,7 @@
       <c r="X22" s="79"/>
       <c r="Y22" s="79"/>
       <c r="Z22" s="79"/>
-      <c r="AA22" s="37"/>
+      <c r="AA22" s="36"/>
     </row>
     <row r="23">
       <c r="A23" s="79"/>
@@ -5532,7 +5584,7 @@
       <c r="X23" s="79"/>
       <c r="Y23" s="79"/>
       <c r="Z23" s="79"/>
-      <c r="AA23" s="37"/>
+      <c r="AA23" s="36"/>
     </row>
     <row r="24">
       <c r="A24" s="79"/>
@@ -5561,7 +5613,7 @@
       <c r="X24" s="79"/>
       <c r="Y24" s="79"/>
       <c r="Z24" s="79"/>
-      <c r="AA24" s="37"/>
+      <c r="AA24" s="36"/>
     </row>
     <row r="25">
       <c r="A25" s="79"/>
@@ -5594,7 +5646,7 @@
       <c r="X25" s="79"/>
       <c r="Y25" s="79"/>
       <c r="Z25" s="79"/>
-      <c r="AA25" s="37"/>
+      <c r="AA25" s="36"/>
     </row>
     <row r="26">
       <c r="A26" s="79"/>
@@ -5627,7 +5679,7 @@
       <c r="X26" s="79"/>
       <c r="Y26" s="79"/>
       <c r="Z26" s="79"/>
-      <c r="AA26" s="37"/>
+      <c r="AA26" s="36"/>
     </row>
     <row r="27">
       <c r="A27" s="79"/>
@@ -5660,7 +5712,7 @@
       <c r="X27" s="79"/>
       <c r="Y27" s="79"/>
       <c r="Z27" s="79"/>
-      <c r="AA27" s="37"/>
+      <c r="AA27" s="36"/>
     </row>
     <row r="28">
       <c r="A28" s="79"/>
@@ -5836,10 +5888,10 @@
         <v>39</v>
       </c>
       <c r="B12" s="106">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C12" s="107">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="13">
@@ -5858,7 +5910,7 @@
         <v>41</v>
       </c>
       <c r="B14" s="106">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="C14" s="108"/>
     </row>
@@ -5936,8 +5988,8 @@
         <v>61</v>
       </c>
       <c r="B22" s="109"/>
-      <c r="C22" s="108">
-        <v>13.0</v>
+      <c r="C22" s="107">
+        <v>14.0</v>
       </c>
     </row>
     <row r="23">
@@ -5955,7 +6007,7 @@
       </c>
       <c r="B24" s="109"/>
       <c r="C24" s="107">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="25">
@@ -5964,7 +6016,7 @@
       </c>
       <c r="B25" s="109"/>
       <c r="C25" s="107">
-        <v>26.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="26">
@@ -5981,8 +6033,8 @@
         <v>65</v>
       </c>
       <c r="B27" s="109"/>
-      <c r="C27" s="108">
-        <v>29.0</v>
+      <c r="C27" s="107">
+        <v>28.0</v>
       </c>
     </row>
     <row r="28">
@@ -6023,7 +6075,7 @@
       </c>
       <c r="B2" s="105">
         <f>COUNTIF(Sheet1!D12:AA13,"&lt;&gt;"&amp;"")</f>
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -6041,7 +6093,7 @@
       </c>
       <c r="B4" s="105">
         <f>COUNTIF(Sheet1!D16:AA17,"&lt;&gt;"&amp;"")</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -6050,7 +6102,7 @@
       </c>
       <c r="B5" s="105">
         <f>COUNTIF(Sheet1!D18:AA19,"&lt;&gt;"&amp;"")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
@@ -6059,7 +6111,7 @@
       </c>
       <c r="B6" s="105">
         <f>COUNTIF(Sheet1!D20:AA21,"&lt;&gt;"&amp;"")</f>
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -6068,7 +6120,7 @@
       </c>
       <c r="B7" s="105">
         <f>COUNTIF(Sheet1!D22:AA23,"&lt;&gt;"&amp;"")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -6077,7 +6129,7 @@
       </c>
       <c r="B8" s="105">
         <f>COUNTIF(Sheet1!V24:AA25,"&lt;&gt;"&amp;"")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -6086,7 +6138,7 @@
       </c>
       <c r="B9" s="105">
         <f>COUNTIF(Sheet1!D26:AA27,"&lt;&gt;"&amp;"")</f>
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
@@ -6095,7 +6147,7 @@
       </c>
       <c r="B10" s="105">
         <f>COUNTIF(Sheet1!D28:AA29,"&lt;&gt;"&amp;"")</f>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
@@ -6104,7 +6156,7 @@
       </c>
       <c r="B11" s="105">
         <f>COUNTIF(Sheet1!D30:AA31,"&lt;&gt;"&amp;"")</f>
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
040 Week 24 data update
</commit_message>
<xml_diff>
--- a/data/WINTER.xlsx
+++ b/data/WINTER.xlsx
@@ -4647,7 +4647,9 @@
       <c r="X5" s="92">
         <v>34.0</v>
       </c>
-      <c r="Y5" s="90"/>
+      <c r="Y5" s="92">
+        <v>30.0</v>
+      </c>
       <c r="Z5" s="94">
         <f t="shared" ref="Z5:Z19" si="1">SUM(B5:W5)</f>
         <v>548</v>
@@ -4715,7 +4717,9 @@
       <c r="X6" s="92">
         <v>34.0</v>
       </c>
-      <c r="Y6" s="90"/>
+      <c r="Y6" s="93">
+        <v>37.0</v>
+      </c>
       <c r="Z6" s="94">
         <f t="shared" si="1"/>
         <v>526</v>
@@ -4787,7 +4791,9 @@
       <c r="X7" s="92">
         <v>25.0</v>
       </c>
-      <c r="Y7" s="90"/>
+      <c r="Y7" s="92">
+        <v>35.0</v>
+      </c>
       <c r="Z7" s="94">
         <f t="shared" si="1"/>
         <v>541</v>
@@ -4923,7 +4929,9 @@
       <c r="X9" s="92">
         <v>32.0</v>
       </c>
-      <c r="Y9" s="90"/>
+      <c r="Y9" s="92">
+        <v>35.0</v>
+      </c>
       <c r="Z9" s="94">
         <f t="shared" si="1"/>
         <v>500</v>
@@ -4989,7 +4997,9 @@
       <c r="X10" s="92">
         <v>26.0</v>
       </c>
-      <c r="Y10" s="90"/>
+      <c r="Y10" s="92">
+        <v>30.0</v>
+      </c>
       <c r="Z10" s="94">
         <f t="shared" si="1"/>
         <v>376</v>
@@ -5277,7 +5287,9 @@
       <c r="X15" s="92">
         <v>35.0</v>
       </c>
-      <c r="Y15" s="90"/>
+      <c r="Y15" s="92">
+        <v>30.0</v>
+      </c>
       <c r="Z15" s="94">
         <f t="shared" si="1"/>
         <v>423</v>
@@ -5457,7 +5469,9 @@
       <c r="X19" s="92">
         <v>34.0</v>
       </c>
-      <c r="Y19" s="90"/>
+      <c r="Y19" s="92">
+        <v>30.0</v>
+      </c>
       <c r="Z19" s="94">
         <f t="shared" si="1"/>
         <v>212</v>
@@ -5792,10 +5806,10 @@
         <v>29</v>
       </c>
       <c r="B2" s="106">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="C2" s="107">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="3">
@@ -5939,10 +5953,10 @@
         <v>44</v>
       </c>
       <c r="B17" s="106">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="C17" s="107">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="18">

</xml_diff>